<commit_message>
Last Update 16-10-2018  1:02:26.19
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -18,7 +18,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Marks'!$C$1:$C$56</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1713,11 +1712,42 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1725,17 +1755,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1758,25 +1782,70 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1806,84 +1875,14 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2207,7 +2206,7 @@
   <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -2220,29 +2219,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="18.75">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="57" t="s">
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -2267,41 +2266,41 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:33" ht="19.5">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="70"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="78"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="57" t="s">
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="58" t="s">
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="81"/>
+      <c r="V2" s="81"/>
+      <c r="W2" s="81"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -2314,41 +2313,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:33" ht="18.75">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="73"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="65"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="57" t="s">
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="58" t="s">
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="58"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="81"/>
+      <c r="R3" s="81"/>
+      <c r="S3" s="81"/>
+      <c r="T3" s="81"/>
+      <c r="U3" s="81"/>
+      <c r="V3" s="81"/>
+      <c r="W3" s="81"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -2361,49 +2360,49 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:33" ht="18.75">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="106">
+      <c r="B4" s="60"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66">
         <v>43344</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
-      <c r="J4" s="107"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="107"/>
-      <c r="M4" s="107"/>
-      <c r="N4" s="107"/>
-      <c r="O4" s="107"/>
-      <c r="P4" s="107"/>
-      <c r="Q4" s="107"/>
-      <c r="R4" s="107"/>
-      <c r="S4" s="107"/>
-      <c r="T4" s="107"/>
-      <c r="U4" s="107"/>
-      <c r="V4" s="107"/>
-      <c r="W4" s="108"/>
-      <c r="X4" s="109"/>
-      <c r="Y4" s="109"/>
-      <c r="Z4" s="109"/>
-      <c r="AA4" s="109"/>
-      <c r="AB4" s="109"/>
-      <c r="AC4" s="109"/>
-      <c r="AD4" s="109"/>
-      <c r="AE4" s="109"/>
-      <c r="AF4" s="109"/>
-      <c r="AG4" s="109"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="68"/>
+      <c r="X4" s="57"/>
+      <c r="Y4" s="57"/>
+      <c r="Z4" s="57"/>
+      <c r="AA4" s="57"/>
+      <c r="AB4" s="57"/>
+      <c r="AC4" s="57"/>
+      <c r="AD4" s="57"/>
+      <c r="AE4" s="57"/>
+      <c r="AF4" s="57"/>
+      <c r="AG4" s="57"/>
     </row>
     <row r="5" spans="1:33">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="79" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="73" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -2497,8 +2496,8 @@
       <c r="AG5" s="12"/>
     </row>
     <row r="6" spans="1:33">
-      <c r="A6" s="64"/>
-      <c r="B6" s="66"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -2593,7 +2592,7 @@
       <c r="A7" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="67"/>
+      <c r="B7" s="75"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -3923,7 +3922,7 @@
       <c r="A21" s="3">
         <v>14</v>
       </c>
-      <c r="B21" s="112" t="s">
+      <c r="B21" s="58" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="6"/>
@@ -7245,10 +7244,10 @@
       <c r="AG55" s="12"/>
     </row>
     <row r="56" spans="1:33">
-      <c r="A56" s="62" t="s">
+      <c r="A56" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="63"/>
+      <c r="B56" s="72"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -7372,10 +7371,10 @@
       </c>
     </row>
     <row r="57" spans="1:33">
-      <c r="A57" s="59" t="s">
+      <c r="A57" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="60"/>
+      <c r="B57" s="70"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -7500,11 +7499,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:W4"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="A56:B56"/>
@@ -7512,6 +7506,11 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:W4"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
@@ -7519,7 +7518,7 @@
     <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -7544,72 +7543,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="96" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="96"/>
-      <c r="E1" s="58" t="s">
+      <c r="D1" s="89"/>
+      <c r="E1" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="96" t="s">
+      <c r="B2" s="87"/>
+      <c r="C2" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="58" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="99"/>
-      <c r="C3" s="96" t="s">
+      <c r="B3" s="88"/>
+      <c r="C3" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="96"/>
-      <c r="E3" s="58" t="s">
+      <c r="D3" s="89"/>
+      <c r="E3" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="83" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="94"/>
-      <c r="B5" s="66"/>
+      <c r="A5" s="84"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -7630,8 +7629,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="95"/>
-      <c r="B6" s="67"/>
+      <c r="A6" s="85"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -8554,10 +8553,10 @@
       <c r="H54" s="42"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="62" t="s">
+      <c r="A55" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="63"/>
+      <c r="B55" s="72"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -8571,10 +8570,10 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="59" t="s">
+      <c r="A56" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="60"/>
+      <c r="B56" s="70"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -8588,10 +8587,10 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="59" t="s">
+      <c r="A57" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="60"/>
+      <c r="B57" s="70"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -8605,10 +8604,10 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="59" t="s">
+      <c r="A58" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="60"/>
+      <c r="B58" s="70"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -8623,13 +8622,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -8639,6 +8631,13 @@
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:H54">
     <cfRule type="cellIs" dxfId="1" priority="17" operator="lessThan">
@@ -8646,7 +8645,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8672,72 +8671,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="96" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="96"/>
-      <c r="E1" s="104" t="s">
+      <c r="D1" s="89"/>
+      <c r="E1" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="105"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="91"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="96" t="s">
+      <c r="B2" s="87"/>
+      <c r="C2" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="58" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="99"/>
-      <c r="C3" s="96" t="s">
+      <c r="B3" s="88"/>
+      <c r="C3" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="96"/>
-      <c r="E3" s="58" t="s">
+      <c r="D3" s="89"/>
+      <c r="E3" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="83" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="103"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="94"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="94"/>
-      <c r="B5" s="66"/>
+      <c r="A5" s="84"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -8758,8 +8757,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="95"/>
-      <c r="B6" s="67"/>
+      <c r="A6" s="85"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -9788,10 +9787,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="62" t="s">
+      <c r="A55" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="63"/>
+      <c r="B55" s="72"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -9804,10 +9803,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="59" t="s">
+      <c r="A56" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="60"/>
+      <c r="B56" s="70"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -9820,10 +9819,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="59" t="s">
+      <c r="A57" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="60"/>
+      <c r="B57" s="70"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -9836,10 +9835,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="59" t="s">
+      <c r="A58" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="60"/>
+      <c r="B58" s="70"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -9853,22 +9852,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
@@ -9876,7 +9875,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9899,147 +9898,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="57" t="s">
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="110" t="s">
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="111" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="111"/>
-      <c r="X1" s="111"/>
-      <c r="Y1" s="111"/>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="111"/>
-      <c r="AB1" s="111"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="112"/>
+      <c r="X1" s="112"/>
+      <c r="Y1" s="112"/>
+      <c r="Z1" s="112"/>
+      <c r="AA1" s="112"/>
+      <c r="AB1" s="112"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="70"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="78"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="57" t="s">
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="110" t="s">
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="111" t="s">
         <v>79</v>
       </c>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
-      <c r="X2" s="111"/>
-      <c r="Y2" s="111"/>
-      <c r="Z2" s="111"/>
-      <c r="AA2" s="111"/>
-      <c r="AB2" s="111"/>
+      <c r="O2" s="112"/>
+      <c r="P2" s="112"/>
+      <c r="Q2" s="112"/>
+      <c r="R2" s="112"/>
+      <c r="S2" s="112"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="112"/>
+      <c r="V2" s="112"/>
+      <c r="W2" s="112"/>
+      <c r="X2" s="112"/>
+      <c r="Y2" s="112"/>
+      <c r="Z2" s="112"/>
+      <c r="AA2" s="112"/>
+      <c r="AB2" s="112"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="81"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="104"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="78" t="s">
+      <c r="F3" s="101" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="77" t="s">
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="110" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="110" t="s">
+      <c r="K3" s="110"/>
+      <c r="L3" s="110"/>
+      <c r="M3" s="110"/>
+      <c r="N3" s="111" t="s">
         <v>80</v>
       </c>
-      <c r="O3" s="111"/>
-      <c r="P3" s="111"/>
-      <c r="Q3" s="111"/>
-      <c r="R3" s="111"/>
-      <c r="S3" s="111"/>
-      <c r="T3" s="111"/>
-      <c r="U3" s="111"/>
-      <c r="V3" s="111"/>
-      <c r="W3" s="111"/>
-      <c r="X3" s="111"/>
-      <c r="Y3" s="111"/>
-      <c r="Z3" s="111"/>
-      <c r="AA3" s="111"/>
-      <c r="AB3" s="111"/>
+      <c r="O3" s="112"/>
+      <c r="P3" s="112"/>
+      <c r="Q3" s="112"/>
+      <c r="R3" s="112"/>
+      <c r="S3" s="112"/>
+      <c r="T3" s="112"/>
+      <c r="U3" s="112"/>
+      <c r="V3" s="112"/>
+      <c r="W3" s="112"/>
+      <c r="X3" s="112"/>
+      <c r="Y3" s="112"/>
+      <c r="Z3" s="112"/>
+      <c r="AA3" s="112"/>
+      <c r="AB3" s="112"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="82"/>
-      <c r="B4" s="83"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="85">
+      <c r="A4" s="105"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="108">
         <v>43344</v>
       </c>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
@@ -10052,45 +10051,45 @@
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="73" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="90" t="s">
+      <c r="D5" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="88" t="s">
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="87" t="s">
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="87"/>
-      <c r="N5" s="88" t="s">
+      <c r="M5" s="95"/>
+      <c r="N5" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="89"/>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="87" t="s">
+      <c r="O5" s="97"/>
+      <c r="P5" s="97"/>
+      <c r="Q5" s="97"/>
+      <c r="R5" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="87"/>
+      <c r="S5" s="95"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="94"/>
-      <c r="B6" s="66"/>
+      <c r="A6" s="84"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -10157,8 +10156,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="94"/>
-      <c r="B7" s="66"/>
+      <c r="A7" s="84"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -10225,8 +10224,8 @@
       <c r="AF7" s="19"/>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="95"/>
-      <c r="B8" s="67"/>
+      <c r="A8" s="85"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -13653,10 +13652,10 @@
       <c r="AF56" s="19"/>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="62" t="s">
+      <c r="A57" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="63"/>
+      <c r="B57" s="72"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -13776,10 +13775,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="59" t="s">
+      <c r="A58" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="60"/>
+      <c r="B58" s="70"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -13900,15 +13899,9 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="N1:AB1"/>
+    <mergeCell ref="N2:AB2"/>
+    <mergeCell ref="N3:AB3"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="F3:I3"/>
@@ -13919,12 +13912,18 @@
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N1:AB1"/>
-    <mergeCell ref="N2:AB2"/>
-    <mergeCell ref="N3:AB3"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Last Update 16-10-2018  1:04:29.76
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -937,7 +937,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2412" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2412" uniqueCount="95">
   <si>
     <t>S.NO</t>
   </si>
@@ -1176,9 +1176,6 @@
     <t>Problem Solving and Python Programming</t>
   </si>
   <si>
-    <t>GE8392</t>
-  </si>
-  <si>
     <t>Mr. Rajasekaran S</t>
   </si>
   <si>
@@ -1219,6 +1216,12 @@
   </si>
   <si>
     <t>18ITA</t>
+  </si>
+  <si>
+    <t>GE8151</t>
+  </si>
+  <si>
+    <t>GE8192</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1372,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1467,15 +1470,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1541,7 +1535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1694,7 +1688,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1719,41 +1713,14 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1782,13 +1749,52 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1803,24 +1809,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1829,6 +1817,42 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1848,42 +1872,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2205,8 +2200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -2219,23 +2214,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="18.75">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="63"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="76"/>
       <c r="J1" s="80" t="s">
         <v>75</v>
       </c>
@@ -2266,23 +2261,23 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:33" ht="19.5">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="78"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="69"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="80" t="s">
         <v>76</v>
       </c>
@@ -2290,7 +2285,7 @@
       <c r="L2" s="80"/>
       <c r="M2" s="80"/>
       <c r="N2" s="81" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="O2" s="81"/>
       <c r="P2" s="81"/>
@@ -2313,23 +2308,23 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:33" ht="18.75">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="65"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="72"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="64" t="s">
+      <c r="F3" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
       <c r="J3" s="80" t="s">
         <v>77</v>
       </c>
@@ -2337,7 +2332,7 @@
       <c r="L3" s="80"/>
       <c r="M3" s="80"/>
       <c r="N3" s="81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O3" s="81"/>
       <c r="P3" s="81"/>
@@ -2360,33 +2355,33 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:33" ht="18.75">
-      <c r="A4" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66">
+      <c r="A4" s="70" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="71"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="77">
         <v>43344</v>
       </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="68"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="78"/>
+      <c r="R4" s="78"/>
+      <c r="S4" s="78"/>
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="79"/>
       <c r="X4" s="57"/>
       <c r="Y4" s="57"/>
       <c r="Z4" s="57"/>
@@ -2399,10 +2394,10 @@
       <c r="AG4" s="57"/>
     </row>
     <row r="5" spans="1:33">
-      <c r="A5" s="79" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="73" t="s">
+      <c r="A5" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="64" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -2496,8 +2491,8 @@
       <c r="AG5" s="12"/>
     </row>
     <row r="6" spans="1:33">
-      <c r="A6" s="79"/>
-      <c r="B6" s="74"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -2590,9 +2585,9 @@
     </row>
     <row r="7" spans="1:33" ht="15" customHeight="1">
       <c r="A7" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="75"/>
+        <v>92</v>
+      </c>
+      <c r="B7" s="66"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -7244,10 +7239,10 @@
       <c r="AG55" s="12"/>
     </row>
     <row r="56" spans="1:33">
-      <c r="A56" s="71" t="s">
+      <c r="A56" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="72"/>
+      <c r="B56" s="63"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -7371,10 +7366,10 @@
       </c>
     </row>
     <row r="57" spans="1:33">
-      <c r="A57" s="69" t="s">
+      <c r="A57" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="70"/>
+      <c r="B57" s="60"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -7499,13 +7494,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F3:I3"/>
@@ -7516,6 +7504,13 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N2:W2"/>
     <mergeCell ref="N3:W3"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7528,7 +7523,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="E2" sqref="E2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -7543,14 +7538,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="89" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="89"/>
+      <c r="D1" s="85"/>
       <c r="E1" s="81" t="s">
         <v>78</v>
       </c>
@@ -7559,56 +7554,56 @@
       <c r="H1" s="81"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="89" t="s">
+      <c r="B2" s="83"/>
+      <c r="C2" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="89"/>
+      <c r="D2" s="85"/>
       <c r="E2" s="81" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="F2" s="81"/>
       <c r="G2" s="81"/>
       <c r="H2" s="81"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="88" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="89" t="s">
+      <c r="A3" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="84"/>
+      <c r="C3" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="89"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F3" s="81"/>
       <c r="G3" s="81"/>
       <c r="H3" s="81"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="87" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="73" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="86" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
+      <c r="C4" s="82" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="84"/>
-      <c r="B5" s="74"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -7619,18 +7614,18 @@
         <v>72</v>
       </c>
       <c r="F5" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="85"/>
-      <c r="B6" s="75"/>
+      <c r="A6" s="89"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -8553,10 +8548,10 @@
       <c r="H54" s="42"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="71" t="s">
+      <c r="A55" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="72"/>
+      <c r="B55" s="63"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -8570,10 +8565,10 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="69" t="s">
+      <c r="A56" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="70"/>
+      <c r="B56" s="60"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -8587,10 +8582,10 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="69" t="s">
+      <c r="A57" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="70"/>
+      <c r="B57" s="60"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -8604,10 +8599,10 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="69" t="s">
+      <c r="A58" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="70"/>
+      <c r="B58" s="60"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -8622,6 +8617,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -8631,13 +8633,6 @@
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:H54">
     <cfRule type="cellIs" dxfId="1" priority="17" operator="lessThan">
@@ -8654,7 +8649,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:H4"/>
+      <selection activeCell="E3" sqref="E3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -8671,72 +8666,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="89" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90" t="s">
+      <c r="D1" s="85"/>
+      <c r="E1" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="91"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="94"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="89" t="s">
+      <c r="B2" s="83"/>
+      <c r="C2" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="89"/>
+      <c r="D2" s="85"/>
       <c r="E2" s="81" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="F2" s="81"/>
       <c r="G2" s="81"/>
       <c r="H2" s="81"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="88" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="89" t="s">
+      <c r="A3" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="84"/>
+      <c r="C3" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="89"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F3" s="81"/>
       <c r="G3" s="81"/>
       <c r="H3" s="81"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="87" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="73" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="92" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="94"/>
+      <c r="C4" s="90" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="92"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="84"/>
-      <c r="B5" s="74"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -8744,21 +8739,21 @@
         <v>71</v>
       </c>
       <c r="E5" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="G5" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="H5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="56" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="85"/>
-      <c r="B6" s="75"/>
+      <c r="A6" s="89"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -9787,10 +9782,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="71" t="s">
+      <c r="A55" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="72"/>
+      <c r="B55" s="63"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -9803,10 +9798,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="69" t="s">
+      <c r="A56" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="70"/>
+      <c r="B56" s="60"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -9819,10 +9814,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="69" t="s">
+      <c r="A57" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="70"/>
+      <c r="B57" s="60"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -9835,10 +9830,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="69" t="s">
+      <c r="A58" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="70"/>
+      <c r="B58" s="60"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -9852,22 +9847,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
@@ -9883,8 +9878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -9898,198 +9893,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="63"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="76"/>
       <c r="J1" s="80" t="s">
         <v>75</v>
       </c>
       <c r="K1" s="80"/>
       <c r="L1" s="80"/>
       <c r="M1" s="80"/>
-      <c r="N1" s="111" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
-      <c r="W1" s="112"/>
-      <c r="X1" s="112"/>
-      <c r="Y1" s="112"/>
-      <c r="Z1" s="112"/>
-      <c r="AA1" s="112"/>
-      <c r="AB1" s="112"/>
+      <c r="N1" s="112" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="113"/>
+      <c r="W1" s="113"/>
+      <c r="X1" s="113"/>
+      <c r="Y1" s="113"/>
+      <c r="Z1" s="113"/>
+      <c r="AA1" s="113"/>
+      <c r="AB1" s="113"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="78"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="69"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="80" t="s">
         <v>76</v>
       </c>
       <c r="K2" s="80"/>
       <c r="L2" s="80"/>
       <c r="M2" s="80"/>
-      <c r="N2" s="111" t="s">
-        <v>79</v>
-      </c>
-      <c r="O2" s="112"/>
-      <c r="P2" s="112"/>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="112"/>
-      <c r="U2" s="112"/>
-      <c r="V2" s="112"/>
-      <c r="W2" s="112"/>
-      <c r="X2" s="112"/>
-      <c r="Y2" s="112"/>
-      <c r="Z2" s="112"/>
-      <c r="AA2" s="112"/>
-      <c r="AB2" s="112"/>
+      <c r="N2" s="112" t="s">
+        <v>94</v>
+      </c>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="113"/>
+      <c r="X2" s="113"/>
+      <c r="Y2" s="113"/>
+      <c r="Z2" s="113"/>
+      <c r="AA2" s="113"/>
+      <c r="AB2" s="113"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="104"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="98"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="101" t="s">
+      <c r="F3" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="110" t="s">
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="110"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="111" t="s">
-        <v>80</v>
-      </c>
-      <c r="O3" s="112"/>
-      <c r="P3" s="112"/>
-      <c r="Q3" s="112"/>
-      <c r="R3" s="112"/>
-      <c r="S3" s="112"/>
-      <c r="T3" s="112"/>
-      <c r="U3" s="112"/>
-      <c r="V3" s="112"/>
-      <c r="W3" s="112"/>
-      <c r="X3" s="112"/>
-      <c r="Y3" s="112"/>
-      <c r="Z3" s="112"/>
-      <c r="AA3" s="112"/>
-      <c r="AB3" s="112"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="112" t="s">
+        <v>79</v>
+      </c>
+      <c r="O3" s="113"/>
+      <c r="P3" s="113"/>
+      <c r="Q3" s="113"/>
+      <c r="R3" s="113"/>
+      <c r="S3" s="113"/>
+      <c r="T3" s="113"/>
+      <c r="U3" s="113"/>
+      <c r="V3" s="113"/>
+      <c r="W3" s="113"/>
+      <c r="X3" s="113"/>
+      <c r="Y3" s="113"/>
+      <c r="Z3" s="113"/>
+      <c r="AA3" s="113"/>
+      <c r="AB3" s="113"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="105"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="108">
+      <c r="A4" s="99"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="102">
         <v>43344</v>
       </c>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="109"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="111"/>
+      <c r="O4" s="111"/>
+      <c r="P4" s="111"/>
+      <c r="Q4" s="111"/>
+      <c r="R4" s="111"/>
+      <c r="S4" s="111"/>
       <c r="T4" s="53"/>
       <c r="U4" s="53"/>
       <c r="V4" s="53"/>
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="64" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="98" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="108" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="96" t="s">
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="95" t="s">
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="107"/>
+      <c r="L5" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="95"/>
-      <c r="N5" s="96" t="s">
+      <c r="M5" s="105"/>
+      <c r="N5" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="97"/>
-      <c r="P5" s="97"/>
-      <c r="Q5" s="97"/>
-      <c r="R5" s="95" t="s">
+      <c r="O5" s="107"/>
+      <c r="P5" s="107"/>
+      <c r="Q5" s="107"/>
+      <c r="R5" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="95"/>
+      <c r="S5" s="105"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="84"/>
-      <c r="B6" s="74"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -10156,8 +10151,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="84"/>
-      <c r="B7" s="74"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -10224,8 +10219,8 @@
       <c r="AF7" s="19"/>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="85"/>
-      <c r="B8" s="75"/>
+      <c r="A8" s="89"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -13652,10 +13647,10 @@
       <c r="AF56" s="19"/>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="71" t="s">
+      <c r="A57" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="72"/>
+      <c r="B57" s="63"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -13775,10 +13770,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="69" t="s">
+      <c r="A58" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="70"/>
+      <c r="B58" s="60"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -13899,6 +13894,15 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
     <mergeCell ref="N1:AB1"/>
     <mergeCell ref="N2:AB2"/>
     <mergeCell ref="N3:AB3"/>
@@ -13912,15 +13916,6 @@
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Last Update 25-10-2018 20:13:43.50
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -703,6 +703,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="AF7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Controll Flow Type, If elif else</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Controll Flow Type, Loops, Branching, Break and Continue</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -937,7 +985,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2412" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="97">
   <si>
     <t>S.NO</t>
   </si>
@@ -1222,6 +1270,12 @@
   </si>
   <si>
     <t>GE8192</t>
+  </si>
+  <si>
+    <t>Lab 4</t>
+  </si>
+  <si>
+    <t>aa</t>
   </si>
 </sst>
 </file>
@@ -1535,7 +1589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1713,6 +1767,15 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1824,6 +1887,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1872,13 +1939,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2200,8 +2260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:W3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -2214,29 +2274,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="18.75">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="80" t="s">
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="83" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -2257,45 +2317,47 @@
       <c r="AC1" s="50"/>
       <c r="AD1" s="50"/>
       <c r="AE1" s="50"/>
-      <c r="AF1" s="50"/>
+      <c r="AF1" s="50" t="s">
+        <v>96</v>
+      </c>
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:33" ht="19.5">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="69"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="80" t="s">
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="81" t="s">
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="81"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="84"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="84"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -2308,41 +2370,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:33" ht="18.75">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="72"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="75"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="80" t="s">
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="81" t="s">
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="81"/>
-      <c r="S3" s="81"/>
-      <c r="T3" s="81"/>
-      <c r="U3" s="81"/>
-      <c r="V3" s="81"/>
-      <c r="W3" s="81"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
+      <c r="T3" s="84"/>
+      <c r="U3" s="84"/>
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -2355,33 +2417,33 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:33" ht="18.75">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="77">
+      <c r="B4" s="74"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="80">
         <v>43344</v>
       </c>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="78"/>
-      <c r="S4" s="78"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="79"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="82"/>
       <c r="X4" s="57"/>
       <c r="Y4" s="57"/>
       <c r="Z4" s="57"/>
@@ -2394,10 +2456,10 @@
       <c r="AG4" s="57"/>
     </row>
     <row r="5" spans="1:33">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="76" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="67" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -2487,12 +2549,16 @@
       <c r="AE5" s="42">
         <v>10</v>
       </c>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="12"/>
+      <c r="AF5" s="12">
+        <v>10</v>
+      </c>
+      <c r="AG5" s="12">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:33">
-      <c r="A6" s="73"/>
-      <c r="B6" s="65"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -2580,14 +2646,18 @@
       <c r="AE6" s="42">
         <v>12</v>
       </c>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="12"/>
+      <c r="AF6" s="12">
+        <v>22</v>
+      </c>
+      <c r="AG6" s="12">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:33" ht="15" customHeight="1">
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="66"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -2675,8 +2745,12 @@
       <c r="AE7" s="49">
         <v>4</v>
       </c>
-      <c r="AF7" s="12"/>
-      <c r="AG7" s="12"/>
+      <c r="AF7" s="12">
+        <v>4</v>
+      </c>
+      <c r="AG7" s="12">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:33" ht="15" customHeight="1">
       <c r="A8" s="3">
@@ -2770,8 +2844,12 @@
       <c r="AE8" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF8" s="12"/>
-      <c r="AG8" s="12"/>
+      <c r="AF8" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG8" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" spans="1:33" ht="15" customHeight="1">
       <c r="A9" s="3">
@@ -2865,8 +2943,12 @@
       <c r="AE9" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="12"/>
-      <c r="AG9" s="12"/>
+      <c r="AF9" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG9" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:33" ht="15" customHeight="1">
       <c r="A10" s="3">
@@ -2960,8 +3042,12 @@
       <c r="AE10" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF10" s="12"/>
-      <c r="AG10" s="12"/>
+      <c r="AF10" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG10" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="11" spans="1:33" ht="15" customHeight="1">
       <c r="A11" s="3">
@@ -3055,8 +3141,12 @@
       <c r="AE11" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF11" s="12"/>
-      <c r="AG11" s="12"/>
+      <c r="AF11" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG11" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="12" spans="1:33" ht="15" customHeight="1">
       <c r="A12" s="3">
@@ -3150,8 +3240,12 @@
       <c r="AE12" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF12" s="12"/>
-      <c r="AG12" s="12"/>
+      <c r="AF12" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG12" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="13" spans="1:33" ht="15" customHeight="1">
       <c r="A13" s="3">
@@ -3245,8 +3339,12 @@
       <c r="AE13" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF13" s="12"/>
-      <c r="AG13" s="12"/>
+      <c r="AF13" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG13" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:33" ht="15" customHeight="1">
       <c r="A14" s="3">
@@ -3340,8 +3438,12 @@
       <c r="AE14" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF14" s="12"/>
-      <c r="AG14" s="12"/>
+      <c r="AF14" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG14" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="15" spans="1:33" ht="15" customHeight="1">
       <c r="A15" s="3">
@@ -3435,8 +3537,12 @@
       <c r="AE15" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF15" s="12"/>
-      <c r="AG15" s="12"/>
+      <c r="AF15" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG15" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="16" spans="1:33" ht="15" customHeight="1">
       <c r="A16" s="3">
@@ -3530,8 +3636,12 @@
       <c r="AE16" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF16" s="12"/>
-      <c r="AG16" s="12"/>
+      <c r="AF16" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG16" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="17" spans="1:33" ht="15" customHeight="1">
       <c r="A17" s="3">
@@ -3625,8 +3735,12 @@
       <c r="AE17" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF17" s="12"/>
-      <c r="AG17" s="12"/>
+      <c r="AF17" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG17" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="18" spans="1:33" ht="15" customHeight="1">
       <c r="A18" s="3">
@@ -3720,8 +3834,12 @@
       <c r="AE18" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF18" s="12"/>
-      <c r="AG18" s="12"/>
+      <c r="AF18" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG18" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="19" spans="1:33" ht="15" customHeight="1">
       <c r="A19" s="3">
@@ -3815,8 +3933,12 @@
       <c r="AE19" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF19" s="12"/>
-      <c r="AG19" s="12"/>
+      <c r="AF19" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG19" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="20" spans="1:33" ht="15" customHeight="1">
       <c r="A20" s="3">
@@ -3910,8 +4032,12 @@
       <c r="AE20" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF20" s="12"/>
-      <c r="AG20" s="12"/>
+      <c r="AF20" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG20" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="21" spans="1:33" ht="15" customHeight="1">
       <c r="A21" s="3">
@@ -4005,8 +4131,12 @@
       <c r="AE21" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF21" s="12"/>
-      <c r="AG21" s="12"/>
+      <c r="AF21" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG21" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="22" spans="1:33" ht="15" customHeight="1">
       <c r="A22" s="3">
@@ -4100,8 +4230,12 @@
       <c r="AE22" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="AF22" s="12"/>
-      <c r="AG22" s="12"/>
+      <c r="AF22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG22" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="23" spans="1:33" ht="15" customHeight="1">
       <c r="A23" s="3">
@@ -4195,8 +4329,12 @@
       <c r="AE23" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF23" s="12"/>
-      <c r="AG23" s="12"/>
+      <c r="AF23" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG23" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="24" spans="1:33" ht="15" customHeight="1">
       <c r="A24" s="3">
@@ -4290,8 +4428,12 @@
       <c r="AE24" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AF24" s="12"/>
-      <c r="AG24" s="12"/>
+      <c r="AF24" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG24" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="1:33" ht="15" customHeight="1">
       <c r="A25" s="3">
@@ -4385,8 +4527,12 @@
       <c r="AE25" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF25" s="12"/>
-      <c r="AG25" s="12"/>
+      <c r="AF25" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG25" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="26" spans="1:33" ht="15" customHeight="1">
       <c r="A26" s="3">
@@ -4480,8 +4626,12 @@
       <c r="AE26" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF26" s="12"/>
-      <c r="AG26" s="12"/>
+      <c r="AF26" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG26" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="27" spans="1:33" ht="15" customHeight="1">
       <c r="A27" s="3">
@@ -4575,8 +4725,12 @@
       <c r="AE27" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF27" s="12"/>
-      <c r="AG27" s="12"/>
+      <c r="AF27" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG27" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="28" spans="1:33" ht="15" customHeight="1">
       <c r="A28" s="3">
@@ -4670,8 +4824,12 @@
       <c r="AE28" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF28" s="12"/>
-      <c r="AG28" s="12"/>
+      <c r="AF28" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG28" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="29" spans="1:33" ht="15" customHeight="1">
       <c r="A29" s="3">
@@ -4765,8 +4923,12 @@
       <c r="AE29" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF29" s="12"/>
-      <c r="AG29" s="12"/>
+      <c r="AF29" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG29" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="30" spans="1:33" ht="15" customHeight="1">
       <c r="A30" s="3">
@@ -4860,8 +5022,12 @@
       <c r="AE30" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF30" s="12"/>
-      <c r="AG30" s="12"/>
+      <c r="AF30" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG30" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="31" spans="1:33" ht="15" customHeight="1">
       <c r="A31" s="3">
@@ -4955,8 +5121,12 @@
       <c r="AE31" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF31" s="12"/>
-      <c r="AG31" s="12"/>
+      <c r="AF31" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG31" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="32" spans="1:33" ht="15" customHeight="1">
       <c r="A32" s="3">
@@ -5050,8 +5220,12 @@
       <c r="AE32" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF32" s="12"/>
-      <c r="AG32" s="12"/>
+      <c r="AF32" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG32" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="33" spans="1:33" ht="15" customHeight="1">
       <c r="A33" s="3">
@@ -5145,8 +5319,12 @@
       <c r="AE33" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF33" s="12"/>
-      <c r="AG33" s="12"/>
+      <c r="AF33" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG33" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="34" spans="1:33" ht="15" customHeight="1">
       <c r="A34" s="3">
@@ -5240,8 +5418,12 @@
       <c r="AE34" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF34" s="12"/>
-      <c r="AG34" s="12"/>
+      <c r="AF34" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG34" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="35" spans="1:33" ht="15" customHeight="1">
       <c r="A35" s="3">
@@ -5335,8 +5517,12 @@
       <c r="AE35" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF35" s="12"/>
-      <c r="AG35" s="12"/>
+      <c r="AF35" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG35" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="1:33" ht="15" customHeight="1">
       <c r="A36" s="3">
@@ -5430,8 +5616,12 @@
       <c r="AE36" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF36" s="12"/>
-      <c r="AG36" s="12"/>
+      <c r="AF36" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG36" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="37" spans="1:33" ht="15" customHeight="1">
       <c r="A37" s="3">
@@ -5525,8 +5715,12 @@
       <c r="AE37" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF37" s="12"/>
-      <c r="AG37" s="12"/>
+      <c r="AF37" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG37" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="38" spans="1:33" ht="15" customHeight="1">
       <c r="A38" s="3">
@@ -5620,8 +5814,12 @@
       <c r="AE38" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF38" s="12"/>
-      <c r="AG38" s="12"/>
+      <c r="AF38" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG38" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="39" spans="1:33" ht="15" customHeight="1">
       <c r="A39" s="3">
@@ -5715,8 +5913,12 @@
       <c r="AE39" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF39" s="12"/>
-      <c r="AG39" s="12"/>
+      <c r="AF39" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG39" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="40" spans="1:33" ht="15" customHeight="1">
       <c r="A40" s="3">
@@ -5810,8 +6012,12 @@
       <c r="AE40" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF40" s="12"/>
-      <c r="AG40" s="12"/>
+      <c r="AF40" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG40" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="41" spans="1:33" ht="15" customHeight="1">
       <c r="A41" s="3">
@@ -5905,8 +6111,12 @@
       <c r="AE41" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF41" s="12"/>
-      <c r="AG41" s="12"/>
+      <c r="AF41" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG41" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="42" spans="1:33" ht="15" customHeight="1">
       <c r="A42" s="3">
@@ -6000,8 +6210,12 @@
       <c r="AE42" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF42" s="12"/>
-      <c r="AG42" s="12"/>
+      <c r="AF42" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG42" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="43" spans="1:33" ht="15" customHeight="1">
       <c r="A43" s="3">
@@ -6095,8 +6309,12 @@
       <c r="AE43" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF43" s="12"/>
-      <c r="AG43" s="12"/>
+      <c r="AF43" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG43" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="44" spans="1:33" ht="15" customHeight="1">
       <c r="A44" s="3">
@@ -6190,8 +6408,12 @@
       <c r="AE44" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF44" s="12"/>
-      <c r="AG44" s="12"/>
+      <c r="AF44" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG44" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="45" spans="1:33" ht="15" customHeight="1">
       <c r="A45" s="3">
@@ -6285,8 +6507,12 @@
       <c r="AE45" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF45" s="12"/>
-      <c r="AG45" s="12"/>
+      <c r="AF45" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG45" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="46" spans="1:33" ht="15" customHeight="1">
       <c r="A46" s="3">
@@ -6380,8 +6606,12 @@
       <c r="AE46" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF46" s="12"/>
-      <c r="AG46" s="12"/>
+      <c r="AF46" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG46" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="47" spans="1:33" ht="15" customHeight="1">
       <c r="A47" s="3">
@@ -6475,8 +6705,12 @@
       <c r="AE47" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF47" s="12"/>
-      <c r="AG47" s="12"/>
+      <c r="AF47" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG47" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="48" spans="1:33" ht="15" customHeight="1">
       <c r="A48" s="3">
@@ -6570,8 +6804,12 @@
       <c r="AE48" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF48" s="12"/>
-      <c r="AG48" s="12"/>
+      <c r="AF48" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG48" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="49" spans="1:33" ht="15" customHeight="1">
       <c r="A49" s="3">
@@ -6665,8 +6903,12 @@
       <c r="AE49" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF49" s="12"/>
-      <c r="AG49" s="12"/>
+      <c r="AF49" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG49" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="50" spans="1:33" ht="15" customHeight="1">
       <c r="A50" s="3">
@@ -6760,8 +7002,12 @@
       <c r="AE50" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF50" s="12"/>
-      <c r="AG50" s="12"/>
+      <c r="AF50" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG50" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="51" spans="1:33" ht="15" customHeight="1">
       <c r="A51" s="3">
@@ -6855,8 +7101,12 @@
       <c r="AE51" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF51" s="12"/>
-      <c r="AG51" s="12"/>
+      <c r="AF51" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG51" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="52" spans="1:33" ht="15" customHeight="1">
       <c r="A52" s="3">
@@ -6950,8 +7200,12 @@
       <c r="AE52" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF52" s="12"/>
-      <c r="AG52" s="12"/>
+      <c r="AF52" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG52" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="53" spans="1:33" ht="15" customHeight="1">
       <c r="A53" s="3">
@@ -7045,8 +7299,12 @@
       <c r="AE53" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF53" s="12"/>
-      <c r="AG53" s="12"/>
+      <c r="AF53" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG53" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="54" spans="1:33" ht="15" customHeight="1">
       <c r="A54" s="3">
@@ -7140,8 +7398,12 @@
       <c r="AE54" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF54" s="12"/>
-      <c r="AG54" s="12"/>
+      <c r="AF54" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG54" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="55" spans="1:33" ht="15" customHeight="1">
       <c r="A55" s="3">
@@ -7235,14 +7497,18 @@
       <c r="AE55" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AF55" s="12"/>
-      <c r="AG55" s="12"/>
+      <c r="AF55" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG55" s="61" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="56" spans="1:33">
-      <c r="A56" s="62" t="s">
+      <c r="A56" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="63"/>
+      <c r="B56" s="66"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -7358,18 +7624,18 @@
       </c>
       <c r="AF56" s="12">
         <f t="shared" ref="AF56" si="21">COUNTIF(AF8:AF55,"A")</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AG56" s="12">
         <f t="shared" ref="AG56" si="22">COUNTIF(AG8:AG55,"A")</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:33">
-      <c r="A57" s="59" t="s">
+      <c r="A57" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="60"/>
+      <c r="B57" s="63"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -7485,11 +7751,11 @@
       </c>
       <c r="AF57" s="24">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="AG57" s="24">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -7538,72 +7804,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="85" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="85"/>
-      <c r="E1" s="81" t="s">
+      <c r="D1" s="88"/>
+      <c r="E1" s="84" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="85" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="E2" s="81" t="s">
+      <c r="D2" s="88"/>
+      <c r="E2" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="87" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="85" t="s">
+      <c r="B3" s="87"/>
+      <c r="C3" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="81" t="s">
+      <c r="D3" s="88"/>
+      <c r="E3" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="88"/>
-      <c r="B5" s="65"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -7624,8 +7890,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="89"/>
-      <c r="B6" s="66"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -8548,10 +8814,10 @@
       <c r="H54" s="42"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="62" t="s">
+      <c r="A55" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="63"/>
+      <c r="B55" s="66"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -8565,10 +8831,10 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="59" t="s">
+      <c r="A56" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="60"/>
+      <c r="B56" s="63"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -8582,10 +8848,10 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="59" t="s">
+      <c r="A57" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="60"/>
+      <c r="B57" s="63"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -8599,10 +8865,10 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="59" t="s">
+      <c r="A58" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="60"/>
+      <c r="B58" s="63"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -8648,8 +8914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:H3"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -8666,72 +8932,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="85" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="85"/>
-      <c r="E1" s="93" t="s">
+      <c r="D1" s="88"/>
+      <c r="E1" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="94"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="97"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="85" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="E2" s="81" t="s">
+      <c r="D2" s="88"/>
+      <c r="E2" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="87" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="85" t="s">
+      <c r="B3" s="87"/>
+      <c r="C3" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="81" t="s">
+      <c r="D3" s="88"/>
+      <c r="E3" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="92"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="95"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="88"/>
-      <c r="B5" s="65"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -8752,8 +9018,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="89"/>
-      <c r="B6" s="66"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -9782,10 +10048,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="62" t="s">
+      <c r="A55" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="63"/>
+      <c r="B55" s="66"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -9798,10 +10064,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="59" t="s">
+      <c r="A56" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="60"/>
+      <c r="B56" s="63"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -9814,10 +10080,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="59" t="s">
+      <c r="A57" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="60"/>
+      <c r="B57" s="63"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -9830,10 +10096,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="59" t="s">
+      <c r="A58" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="60"/>
+      <c r="B58" s="63"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -9878,8 +10144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -9893,198 +10159,202 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="80" t="s">
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="83" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="112" t="s">
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="113"/>
-      <c r="P1" s="113"/>
-      <c r="Q1" s="113"/>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="113"/>
-      <c r="V1" s="113"/>
-      <c r="W1" s="113"/>
-      <c r="X1" s="113"/>
-      <c r="Y1" s="113"/>
-      <c r="Z1" s="113"/>
-      <c r="AA1" s="113"/>
-      <c r="AB1" s="113"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="99"/>
+      <c r="Z1" s="99"/>
+      <c r="AA1" s="99"/>
+      <c r="AB1" s="99"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="69"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="80" t="s">
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="112" t="s">
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="98" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="113"/>
-      <c r="V2" s="113"/>
-      <c r="W2" s="113"/>
-      <c r="X2" s="113"/>
-      <c r="Y2" s="113"/>
-      <c r="Z2" s="113"/>
-      <c r="AA2" s="113"/>
-      <c r="AB2" s="113"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="99"/>
+      <c r="T2" s="99"/>
+      <c r="U2" s="99"/>
+      <c r="V2" s="99"/>
+      <c r="W2" s="99"/>
+      <c r="X2" s="99"/>
+      <c r="Y2" s="99"/>
+      <c r="Z2" s="99"/>
+      <c r="AA2" s="99"/>
+      <c r="AB2" s="99"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="98"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="103"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="100" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="104" t="s">
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="112" t="s">
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="113"/>
-      <c r="P3" s="113"/>
-      <c r="Q3" s="113"/>
-      <c r="R3" s="113"/>
-      <c r="S3" s="113"/>
-      <c r="T3" s="113"/>
-      <c r="U3" s="113"/>
-      <c r="V3" s="113"/>
-      <c r="W3" s="113"/>
-      <c r="X3" s="113"/>
-      <c r="Y3" s="113"/>
-      <c r="Z3" s="113"/>
-      <c r="AA3" s="113"/>
-      <c r="AB3" s="113"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
+      <c r="Q3" s="99"/>
+      <c r="R3" s="99"/>
+      <c r="S3" s="99"/>
+      <c r="T3" s="99"/>
+      <c r="U3" s="99"/>
+      <c r="V3" s="99"/>
+      <c r="W3" s="99"/>
+      <c r="X3" s="99"/>
+      <c r="Y3" s="99"/>
+      <c r="Z3" s="99"/>
+      <c r="AA3" s="99"/>
+      <c r="AB3" s="99"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="99"/>
-      <c r="B4" s="100"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="102">
+      <c r="A4" s="104"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="107">
         <v>43344</v>
       </c>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
-      <c r="N4" s="111"/>
-      <c r="O4" s="111"/>
-      <c r="P4" s="111"/>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="111"/>
-      <c r="S4" s="111"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="108"/>
+      <c r="J4" s="108"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="108"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
       <c r="T4" s="53"/>
       <c r="U4" s="53"/>
       <c r="V4" s="53"/>
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="67" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="108" t="s">
+      <c r="D5" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="106" t="s">
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="111" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="105" t="s">
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="105"/>
-      <c r="N5" s="106" t="s">
+      <c r="M5" s="110"/>
+      <c r="N5" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="107"/>
-      <c r="P5" s="107"/>
-      <c r="Q5" s="107"/>
-      <c r="R5" s="105" t="s">
+      <c r="O5" s="112"/>
+      <c r="P5" s="112"/>
+      <c r="Q5" s="112"/>
+      <c r="R5" s="110" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="105"/>
+      <c r="S5" s="110"/>
+      <c r="T5" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="U5" s="76"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="88"/>
-      <c r="B6" s="65"/>
+      <c r="A6" s="91"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -10136,8 +10406,12 @@
       <c r="S6" s="19">
         <v>10</v>
       </c>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
+      <c r="T6" s="19">
+        <v>10</v>
+      </c>
+      <c r="U6" s="59">
+        <v>10</v>
+      </c>
       <c r="V6" s="19"/>
       <c r="W6" s="19"/>
       <c r="X6" s="19"/>
@@ -10151,8 +10425,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="88"/>
-      <c r="B7" s="65"/>
+      <c r="A7" s="91"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -10204,8 +10478,12 @@
       <c r="S7" s="19">
         <v>10</v>
       </c>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
+      <c r="T7" s="19">
+        <v>17</v>
+      </c>
+      <c r="U7" s="59">
+        <v>17</v>
+      </c>
       <c r="V7" s="19"/>
       <c r="W7" s="19"/>
       <c r="X7" s="19"/>
@@ -10219,8 +10497,8 @@
       <c r="AF7" s="19"/>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="89"/>
-      <c r="B8" s="66"/>
+      <c r="A8" s="92"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -10272,8 +10550,12 @@
       <c r="S8" s="19">
         <v>2</v>
       </c>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
+      <c r="T8" s="19">
+        <v>3</v>
+      </c>
+      <c r="U8" s="59">
+        <v>4</v>
+      </c>
       <c r="V8" s="19"/>
       <c r="W8" s="19"/>
       <c r="X8" s="19"/>
@@ -10342,8 +10624,12 @@
       <c r="S9" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
+      <c r="T9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U9" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V9" s="19"/>
       <c r="W9" s="19"/>
       <c r="X9" s="19"/>
@@ -10412,8 +10698,12 @@
       <c r="S10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
+      <c r="T10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U10" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V10" s="19"/>
       <c r="W10" s="19"/>
       <c r="X10" s="19"/>
@@ -10482,8 +10772,12 @@
       <c r="S11" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
+      <c r="T11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U11" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V11" s="19"/>
       <c r="W11" s="19"/>
       <c r="X11" s="19"/>
@@ -10552,8 +10846,12 @@
       <c r="S12" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
+      <c r="T12" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U12" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V12" s="19"/>
       <c r="W12" s="19"/>
       <c r="X12" s="19"/>
@@ -10622,8 +10920,12 @@
       <c r="S13" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
+      <c r="T13" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U13" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V13" s="19"/>
       <c r="W13" s="19"/>
       <c r="X13" s="19"/>
@@ -10692,8 +10994,12 @@
       <c r="S14" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T14" s="19"/>
-      <c r="U14" s="19"/>
+      <c r="T14" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U14" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V14" s="19"/>
       <c r="W14" s="19"/>
       <c r="X14" s="19"/>
@@ -10762,8 +11068,12 @@
       <c r="S15" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
+      <c r="T15" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U15" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V15" s="19"/>
       <c r="W15" s="19"/>
       <c r="X15" s="19"/>
@@ -10832,8 +11142,12 @@
       <c r="S16" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T16" s="19"/>
-      <c r="U16" s="19"/>
+      <c r="T16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U16" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V16" s="19"/>
       <c r="W16" s="19"/>
       <c r="X16" s="19"/>
@@ -10902,8 +11216,12 @@
       <c r="S17" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
+      <c r="T17" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U17" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V17" s="19"/>
       <c r="W17" s="19"/>
       <c r="X17" s="19"/>
@@ -10972,8 +11290,12 @@
       <c r="S18" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
+      <c r="T18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U18" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V18" s="19"/>
       <c r="W18" s="19"/>
       <c r="X18" s="19"/>
@@ -11042,8 +11364,12 @@
       <c r="S19" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
+      <c r="T19" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U19" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V19" s="19"/>
       <c r="W19" s="19"/>
       <c r="X19" s="19"/>
@@ -11112,8 +11438,12 @@
       <c r="S20" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T20" s="19"/>
-      <c r="U20" s="19"/>
+      <c r="T20" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U20" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V20" s="19"/>
       <c r="W20" s="19"/>
       <c r="X20" s="19"/>
@@ -11182,8 +11512,12 @@
       <c r="S21" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
+      <c r="T21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U21" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V21" s="19"/>
       <c r="W21" s="19"/>
       <c r="X21" s="19"/>
@@ -11252,8 +11586,12 @@
       <c r="S22" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T22" s="19"/>
-      <c r="U22" s="19"/>
+      <c r="T22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U22" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V22" s="19"/>
       <c r="W22" s="19"/>
       <c r="X22" s="19"/>
@@ -11322,8 +11660,12 @@
       <c r="S23" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T23" s="19"/>
-      <c r="U23" s="19"/>
+      <c r="T23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U23" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V23" s="19"/>
       <c r="W23" s="19"/>
       <c r="X23" s="19"/>
@@ -11392,8 +11734,12 @@
       <c r="S24" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T24" s="19"/>
-      <c r="U24" s="19"/>
+      <c r="T24" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U24" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V24" s="19"/>
       <c r="W24" s="19"/>
       <c r="X24" s="19"/>
@@ -11462,8 +11808,12 @@
       <c r="S25" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
+      <c r="T25" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U25" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V25" s="19"/>
       <c r="W25" s="19"/>
       <c r="X25" s="19"/>
@@ -11532,8 +11882,12 @@
       <c r="S26" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T26" s="19"/>
-      <c r="U26" s="19"/>
+      <c r="T26" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U26" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V26" s="19"/>
       <c r="W26" s="19"/>
       <c r="X26" s="19"/>
@@ -11602,8 +11956,12 @@
       <c r="S27" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T27" s="19"/>
-      <c r="U27" s="19"/>
+      <c r="T27" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U27" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V27" s="19"/>
       <c r="W27" s="19"/>
       <c r="X27" s="19"/>
@@ -11672,8 +12030,12 @@
       <c r="S28" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T28" s="19"/>
-      <c r="U28" s="19"/>
+      <c r="T28" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U28" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V28" s="19"/>
       <c r="W28" s="19"/>
       <c r="X28" s="19"/>
@@ -11742,8 +12104,12 @@
       <c r="S29" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T29" s="19"/>
-      <c r="U29" s="19"/>
+      <c r="T29" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U29" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V29" s="19"/>
       <c r="W29" s="19"/>
       <c r="X29" s="19"/>
@@ -11812,8 +12178,12 @@
       <c r="S30" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T30" s="19"/>
-      <c r="U30" s="19"/>
+      <c r="T30" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U30" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V30" s="19"/>
       <c r="W30" s="19"/>
       <c r="X30" s="19"/>
@@ -11882,8 +12252,12 @@
       <c r="S31" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
+      <c r="T31" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U31" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V31" s="19"/>
       <c r="W31" s="19"/>
       <c r="X31" s="19"/>
@@ -11952,8 +12326,12 @@
       <c r="S32" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
+      <c r="T32" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U32" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V32" s="19"/>
       <c r="W32" s="19"/>
       <c r="X32" s="19"/>
@@ -12022,8 +12400,12 @@
       <c r="S33" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T33" s="19"/>
-      <c r="U33" s="19"/>
+      <c r="T33" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U33" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V33" s="19"/>
       <c r="W33" s="19"/>
       <c r="X33" s="19"/>
@@ -12092,8 +12474,12 @@
       <c r="S34" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
+      <c r="T34" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U34" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V34" s="19"/>
       <c r="W34" s="19"/>
       <c r="X34" s="19"/>
@@ -12162,8 +12548,12 @@
       <c r="S35" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T35" s="19"/>
-      <c r="U35" s="19"/>
+      <c r="T35" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U35" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V35" s="19"/>
       <c r="W35" s="19"/>
       <c r="X35" s="19"/>
@@ -12232,8 +12622,12 @@
       <c r="S36" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T36" s="19"/>
-      <c r="U36" s="19"/>
+      <c r="T36" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U36" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V36" s="19"/>
       <c r="W36" s="19"/>
       <c r="X36" s="19"/>
@@ -12302,8 +12696,12 @@
       <c r="S37" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
+      <c r="T37" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U37" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V37" s="19"/>
       <c r="W37" s="19"/>
       <c r="X37" s="19"/>
@@ -12372,8 +12770,12 @@
       <c r="S38" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
+      <c r="T38" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U38" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V38" s="19"/>
       <c r="W38" s="19"/>
       <c r="X38" s="19"/>
@@ -12442,8 +12844,12 @@
       <c r="S39" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T39" s="19"/>
-      <c r="U39" s="19"/>
+      <c r="T39" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U39" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V39" s="19"/>
       <c r="W39" s="19"/>
       <c r="X39" s="19"/>
@@ -12512,8 +12918,12 @@
       <c r="S40" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="T40" s="19"/>
-      <c r="U40" s="19"/>
+      <c r="T40" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U40" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V40" s="19"/>
       <c r="W40" s="19"/>
       <c r="X40" s="19"/>
@@ -12582,8 +12992,12 @@
       <c r="S41" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T41" s="19"/>
-      <c r="U41" s="19"/>
+      <c r="T41" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U41" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V41" s="19"/>
       <c r="W41" s="19"/>
       <c r="X41" s="19"/>
@@ -12652,8 +13066,12 @@
       <c r="S42" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T42" s="19"/>
-      <c r="U42" s="19"/>
+      <c r="T42" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U42" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V42" s="19"/>
       <c r="W42" s="19"/>
       <c r="X42" s="19"/>
@@ -12722,8 +13140,12 @@
       <c r="S43" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T43" s="19"/>
-      <c r="U43" s="19"/>
+      <c r="T43" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U43" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V43" s="19"/>
       <c r="W43" s="19"/>
       <c r="X43" s="19"/>
@@ -12792,8 +13214,12 @@
       <c r="S44" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T44" s="19"/>
-      <c r="U44" s="19"/>
+      <c r="T44" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U44" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V44" s="19"/>
       <c r="W44" s="19"/>
       <c r="X44" s="19"/>
@@ -12862,8 +13288,12 @@
       <c r="S45" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T45" s="19"/>
-      <c r="U45" s="19"/>
+      <c r="T45" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U45" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V45" s="19"/>
       <c r="W45" s="19"/>
       <c r="X45" s="19"/>
@@ -12932,8 +13362,12 @@
       <c r="S46" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T46" s="19"/>
-      <c r="U46" s="19"/>
+      <c r="T46" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U46" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V46" s="19"/>
       <c r="W46" s="19"/>
       <c r="X46" s="19"/>
@@ -13002,8 +13436,12 @@
       <c r="S47" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T47" s="19"/>
-      <c r="U47" s="19"/>
+      <c r="T47" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U47" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V47" s="19"/>
       <c r="W47" s="19"/>
       <c r="X47" s="19"/>
@@ -13072,8 +13510,12 @@
       <c r="S48" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T48" s="19"/>
-      <c r="U48" s="19"/>
+      <c r="T48" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U48" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V48" s="19"/>
       <c r="W48" s="19"/>
       <c r="X48" s="19"/>
@@ -13142,8 +13584,12 @@
       <c r="S49" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="T49" s="19"/>
-      <c r="U49" s="19"/>
+      <c r="T49" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="U49" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V49" s="19"/>
       <c r="W49" s="19"/>
       <c r="X49" s="19"/>
@@ -13212,8 +13658,12 @@
       <c r="S50" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T50" s="19"/>
-      <c r="U50" s="19"/>
+      <c r="T50" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U50" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V50" s="19"/>
       <c r="W50" s="19"/>
       <c r="X50" s="19"/>
@@ -13282,8 +13732,12 @@
       <c r="S51" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T51" s="19"/>
-      <c r="U51" s="19"/>
+      <c r="T51" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U51" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V51" s="19"/>
       <c r="W51" s="19"/>
       <c r="X51" s="19"/>
@@ -13352,8 +13806,12 @@
       <c r="S52" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T52" s="19"/>
-      <c r="U52" s="19"/>
+      <c r="T52" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U52" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V52" s="19"/>
       <c r="W52" s="19"/>
       <c r="X52" s="19"/>
@@ -13422,8 +13880,12 @@
       <c r="S53" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T53" s="19"/>
-      <c r="U53" s="19"/>
+      <c r="T53" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U53" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V53" s="19"/>
       <c r="W53" s="19"/>
       <c r="X53" s="19"/>
@@ -13492,8 +13954,12 @@
       <c r="S54" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T54" s="19"/>
-      <c r="U54" s="19"/>
+      <c r="T54" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U54" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V54" s="19"/>
       <c r="W54" s="19"/>
       <c r="X54" s="19"/>
@@ -13562,8 +14028,12 @@
       <c r="S55" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T55" s="19"/>
-      <c r="U55" s="19"/>
+      <c r="T55" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U55" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V55" s="19"/>
       <c r="W55" s="19"/>
       <c r="X55" s="19"/>
@@ -13632,8 +14102,12 @@
       <c r="S56" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="T56" s="19"/>
-      <c r="U56" s="19"/>
+      <c r="T56" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="U56" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="V56" s="19"/>
       <c r="W56" s="19"/>
       <c r="X56" s="19"/>
@@ -13647,10 +14121,10 @@
       <c r="AF56" s="19"/>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="62" t="s">
+      <c r="A57" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="63"/>
+      <c r="B57" s="66"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -13718,11 +14192,11 @@
       </c>
       <c r="T57" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U57" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="V57" s="19">
         <f t="shared" si="0"/>
@@ -13770,10 +14244,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="59" t="s">
+      <c r="A58" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="60"/>
+      <c r="B58" s="63"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -13841,11 +14315,11 @@
       </c>
       <c r="T58" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="U58" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="V58" s="24">
         <f t="shared" si="1"/>
@@ -13893,9 +14367,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="N5:Q5"/>
+  <mergeCells count="23">
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:B58"/>
@@ -13903,6 +14375,7 @@
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="B5:B8"/>
+    <mergeCell ref="T5:U5"/>
     <mergeCell ref="N1:AB1"/>
     <mergeCell ref="N2:AB2"/>
     <mergeCell ref="N3:AB3"/>
@@ -13916,6 +14389,8 @@
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="N5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Last Update 29-10-2018 12:10:20.97
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -985,7 +985,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="96">
   <si>
     <t>S.NO</t>
   </si>
@@ -1273,9 +1273,6 @@
   </si>
   <si>
     <t>Lab 4</t>
-  </si>
-  <si>
-    <t>aa</t>
   </si>
 </sst>
 </file>
@@ -1589,7 +1586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1772,6 +1769,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2258,10 +2258,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG57"/>
+  <dimension ref="A1:BL57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AF7" sqref="AF7"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="R5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -2269,34 +2272,35 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
-    <col min="4" max="33" width="4.140625" style="2" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="64" width="4.140625" style="2" customWidth="1"/>
+    <col min="65" max="96" width="4.140625" style="1" customWidth="1"/>
+    <col min="97" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="18.75">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:64" ht="18.75">
+      <c r="A1" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="83" t="s">
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -2317,47 +2321,45 @@
       <c r="AC1" s="50"/>
       <c r="AD1" s="50"/>
       <c r="AE1" s="50"/>
-      <c r="AF1" s="50" t="s">
-        <v>96</v>
-      </c>
+      <c r="AF1" s="50"/>
       <c r="AG1" s="50"/>
     </row>
-    <row r="2" spans="1:33" ht="19.5">
-      <c r="A2" s="70" t="s">
+    <row r="2" spans="1:64" ht="19.5">
+      <c r="A2" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="72"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="73"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="83" t="s">
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="84" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="84" t="s">
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="84"/>
-      <c r="S2" s="84"/>
-      <c r="T2" s="84"/>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -2369,42 +2371,42 @@
       <c r="AF2" s="50"/>
       <c r="AG2" s="50"/>
     </row>
-    <row r="3" spans="1:33" ht="18.75">
-      <c r="A3" s="73" t="s">
+    <row r="3" spans="1:64" ht="18.75">
+      <c r="A3" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="75"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="76"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="64" t="s">
+      <c r="F3" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="83" t="s">
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="84" t="s">
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="84"/>
-      <c r="S3" s="84"/>
-      <c r="T3" s="84"/>
-      <c r="U3" s="84"/>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -2416,34 +2418,34 @@
       <c r="AF3" s="51"/>
       <c r="AG3" s="51"/>
     </row>
-    <row r="4" spans="1:33" ht="18.75">
-      <c r="A4" s="73" t="s">
+    <row r="4" spans="1:64" ht="18.75">
+      <c r="A4" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="80">
+      <c r="B4" s="75"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="81">
         <v>43344</v>
       </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="82"/>
+      <c r="T4" s="82"/>
+      <c r="U4" s="82"/>
+      <c r="V4" s="82"/>
+      <c r="W4" s="83"/>
       <c r="X4" s="57"/>
       <c r="Y4" s="57"/>
       <c r="Z4" s="57"/>
@@ -2454,12 +2456,43 @@
       <c r="AE4" s="57"/>
       <c r="AF4" s="57"/>
       <c r="AG4" s="57"/>
-    </row>
-    <row r="5" spans="1:33">
-      <c r="A5" s="76" t="s">
+      <c r="AH4" s="62"/>
+      <c r="AI4" s="62"/>
+      <c r="AJ4" s="62"/>
+      <c r="AK4" s="62"/>
+      <c r="AL4" s="62"/>
+      <c r="AM4" s="62"/>
+      <c r="AN4" s="62"/>
+      <c r="AO4" s="62"/>
+      <c r="AP4" s="62"/>
+      <c r="AQ4" s="62"/>
+      <c r="AR4" s="62"/>
+      <c r="AS4" s="62"/>
+      <c r="AT4" s="62"/>
+      <c r="AU4" s="62"/>
+      <c r="AV4" s="62"/>
+      <c r="AW4" s="62"/>
+      <c r="AX4" s="62"/>
+      <c r="AY4" s="62"/>
+      <c r="AZ4" s="62"/>
+      <c r="BA4" s="62"/>
+      <c r="BB4" s="62"/>
+      <c r="BC4" s="62"/>
+      <c r="BD4" s="62"/>
+      <c r="BE4" s="62"/>
+      <c r="BF4" s="62"/>
+      <c r="BG4" s="62"/>
+      <c r="BH4" s="62"/>
+      <c r="BI4" s="62"/>
+      <c r="BJ4" s="62"/>
+      <c r="BK4" s="62"/>
+      <c r="BL4" s="62"/>
+    </row>
+    <row r="5" spans="1:64">
+      <c r="A5" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="68" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -2555,10 +2588,57 @@
       <c r="AG5" s="12">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:33">
-      <c r="A6" s="76"/>
-      <c r="B6" s="68"/>
+      <c r="AH5" s="62">
+        <v>10</v>
+      </c>
+      <c r="AI5" s="62">
+        <v>10</v>
+      </c>
+      <c r="AJ5" s="62">
+        <v>10</v>
+      </c>
+      <c r="AK5" s="62">
+        <v>10</v>
+      </c>
+      <c r="AL5" s="62">
+        <v>10</v>
+      </c>
+      <c r="AM5" s="62">
+        <v>10</v>
+      </c>
+      <c r="AN5" s="62">
+        <v>10</v>
+      </c>
+      <c r="AO5" s="62">
+        <v>10</v>
+      </c>
+      <c r="AP5" s="62"/>
+      <c r="AQ5" s="62"/>
+      <c r="AR5" s="62"/>
+      <c r="AS5" s="62"/>
+      <c r="AT5" s="62"/>
+      <c r="AU5" s="62"/>
+      <c r="AV5" s="62"/>
+      <c r="AW5" s="62"/>
+      <c r="AX5" s="62"/>
+      <c r="AY5" s="62"/>
+      <c r="AZ5" s="62"/>
+      <c r="BA5" s="62"/>
+      <c r="BB5" s="62"/>
+      <c r="BC5" s="62"/>
+      <c r="BD5" s="62"/>
+      <c r="BE5" s="62"/>
+      <c r="BF5" s="62"/>
+      <c r="BG5" s="62"/>
+      <c r="BH5" s="62"/>
+      <c r="BI5" s="62"/>
+      <c r="BJ5" s="62"/>
+      <c r="BK5" s="62"/>
+      <c r="BL5" s="62"/>
+    </row>
+    <row r="6" spans="1:64">
+      <c r="A6" s="77"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -2652,12 +2732,59 @@
       <c r="AG6" s="12">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" ht="15" customHeight="1">
+      <c r="AH6" s="62">
+        <v>26</v>
+      </c>
+      <c r="AI6" s="62">
+        <v>26</v>
+      </c>
+      <c r="AJ6" s="62">
+        <v>26</v>
+      </c>
+      <c r="AK6" s="62">
+        <v>26</v>
+      </c>
+      <c r="AL6" s="62">
+        <v>26</v>
+      </c>
+      <c r="AM6" s="62">
+        <v>26</v>
+      </c>
+      <c r="AN6" s="62">
+        <v>26</v>
+      </c>
+      <c r="AO6" s="62">
+        <v>26</v>
+      </c>
+      <c r="AP6" s="62"/>
+      <c r="AQ6" s="62"/>
+      <c r="AR6" s="62"/>
+      <c r="AS6" s="62"/>
+      <c r="AT6" s="62"/>
+      <c r="AU6" s="62"/>
+      <c r="AV6" s="62"/>
+      <c r="AW6" s="62"/>
+      <c r="AX6" s="62"/>
+      <c r="AY6" s="62"/>
+      <c r="AZ6" s="62"/>
+      <c r="BA6" s="62"/>
+      <c r="BB6" s="62"/>
+      <c r="BC6" s="62"/>
+      <c r="BD6" s="62"/>
+      <c r="BE6" s="62"/>
+      <c r="BF6" s="62"/>
+      <c r="BG6" s="62"/>
+      <c r="BH6" s="62"/>
+      <c r="BI6" s="62"/>
+      <c r="BJ6" s="62"/>
+      <c r="BK6" s="62"/>
+      <c r="BL6" s="62"/>
+    </row>
+    <row r="7" spans="1:64" ht="15" customHeight="1">
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="69"/>
+      <c r="B7" s="70"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -2751,8 +2878,55 @@
       <c r="AG7" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" ht="15" customHeight="1">
+      <c r="AH7" s="62">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="62">
+        <v>2</v>
+      </c>
+      <c r="AJ7" s="62">
+        <v>3</v>
+      </c>
+      <c r="AK7" s="62">
+        <v>4</v>
+      </c>
+      <c r="AL7" s="62">
+        <v>5</v>
+      </c>
+      <c r="AM7" s="62">
+        <v>6</v>
+      </c>
+      <c r="AN7" s="62">
+        <v>7</v>
+      </c>
+      <c r="AO7" s="62">
+        <v>8</v>
+      </c>
+      <c r="AP7" s="62"/>
+      <c r="AQ7" s="62"/>
+      <c r="AR7" s="62"/>
+      <c r="AS7" s="62"/>
+      <c r="AT7" s="62"/>
+      <c r="AU7" s="62"/>
+      <c r="AV7" s="62"/>
+      <c r="AW7" s="62"/>
+      <c r="AX7" s="62"/>
+      <c r="AY7" s="62"/>
+      <c r="AZ7" s="62"/>
+      <c r="BA7" s="62"/>
+      <c r="BB7" s="62"/>
+      <c r="BC7" s="62"/>
+      <c r="BD7" s="62"/>
+      <c r="BE7" s="62"/>
+      <c r="BF7" s="62"/>
+      <c r="BG7" s="62"/>
+      <c r="BH7" s="62"/>
+      <c r="BI7" s="62"/>
+      <c r="BJ7" s="62"/>
+      <c r="BK7" s="62"/>
+      <c r="BL7" s="62"/>
+    </row>
+    <row r="8" spans="1:64" ht="15" customHeight="1">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -2850,8 +3024,55 @@
       <c r="AG8" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" ht="15" customHeight="1">
+      <c r="AH8" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI8" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ8" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK8" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL8" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM8" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN8" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO8" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP8" s="62"/>
+      <c r="AQ8" s="62"/>
+      <c r="AR8" s="62"/>
+      <c r="AS8" s="62"/>
+      <c r="AT8" s="62"/>
+      <c r="AU8" s="62"/>
+      <c r="AV8" s="62"/>
+      <c r="AW8" s="62"/>
+      <c r="AX8" s="62"/>
+      <c r="AY8" s="62"/>
+      <c r="AZ8" s="62"/>
+      <c r="BA8" s="62"/>
+      <c r="BB8" s="62"/>
+      <c r="BC8" s="62"/>
+      <c r="BD8" s="62"/>
+      <c r="BE8" s="62"/>
+      <c r="BF8" s="62"/>
+      <c r="BG8" s="62"/>
+      <c r="BH8" s="62"/>
+      <c r="BI8" s="62"/>
+      <c r="BJ8" s="62"/>
+      <c r="BK8" s="62"/>
+      <c r="BL8" s="62"/>
+    </row>
+    <row r="9" spans="1:64" ht="15" customHeight="1">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -2949,8 +3170,55 @@
       <c r="AG9" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:33" ht="15" customHeight="1">
+      <c r="AH9" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI9" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ9" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK9" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL9" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM9" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN9" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO9" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP9" s="62"/>
+      <c r="AQ9" s="62"/>
+      <c r="AR9" s="62"/>
+      <c r="AS9" s="62"/>
+      <c r="AT9" s="62"/>
+      <c r="AU9" s="62"/>
+      <c r="AV9" s="62"/>
+      <c r="AW9" s="62"/>
+      <c r="AX9" s="62"/>
+      <c r="AY9" s="62"/>
+      <c r="AZ9" s="62"/>
+      <c r="BA9" s="62"/>
+      <c r="BB9" s="62"/>
+      <c r="BC9" s="62"/>
+      <c r="BD9" s="62"/>
+      <c r="BE9" s="62"/>
+      <c r="BF9" s="62"/>
+      <c r="BG9" s="62"/>
+      <c r="BH9" s="62"/>
+      <c r="BI9" s="62"/>
+      <c r="BJ9" s="62"/>
+      <c r="BK9" s="62"/>
+      <c r="BL9" s="62"/>
+    </row>
+    <row r="10" spans="1:64" ht="15" customHeight="1">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -3048,8 +3316,55 @@
       <c r="AG10" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:33" ht="15" customHeight="1">
+      <c r="AH10" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI10" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ10" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK10" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL10" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM10" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN10" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO10" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP10" s="62"/>
+      <c r="AQ10" s="62"/>
+      <c r="AR10" s="62"/>
+      <c r="AS10" s="62"/>
+      <c r="AT10" s="62"/>
+      <c r="AU10" s="62"/>
+      <c r="AV10" s="62"/>
+      <c r="AW10" s="62"/>
+      <c r="AX10" s="62"/>
+      <c r="AY10" s="62"/>
+      <c r="AZ10" s="62"/>
+      <c r="BA10" s="62"/>
+      <c r="BB10" s="62"/>
+      <c r="BC10" s="62"/>
+      <c r="BD10" s="62"/>
+      <c r="BE10" s="62"/>
+      <c r="BF10" s="62"/>
+      <c r="BG10" s="62"/>
+      <c r="BH10" s="62"/>
+      <c r="BI10" s="62"/>
+      <c r="BJ10" s="62"/>
+      <c r="BK10" s="62"/>
+      <c r="BL10" s="62"/>
+    </row>
+    <row r="11" spans="1:64" ht="15" customHeight="1">
       <c r="A11" s="3">
         <v>4</v>
       </c>
@@ -3147,8 +3462,55 @@
       <c r="AG11" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:33" ht="15" customHeight="1">
+      <c r="AH11" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI11" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ11" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK11" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL11" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM11" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN11" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO11" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP11" s="62"/>
+      <c r="AQ11" s="62"/>
+      <c r="AR11" s="62"/>
+      <c r="AS11" s="62"/>
+      <c r="AT11" s="62"/>
+      <c r="AU11" s="62"/>
+      <c r="AV11" s="62"/>
+      <c r="AW11" s="62"/>
+      <c r="AX11" s="62"/>
+      <c r="AY11" s="62"/>
+      <c r="AZ11" s="62"/>
+      <c r="BA11" s="62"/>
+      <c r="BB11" s="62"/>
+      <c r="BC11" s="62"/>
+      <c r="BD11" s="62"/>
+      <c r="BE11" s="62"/>
+      <c r="BF11" s="62"/>
+      <c r="BG11" s="62"/>
+      <c r="BH11" s="62"/>
+      <c r="BI11" s="62"/>
+      <c r="BJ11" s="62"/>
+      <c r="BK11" s="62"/>
+      <c r="BL11" s="62"/>
+    </row>
+    <row r="12" spans="1:64" ht="15" customHeight="1">
       <c r="A12" s="3">
         <v>5</v>
       </c>
@@ -3246,8 +3608,55 @@
       <c r="AG12" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" ht="15" customHeight="1">
+      <c r="AH12" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI12" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ12" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK12" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL12" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM12" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN12" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO12" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP12" s="62"/>
+      <c r="AQ12" s="62"/>
+      <c r="AR12" s="62"/>
+      <c r="AS12" s="62"/>
+      <c r="AT12" s="62"/>
+      <c r="AU12" s="62"/>
+      <c r="AV12" s="62"/>
+      <c r="AW12" s="62"/>
+      <c r="AX12" s="62"/>
+      <c r="AY12" s="62"/>
+      <c r="AZ12" s="62"/>
+      <c r="BA12" s="62"/>
+      <c r="BB12" s="62"/>
+      <c r="BC12" s="62"/>
+      <c r="BD12" s="62"/>
+      <c r="BE12" s="62"/>
+      <c r="BF12" s="62"/>
+      <c r="BG12" s="62"/>
+      <c r="BH12" s="62"/>
+      <c r="BI12" s="62"/>
+      <c r="BJ12" s="62"/>
+      <c r="BK12" s="62"/>
+      <c r="BL12" s="62"/>
+    </row>
+    <row r="13" spans="1:64" ht="15" customHeight="1">
       <c r="A13" s="3">
         <v>6</v>
       </c>
@@ -3345,8 +3754,55 @@
       <c r="AG13" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" ht="15" customHeight="1">
+      <c r="AH13" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI13" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ13" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK13" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL13" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM13" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN13" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO13" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP13" s="62"/>
+      <c r="AQ13" s="62"/>
+      <c r="AR13" s="62"/>
+      <c r="AS13" s="62"/>
+      <c r="AT13" s="62"/>
+      <c r="AU13" s="62"/>
+      <c r="AV13" s="62"/>
+      <c r="AW13" s="62"/>
+      <c r="AX13" s="62"/>
+      <c r="AY13" s="62"/>
+      <c r="AZ13" s="62"/>
+      <c r="BA13" s="62"/>
+      <c r="BB13" s="62"/>
+      <c r="BC13" s="62"/>
+      <c r="BD13" s="62"/>
+      <c r="BE13" s="62"/>
+      <c r="BF13" s="62"/>
+      <c r="BG13" s="62"/>
+      <c r="BH13" s="62"/>
+      <c r="BI13" s="62"/>
+      <c r="BJ13" s="62"/>
+      <c r="BK13" s="62"/>
+      <c r="BL13" s="62"/>
+    </row>
+    <row r="14" spans="1:64" ht="15" customHeight="1">
       <c r="A14" s="3">
         <v>7</v>
       </c>
@@ -3444,8 +3900,55 @@
       <c r="AG14" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" ht="15" customHeight="1">
+      <c r="AH14" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI14" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ14" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK14" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL14" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM14" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN14" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO14" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP14" s="62"/>
+      <c r="AQ14" s="62"/>
+      <c r="AR14" s="62"/>
+      <c r="AS14" s="62"/>
+      <c r="AT14" s="62"/>
+      <c r="AU14" s="62"/>
+      <c r="AV14" s="62"/>
+      <c r="AW14" s="62"/>
+      <c r="AX14" s="62"/>
+      <c r="AY14" s="62"/>
+      <c r="AZ14" s="62"/>
+      <c r="BA14" s="62"/>
+      <c r="BB14" s="62"/>
+      <c r="BC14" s="62"/>
+      <c r="BD14" s="62"/>
+      <c r="BE14" s="62"/>
+      <c r="BF14" s="62"/>
+      <c r="BG14" s="62"/>
+      <c r="BH14" s="62"/>
+      <c r="BI14" s="62"/>
+      <c r="BJ14" s="62"/>
+      <c r="BK14" s="62"/>
+      <c r="BL14" s="62"/>
+    </row>
+    <row r="15" spans="1:64" ht="15" customHeight="1">
       <c r="A15" s="3">
         <v>8</v>
       </c>
@@ -3543,8 +4046,55 @@
       <c r="AG15" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:33" ht="15" customHeight="1">
+      <c r="AH15" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI15" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ15" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK15" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL15" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM15" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN15" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO15" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP15" s="62"/>
+      <c r="AQ15" s="62"/>
+      <c r="AR15" s="62"/>
+      <c r="AS15" s="62"/>
+      <c r="AT15" s="62"/>
+      <c r="AU15" s="62"/>
+      <c r="AV15" s="62"/>
+      <c r="AW15" s="62"/>
+      <c r="AX15" s="62"/>
+      <c r="AY15" s="62"/>
+      <c r="AZ15" s="62"/>
+      <c r="BA15" s="62"/>
+      <c r="BB15" s="62"/>
+      <c r="BC15" s="62"/>
+      <c r="BD15" s="62"/>
+      <c r="BE15" s="62"/>
+      <c r="BF15" s="62"/>
+      <c r="BG15" s="62"/>
+      <c r="BH15" s="62"/>
+      <c r="BI15" s="62"/>
+      <c r="BJ15" s="62"/>
+      <c r="BK15" s="62"/>
+      <c r="BL15" s="62"/>
+    </row>
+    <row r="16" spans="1:64" ht="15" customHeight="1">
       <c r="A16" s="3">
         <v>9</v>
       </c>
@@ -3642,8 +4192,55 @@
       <c r="AG16" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:33" ht="15" customHeight="1">
+      <c r="AH16" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI16" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ16" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK16" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL16" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM16" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN16" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO16" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP16" s="62"/>
+      <c r="AQ16" s="62"/>
+      <c r="AR16" s="62"/>
+      <c r="AS16" s="62"/>
+      <c r="AT16" s="62"/>
+      <c r="AU16" s="62"/>
+      <c r="AV16" s="62"/>
+      <c r="AW16" s="62"/>
+      <c r="AX16" s="62"/>
+      <c r="AY16" s="62"/>
+      <c r="AZ16" s="62"/>
+      <c r="BA16" s="62"/>
+      <c r="BB16" s="62"/>
+      <c r="BC16" s="62"/>
+      <c r="BD16" s="62"/>
+      <c r="BE16" s="62"/>
+      <c r="BF16" s="62"/>
+      <c r="BG16" s="62"/>
+      <c r="BH16" s="62"/>
+      <c r="BI16" s="62"/>
+      <c r="BJ16" s="62"/>
+      <c r="BK16" s="62"/>
+      <c r="BL16" s="62"/>
+    </row>
+    <row r="17" spans="1:64" ht="15" customHeight="1">
       <c r="A17" s="3">
         <v>10</v>
       </c>
@@ -3741,8 +4338,55 @@
       <c r="AG17" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:33" ht="15" customHeight="1">
+      <c r="AH17" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI17" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ17" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK17" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL17" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM17" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN17" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO17" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP17" s="62"/>
+      <c r="AQ17" s="62"/>
+      <c r="AR17" s="62"/>
+      <c r="AS17" s="62"/>
+      <c r="AT17" s="62"/>
+      <c r="AU17" s="62"/>
+      <c r="AV17" s="62"/>
+      <c r="AW17" s="62"/>
+      <c r="AX17" s="62"/>
+      <c r="AY17" s="62"/>
+      <c r="AZ17" s="62"/>
+      <c r="BA17" s="62"/>
+      <c r="BB17" s="62"/>
+      <c r="BC17" s="62"/>
+      <c r="BD17" s="62"/>
+      <c r="BE17" s="62"/>
+      <c r="BF17" s="62"/>
+      <c r="BG17" s="62"/>
+      <c r="BH17" s="62"/>
+      <c r="BI17" s="62"/>
+      <c r="BJ17" s="62"/>
+      <c r="BK17" s="62"/>
+      <c r="BL17" s="62"/>
+    </row>
+    <row r="18" spans="1:64" ht="15" customHeight="1">
       <c r="A18" s="3">
         <v>11</v>
       </c>
@@ -3840,8 +4484,55 @@
       <c r="AG18" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:33" ht="15" customHeight="1">
+      <c r="AH18" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI18" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ18" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK18" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL18" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM18" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN18" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO18" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP18" s="62"/>
+      <c r="AQ18" s="62"/>
+      <c r="AR18" s="62"/>
+      <c r="AS18" s="62"/>
+      <c r="AT18" s="62"/>
+      <c r="AU18" s="62"/>
+      <c r="AV18" s="62"/>
+      <c r="AW18" s="62"/>
+      <c r="AX18" s="62"/>
+      <c r="AY18" s="62"/>
+      <c r="AZ18" s="62"/>
+      <c r="BA18" s="62"/>
+      <c r="BB18" s="62"/>
+      <c r="BC18" s="62"/>
+      <c r="BD18" s="62"/>
+      <c r="BE18" s="62"/>
+      <c r="BF18" s="62"/>
+      <c r="BG18" s="62"/>
+      <c r="BH18" s="62"/>
+      <c r="BI18" s="62"/>
+      <c r="BJ18" s="62"/>
+      <c r="BK18" s="62"/>
+      <c r="BL18" s="62"/>
+    </row>
+    <row r="19" spans="1:64" ht="15" customHeight="1">
       <c r="A19" s="3">
         <v>12</v>
       </c>
@@ -3939,8 +4630,55 @@
       <c r="AG19" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:33" ht="15" customHeight="1">
+      <c r="AH19" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI19" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ19" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK19" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL19" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM19" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN19" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO19" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP19" s="62"/>
+      <c r="AQ19" s="62"/>
+      <c r="AR19" s="62"/>
+      <c r="AS19" s="62"/>
+      <c r="AT19" s="62"/>
+      <c r="AU19" s="62"/>
+      <c r="AV19" s="62"/>
+      <c r="AW19" s="62"/>
+      <c r="AX19" s="62"/>
+      <c r="AY19" s="62"/>
+      <c r="AZ19" s="62"/>
+      <c r="BA19" s="62"/>
+      <c r="BB19" s="62"/>
+      <c r="BC19" s="62"/>
+      <c r="BD19" s="62"/>
+      <c r="BE19" s="62"/>
+      <c r="BF19" s="62"/>
+      <c r="BG19" s="62"/>
+      <c r="BH19" s="62"/>
+      <c r="BI19" s="62"/>
+      <c r="BJ19" s="62"/>
+      <c r="BK19" s="62"/>
+      <c r="BL19" s="62"/>
+    </row>
+    <row r="20" spans="1:64" ht="15" customHeight="1">
       <c r="A20" s="3">
         <v>13</v>
       </c>
@@ -4038,8 +4776,55 @@
       <c r="AG20" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:33" ht="15" customHeight="1">
+      <c r="AH20" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI20" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ20" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK20" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL20" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM20" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN20" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO20" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP20" s="62"/>
+      <c r="AQ20" s="62"/>
+      <c r="AR20" s="62"/>
+      <c r="AS20" s="62"/>
+      <c r="AT20" s="62"/>
+      <c r="AU20" s="62"/>
+      <c r="AV20" s="62"/>
+      <c r="AW20" s="62"/>
+      <c r="AX20" s="62"/>
+      <c r="AY20" s="62"/>
+      <c r="AZ20" s="62"/>
+      <c r="BA20" s="62"/>
+      <c r="BB20" s="62"/>
+      <c r="BC20" s="62"/>
+      <c r="BD20" s="62"/>
+      <c r="BE20" s="62"/>
+      <c r="BF20" s="62"/>
+      <c r="BG20" s="62"/>
+      <c r="BH20" s="62"/>
+      <c r="BI20" s="62"/>
+      <c r="BJ20" s="62"/>
+      <c r="BK20" s="62"/>
+      <c r="BL20" s="62"/>
+    </row>
+    <row r="21" spans="1:64" ht="15" customHeight="1">
       <c r="A21" s="3">
         <v>14</v>
       </c>
@@ -4137,8 +4922,55 @@
       <c r="AG21" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="1:33" ht="15" customHeight="1">
+      <c r="AH21" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI21" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ21" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK21" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL21" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM21" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN21" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO21" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP21" s="62"/>
+      <c r="AQ21" s="62"/>
+      <c r="AR21" s="62"/>
+      <c r="AS21" s="62"/>
+      <c r="AT21" s="62"/>
+      <c r="AU21" s="62"/>
+      <c r="AV21" s="62"/>
+      <c r="AW21" s="62"/>
+      <c r="AX21" s="62"/>
+      <c r="AY21" s="62"/>
+      <c r="AZ21" s="62"/>
+      <c r="BA21" s="62"/>
+      <c r="BB21" s="62"/>
+      <c r="BC21" s="62"/>
+      <c r="BD21" s="62"/>
+      <c r="BE21" s="62"/>
+      <c r="BF21" s="62"/>
+      <c r="BG21" s="62"/>
+      <c r="BH21" s="62"/>
+      <c r="BI21" s="62"/>
+      <c r="BJ21" s="62"/>
+      <c r="BK21" s="62"/>
+      <c r="BL21" s="62"/>
+    </row>
+    <row r="22" spans="1:64" ht="15" customHeight="1">
       <c r="A22" s="3">
         <v>15</v>
       </c>
@@ -4236,8 +5068,55 @@
       <c r="AG22" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:33" ht="15" customHeight="1">
+      <c r="AH22" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI22" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ22" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK22" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL22" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM22" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN22" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO22" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP22" s="62"/>
+      <c r="AQ22" s="62"/>
+      <c r="AR22" s="62"/>
+      <c r="AS22" s="62"/>
+      <c r="AT22" s="62"/>
+      <c r="AU22" s="62"/>
+      <c r="AV22" s="62"/>
+      <c r="AW22" s="62"/>
+      <c r="AX22" s="62"/>
+      <c r="AY22" s="62"/>
+      <c r="AZ22" s="62"/>
+      <c r="BA22" s="62"/>
+      <c r="BB22" s="62"/>
+      <c r="BC22" s="62"/>
+      <c r="BD22" s="62"/>
+      <c r="BE22" s="62"/>
+      <c r="BF22" s="62"/>
+      <c r="BG22" s="62"/>
+      <c r="BH22" s="62"/>
+      <c r="BI22" s="62"/>
+      <c r="BJ22" s="62"/>
+      <c r="BK22" s="62"/>
+      <c r="BL22" s="62"/>
+    </row>
+    <row r="23" spans="1:64" ht="15" customHeight="1">
       <c r="A23" s="3">
         <v>16</v>
       </c>
@@ -4335,8 +5214,55 @@
       <c r="AG23" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="1:33" ht="15" customHeight="1">
+      <c r="AH23" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI23" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ23" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK23" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL23" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM23" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN23" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO23" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP23" s="62"/>
+      <c r="AQ23" s="62"/>
+      <c r="AR23" s="62"/>
+      <c r="AS23" s="62"/>
+      <c r="AT23" s="62"/>
+      <c r="AU23" s="62"/>
+      <c r="AV23" s="62"/>
+      <c r="AW23" s="62"/>
+      <c r="AX23" s="62"/>
+      <c r="AY23" s="62"/>
+      <c r="AZ23" s="62"/>
+      <c r="BA23" s="62"/>
+      <c r="BB23" s="62"/>
+      <c r="BC23" s="62"/>
+      <c r="BD23" s="62"/>
+      <c r="BE23" s="62"/>
+      <c r="BF23" s="62"/>
+      <c r="BG23" s="62"/>
+      <c r="BH23" s="62"/>
+      <c r="BI23" s="62"/>
+      <c r="BJ23" s="62"/>
+      <c r="BK23" s="62"/>
+      <c r="BL23" s="62"/>
+    </row>
+    <row r="24" spans="1:64" ht="15" customHeight="1">
       <c r="A24" s="3">
         <v>17</v>
       </c>
@@ -4434,8 +5360,55 @@
       <c r="AG24" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:33" ht="15" customHeight="1">
+      <c r="AH24" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI24" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ24" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK24" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL24" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM24" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN24" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO24" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP24" s="62"/>
+      <c r="AQ24" s="62"/>
+      <c r="AR24" s="62"/>
+      <c r="AS24" s="62"/>
+      <c r="AT24" s="62"/>
+      <c r="AU24" s="62"/>
+      <c r="AV24" s="62"/>
+      <c r="AW24" s="62"/>
+      <c r="AX24" s="62"/>
+      <c r="AY24" s="62"/>
+      <c r="AZ24" s="62"/>
+      <c r="BA24" s="62"/>
+      <c r="BB24" s="62"/>
+      <c r="BC24" s="62"/>
+      <c r="BD24" s="62"/>
+      <c r="BE24" s="62"/>
+      <c r="BF24" s="62"/>
+      <c r="BG24" s="62"/>
+      <c r="BH24" s="62"/>
+      <c r="BI24" s="62"/>
+      <c r="BJ24" s="62"/>
+      <c r="BK24" s="62"/>
+      <c r="BL24" s="62"/>
+    </row>
+    <row r="25" spans="1:64" ht="15" customHeight="1">
       <c r="A25" s="3">
         <v>18</v>
       </c>
@@ -4533,8 +5506,55 @@
       <c r="AG25" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="1:33" ht="15" customHeight="1">
+      <c r="AH25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP25" s="62"/>
+      <c r="AQ25" s="62"/>
+      <c r="AR25" s="62"/>
+      <c r="AS25" s="62"/>
+      <c r="AT25" s="62"/>
+      <c r="AU25" s="62"/>
+      <c r="AV25" s="62"/>
+      <c r="AW25" s="62"/>
+      <c r="AX25" s="62"/>
+      <c r="AY25" s="62"/>
+      <c r="AZ25" s="62"/>
+      <c r="BA25" s="62"/>
+      <c r="BB25" s="62"/>
+      <c r="BC25" s="62"/>
+      <c r="BD25" s="62"/>
+      <c r="BE25" s="62"/>
+      <c r="BF25" s="62"/>
+      <c r="BG25" s="62"/>
+      <c r="BH25" s="62"/>
+      <c r="BI25" s="62"/>
+      <c r="BJ25" s="62"/>
+      <c r="BK25" s="62"/>
+      <c r="BL25" s="62"/>
+    </row>
+    <row r="26" spans="1:64" ht="15" customHeight="1">
       <c r="A26" s="3">
         <v>19</v>
       </c>
@@ -4632,8 +5652,55 @@
       <c r="AG26" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:33" ht="15" customHeight="1">
+      <c r="AH26" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI26" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ26" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK26" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL26" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM26" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN26" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO26" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP26" s="62"/>
+      <c r="AQ26" s="62"/>
+      <c r="AR26" s="62"/>
+      <c r="AS26" s="62"/>
+      <c r="AT26" s="62"/>
+      <c r="AU26" s="62"/>
+      <c r="AV26" s="62"/>
+      <c r="AW26" s="62"/>
+      <c r="AX26" s="62"/>
+      <c r="AY26" s="62"/>
+      <c r="AZ26" s="62"/>
+      <c r="BA26" s="62"/>
+      <c r="BB26" s="62"/>
+      <c r="BC26" s="62"/>
+      <c r="BD26" s="62"/>
+      <c r="BE26" s="62"/>
+      <c r="BF26" s="62"/>
+      <c r="BG26" s="62"/>
+      <c r="BH26" s="62"/>
+      <c r="BI26" s="62"/>
+      <c r="BJ26" s="62"/>
+      <c r="BK26" s="62"/>
+      <c r="BL26" s="62"/>
+    </row>
+    <row r="27" spans="1:64" ht="15" customHeight="1">
       <c r="A27" s="3">
         <v>20</v>
       </c>
@@ -4731,8 +5798,55 @@
       <c r="AG27" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="1:33" ht="15" customHeight="1">
+      <c r="AH27" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI27" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ27" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK27" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL27" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM27" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN27" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO27" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP27" s="62"/>
+      <c r="AQ27" s="62"/>
+      <c r="AR27" s="62"/>
+      <c r="AS27" s="62"/>
+      <c r="AT27" s="62"/>
+      <c r="AU27" s="62"/>
+      <c r="AV27" s="62"/>
+      <c r="AW27" s="62"/>
+      <c r="AX27" s="62"/>
+      <c r="AY27" s="62"/>
+      <c r="AZ27" s="62"/>
+      <c r="BA27" s="62"/>
+      <c r="BB27" s="62"/>
+      <c r="BC27" s="62"/>
+      <c r="BD27" s="62"/>
+      <c r="BE27" s="62"/>
+      <c r="BF27" s="62"/>
+      <c r="BG27" s="62"/>
+      <c r="BH27" s="62"/>
+      <c r="BI27" s="62"/>
+      <c r="BJ27" s="62"/>
+      <c r="BK27" s="62"/>
+      <c r="BL27" s="62"/>
+    </row>
+    <row r="28" spans="1:64" ht="15" customHeight="1">
       <c r="A28" s="3">
         <v>21</v>
       </c>
@@ -4830,8 +5944,55 @@
       <c r="AG28" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:33" ht="15" customHeight="1">
+      <c r="AH28" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI28" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ28" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK28" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL28" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM28" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN28" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO28" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP28" s="62"/>
+      <c r="AQ28" s="62"/>
+      <c r="AR28" s="62"/>
+      <c r="AS28" s="62"/>
+      <c r="AT28" s="62"/>
+      <c r="AU28" s="62"/>
+      <c r="AV28" s="62"/>
+      <c r="AW28" s="62"/>
+      <c r="AX28" s="62"/>
+      <c r="AY28" s="62"/>
+      <c r="AZ28" s="62"/>
+      <c r="BA28" s="62"/>
+      <c r="BB28" s="62"/>
+      <c r="BC28" s="62"/>
+      <c r="BD28" s="62"/>
+      <c r="BE28" s="62"/>
+      <c r="BF28" s="62"/>
+      <c r="BG28" s="62"/>
+      <c r="BH28" s="62"/>
+      <c r="BI28" s="62"/>
+      <c r="BJ28" s="62"/>
+      <c r="BK28" s="62"/>
+      <c r="BL28" s="62"/>
+    </row>
+    <row r="29" spans="1:64" ht="15" customHeight="1">
       <c r="A29" s="3">
         <v>22</v>
       </c>
@@ -4929,8 +6090,55 @@
       <c r="AG29" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="1:33" ht="15" customHeight="1">
+      <c r="AH29" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI29" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ29" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK29" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL29" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM29" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN29" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO29" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP29" s="62"/>
+      <c r="AQ29" s="62"/>
+      <c r="AR29" s="62"/>
+      <c r="AS29" s="62"/>
+      <c r="AT29" s="62"/>
+      <c r="AU29" s="62"/>
+      <c r="AV29" s="62"/>
+      <c r="AW29" s="62"/>
+      <c r="AX29" s="62"/>
+      <c r="AY29" s="62"/>
+      <c r="AZ29" s="62"/>
+      <c r="BA29" s="62"/>
+      <c r="BB29" s="62"/>
+      <c r="BC29" s="62"/>
+      <c r="BD29" s="62"/>
+      <c r="BE29" s="62"/>
+      <c r="BF29" s="62"/>
+      <c r="BG29" s="62"/>
+      <c r="BH29" s="62"/>
+      <c r="BI29" s="62"/>
+      <c r="BJ29" s="62"/>
+      <c r="BK29" s="62"/>
+      <c r="BL29" s="62"/>
+    </row>
+    <row r="30" spans="1:64" ht="15" customHeight="1">
       <c r="A30" s="3">
         <v>23</v>
       </c>
@@ -5028,8 +6236,55 @@
       <c r="AG30" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:33" ht="15" customHeight="1">
+      <c r="AH30" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI30" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ30" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK30" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL30" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM30" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN30" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO30" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP30" s="62"/>
+      <c r="AQ30" s="62"/>
+      <c r="AR30" s="62"/>
+      <c r="AS30" s="62"/>
+      <c r="AT30" s="62"/>
+      <c r="AU30" s="62"/>
+      <c r="AV30" s="62"/>
+      <c r="AW30" s="62"/>
+      <c r="AX30" s="62"/>
+      <c r="AY30" s="62"/>
+      <c r="AZ30" s="62"/>
+      <c r="BA30" s="62"/>
+      <c r="BB30" s="62"/>
+      <c r="BC30" s="62"/>
+      <c r="BD30" s="62"/>
+      <c r="BE30" s="62"/>
+      <c r="BF30" s="62"/>
+      <c r="BG30" s="62"/>
+      <c r="BH30" s="62"/>
+      <c r="BI30" s="62"/>
+      <c r="BJ30" s="62"/>
+      <c r="BK30" s="62"/>
+      <c r="BL30" s="62"/>
+    </row>
+    <row r="31" spans="1:64" ht="15" customHeight="1">
       <c r="A31" s="3">
         <v>24</v>
       </c>
@@ -5127,8 +6382,55 @@
       <c r="AG31" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:33" ht="15" customHeight="1">
+      <c r="AH31" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI31" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ31" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK31" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL31" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM31" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN31" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO31" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP31" s="62"/>
+      <c r="AQ31" s="62"/>
+      <c r="AR31" s="62"/>
+      <c r="AS31" s="62"/>
+      <c r="AT31" s="62"/>
+      <c r="AU31" s="62"/>
+      <c r="AV31" s="62"/>
+      <c r="AW31" s="62"/>
+      <c r="AX31" s="62"/>
+      <c r="AY31" s="62"/>
+      <c r="AZ31" s="62"/>
+      <c r="BA31" s="62"/>
+      <c r="BB31" s="62"/>
+      <c r="BC31" s="62"/>
+      <c r="BD31" s="62"/>
+      <c r="BE31" s="62"/>
+      <c r="BF31" s="62"/>
+      <c r="BG31" s="62"/>
+      <c r="BH31" s="62"/>
+      <c r="BI31" s="62"/>
+      <c r="BJ31" s="62"/>
+      <c r="BK31" s="62"/>
+      <c r="BL31" s="62"/>
+    </row>
+    <row r="32" spans="1:64" ht="15" customHeight="1">
       <c r="A32" s="3">
         <v>25</v>
       </c>
@@ -5226,8 +6528,55 @@
       <c r="AG32" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" spans="1:33" ht="15" customHeight="1">
+      <c r="AH32" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI32" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ32" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK32" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL32" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM32" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN32" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO32" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP32" s="62"/>
+      <c r="AQ32" s="62"/>
+      <c r="AR32" s="62"/>
+      <c r="AS32" s="62"/>
+      <c r="AT32" s="62"/>
+      <c r="AU32" s="62"/>
+      <c r="AV32" s="62"/>
+      <c r="AW32" s="62"/>
+      <c r="AX32" s="62"/>
+      <c r="AY32" s="62"/>
+      <c r="AZ32" s="62"/>
+      <c r="BA32" s="62"/>
+      <c r="BB32" s="62"/>
+      <c r="BC32" s="62"/>
+      <c r="BD32" s="62"/>
+      <c r="BE32" s="62"/>
+      <c r="BF32" s="62"/>
+      <c r="BG32" s="62"/>
+      <c r="BH32" s="62"/>
+      <c r="BI32" s="62"/>
+      <c r="BJ32" s="62"/>
+      <c r="BK32" s="62"/>
+      <c r="BL32" s="62"/>
+    </row>
+    <row r="33" spans="1:64" ht="15" customHeight="1">
       <c r="A33" s="3">
         <v>26</v>
       </c>
@@ -5325,8 +6674,55 @@
       <c r="AG33" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" spans="1:33" ht="15" customHeight="1">
+      <c r="AH33" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI33" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ33" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK33" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL33" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM33" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN33" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO33" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP33" s="62"/>
+      <c r="AQ33" s="62"/>
+      <c r="AR33" s="62"/>
+      <c r="AS33" s="62"/>
+      <c r="AT33" s="62"/>
+      <c r="AU33" s="62"/>
+      <c r="AV33" s="62"/>
+      <c r="AW33" s="62"/>
+      <c r="AX33" s="62"/>
+      <c r="AY33" s="62"/>
+      <c r="AZ33" s="62"/>
+      <c r="BA33" s="62"/>
+      <c r="BB33" s="62"/>
+      <c r="BC33" s="62"/>
+      <c r="BD33" s="62"/>
+      <c r="BE33" s="62"/>
+      <c r="BF33" s="62"/>
+      <c r="BG33" s="62"/>
+      <c r="BH33" s="62"/>
+      <c r="BI33" s="62"/>
+      <c r="BJ33" s="62"/>
+      <c r="BK33" s="62"/>
+      <c r="BL33" s="62"/>
+    </row>
+    <row r="34" spans="1:64" ht="15" customHeight="1">
       <c r="A34" s="3">
         <v>27</v>
       </c>
@@ -5424,8 +6820,55 @@
       <c r="AG34" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="35" spans="1:33" ht="15" customHeight="1">
+      <c r="AH34" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI34" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ34" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK34" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL34" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM34" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN34" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO34" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP34" s="62"/>
+      <c r="AQ34" s="62"/>
+      <c r="AR34" s="62"/>
+      <c r="AS34" s="62"/>
+      <c r="AT34" s="62"/>
+      <c r="AU34" s="62"/>
+      <c r="AV34" s="62"/>
+      <c r="AW34" s="62"/>
+      <c r="AX34" s="62"/>
+      <c r="AY34" s="62"/>
+      <c r="AZ34" s="62"/>
+      <c r="BA34" s="62"/>
+      <c r="BB34" s="62"/>
+      <c r="BC34" s="62"/>
+      <c r="BD34" s="62"/>
+      <c r="BE34" s="62"/>
+      <c r="BF34" s="62"/>
+      <c r="BG34" s="62"/>
+      <c r="BH34" s="62"/>
+      <c r="BI34" s="62"/>
+      <c r="BJ34" s="62"/>
+      <c r="BK34" s="62"/>
+      <c r="BL34" s="62"/>
+    </row>
+    <row r="35" spans="1:64" ht="15" customHeight="1">
       <c r="A35" s="3">
         <v>28</v>
       </c>
@@ -5523,8 +6966,55 @@
       <c r="AG35" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:33" ht="15" customHeight="1">
+      <c r="AH35" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI35" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ35" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK35" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL35" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM35" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN35" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO35" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP35" s="62"/>
+      <c r="AQ35" s="62"/>
+      <c r="AR35" s="62"/>
+      <c r="AS35" s="62"/>
+      <c r="AT35" s="62"/>
+      <c r="AU35" s="62"/>
+      <c r="AV35" s="62"/>
+      <c r="AW35" s="62"/>
+      <c r="AX35" s="62"/>
+      <c r="AY35" s="62"/>
+      <c r="AZ35" s="62"/>
+      <c r="BA35" s="62"/>
+      <c r="BB35" s="62"/>
+      <c r="BC35" s="62"/>
+      <c r="BD35" s="62"/>
+      <c r="BE35" s="62"/>
+      <c r="BF35" s="62"/>
+      <c r="BG35" s="62"/>
+      <c r="BH35" s="62"/>
+      <c r="BI35" s="62"/>
+      <c r="BJ35" s="62"/>
+      <c r="BK35" s="62"/>
+      <c r="BL35" s="62"/>
+    </row>
+    <row r="36" spans="1:64" ht="15" customHeight="1">
       <c r="A36" s="3">
         <v>29</v>
       </c>
@@ -5622,8 +7112,55 @@
       <c r="AG36" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="37" spans="1:33" ht="15" customHeight="1">
+      <c r="AH36" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI36" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ36" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK36" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL36" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM36" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN36" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO36" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP36" s="62"/>
+      <c r="AQ36" s="62"/>
+      <c r="AR36" s="62"/>
+      <c r="AS36" s="62"/>
+      <c r="AT36" s="62"/>
+      <c r="AU36" s="62"/>
+      <c r="AV36" s="62"/>
+      <c r="AW36" s="62"/>
+      <c r="AX36" s="62"/>
+      <c r="AY36" s="62"/>
+      <c r="AZ36" s="62"/>
+      <c r="BA36" s="62"/>
+      <c r="BB36" s="62"/>
+      <c r="BC36" s="62"/>
+      <c r="BD36" s="62"/>
+      <c r="BE36" s="62"/>
+      <c r="BF36" s="62"/>
+      <c r="BG36" s="62"/>
+      <c r="BH36" s="62"/>
+      <c r="BI36" s="62"/>
+      <c r="BJ36" s="62"/>
+      <c r="BK36" s="62"/>
+      <c r="BL36" s="62"/>
+    </row>
+    <row r="37" spans="1:64" ht="15" customHeight="1">
       <c r="A37" s="3">
         <v>30</v>
       </c>
@@ -5721,8 +7258,55 @@
       <c r="AG37" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="38" spans="1:33" ht="15" customHeight="1">
+      <c r="AH37" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI37" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ37" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK37" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL37" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM37" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN37" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO37" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP37" s="62"/>
+      <c r="AQ37" s="62"/>
+      <c r="AR37" s="62"/>
+      <c r="AS37" s="62"/>
+      <c r="AT37" s="62"/>
+      <c r="AU37" s="62"/>
+      <c r="AV37" s="62"/>
+      <c r="AW37" s="62"/>
+      <c r="AX37" s="62"/>
+      <c r="AY37" s="62"/>
+      <c r="AZ37" s="62"/>
+      <c r="BA37" s="62"/>
+      <c r="BB37" s="62"/>
+      <c r="BC37" s="62"/>
+      <c r="BD37" s="62"/>
+      <c r="BE37" s="62"/>
+      <c r="BF37" s="62"/>
+      <c r="BG37" s="62"/>
+      <c r="BH37" s="62"/>
+      <c r="BI37" s="62"/>
+      <c r="BJ37" s="62"/>
+      <c r="BK37" s="62"/>
+      <c r="BL37" s="62"/>
+    </row>
+    <row r="38" spans="1:64" ht="15" customHeight="1">
       <c r="A38" s="3">
         <v>31</v>
       </c>
@@ -5820,8 +7404,55 @@
       <c r="AG38" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="39" spans="1:33" ht="15" customHeight="1">
+      <c r="AH38" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI38" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ38" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK38" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL38" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM38" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN38" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO38" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP38" s="62"/>
+      <c r="AQ38" s="62"/>
+      <c r="AR38" s="62"/>
+      <c r="AS38" s="62"/>
+      <c r="AT38" s="62"/>
+      <c r="AU38" s="62"/>
+      <c r="AV38" s="62"/>
+      <c r="AW38" s="62"/>
+      <c r="AX38" s="62"/>
+      <c r="AY38" s="62"/>
+      <c r="AZ38" s="62"/>
+      <c r="BA38" s="62"/>
+      <c r="BB38" s="62"/>
+      <c r="BC38" s="62"/>
+      <c r="BD38" s="62"/>
+      <c r="BE38" s="62"/>
+      <c r="BF38" s="62"/>
+      <c r="BG38" s="62"/>
+      <c r="BH38" s="62"/>
+      <c r="BI38" s="62"/>
+      <c r="BJ38" s="62"/>
+      <c r="BK38" s="62"/>
+      <c r="BL38" s="62"/>
+    </row>
+    <row r="39" spans="1:64" ht="15" customHeight="1">
       <c r="A39" s="3">
         <v>32</v>
       </c>
@@ -5919,8 +7550,55 @@
       <c r="AG39" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="40" spans="1:33" ht="15" customHeight="1">
+      <c r="AH39" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI39" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ39" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK39" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL39" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM39" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN39" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO39" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP39" s="62"/>
+      <c r="AQ39" s="62"/>
+      <c r="AR39" s="62"/>
+      <c r="AS39" s="62"/>
+      <c r="AT39" s="62"/>
+      <c r="AU39" s="62"/>
+      <c r="AV39" s="62"/>
+      <c r="AW39" s="62"/>
+      <c r="AX39" s="62"/>
+      <c r="AY39" s="62"/>
+      <c r="AZ39" s="62"/>
+      <c r="BA39" s="62"/>
+      <c r="BB39" s="62"/>
+      <c r="BC39" s="62"/>
+      <c r="BD39" s="62"/>
+      <c r="BE39" s="62"/>
+      <c r="BF39" s="62"/>
+      <c r="BG39" s="62"/>
+      <c r="BH39" s="62"/>
+      <c r="BI39" s="62"/>
+      <c r="BJ39" s="62"/>
+      <c r="BK39" s="62"/>
+      <c r="BL39" s="62"/>
+    </row>
+    <row r="40" spans="1:64" ht="15" customHeight="1">
       <c r="A40" s="3">
         <v>33</v>
       </c>
@@ -6018,8 +7696,55 @@
       <c r="AG40" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="41" spans="1:33" ht="15" customHeight="1">
+      <c r="AH40" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI40" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ40" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK40" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL40" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM40" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN40" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO40" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP40" s="62"/>
+      <c r="AQ40" s="62"/>
+      <c r="AR40" s="62"/>
+      <c r="AS40" s="62"/>
+      <c r="AT40" s="62"/>
+      <c r="AU40" s="62"/>
+      <c r="AV40" s="62"/>
+      <c r="AW40" s="62"/>
+      <c r="AX40" s="62"/>
+      <c r="AY40" s="62"/>
+      <c r="AZ40" s="62"/>
+      <c r="BA40" s="62"/>
+      <c r="BB40" s="62"/>
+      <c r="BC40" s="62"/>
+      <c r="BD40" s="62"/>
+      <c r="BE40" s="62"/>
+      <c r="BF40" s="62"/>
+      <c r="BG40" s="62"/>
+      <c r="BH40" s="62"/>
+      <c r="BI40" s="62"/>
+      <c r="BJ40" s="62"/>
+      <c r="BK40" s="62"/>
+      <c r="BL40" s="62"/>
+    </row>
+    <row r="41" spans="1:64" ht="15" customHeight="1">
       <c r="A41" s="3">
         <v>34</v>
       </c>
@@ -6117,8 +7842,55 @@
       <c r="AG41" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="42" spans="1:33" ht="15" customHeight="1">
+      <c r="AH41" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI41" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ41" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK41" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL41" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM41" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN41" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO41" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP41" s="62"/>
+      <c r="AQ41" s="62"/>
+      <c r="AR41" s="62"/>
+      <c r="AS41" s="62"/>
+      <c r="AT41" s="62"/>
+      <c r="AU41" s="62"/>
+      <c r="AV41" s="62"/>
+      <c r="AW41" s="62"/>
+      <c r="AX41" s="62"/>
+      <c r="AY41" s="62"/>
+      <c r="AZ41" s="62"/>
+      <c r="BA41" s="62"/>
+      <c r="BB41" s="62"/>
+      <c r="BC41" s="62"/>
+      <c r="BD41" s="62"/>
+      <c r="BE41" s="62"/>
+      <c r="BF41" s="62"/>
+      <c r="BG41" s="62"/>
+      <c r="BH41" s="62"/>
+      <c r="BI41" s="62"/>
+      <c r="BJ41" s="62"/>
+      <c r="BK41" s="62"/>
+      <c r="BL41" s="62"/>
+    </row>
+    <row r="42" spans="1:64" ht="15" customHeight="1">
       <c r="A42" s="3">
         <v>35</v>
       </c>
@@ -6216,8 +7988,55 @@
       <c r="AG42" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="43" spans="1:33" ht="15" customHeight="1">
+      <c r="AH42" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI42" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ42" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK42" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL42" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM42" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN42" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO42" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP42" s="62"/>
+      <c r="AQ42" s="62"/>
+      <c r="AR42" s="62"/>
+      <c r="AS42" s="62"/>
+      <c r="AT42" s="62"/>
+      <c r="AU42" s="62"/>
+      <c r="AV42" s="62"/>
+      <c r="AW42" s="62"/>
+      <c r="AX42" s="62"/>
+      <c r="AY42" s="62"/>
+      <c r="AZ42" s="62"/>
+      <c r="BA42" s="62"/>
+      <c r="BB42" s="62"/>
+      <c r="BC42" s="62"/>
+      <c r="BD42" s="62"/>
+      <c r="BE42" s="62"/>
+      <c r="BF42" s="62"/>
+      <c r="BG42" s="62"/>
+      <c r="BH42" s="62"/>
+      <c r="BI42" s="62"/>
+      <c r="BJ42" s="62"/>
+      <c r="BK42" s="62"/>
+      <c r="BL42" s="62"/>
+    </row>
+    <row r="43" spans="1:64" ht="15" customHeight="1">
       <c r="A43" s="3">
         <v>36</v>
       </c>
@@ -6315,8 +8134,55 @@
       <c r="AG43" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="44" spans="1:33" ht="15" customHeight="1">
+      <c r="AH43" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI43" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ43" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK43" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL43" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM43" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN43" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO43" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP43" s="62"/>
+      <c r="AQ43" s="62"/>
+      <c r="AR43" s="62"/>
+      <c r="AS43" s="62"/>
+      <c r="AT43" s="62"/>
+      <c r="AU43" s="62"/>
+      <c r="AV43" s="62"/>
+      <c r="AW43" s="62"/>
+      <c r="AX43" s="62"/>
+      <c r="AY43" s="62"/>
+      <c r="AZ43" s="62"/>
+      <c r="BA43" s="62"/>
+      <c r="BB43" s="62"/>
+      <c r="BC43" s="62"/>
+      <c r="BD43" s="62"/>
+      <c r="BE43" s="62"/>
+      <c r="BF43" s="62"/>
+      <c r="BG43" s="62"/>
+      <c r="BH43" s="62"/>
+      <c r="BI43" s="62"/>
+      <c r="BJ43" s="62"/>
+      <c r="BK43" s="62"/>
+      <c r="BL43" s="62"/>
+    </row>
+    <row r="44" spans="1:64" ht="15" customHeight="1">
       <c r="A44" s="3">
         <v>37</v>
       </c>
@@ -6414,8 +8280,55 @@
       <c r="AG44" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="45" spans="1:33" ht="15" customHeight="1">
+      <c r="AH44" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI44" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ44" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK44" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL44" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM44" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN44" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO44" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP44" s="62"/>
+      <c r="AQ44" s="62"/>
+      <c r="AR44" s="62"/>
+      <c r="AS44" s="62"/>
+      <c r="AT44" s="62"/>
+      <c r="AU44" s="62"/>
+      <c r="AV44" s="62"/>
+      <c r="AW44" s="62"/>
+      <c r="AX44" s="62"/>
+      <c r="AY44" s="62"/>
+      <c r="AZ44" s="62"/>
+      <c r="BA44" s="62"/>
+      <c r="BB44" s="62"/>
+      <c r="BC44" s="62"/>
+      <c r="BD44" s="62"/>
+      <c r="BE44" s="62"/>
+      <c r="BF44" s="62"/>
+      <c r="BG44" s="62"/>
+      <c r="BH44" s="62"/>
+      <c r="BI44" s="62"/>
+      <c r="BJ44" s="62"/>
+      <c r="BK44" s="62"/>
+      <c r="BL44" s="62"/>
+    </row>
+    <row r="45" spans="1:64" ht="15" customHeight="1">
       <c r="A45" s="3">
         <v>38</v>
       </c>
@@ -6513,8 +8426,55 @@
       <c r="AG45" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:33" ht="15" customHeight="1">
+      <c r="AH45" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI45" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ45" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK45" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL45" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM45" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN45" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO45" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP45" s="62"/>
+      <c r="AQ45" s="62"/>
+      <c r="AR45" s="62"/>
+      <c r="AS45" s="62"/>
+      <c r="AT45" s="62"/>
+      <c r="AU45" s="62"/>
+      <c r="AV45" s="62"/>
+      <c r="AW45" s="62"/>
+      <c r="AX45" s="62"/>
+      <c r="AY45" s="62"/>
+      <c r="AZ45" s="62"/>
+      <c r="BA45" s="62"/>
+      <c r="BB45" s="62"/>
+      <c r="BC45" s="62"/>
+      <c r="BD45" s="62"/>
+      <c r="BE45" s="62"/>
+      <c r="BF45" s="62"/>
+      <c r="BG45" s="62"/>
+      <c r="BH45" s="62"/>
+      <c r="BI45" s="62"/>
+      <c r="BJ45" s="62"/>
+      <c r="BK45" s="62"/>
+      <c r="BL45" s="62"/>
+    </row>
+    <row r="46" spans="1:64" ht="15" customHeight="1">
       <c r="A46" s="3">
         <v>39</v>
       </c>
@@ -6612,8 +8572,55 @@
       <c r="AG46" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="47" spans="1:33" ht="15" customHeight="1">
+      <c r="AH46" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI46" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ46" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK46" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL46" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM46" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN46" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO46" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP46" s="62"/>
+      <c r="AQ46" s="62"/>
+      <c r="AR46" s="62"/>
+      <c r="AS46" s="62"/>
+      <c r="AT46" s="62"/>
+      <c r="AU46" s="62"/>
+      <c r="AV46" s="62"/>
+      <c r="AW46" s="62"/>
+      <c r="AX46" s="62"/>
+      <c r="AY46" s="62"/>
+      <c r="AZ46" s="62"/>
+      <c r="BA46" s="62"/>
+      <c r="BB46" s="62"/>
+      <c r="BC46" s="62"/>
+      <c r="BD46" s="62"/>
+      <c r="BE46" s="62"/>
+      <c r="BF46" s="62"/>
+      <c r="BG46" s="62"/>
+      <c r="BH46" s="62"/>
+      <c r="BI46" s="62"/>
+      <c r="BJ46" s="62"/>
+      <c r="BK46" s="62"/>
+      <c r="BL46" s="62"/>
+    </row>
+    <row r="47" spans="1:64" ht="15" customHeight="1">
       <c r="A47" s="3">
         <v>40</v>
       </c>
@@ -6711,8 +8718,55 @@
       <c r="AG47" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:33" ht="15" customHeight="1">
+      <c r="AH47" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI47" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ47" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK47" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL47" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM47" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN47" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO47" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP47" s="62"/>
+      <c r="AQ47" s="62"/>
+      <c r="AR47" s="62"/>
+      <c r="AS47" s="62"/>
+      <c r="AT47" s="62"/>
+      <c r="AU47" s="62"/>
+      <c r="AV47" s="62"/>
+      <c r="AW47" s="62"/>
+      <c r="AX47" s="62"/>
+      <c r="AY47" s="62"/>
+      <c r="AZ47" s="62"/>
+      <c r="BA47" s="62"/>
+      <c r="BB47" s="62"/>
+      <c r="BC47" s="62"/>
+      <c r="BD47" s="62"/>
+      <c r="BE47" s="62"/>
+      <c r="BF47" s="62"/>
+      <c r="BG47" s="62"/>
+      <c r="BH47" s="62"/>
+      <c r="BI47" s="62"/>
+      <c r="BJ47" s="62"/>
+      <c r="BK47" s="62"/>
+      <c r="BL47" s="62"/>
+    </row>
+    <row r="48" spans="1:64" ht="15" customHeight="1">
       <c r="A48" s="3">
         <v>41</v>
       </c>
@@ -6810,8 +8864,55 @@
       <c r="AG48" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="49" spans="1:33" ht="15" customHeight="1">
+      <c r="AH48" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI48" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ48" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK48" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL48" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM48" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN48" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO48" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP48" s="62"/>
+      <c r="AQ48" s="62"/>
+      <c r="AR48" s="62"/>
+      <c r="AS48" s="62"/>
+      <c r="AT48" s="62"/>
+      <c r="AU48" s="62"/>
+      <c r="AV48" s="62"/>
+      <c r="AW48" s="62"/>
+      <c r="AX48" s="62"/>
+      <c r="AY48" s="62"/>
+      <c r="AZ48" s="62"/>
+      <c r="BA48" s="62"/>
+      <c r="BB48" s="62"/>
+      <c r="BC48" s="62"/>
+      <c r="BD48" s="62"/>
+      <c r="BE48" s="62"/>
+      <c r="BF48" s="62"/>
+      <c r="BG48" s="62"/>
+      <c r="BH48" s="62"/>
+      <c r="BI48" s="62"/>
+      <c r="BJ48" s="62"/>
+      <c r="BK48" s="62"/>
+      <c r="BL48" s="62"/>
+    </row>
+    <row r="49" spans="1:64" ht="15" customHeight="1">
       <c r="A49" s="3">
         <v>42</v>
       </c>
@@ -6909,8 +9010,55 @@
       <c r="AG49" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="50" spans="1:33" ht="15" customHeight="1">
+      <c r="AH49" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI49" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ49" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK49" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL49" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM49" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN49" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO49" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP49" s="62"/>
+      <c r="AQ49" s="62"/>
+      <c r="AR49" s="62"/>
+      <c r="AS49" s="62"/>
+      <c r="AT49" s="62"/>
+      <c r="AU49" s="62"/>
+      <c r="AV49" s="62"/>
+      <c r="AW49" s="62"/>
+      <c r="AX49" s="62"/>
+      <c r="AY49" s="62"/>
+      <c r="AZ49" s="62"/>
+      <c r="BA49" s="62"/>
+      <c r="BB49" s="62"/>
+      <c r="BC49" s="62"/>
+      <c r="BD49" s="62"/>
+      <c r="BE49" s="62"/>
+      <c r="BF49" s="62"/>
+      <c r="BG49" s="62"/>
+      <c r="BH49" s="62"/>
+      <c r="BI49" s="62"/>
+      <c r="BJ49" s="62"/>
+      <c r="BK49" s="62"/>
+      <c r="BL49" s="62"/>
+    </row>
+    <row r="50" spans="1:64" ht="15" customHeight="1">
       <c r="A50" s="3">
         <v>43</v>
       </c>
@@ -7008,8 +9156,55 @@
       <c r="AG50" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="51" spans="1:33" ht="15" customHeight="1">
+      <c r="AH50" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI50" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ50" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK50" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL50" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM50" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN50" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO50" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP50" s="62"/>
+      <c r="AQ50" s="62"/>
+      <c r="AR50" s="62"/>
+      <c r="AS50" s="62"/>
+      <c r="AT50" s="62"/>
+      <c r="AU50" s="62"/>
+      <c r="AV50" s="62"/>
+      <c r="AW50" s="62"/>
+      <c r="AX50" s="62"/>
+      <c r="AY50" s="62"/>
+      <c r="AZ50" s="62"/>
+      <c r="BA50" s="62"/>
+      <c r="BB50" s="62"/>
+      <c r="BC50" s="62"/>
+      <c r="BD50" s="62"/>
+      <c r="BE50" s="62"/>
+      <c r="BF50" s="62"/>
+      <c r="BG50" s="62"/>
+      <c r="BH50" s="62"/>
+      <c r="BI50" s="62"/>
+      <c r="BJ50" s="62"/>
+      <c r="BK50" s="62"/>
+      <c r="BL50" s="62"/>
+    </row>
+    <row r="51" spans="1:64" ht="15" customHeight="1">
       <c r="A51" s="3">
         <v>44</v>
       </c>
@@ -7107,8 +9302,55 @@
       <c r="AG51" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="52" spans="1:33" ht="15" customHeight="1">
+      <c r="AH51" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI51" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ51" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK51" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL51" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM51" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN51" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO51" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP51" s="62"/>
+      <c r="AQ51" s="62"/>
+      <c r="AR51" s="62"/>
+      <c r="AS51" s="62"/>
+      <c r="AT51" s="62"/>
+      <c r="AU51" s="62"/>
+      <c r="AV51" s="62"/>
+      <c r="AW51" s="62"/>
+      <c r="AX51" s="62"/>
+      <c r="AY51" s="62"/>
+      <c r="AZ51" s="62"/>
+      <c r="BA51" s="62"/>
+      <c r="BB51" s="62"/>
+      <c r="BC51" s="62"/>
+      <c r="BD51" s="62"/>
+      <c r="BE51" s="62"/>
+      <c r="BF51" s="62"/>
+      <c r="BG51" s="62"/>
+      <c r="BH51" s="62"/>
+      <c r="BI51" s="62"/>
+      <c r="BJ51" s="62"/>
+      <c r="BK51" s="62"/>
+      <c r="BL51" s="62"/>
+    </row>
+    <row r="52" spans="1:64" ht="15" customHeight="1">
       <c r="A52" s="3">
         <v>45</v>
       </c>
@@ -7206,8 +9448,55 @@
       <c r="AG52" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="53" spans="1:33" ht="15" customHeight="1">
+      <c r="AH52" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI52" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ52" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK52" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL52" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM52" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN52" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO52" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP52" s="62"/>
+      <c r="AQ52" s="62"/>
+      <c r="AR52" s="62"/>
+      <c r="AS52" s="62"/>
+      <c r="AT52" s="62"/>
+      <c r="AU52" s="62"/>
+      <c r="AV52" s="62"/>
+      <c r="AW52" s="62"/>
+      <c r="AX52" s="62"/>
+      <c r="AY52" s="62"/>
+      <c r="AZ52" s="62"/>
+      <c r="BA52" s="62"/>
+      <c r="BB52" s="62"/>
+      <c r="BC52" s="62"/>
+      <c r="BD52" s="62"/>
+      <c r="BE52" s="62"/>
+      <c r="BF52" s="62"/>
+      <c r="BG52" s="62"/>
+      <c r="BH52" s="62"/>
+      <c r="BI52" s="62"/>
+      <c r="BJ52" s="62"/>
+      <c r="BK52" s="62"/>
+      <c r="BL52" s="62"/>
+    </row>
+    <row r="53" spans="1:64" ht="15" customHeight="1">
       <c r="A53" s="3">
         <v>46</v>
       </c>
@@ -7305,8 +9594,55 @@
       <c r="AG53" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="54" spans="1:33" ht="15" customHeight="1">
+      <c r="AH53" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI53" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ53" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK53" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL53" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM53" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN53" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO53" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP53" s="62"/>
+      <c r="AQ53" s="62"/>
+      <c r="AR53" s="62"/>
+      <c r="AS53" s="62"/>
+      <c r="AT53" s="62"/>
+      <c r="AU53" s="62"/>
+      <c r="AV53" s="62"/>
+      <c r="AW53" s="62"/>
+      <c r="AX53" s="62"/>
+      <c r="AY53" s="62"/>
+      <c r="AZ53" s="62"/>
+      <c r="BA53" s="62"/>
+      <c r="BB53" s="62"/>
+      <c r="BC53" s="62"/>
+      <c r="BD53" s="62"/>
+      <c r="BE53" s="62"/>
+      <c r="BF53" s="62"/>
+      <c r="BG53" s="62"/>
+      <c r="BH53" s="62"/>
+      <c r="BI53" s="62"/>
+      <c r="BJ53" s="62"/>
+      <c r="BK53" s="62"/>
+      <c r="BL53" s="62"/>
+    </row>
+    <row r="54" spans="1:64" ht="15" customHeight="1">
       <c r="A54" s="3">
         <v>47</v>
       </c>
@@ -7404,8 +9740,55 @@
       <c r="AG54" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:33" ht="15" customHeight="1">
+      <c r="AH54" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI54" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ54" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK54" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL54" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM54" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN54" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO54" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP54" s="62"/>
+      <c r="AQ54" s="62"/>
+      <c r="AR54" s="62"/>
+      <c r="AS54" s="62"/>
+      <c r="AT54" s="62"/>
+      <c r="AU54" s="62"/>
+      <c r="AV54" s="62"/>
+      <c r="AW54" s="62"/>
+      <c r="AX54" s="62"/>
+      <c r="AY54" s="62"/>
+      <c r="AZ54" s="62"/>
+      <c r="BA54" s="62"/>
+      <c r="BB54" s="62"/>
+      <c r="BC54" s="62"/>
+      <c r="BD54" s="62"/>
+      <c r="BE54" s="62"/>
+      <c r="BF54" s="62"/>
+      <c r="BG54" s="62"/>
+      <c r="BH54" s="62"/>
+      <c r="BI54" s="62"/>
+      <c r="BJ54" s="62"/>
+      <c r="BK54" s="62"/>
+      <c r="BL54" s="62"/>
+    </row>
+    <row r="55" spans="1:64" ht="15" customHeight="1">
       <c r="A55" s="3">
         <v>48</v>
       </c>
@@ -7503,12 +9886,59 @@
       <c r="AG55" s="61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:33">
-      <c r="A56" s="65" t="s">
+      <c r="AH55" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI55" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ55" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK55" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL55" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM55" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN55" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO55" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP55" s="62"/>
+      <c r="AQ55" s="62"/>
+      <c r="AR55" s="62"/>
+      <c r="AS55" s="62"/>
+      <c r="AT55" s="62"/>
+      <c r="AU55" s="62"/>
+      <c r="AV55" s="62"/>
+      <c r="AW55" s="62"/>
+      <c r="AX55" s="62"/>
+      <c r="AY55" s="62"/>
+      <c r="AZ55" s="62"/>
+      <c r="BA55" s="62"/>
+      <c r="BB55" s="62"/>
+      <c r="BC55" s="62"/>
+      <c r="BD55" s="62"/>
+      <c r="BE55" s="62"/>
+      <c r="BF55" s="62"/>
+      <c r="BG55" s="62"/>
+      <c r="BH55" s="62"/>
+      <c r="BI55" s="62"/>
+      <c r="BJ55" s="62"/>
+      <c r="BK55" s="62"/>
+      <c r="BL55" s="62"/>
+    </row>
+    <row r="56" spans="1:64">
+      <c r="A56" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="66"/>
+      <c r="B56" s="67"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -7627,22 +10057,146 @@
         <v>11</v>
       </c>
       <c r="AG56" s="12">
-        <f t="shared" ref="AG56" si="22">COUNTIF(AG8:AG55,"A")</f>
+        <f t="shared" ref="AG56:BL56" si="22">COUNTIF(AG8:AG55,"A")</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="57" spans="1:33">
-      <c r="A57" s="62" t="s">
+      <c r="AH56" s="62">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AI56" s="62">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AJ56" s="62">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AK56" s="62">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AL56" s="62">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AM56" s="62">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AN56" s="62">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AO56" s="62">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AP56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AQ56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AR56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AS56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AT56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AU56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AV56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AW56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AX56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AY56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AZ56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BA56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BB56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BC56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BD56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BE56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BF56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BG56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BH56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BI56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BJ56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BK56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="BL56" s="62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:64">
+      <c r="A57" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="63"/>
+      <c r="B57" s="64"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
         <v>48</v>
       </c>
       <c r="E57" s="24">
-        <f t="shared" ref="E57:AG57" si="23">(48-E56)</f>
+        <f t="shared" ref="E57:BL57" si="23">(48-E56)</f>
         <v>48</v>
       </c>
       <c r="F57" s="24">
@@ -7756,6 +10310,130 @@
       <c r="AG57" s="24">
         <f t="shared" si="23"/>
         <v>37</v>
+      </c>
+      <c r="AH57" s="62">
+        <f t="shared" si="23"/>
+        <v>47</v>
+      </c>
+      <c r="AI57" s="62">
+        <f t="shared" si="23"/>
+        <v>47</v>
+      </c>
+      <c r="AJ57" s="62">
+        <f t="shared" si="23"/>
+        <v>47</v>
+      </c>
+      <c r="AK57" s="62">
+        <f t="shared" si="23"/>
+        <v>47</v>
+      </c>
+      <c r="AL57" s="62">
+        <f t="shared" si="23"/>
+        <v>47</v>
+      </c>
+      <c r="AM57" s="62">
+        <f t="shared" si="23"/>
+        <v>47</v>
+      </c>
+      <c r="AN57" s="62">
+        <f t="shared" si="23"/>
+        <v>47</v>
+      </c>
+      <c r="AO57" s="62">
+        <f t="shared" si="23"/>
+        <v>47</v>
+      </c>
+      <c r="AP57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="AQ57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="AR57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="AS57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="AT57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="AU57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="AV57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="AW57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="AX57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="AY57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="AZ57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="BA57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="BB57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="BC57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="BD57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="BE57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="BF57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="BG57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="BH57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="BI57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="BJ57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="BK57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
+      </c>
+      <c r="BL57" s="62">
+        <f t="shared" si="23"/>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -7788,7 +10466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:H2"/>
     </sheetView>
   </sheetViews>
@@ -7804,72 +10482,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="88" t="s">
+      <c r="B1" s="90"/>
+      <c r="C1" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="88"/>
-      <c r="E1" s="84" t="s">
+      <c r="D1" s="89"/>
+      <c r="E1" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="88" t="s">
+      <c r="B2" s="87"/>
+      <c r="C2" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="84" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="88" t="s">
+      <c r="B3" s="88"/>
+      <c r="C3" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="E3" s="84" t="s">
+      <c r="D3" s="89"/>
+      <c r="E3" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="91"/>
-      <c r="B5" s="68"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -7890,8 +10568,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="92"/>
-      <c r="B6" s="69"/>
+      <c r="A6" s="93"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -8814,10 +11492,10 @@
       <c r="H54" s="42"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="65" t="s">
+      <c r="A55" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="66"/>
+      <c r="B55" s="67"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -8831,10 +11509,10 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="62" t="s">
+      <c r="A56" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="63"/>
+      <c r="B56" s="64"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -8848,10 +11526,10 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="62" t="s">
+      <c r="A57" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="63"/>
+      <c r="B57" s="64"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -8865,10 +11543,10 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="62" t="s">
+      <c r="A58" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="63"/>
+      <c r="B58" s="64"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -8914,8 +11592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -8932,72 +11610,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="88" t="s">
+      <c r="B1" s="90"/>
+      <c r="C1" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="88"/>
-      <c r="E1" s="96" t="s">
+      <c r="D1" s="89"/>
+      <c r="E1" s="97" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="98"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="88" t="s">
+      <c r="B2" s="87"/>
+      <c r="C2" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="84" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="88" t="s">
+      <c r="B3" s="88"/>
+      <c r="C3" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="E3" s="84" t="s">
+      <c r="D3" s="89"/>
+      <c r="E3" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="96"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="91"/>
-      <c r="B5" s="68"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -9018,8 +11696,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="92"/>
-      <c r="B6" s="69"/>
+      <c r="A6" s="93"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -10048,10 +12726,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="65" t="s">
+      <c r="A55" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="66"/>
+      <c r="B55" s="67"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -10064,10 +12742,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="62" t="s">
+      <c r="A56" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="63"/>
+      <c r="B56" s="64"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -10080,10 +12758,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="62" t="s">
+      <c r="A57" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="63"/>
+      <c r="B57" s="64"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -10096,10 +12774,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="62" t="s">
+      <c r="A58" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="63"/>
+      <c r="B58" s="64"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -10159,147 +12837,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="83" t="s">
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="98" t="s">
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
-      <c r="W1" s="99"/>
-      <c r="X1" s="99"/>
-      <c r="Y1" s="99"/>
-      <c r="Z1" s="99"/>
-      <c r="AA1" s="99"/>
-      <c r="AB1" s="99"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="100"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="72"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="73"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="83" t="s">
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="84" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="98" t="s">
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="99"/>
-      <c r="R2" s="99"/>
-      <c r="S2" s="99"/>
-      <c r="T2" s="99"/>
-      <c r="U2" s="99"/>
-      <c r="V2" s="99"/>
-      <c r="W2" s="99"/>
-      <c r="X2" s="99"/>
-      <c r="Y2" s="99"/>
-      <c r="Z2" s="99"/>
-      <c r="AA2" s="99"/>
-      <c r="AB2" s="99"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="100"/>
+      <c r="R2" s="100"/>
+      <c r="S2" s="100"/>
+      <c r="T2" s="100"/>
+      <c r="U2" s="100"/>
+      <c r="V2" s="100"/>
+      <c r="W2" s="100"/>
+      <c r="X2" s="100"/>
+      <c r="Y2" s="100"/>
+      <c r="Z2" s="100"/>
+      <c r="AA2" s="100"/>
+      <c r="AB2" s="100"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="102"/>
-      <c r="C3" s="103"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="104"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="100" t="s">
+      <c r="F3" s="101" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="109" t="s">
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="110" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="109"/>
-      <c r="L3" s="109"/>
-      <c r="M3" s="109"/>
-      <c r="N3" s="98" t="s">
+      <c r="K3" s="110"/>
+      <c r="L3" s="110"/>
+      <c r="M3" s="110"/>
+      <c r="N3" s="99" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
-      <c r="Q3" s="99"/>
-      <c r="R3" s="99"/>
-      <c r="S3" s="99"/>
-      <c r="T3" s="99"/>
-      <c r="U3" s="99"/>
-      <c r="V3" s="99"/>
-      <c r="W3" s="99"/>
-      <c r="X3" s="99"/>
-      <c r="Y3" s="99"/>
-      <c r="Z3" s="99"/>
-      <c r="AA3" s="99"/>
-      <c r="AB3" s="99"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="100"/>
+      <c r="R3" s="100"/>
+      <c r="S3" s="100"/>
+      <c r="T3" s="100"/>
+      <c r="U3" s="100"/>
+      <c r="V3" s="100"/>
+      <c r="W3" s="100"/>
+      <c r="X3" s="100"/>
+      <c r="Y3" s="100"/>
+      <c r="Z3" s="100"/>
+      <c r="AA3" s="100"/>
+      <c r="AB3" s="100"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="104"/>
-      <c r="B4" s="105"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="107">
+      <c r="A4" s="105"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="108">
         <v>43344</v>
       </c>
-      <c r="E4" s="108"/>
-      <c r="F4" s="108"/>
-      <c r="G4" s="108"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="108"/>
-      <c r="J4" s="108"/>
-      <c r="K4" s="108"/>
-      <c r="L4" s="108"/>
-      <c r="M4" s="108"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60"/>
       <c r="P4" s="60"/>
@@ -10312,49 +12990,49 @@
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="90" t="s">
+      <c r="A5" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="68" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="113" t="s">
+      <c r="D5" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="114"/>
-      <c r="F5" s="114"/>
-      <c r="G5" s="115"/>
-      <c r="H5" s="111" t="s">
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="112" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="110" t="s">
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
+      <c r="K5" s="113"/>
+      <c r="L5" s="111" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111" t="s">
+      <c r="M5" s="111"/>
+      <c r="N5" s="112" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="112"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="110" t="s">
+      <c r="O5" s="113"/>
+      <c r="P5" s="113"/>
+      <c r="Q5" s="113"/>
+      <c r="R5" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="110"/>
-      <c r="T5" s="76" t="s">
+      <c r="S5" s="111"/>
+      <c r="T5" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="76"/>
+      <c r="U5" s="77"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="91"/>
-      <c r="B6" s="68"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -10425,8 +13103,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="91"/>
-      <c r="B7" s="68"/>
+      <c r="A7" s="92"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -10497,8 +13175,8 @@
       <c r="AF7" s="19"/>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="92"/>
-      <c r="B8" s="69"/>
+      <c r="A8" s="93"/>
+      <c r="B8" s="70"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -14121,10 +16799,10 @@
       <c r="AF56" s="19"/>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="65" t="s">
+      <c r="A57" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="66"/>
+      <c r="B57" s="67"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -14244,10 +16922,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="62" t="s">
+      <c r="A58" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="63"/>
+      <c r="B58" s="64"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>

</xml_diff>

<commit_message>
Last Update 01-11-2018  9:32:42.68
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
     <sheet name="Test Marks" sheetId="5" r:id="rId2"/>
     <sheet name="Expected Internal Marks" sheetId="6" r:id="rId3"/>
     <sheet name="Lab Attendance" sheetId="4" r:id="rId4"/>
+    <sheet name="UT-2-Satement" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attendance!$AC$1:$AC$57</definedName>
@@ -985,7 +986,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3206" uniqueCount="117">
   <si>
     <t>S.NO</t>
   </si>
@@ -1274,6 +1275,69 @@
   <si>
     <t>Lab 4</t>
   </si>
+  <si>
+    <t xml:space="preserve">KGiSL Institute of Technology </t>
+  </si>
+  <si>
+    <t>Batch:</t>
+  </si>
+  <si>
+    <t>Semester:</t>
+  </si>
+  <si>
+    <t>Subject Name</t>
+  </si>
+  <si>
+    <t>Year &amp; Sec.</t>
+  </si>
+  <si>
+    <t>Date of Exam</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Statement of Marks - Unit Test-II-OCT-2018</t>
+  </si>
+  <si>
+    <t>2018-2022</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Marks (50)</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>ARAVINDRAJ</t>
+  </si>
+  <si>
+    <t>No.of  Students Passed:</t>
+  </si>
+  <si>
+    <t>No.of  Students Failed:</t>
+  </si>
+  <si>
+    <t>No.of  Students Absent:</t>
+  </si>
+  <si>
+    <t>Subject Pass Percentage:</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>HoD</t>
+  </si>
+  <si>
+    <t>Principal</t>
+  </si>
 </sst>
 </file>
 
@@ -1282,7 +1346,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1377,6 +1441,59 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1583,10 +1700,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1776,14 +1894,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1812,41 +1969,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1860,17 +1996,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1881,11 +2011,23 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1921,29 +2063,131 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -2264,7 +2508,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="R5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AA1" sqref="AA1"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -2278,29 +2522,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="18.75">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="84" t="s">
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -2325,41 +2569,41 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:64" ht="19.5">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="86"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="84" t="s">
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="85" t="s">
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="85"/>
-      <c r="W2" s="85"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="76"/>
+      <c r="W2" s="76"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -2372,41 +2616,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:64" ht="18.75">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="76"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="71"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="84" t="s">
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="85" t="s">
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="85"/>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -2419,33 +2663,33 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:64" ht="18.75">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="81">
+      <c r="B4" s="66"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="72">
         <v>43344</v>
       </c>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="82"/>
-      <c r="U4" s="82"/>
-      <c r="V4" s="82"/>
-      <c r="W4" s="83"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
+      <c r="V4" s="73"/>
+      <c r="W4" s="74"/>
       <c r="X4" s="57"/>
       <c r="Y4" s="57"/>
       <c r="Z4" s="57"/>
@@ -2489,10 +2733,10 @@
       <c r="BL4" s="62"/>
     </row>
     <row r="5" spans="1:64">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="81" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -2612,8 +2856,12 @@
       <c r="AO5" s="62">
         <v>10</v>
       </c>
-      <c r="AP5" s="62"/>
-      <c r="AQ5" s="62"/>
+      <c r="AP5" s="62">
+        <v>10</v>
+      </c>
+      <c r="AQ5" s="62">
+        <v>10</v>
+      </c>
       <c r="AR5" s="62"/>
       <c r="AS5" s="62"/>
       <c r="AT5" s="62"/>
@@ -2637,8 +2885,8 @@
       <c r="BL5" s="62"/>
     </row>
     <row r="6" spans="1:64">
-      <c r="A6" s="77"/>
-      <c r="B6" s="69"/>
+      <c r="A6" s="87"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -2756,8 +3004,12 @@
       <c r="AO6" s="62">
         <v>26</v>
       </c>
-      <c r="AP6" s="62"/>
-      <c r="AQ6" s="62"/>
+      <c r="AP6" s="62">
+        <v>29</v>
+      </c>
+      <c r="AQ6" s="62">
+        <v>30</v>
+      </c>
       <c r="AR6" s="62"/>
       <c r="AS6" s="62"/>
       <c r="AT6" s="62"/>
@@ -2784,7 +3036,7 @@
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="70"/>
+      <c r="B7" s="83"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -2902,8 +3154,12 @@
       <c r="AO7" s="62">
         <v>8</v>
       </c>
-      <c r="AP7" s="62"/>
-      <c r="AQ7" s="62"/>
+      <c r="AP7" s="62">
+        <v>5</v>
+      </c>
+      <c r="AQ7" s="62">
+        <v>5</v>
+      </c>
       <c r="AR7" s="62"/>
       <c r="AS7" s="62"/>
       <c r="AT7" s="62"/>
@@ -3048,8 +3304,12 @@
       <c r="AO8" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP8" s="62"/>
-      <c r="AQ8" s="62"/>
+      <c r="AP8" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ8" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR8" s="62"/>
       <c r="AS8" s="62"/>
       <c r="AT8" s="62"/>
@@ -3194,8 +3454,12 @@
       <c r="AO9" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP9" s="62"/>
-      <c r="AQ9" s="62"/>
+      <c r="AP9" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ9" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR9" s="62"/>
       <c r="AS9" s="62"/>
       <c r="AT9" s="62"/>
@@ -3340,8 +3604,12 @@
       <c r="AO10" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP10" s="62"/>
-      <c r="AQ10" s="62"/>
+      <c r="AP10" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ10" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR10" s="62"/>
       <c r="AS10" s="62"/>
       <c r="AT10" s="62"/>
@@ -3486,8 +3754,12 @@
       <c r="AO11" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP11" s="62"/>
-      <c r="AQ11" s="62"/>
+      <c r="AP11" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ11" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR11" s="62"/>
       <c r="AS11" s="62"/>
       <c r="AT11" s="62"/>
@@ -3632,8 +3904,12 @@
       <c r="AO12" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP12" s="62"/>
-      <c r="AQ12" s="62"/>
+      <c r="AP12" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ12" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR12" s="62"/>
       <c r="AS12" s="62"/>
       <c r="AT12" s="62"/>
@@ -3778,8 +4054,12 @@
       <c r="AO13" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP13" s="62"/>
-      <c r="AQ13" s="62"/>
+      <c r="AP13" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ13" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR13" s="62"/>
       <c r="AS13" s="62"/>
       <c r="AT13" s="62"/>
@@ -3924,8 +4204,12 @@
       <c r="AO14" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP14" s="62"/>
-      <c r="AQ14" s="62"/>
+      <c r="AP14" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ14" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR14" s="62"/>
       <c r="AS14" s="62"/>
       <c r="AT14" s="62"/>
@@ -4046,17 +4330,17 @@
       <c r="AG15" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="AH15" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI15" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ15" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK15" s="62" t="s">
-        <v>54</v>
+      <c r="AH15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK15" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="AL15" s="62" t="s">
         <v>54</v>
@@ -4070,8 +4354,12 @@
       <c r="AO15" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP15" s="62"/>
-      <c r="AQ15" s="62"/>
+      <c r="AP15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ15" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR15" s="62"/>
       <c r="AS15" s="62"/>
       <c r="AT15" s="62"/>
@@ -4216,8 +4504,12 @@
       <c r="AO16" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP16" s="62"/>
-      <c r="AQ16" s="62"/>
+      <c r="AP16" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ16" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR16" s="62"/>
       <c r="AS16" s="62"/>
       <c r="AT16" s="62"/>
@@ -4362,8 +4654,12 @@
       <c r="AO17" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP17" s="62"/>
-      <c r="AQ17" s="62"/>
+      <c r="AP17" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ17" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR17" s="62"/>
       <c r="AS17" s="62"/>
       <c r="AT17" s="62"/>
@@ -4508,8 +4804,12 @@
       <c r="AO18" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP18" s="62"/>
-      <c r="AQ18" s="62"/>
+      <c r="AP18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ18" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR18" s="62"/>
       <c r="AS18" s="62"/>
       <c r="AT18" s="62"/>
@@ -4654,8 +4954,12 @@
       <c r="AO19" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP19" s="62"/>
-      <c r="AQ19" s="62"/>
+      <c r="AP19" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ19" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR19" s="62"/>
       <c r="AS19" s="62"/>
       <c r="AT19" s="62"/>
@@ -4800,8 +5104,12 @@
       <c r="AO20" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP20" s="62"/>
-      <c r="AQ20" s="62"/>
+      <c r="AP20" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ20" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AR20" s="62"/>
       <c r="AS20" s="62"/>
       <c r="AT20" s="62"/>
@@ -4946,8 +5254,12 @@
       <c r="AO21" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP21" s="62"/>
-      <c r="AQ21" s="62"/>
+      <c r="AP21" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ21" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR21" s="62"/>
       <c r="AS21" s="62"/>
       <c r="AT21" s="62"/>
@@ -5092,8 +5404,12 @@
       <c r="AO22" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP22" s="62"/>
-      <c r="AQ22" s="62"/>
+      <c r="AP22" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ22" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR22" s="62"/>
       <c r="AS22" s="62"/>
       <c r="AT22" s="62"/>
@@ -5238,8 +5554,12 @@
       <c r="AO23" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP23" s="62"/>
-      <c r="AQ23" s="62"/>
+      <c r="AP23" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ23" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR23" s="62"/>
       <c r="AS23" s="62"/>
       <c r="AT23" s="62"/>
@@ -5384,8 +5704,12 @@
       <c r="AO24" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP24" s="62"/>
-      <c r="AQ24" s="62"/>
+      <c r="AP24" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ24" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR24" s="62"/>
       <c r="AS24" s="62"/>
       <c r="AT24" s="62"/>
@@ -5530,8 +5854,12 @@
       <c r="AO25" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AP25" s="62"/>
-      <c r="AQ25" s="62"/>
+      <c r="AP25" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ25" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR25" s="62"/>
       <c r="AS25" s="62"/>
       <c r="AT25" s="62"/>
@@ -5676,8 +6004,12 @@
       <c r="AO26" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP26" s="62"/>
-      <c r="AQ26" s="62"/>
+      <c r="AP26" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ26" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR26" s="62"/>
       <c r="AS26" s="62"/>
       <c r="AT26" s="62"/>
@@ -5822,8 +6154,12 @@
       <c r="AO27" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP27" s="62"/>
-      <c r="AQ27" s="62"/>
+      <c r="AP27" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ27" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR27" s="62"/>
       <c r="AS27" s="62"/>
       <c r="AT27" s="62"/>
@@ -5968,8 +6304,12 @@
       <c r="AO28" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP28" s="62"/>
-      <c r="AQ28" s="62"/>
+      <c r="AP28" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ28" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR28" s="62"/>
       <c r="AS28" s="62"/>
       <c r="AT28" s="62"/>
@@ -6114,8 +6454,12 @@
       <c r="AO29" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP29" s="62"/>
-      <c r="AQ29" s="62"/>
+      <c r="AP29" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ29" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR29" s="62"/>
       <c r="AS29" s="62"/>
       <c r="AT29" s="62"/>
@@ -6260,8 +6604,12 @@
       <c r="AO30" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP30" s="62"/>
-      <c r="AQ30" s="62"/>
+      <c r="AP30" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ30" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR30" s="62"/>
       <c r="AS30" s="62"/>
       <c r="AT30" s="62"/>
@@ -6406,8 +6754,12 @@
       <c r="AO31" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP31" s="62"/>
-      <c r="AQ31" s="62"/>
+      <c r="AP31" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ31" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR31" s="62"/>
       <c r="AS31" s="62"/>
       <c r="AT31" s="62"/>
@@ -6552,8 +6904,12 @@
       <c r="AO32" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP32" s="62"/>
-      <c r="AQ32" s="62"/>
+      <c r="AP32" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ32" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR32" s="62"/>
       <c r="AS32" s="62"/>
       <c r="AT32" s="62"/>
@@ -6698,8 +7054,12 @@
       <c r="AO33" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP33" s="62"/>
-      <c r="AQ33" s="62"/>
+      <c r="AP33" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ33" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR33" s="62"/>
       <c r="AS33" s="62"/>
       <c r="AT33" s="62"/>
@@ -6844,8 +7204,12 @@
       <c r="AO34" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP34" s="62"/>
-      <c r="AQ34" s="62"/>
+      <c r="AP34" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ34" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR34" s="62"/>
       <c r="AS34" s="62"/>
       <c r="AT34" s="62"/>
@@ -6990,8 +7354,12 @@
       <c r="AO35" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP35" s="62"/>
-      <c r="AQ35" s="62"/>
+      <c r="AP35" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ35" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR35" s="62"/>
       <c r="AS35" s="62"/>
       <c r="AT35" s="62"/>
@@ -7136,8 +7504,12 @@
       <c r="AO36" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP36" s="62"/>
-      <c r="AQ36" s="62"/>
+      <c r="AP36" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ36" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR36" s="62"/>
       <c r="AS36" s="62"/>
       <c r="AT36" s="62"/>
@@ -7282,8 +7654,12 @@
       <c r="AO37" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP37" s="62"/>
-      <c r="AQ37" s="62"/>
+      <c r="AP37" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ37" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AR37" s="62"/>
       <c r="AS37" s="62"/>
       <c r="AT37" s="62"/>
@@ -7428,8 +7804,12 @@
       <c r="AO38" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP38" s="62"/>
-      <c r="AQ38" s="62"/>
+      <c r="AP38" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ38" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR38" s="62"/>
       <c r="AS38" s="62"/>
       <c r="AT38" s="62"/>
@@ -7574,8 +7954,12 @@
       <c r="AO39" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP39" s="62"/>
-      <c r="AQ39" s="62"/>
+      <c r="AP39" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ39" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR39" s="62"/>
       <c r="AS39" s="62"/>
       <c r="AT39" s="62"/>
@@ -7720,8 +8104,12 @@
       <c r="AO40" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP40" s="62"/>
-      <c r="AQ40" s="62"/>
+      <c r="AP40" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ40" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR40" s="62"/>
       <c r="AS40" s="62"/>
       <c r="AT40" s="62"/>
@@ -7866,8 +8254,12 @@
       <c r="AO41" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP41" s="62"/>
-      <c r="AQ41" s="62"/>
+      <c r="AP41" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ41" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR41" s="62"/>
       <c r="AS41" s="62"/>
       <c r="AT41" s="62"/>
@@ -8012,8 +8404,12 @@
       <c r="AO42" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP42" s="62"/>
-      <c r="AQ42" s="62"/>
+      <c r="AP42" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ42" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR42" s="62"/>
       <c r="AS42" s="62"/>
       <c r="AT42" s="62"/>
@@ -8158,8 +8554,12 @@
       <c r="AO43" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP43" s="62"/>
-      <c r="AQ43" s="62"/>
+      <c r="AP43" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ43" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR43" s="62"/>
       <c r="AS43" s="62"/>
       <c r="AT43" s="62"/>
@@ -8304,8 +8704,12 @@
       <c r="AO44" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP44" s="62"/>
-      <c r="AQ44" s="62"/>
+      <c r="AP44" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ44" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR44" s="62"/>
       <c r="AS44" s="62"/>
       <c r="AT44" s="62"/>
@@ -8450,8 +8854,12 @@
       <c r="AO45" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP45" s="62"/>
-      <c r="AQ45" s="62"/>
+      <c r="AP45" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ45" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR45" s="62"/>
       <c r="AS45" s="62"/>
       <c r="AT45" s="62"/>
@@ -8596,8 +9004,12 @@
       <c r="AO46" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP46" s="62"/>
-      <c r="AQ46" s="62"/>
+      <c r="AP46" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ46" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR46" s="62"/>
       <c r="AS46" s="62"/>
       <c r="AT46" s="62"/>
@@ -8742,8 +9154,12 @@
       <c r="AO47" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP47" s="62"/>
-      <c r="AQ47" s="62"/>
+      <c r="AP47" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ47" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR47" s="62"/>
       <c r="AS47" s="62"/>
       <c r="AT47" s="62"/>
@@ -8888,8 +9304,12 @@
       <c r="AO48" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP48" s="62"/>
-      <c r="AQ48" s="62"/>
+      <c r="AP48" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ48" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR48" s="62"/>
       <c r="AS48" s="62"/>
       <c r="AT48" s="62"/>
@@ -9034,8 +9454,12 @@
       <c r="AO49" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP49" s="62"/>
-      <c r="AQ49" s="62"/>
+      <c r="AP49" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ49" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR49" s="62"/>
       <c r="AS49" s="62"/>
       <c r="AT49" s="62"/>
@@ -9180,8 +9604,12 @@
       <c r="AO50" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP50" s="62"/>
-      <c r="AQ50" s="62"/>
+      <c r="AP50" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ50" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR50" s="62"/>
       <c r="AS50" s="62"/>
       <c r="AT50" s="62"/>
@@ -9326,8 +9754,12 @@
       <c r="AO51" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP51" s="62"/>
-      <c r="AQ51" s="62"/>
+      <c r="AP51" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ51" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR51" s="62"/>
       <c r="AS51" s="62"/>
       <c r="AT51" s="62"/>
@@ -9472,8 +9904,12 @@
       <c r="AO52" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP52" s="62"/>
-      <c r="AQ52" s="62"/>
+      <c r="AP52" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ52" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR52" s="62"/>
       <c r="AS52" s="62"/>
       <c r="AT52" s="62"/>
@@ -9618,8 +10054,12 @@
       <c r="AO53" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP53" s="62"/>
-      <c r="AQ53" s="62"/>
+      <c r="AP53" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ53" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR53" s="62"/>
       <c r="AS53" s="62"/>
       <c r="AT53" s="62"/>
@@ -9764,8 +10204,12 @@
       <c r="AO54" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP54" s="62"/>
-      <c r="AQ54" s="62"/>
+      <c r="AP54" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ54" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR54" s="62"/>
       <c r="AS54" s="62"/>
       <c r="AT54" s="62"/>
@@ -9910,8 +10354,12 @@
       <c r="AO55" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AP55" s="62"/>
-      <c r="AQ55" s="62"/>
+      <c r="AP55" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ55" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AR55" s="62"/>
       <c r="AS55" s="62"/>
       <c r="AT55" s="62"/>
@@ -9935,10 +10383,10 @@
       <c r="BL55" s="62"/>
     </row>
     <row r="56" spans="1:64">
-      <c r="A56" s="66" t="s">
+      <c r="A56" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="67"/>
+      <c r="B56" s="80"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -10062,19 +10510,19 @@
       </c>
       <c r="AH56" s="62">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI56" s="62">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ56" s="62">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK56" s="62">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL56" s="62">
         <f t="shared" si="22"/>
@@ -10094,11 +10542,11 @@
       </c>
       <c r="AP56" s="62">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AQ56" s="62">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR56" s="62">
         <f t="shared" si="22"/>
@@ -10186,10 +10634,10 @@
       </c>
     </row>
     <row r="57" spans="1:64">
-      <c r="A57" s="63" t="s">
+      <c r="A57" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="64"/>
+      <c r="B57" s="78"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -10313,19 +10761,19 @@
       </c>
       <c r="AH57" s="62">
         <f t="shared" si="23"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AI57" s="62">
         <f t="shared" si="23"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AJ57" s="62">
         <f t="shared" si="23"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AK57" s="62">
         <f t="shared" si="23"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AL57" s="62">
         <f t="shared" si="23"/>
@@ -10345,11 +10793,11 @@
       </c>
       <c r="AP57" s="62">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AQ57" s="62">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AR57" s="62">
         <f t="shared" si="23"/>
@@ -10438,6 +10886,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F3:I3"/>
@@ -10448,13 +10903,6 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10466,8 +10914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:H2"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -10482,72 +10930,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="89" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="89"/>
-      <c r="E1" s="85" t="s">
+      <c r="D1" s="95"/>
+      <c r="E1" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="89" t="s">
+      <c r="B2" s="93"/>
+      <c r="C2" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="85" t="s">
+      <c r="D2" s="95"/>
+      <c r="E2" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="89" t="s">
+      <c r="B3" s="94"/>
+      <c r="C3" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="85" t="s">
+      <c r="D3" s="95"/>
+      <c r="E3" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="92"/>
-      <c r="B5" s="69"/>
+      <c r="A5" s="90"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -10568,8 +11016,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="93"/>
-      <c r="B6" s="70"/>
+      <c r="A6" s="91"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -11492,10 +11940,10 @@
       <c r="H54" s="42"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="67"/>
+      <c r="B55" s="80"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -11509,10 +11957,10 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="63" t="s">
+      <c r="A56" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="64"/>
+      <c r="B56" s="78"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -11526,10 +11974,10 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="63" t="s">
+      <c r="A57" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="64"/>
+      <c r="B57" s="78"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -11543,10 +11991,10 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="63" t="s">
+      <c r="A58" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="64"/>
+      <c r="B58" s="78"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -11561,13 +12009,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -11577,9 +12018,16 @@
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:H54">
-    <cfRule type="cellIs" dxfId="1" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="17" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11593,7 +12041,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="D7" sqref="D7:D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -11610,72 +12058,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="89" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="89"/>
-      <c r="E1" s="97" t="s">
+      <c r="D1" s="95"/>
+      <c r="E1" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="98"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="97"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="89" t="s">
+      <c r="B2" s="93"/>
+      <c r="C2" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="85" t="s">
+      <c r="D2" s="95"/>
+      <c r="E2" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="89" t="s">
+      <c r="B3" s="94"/>
+      <c r="C3" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="85" t="s">
+      <c r="D3" s="95"/>
+      <c r="E3" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="96"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="100"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="92"/>
-      <c r="B5" s="69"/>
+      <c r="A5" s="90"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -11696,8 +12144,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="93"/>
-      <c r="B6" s="70"/>
+      <c r="A6" s="91"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -12726,10 +13174,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="67"/>
+      <c r="B55" s="80"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -12742,10 +13190,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="63" t="s">
+      <c r="A56" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="64"/>
+      <c r="B56" s="78"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -12758,10 +13206,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="63" t="s">
+      <c r="A57" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="64"/>
+      <c r="B57" s="78"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -12774,10 +13222,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="63" t="s">
+      <c r="A58" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="64"/>
+      <c r="B58" s="78"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -12791,25 +13239,25 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12822,8 +13270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -12837,147 +13285,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="84" t="s">
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="99" t="s">
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="100"/>
-      <c r="V1" s="100"/>
-      <c r="W1" s="100"/>
-      <c r="X1" s="100"/>
-      <c r="Y1" s="100"/>
-      <c r="Z1" s="100"/>
-      <c r="AA1" s="100"/>
-      <c r="AB1" s="100"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="108"/>
+      <c r="R1" s="108"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="108"/>
+      <c r="X1" s="108"/>
+      <c r="Y1" s="108"/>
+      <c r="Z1" s="108"/>
+      <c r="AA1" s="108"/>
+      <c r="AB1" s="108"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="86"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="84" t="s">
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="99" t="s">
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="107" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="100"/>
-      <c r="S2" s="100"/>
-      <c r="T2" s="100"/>
-      <c r="U2" s="100"/>
-      <c r="V2" s="100"/>
-      <c r="W2" s="100"/>
-      <c r="X2" s="100"/>
-      <c r="Y2" s="100"/>
-      <c r="Z2" s="100"/>
-      <c r="AA2" s="100"/>
-      <c r="AB2" s="100"/>
+      <c r="O2" s="108"/>
+      <c r="P2" s="108"/>
+      <c r="Q2" s="108"/>
+      <c r="R2" s="108"/>
+      <c r="S2" s="108"/>
+      <c r="T2" s="108"/>
+      <c r="U2" s="108"/>
+      <c r="V2" s="108"/>
+      <c r="W2" s="108"/>
+      <c r="X2" s="108"/>
+      <c r="Y2" s="108"/>
+      <c r="Z2" s="108"/>
+      <c r="AA2" s="108"/>
+      <c r="AB2" s="108"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="104"/>
+      <c r="B3" s="111"/>
+      <c r="C3" s="112"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="101" t="s">
+      <c r="F3" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="110" t="s">
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="110"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="99" t="s">
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="107" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="100"/>
-      <c r="P3" s="100"/>
-      <c r="Q3" s="100"/>
-      <c r="R3" s="100"/>
-      <c r="S3" s="100"/>
-      <c r="T3" s="100"/>
-      <c r="U3" s="100"/>
-      <c r="V3" s="100"/>
-      <c r="W3" s="100"/>
-      <c r="X3" s="100"/>
-      <c r="Y3" s="100"/>
-      <c r="Z3" s="100"/>
-      <c r="AA3" s="100"/>
-      <c r="AB3" s="100"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="108"/>
+      <c r="S3" s="108"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="108"/>
+      <c r="V3" s="108"/>
+      <c r="W3" s="108"/>
+      <c r="X3" s="108"/>
+      <c r="Y3" s="108"/>
+      <c r="Z3" s="108"/>
+      <c r="AA3" s="108"/>
+      <c r="AB3" s="108"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="105"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="108">
+      <c r="A4" s="113"/>
+      <c r="B4" s="114"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="116">
         <v>43344</v>
       </c>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="109"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="117"/>
+      <c r="I4" s="117"/>
+      <c r="J4" s="117"/>
+      <c r="K4" s="117"/>
+      <c r="L4" s="117"/>
+      <c r="M4" s="117"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60"/>
       <c r="P4" s="60"/>
@@ -12990,49 +13438,49 @@
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="81" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="112" t="s">
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="113"/>
-      <c r="J5" s="113"/>
-      <c r="K5" s="113"/>
-      <c r="L5" s="111" t="s">
+      <c r="I5" s="106"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="101" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="111"/>
-      <c r="N5" s="112" t="s">
+      <c r="M5" s="101"/>
+      <c r="N5" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="113"/>
-      <c r="P5" s="113"/>
-      <c r="Q5" s="113"/>
-      <c r="R5" s="111" t="s">
+      <c r="O5" s="106"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="106"/>
+      <c r="R5" s="101" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="111"/>
-      <c r="T5" s="77" t="s">
+      <c r="S5" s="101"/>
+      <c r="T5" s="87" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="77"/>
+      <c r="U5" s="87"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="92"/>
-      <c r="B6" s="69"/>
+      <c r="A6" s="90"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -13103,8 +13551,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="92"/>
-      <c r="B7" s="69"/>
+      <c r="A7" s="90"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -13175,8 +13623,8 @@
       <c r="AF7" s="19"/>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="93"/>
-      <c r="B8" s="70"/>
+      <c r="A8" s="91"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -16799,10 +17247,10 @@
       <c r="AF56" s="19"/>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="66" t="s">
+      <c r="A57" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="67"/>
+      <c r="B57" s="80"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -16922,10 +17370,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="63" t="s">
+      <c r="A58" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="64"/>
+      <c r="B58" s="78"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -17046,13 +17494,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
     <mergeCell ref="T5:U5"/>
     <mergeCell ref="N1:AB1"/>
     <mergeCell ref="N2:AB2"/>
@@ -17069,9 +17510,875 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="125" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="135" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="136" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="137" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="137" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+    </row>
+    <row r="4" spans="1:4" s="141" customFormat="1" ht="28.5">
+      <c r="A4" s="139" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="138" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="140" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="138" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="141" customFormat="1" ht="28.5">
+      <c r="A5" s="139" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="138" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="140" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="138" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="141" customFormat="1" ht="28.5">
+      <c r="A6" s="139" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="138" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="140" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="142">
+        <v>43385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1">
+      <c r="A7" s="121" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="120" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="120" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="130" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="141" customFormat="1">
+      <c r="A8" s="121">
+        <v>1</v>
+      </c>
+      <c r="B8" s="143" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="126">
+        <v>39</v>
+      </c>
+      <c r="D8" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="141" customFormat="1">
+      <c r="A9" s="121">
+        <v>2</v>
+      </c>
+      <c r="B9" s="143" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="127">
+        <v>19</v>
+      </c>
+      <c r="D9" s="126" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="141" customFormat="1">
+      <c r="A10" s="121">
+        <v>3</v>
+      </c>
+      <c r="B10" s="143" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="126">
+        <v>23</v>
+      </c>
+      <c r="D10" s="126" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="141" customFormat="1">
+      <c r="A11" s="121">
+        <v>4</v>
+      </c>
+      <c r="B11" s="144" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="126">
+        <v>25</v>
+      </c>
+      <c r="D11" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="141" customFormat="1">
+      <c r="A12" s="121">
+        <v>5</v>
+      </c>
+      <c r="B12" s="143" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="126">
+        <v>35</v>
+      </c>
+      <c r="D12" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="141" customFormat="1">
+      <c r="A13" s="121">
+        <v>6</v>
+      </c>
+      <c r="B13" s="143" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="126">
+        <v>28</v>
+      </c>
+      <c r="D13" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="141" customFormat="1">
+      <c r="A14" s="121">
+        <v>7</v>
+      </c>
+      <c r="B14" s="143" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="126">
+        <v>35</v>
+      </c>
+      <c r="D14" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="141" customFormat="1">
+      <c r="A15" s="121">
+        <v>8</v>
+      </c>
+      <c r="B15" s="143" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="126">
+        <v>39</v>
+      </c>
+      <c r="D15" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="141" customFormat="1">
+      <c r="A16" s="121">
+        <v>9</v>
+      </c>
+      <c r="B16" s="143" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="126">
+        <v>32</v>
+      </c>
+      <c r="D16" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="141" customFormat="1">
+      <c r="A17" s="121">
+        <v>10</v>
+      </c>
+      <c r="B17" s="143" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="126">
+        <v>33</v>
+      </c>
+      <c r="D17" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="141" customFormat="1">
+      <c r="A18" s="121">
+        <v>11</v>
+      </c>
+      <c r="B18" s="143" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="126">
+        <v>38</v>
+      </c>
+      <c r="D18" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="141" customFormat="1">
+      <c r="A19" s="121">
+        <v>12</v>
+      </c>
+      <c r="B19" s="143" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="126">
+        <v>31</v>
+      </c>
+      <c r="D19" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="141" customFormat="1">
+      <c r="A20" s="121">
+        <v>13</v>
+      </c>
+      <c r="B20" s="143" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="126">
+        <v>26</v>
+      </c>
+      <c r="D20" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="141" customFormat="1">
+      <c r="A21" s="121">
+        <v>14</v>
+      </c>
+      <c r="B21" s="145" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="126">
+        <v>31</v>
+      </c>
+      <c r="D21" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="141" customFormat="1">
+      <c r="A22" s="121">
+        <v>15</v>
+      </c>
+      <c r="B22" s="145" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="126">
+        <v>27</v>
+      </c>
+      <c r="D22" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="141" customFormat="1">
+      <c r="A23" s="121">
+        <v>16</v>
+      </c>
+      <c r="B23" s="143" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="126">
+        <v>33</v>
+      </c>
+      <c r="D23" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="141" customFormat="1">
+      <c r="A24" s="121">
+        <v>17</v>
+      </c>
+      <c r="B24" s="143" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="126">
+        <v>31</v>
+      </c>
+      <c r="D24" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="141" customFormat="1" ht="30">
+      <c r="A25" s="121">
+        <v>18</v>
+      </c>
+      <c r="B25" s="143" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="126">
+        <v>31</v>
+      </c>
+      <c r="D25" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="141" customFormat="1">
+      <c r="A26" s="121">
+        <v>19</v>
+      </c>
+      <c r="B26" s="143" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="126">
+        <v>44</v>
+      </c>
+      <c r="D26" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="141" customFormat="1">
+      <c r="A27" s="121">
+        <v>20</v>
+      </c>
+      <c r="B27" s="143" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="126">
+        <v>35</v>
+      </c>
+      <c r="D27" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="141" customFormat="1">
+      <c r="A28" s="121">
+        <v>21</v>
+      </c>
+      <c r="B28" s="143" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="126">
+        <v>23</v>
+      </c>
+      <c r="D28" s="126" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="141" customFormat="1">
+      <c r="A29" s="121">
+        <v>22</v>
+      </c>
+      <c r="B29" s="143" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="126">
+        <v>35</v>
+      </c>
+      <c r="D29" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="141" customFormat="1">
+      <c r="A30" s="121">
+        <v>23</v>
+      </c>
+      <c r="B30" s="146" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="126">
+        <v>31</v>
+      </c>
+      <c r="D30" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="141" customFormat="1">
+      <c r="A31" s="121">
+        <v>24</v>
+      </c>
+      <c r="B31" s="147" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="126">
+        <v>35</v>
+      </c>
+      <c r="D31" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="141" customFormat="1">
+      <c r="A32" s="121">
+        <v>25</v>
+      </c>
+      <c r="B32" s="145" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="126">
+        <v>36</v>
+      </c>
+      <c r="D32" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="141" customFormat="1" ht="30">
+      <c r="A33" s="121">
+        <v>26</v>
+      </c>
+      <c r="B33" s="143" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="126">
+        <v>47</v>
+      </c>
+      <c r="D33" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="141" customFormat="1">
+      <c r="A34" s="121">
+        <v>27</v>
+      </c>
+      <c r="B34" s="147" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="126">
+        <v>25</v>
+      </c>
+      <c r="D34" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="141" customFormat="1">
+      <c r="A35" s="121">
+        <v>28</v>
+      </c>
+      <c r="B35" s="143" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="126">
+        <v>49</v>
+      </c>
+      <c r="D35" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="141" customFormat="1">
+      <c r="A36" s="121">
+        <v>29</v>
+      </c>
+      <c r="B36" s="145" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="126">
+        <v>33</v>
+      </c>
+      <c r="D36" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="141" customFormat="1">
+      <c r="A37" s="121">
+        <v>30</v>
+      </c>
+      <c r="B37" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="126">
+        <v>32</v>
+      </c>
+      <c r="D37" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="141" customFormat="1">
+      <c r="A38" s="121">
+        <v>31</v>
+      </c>
+      <c r="B38" s="145" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="126">
+        <v>42</v>
+      </c>
+      <c r="D38" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="141" customFormat="1">
+      <c r="A39" s="121">
+        <v>32</v>
+      </c>
+      <c r="B39" s="143" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="126">
+        <v>42</v>
+      </c>
+      <c r="D39" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="141" customFormat="1">
+      <c r="A40" s="121">
+        <v>33</v>
+      </c>
+      <c r="B40" s="143" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="126">
+        <v>38</v>
+      </c>
+      <c r="D40" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="141" customFormat="1" ht="30">
+      <c r="A41" s="121">
+        <v>34</v>
+      </c>
+      <c r="B41" s="143" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="126">
+        <v>36</v>
+      </c>
+      <c r="D41" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="141" customFormat="1">
+      <c r="A42" s="121">
+        <v>35</v>
+      </c>
+      <c r="B42" s="143" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="126">
+        <v>34</v>
+      </c>
+      <c r="D42" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="141" customFormat="1">
+      <c r="A43" s="121">
+        <v>36</v>
+      </c>
+      <c r="B43" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="126">
+        <v>19</v>
+      </c>
+      <c r="D43" s="126" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="141" customFormat="1">
+      <c r="A44" s="121">
+        <v>37</v>
+      </c>
+      <c r="B44" s="145" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="126">
+        <v>25</v>
+      </c>
+      <c r="D44" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="141" customFormat="1">
+      <c r="A45" s="121">
+        <v>38</v>
+      </c>
+      <c r="B45" s="143" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="126">
+        <v>25</v>
+      </c>
+      <c r="D45" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="141" customFormat="1">
+      <c r="A46" s="121">
+        <v>39</v>
+      </c>
+      <c r="B46" s="147" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="126">
+        <v>32</v>
+      </c>
+      <c r="D46" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="141" customFormat="1">
+      <c r="A47" s="121">
+        <v>40</v>
+      </c>
+      <c r="B47" s="143" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="126">
+        <v>33</v>
+      </c>
+      <c r="D47" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="141" customFormat="1">
+      <c r="A48" s="121">
+        <v>41</v>
+      </c>
+      <c r="B48" s="143" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="126">
+        <v>25</v>
+      </c>
+      <c r="D48" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="141" customFormat="1">
+      <c r="A49" s="121">
+        <v>42</v>
+      </c>
+      <c r="B49" s="143" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="126">
+        <v>36</v>
+      </c>
+      <c r="D49" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="141" customFormat="1">
+      <c r="A50" s="121">
+        <v>43</v>
+      </c>
+      <c r="B50" s="145" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="126">
+        <v>42</v>
+      </c>
+      <c r="D50" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="141" customFormat="1">
+      <c r="A51" s="121">
+        <v>44</v>
+      </c>
+      <c r="B51" s="145" t="s">
+        <v>43</v>
+      </c>
+      <c r="C51" s="126">
+        <v>37</v>
+      </c>
+      <c r="D51" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="141" customFormat="1">
+      <c r="A52" s="121">
+        <v>45</v>
+      </c>
+      <c r="B52" s="143" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="126">
+        <v>27</v>
+      </c>
+      <c r="D52" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="141" customFormat="1">
+      <c r="A53" s="121">
+        <v>46</v>
+      </c>
+      <c r="B53" s="143" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="126">
+        <v>37</v>
+      </c>
+      <c r="D53" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="141" customFormat="1">
+      <c r="A54" s="121">
+        <v>47</v>
+      </c>
+      <c r="B54" s="143" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="126">
+        <v>30</v>
+      </c>
+      <c r="D54" s="126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="141" customFormat="1">
+      <c r="A55" s="119">
+        <v>48</v>
+      </c>
+      <c r="B55" s="148" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" s="128">
+        <v>46</v>
+      </c>
+      <c r="D55" s="128" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="122" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="122"/>
+      <c r="C56" s="122"/>
+      <c r="D56" s="131">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="122" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="122"/>
+      <c r="C57" s="122"/>
+      <c r="D57" s="132">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="122" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="122"/>
+      <c r="C58" s="122"/>
+      <c r="D58" s="132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="122" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" s="122"/>
+      <c r="C59" s="122"/>
+      <c r="D59" s="132">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="123"/>
+      <c r="B60" s="123"/>
+      <c r="C60" s="123"/>
+      <c r="D60" s="133"/>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="123"/>
+      <c r="B61" s="123"/>
+      <c r="C61" s="123"/>
+      <c r="D61" s="133"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="129"/>
+      <c r="B62" s="129"/>
+      <c r="C62" s="129"/>
+      <c r="D62" s="133"/>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="124" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="124"/>
+      <c r="C63" s="124" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="134" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C25:C55 C8:C23">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Last Update 08-11-2018 14:37:09.60
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -1074,6 +1074,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="Z5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Merge Sort
+Matrix Multiplecation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D7" authorId="0">
       <text>
         <r>
@@ -1178,7 +1203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3640" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3833" uniqueCount="119">
   <si>
     <t>S.NO</t>
   </si>
@@ -1532,6 +1557,9 @@
   </si>
   <si>
     <t>Lab 5</t>
+  </si>
+  <si>
+    <t>Lab 6</t>
   </si>
 </sst>
 </file>
@@ -1905,7 +1933,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2192,35 +2220,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2231,17 +2241,14 @@
     <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2270,8 +2277,44 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2285,24 +2328,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2312,23 +2337,11 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2362,6 +2375,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2762,29 +2793,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="18.75">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="112" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="99" t="s">
+      <c r="F1" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="107" t="s">
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="119" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -2809,41 +2840,41 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:64" ht="19.5">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="118"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="111"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="102" t="s">
+      <c r="F2" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="107" t="s">
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="119" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="108" t="s">
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="120" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="108"/>
-      <c r="P2" s="108"/>
-      <c r="Q2" s="108"/>
-      <c r="R2" s="108"/>
-      <c r="S2" s="108"/>
-      <c r="T2" s="108"/>
-      <c r="U2" s="108"/>
-      <c r="V2" s="108"/>
-      <c r="W2" s="108"/>
+      <c r="O2" s="120"/>
+      <c r="P2" s="120"/>
+      <c r="Q2" s="120"/>
+      <c r="R2" s="120"/>
+      <c r="S2" s="120"/>
+      <c r="T2" s="120"/>
+      <c r="U2" s="120"/>
+      <c r="V2" s="120"/>
+      <c r="W2" s="120"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -2856,41 +2887,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:64" ht="18.75">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="112" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="103"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="114"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="103" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="107" t="s">
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="119" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="108" t="s">
+      <c r="K3" s="119"/>
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="120" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108"/>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108"/>
-      <c r="W3" s="108"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="120"/>
+      <c r="R3" s="120"/>
+      <c r="S3" s="120"/>
+      <c r="T3" s="120"/>
+      <c r="U3" s="120"/>
+      <c r="V3" s="120"/>
+      <c r="W3" s="120"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -2903,56 +2934,56 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:64" ht="18.75">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="112" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="104">
+      <c r="B4" s="113"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="98">
         <v>43344</v>
       </c>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="105"/>
-      <c r="P4" s="105"/>
-      <c r="Q4" s="105"/>
-      <c r="R4" s="105"/>
-      <c r="S4" s="105"/>
-      <c r="T4" s="105"/>
-      <c r="U4" s="105"/>
-      <c r="V4" s="105"/>
-      <c r="W4" s="106"/>
-      <c r="X4" s="104">
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="99"/>
+      <c r="U4" s="99"/>
+      <c r="V4" s="99"/>
+      <c r="W4" s="100"/>
+      <c r="X4" s="98">
         <v>43374</v>
       </c>
-      <c r="Y4" s="105"/>
-      <c r="Z4" s="105"/>
-      <c r="AA4" s="105"/>
-      <c r="AB4" s="105"/>
-      <c r="AC4" s="105"/>
-      <c r="AD4" s="105"/>
-      <c r="AE4" s="105"/>
-      <c r="AF4" s="105"/>
-      <c r="AG4" s="105"/>
-      <c r="AH4" s="105"/>
-      <c r="AI4" s="105"/>
-      <c r="AJ4" s="105"/>
-      <c r="AK4" s="105"/>
-      <c r="AL4" s="105"/>
-      <c r="AM4" s="105"/>
-      <c r="AN4" s="105"/>
-      <c r="AO4" s="105"/>
-      <c r="AP4" s="105"/>
-      <c r="AQ4" s="105"/>
-      <c r="AR4" s="106"/>
+      <c r="Y4" s="99"/>
+      <c r="Z4" s="99"/>
+      <c r="AA4" s="99"/>
+      <c r="AB4" s="99"/>
+      <c r="AC4" s="99"/>
+      <c r="AD4" s="99"/>
+      <c r="AE4" s="99"/>
+      <c r="AF4" s="99"/>
+      <c r="AG4" s="99"/>
+      <c r="AH4" s="99"/>
+      <c r="AI4" s="99"/>
+      <c r="AJ4" s="99"/>
+      <c r="AK4" s="99"/>
+      <c r="AL4" s="99"/>
+      <c r="AM4" s="99"/>
+      <c r="AN4" s="99"/>
+      <c r="AO4" s="99"/>
+      <c r="AP4" s="99"/>
+      <c r="AQ4" s="99"/>
+      <c r="AR4" s="100"/>
       <c r="AS4" s="61"/>
       <c r="AT4" s="61"/>
       <c r="AU4" s="61"/>
@@ -2975,10 +3006,10 @@
       <c r="BL4" s="61"/>
     </row>
     <row r="5" spans="1:64">
-      <c r="A5" s="119" t="s">
+      <c r="A5" s="115" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="113" t="s">
+      <c r="B5" s="106" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -3137,8 +3168,8 @@
       <c r="BL5" s="61"/>
     </row>
     <row r="6" spans="1:64">
-      <c r="A6" s="119"/>
-      <c r="B6" s="114"/>
+      <c r="A6" s="115"/>
+      <c r="B6" s="107"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -3298,7 +3329,7 @@
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="115"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -3425,13 +3456,13 @@
       <c r="AR7" s="2">
         <v>4</v>
       </c>
-      <c r="AS7" s="96">
+      <c r="AS7" s="95">
         <v>1</v>
       </c>
-      <c r="AT7" s="96">
+      <c r="AT7" s="95">
         <v>2</v>
       </c>
-      <c r="AU7" s="96">
+      <c r="AU7" s="95">
         <v>3</v>
       </c>
       <c r="AV7" s="93">
@@ -11135,10 +11166,10 @@
       <c r="BL55" s="61"/>
     </row>
     <row r="56" spans="1:64">
-      <c r="A56" s="111" t="s">
+      <c r="A56" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="112"/>
+      <c r="B56" s="105"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -11386,10 +11417,10 @@
       </c>
     </row>
     <row r="57" spans="1:64">
-      <c r="A57" s="109" t="s">
+      <c r="A57" s="101" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="110"/>
+      <c r="B57" s="102"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -11638,14 +11669,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="X4:AR4"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F3:I3"/>
@@ -11656,6 +11679,14 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N2:W2"/>
     <mergeCell ref="N3:W3"/>
+    <mergeCell ref="X4:AR4"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -11667,8 +11698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F54"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -11683,72 +11714,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="125" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="127" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="124" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="127"/>
-      <c r="E1" s="108" t="s">
+      <c r="D1" s="124"/>
+      <c r="E1" s="120" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="127" t="s">
+      <c r="B2" s="122"/>
+      <c r="C2" s="124" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="127"/>
-      <c r="E2" s="108" t="s">
+      <c r="D2" s="124"/>
+      <c r="E2" s="120" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="123" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="127" t="s">
+      <c r="B3" s="123"/>
+      <c r="C3" s="124" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="127"/>
-      <c r="E3" s="108" t="s">
+      <c r="D3" s="124"/>
+      <c r="E3" s="120" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="126" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="106" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="124" t="s">
+      <c r="C4" s="121" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="122"/>
-      <c r="B5" s="114"/>
+      <c r="A5" s="127"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -11769,8 +11800,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="123"/>
-      <c r="B6" s="115"/>
+      <c r="A6" s="128"/>
+      <c r="B6" s="108"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -11826,8 +11857,8 @@
       <c r="E8" s="45">
         <v>19</v>
       </c>
-      <c r="F8" s="95">
-        <v>39</v>
+      <c r="F8" s="94">
+        <v>41</v>
       </c>
       <c r="G8" s="45"/>
       <c r="H8" s="45"/>
@@ -12140,7 +12171,7 @@
       <c r="E23" s="30">
         <v>31</v>
       </c>
-      <c r="F23" s="95">
+      <c r="F23" s="94">
         <v>26</v>
       </c>
       <c r="G23" s="45"/>
@@ -12243,7 +12274,7 @@
       </c>
       <c r="E28" s="30"/>
       <c r="F28" s="42">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G28" s="42"/>
       <c r="H28" s="42"/>
@@ -12473,7 +12504,7 @@
         <v>22</v>
       </c>
       <c r="F39" s="42">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G39" s="42"/>
       <c r="H39" s="42"/>
@@ -12493,7 +12524,7 @@
       </c>
       <c r="E40" s="30"/>
       <c r="F40" s="42">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G40" s="42"/>
       <c r="H40" s="42"/>
@@ -12513,7 +12544,7 @@
       </c>
       <c r="E41" s="30"/>
       <c r="F41" s="42">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G41" s="42"/>
       <c r="H41" s="42"/>
@@ -12783,16 +12814,16 @@
       </c>
       <c r="E54" s="30"/>
       <c r="F54" s="42">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G54" s="42"/>
       <c r="H54" s="42"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="111" t="s">
+      <c r="A55" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="112"/>
+      <c r="B55" s="105"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -12808,10 +12839,10 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="109" t="s">
+      <c r="A56" s="101" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="110"/>
+      <c r="B56" s="102"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -12827,10 +12858,10 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="109" t="s">
+      <c r="A57" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="110"/>
+      <c r="B57" s="102"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -12846,10 +12877,10 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="109" t="s">
+      <c r="A58" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="110"/>
+      <c r="B58" s="102"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -12866,6 +12897,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -12875,13 +12913,6 @@
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:H54">
     <cfRule type="cellIs" dxfId="5" priority="17" operator="lessThan">
@@ -12897,8 +12928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -12915,72 +12946,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="125" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="127" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="124" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="127"/>
-      <c r="E1" s="128" t="s">
+      <c r="D1" s="124"/>
+      <c r="E1" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="129"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="133"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="127" t="s">
+      <c r="B2" s="122"/>
+      <c r="C2" s="124" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="127"/>
-      <c r="E2" s="108" t="s">
+      <c r="D2" s="124"/>
+      <c r="E2" s="120" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="123" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="127" t="s">
+      <c r="B3" s="123"/>
+      <c r="C3" s="124" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="127"/>
-      <c r="E3" s="108" t="s">
+      <c r="D3" s="124"/>
+      <c r="E3" s="120" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="126" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="106" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="130" t="s">
+      <c r="C4" s="129" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="131"/>
-      <c r="E4" s="131"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="131"/>
-      <c r="H4" s="132"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="131"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="122"/>
-      <c r="B5" s="114"/>
+      <c r="A5" s="127"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -13001,8 +13032,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="123"/>
-      <c r="B6" s="115"/>
+      <c r="A6" s="128"/>
+      <c r="B6" s="108"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -13035,7 +13066,7 @@
       <c r="D7" s="42">
         <v>39</v>
       </c>
-      <c r="E7" s="94">
+      <c r="E7" s="96">
         <v>31</v>
       </c>
       <c r="F7" s="42"/>
@@ -13058,14 +13089,14 @@
       <c r="D8" s="45">
         <v>19</v>
       </c>
-      <c r="E8" s="95">
-        <v>39</v>
+      <c r="E8" s="97">
+        <v>41</v>
       </c>
       <c r="F8" s="45"/>
       <c r="G8" s="45"/>
       <c r="H8" s="55">
         <f t="shared" ref="H8:H54" si="0">(SUM(C8:E8)/300)*20</f>
-        <v>6.0666666666666664</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
@@ -13081,7 +13112,7 @@
       <c r="D9" s="42">
         <v>23</v>
       </c>
-      <c r="E9" s="94">
+      <c r="E9" s="96">
         <v>30</v>
       </c>
       <c r="F9" s="42"/>
@@ -13104,7 +13135,7 @@
       <c r="D10" s="42">
         <v>25</v>
       </c>
-      <c r="E10" s="94">
+      <c r="E10" s="96">
         <v>28</v>
       </c>
       <c r="F10" s="42"/>
@@ -13127,7 +13158,7 @@
       <c r="D11" s="42">
         <v>35</v>
       </c>
-      <c r="E11" s="94">
+      <c r="E11" s="96">
         <v>35</v>
       </c>
       <c r="F11" s="42"/>
@@ -13173,7 +13204,7 @@
       <c r="D13" s="42">
         <v>35</v>
       </c>
-      <c r="E13" s="94">
+      <c r="E13" s="96">
         <v>41</v>
       </c>
       <c r="F13" s="42"/>
@@ -13196,7 +13227,7 @@
       <c r="D14" s="42">
         <v>39</v>
       </c>
-      <c r="E14" s="94">
+      <c r="E14" s="96">
         <v>35</v>
       </c>
       <c r="F14" s="42"/>
@@ -13219,7 +13250,7 @@
       <c r="D15" s="42">
         <v>32</v>
       </c>
-      <c r="E15" s="94">
+      <c r="E15" s="96">
         <v>22</v>
       </c>
       <c r="F15" s="42"/>
@@ -13242,7 +13273,7 @@
       <c r="D16" s="42">
         <v>33</v>
       </c>
-      <c r="E16" s="94">
+      <c r="E16" s="96">
         <v>27</v>
       </c>
       <c r="F16" s="42"/>
@@ -13265,7 +13296,7 @@
       <c r="D17" s="42">
         <v>38</v>
       </c>
-      <c r="E17" s="94">
+      <c r="E17" s="96">
         <v>39</v>
       </c>
       <c r="F17" s="42"/>
@@ -13288,7 +13319,7 @@
       <c r="D18" s="42">
         <v>31</v>
       </c>
-      <c r="E18" s="94">
+      <c r="E18" s="96">
         <v>25</v>
       </c>
       <c r="F18" s="42"/>
@@ -13311,7 +13342,7 @@
       <c r="D19" s="42">
         <v>26</v>
       </c>
-      <c r="E19" s="94">
+      <c r="E19" s="96">
         <v>29</v>
       </c>
       <c r="F19" s="42"/>
@@ -13334,7 +13365,7 @@
       <c r="D20" s="42">
         <v>31</v>
       </c>
-      <c r="E20" s="94">
+      <c r="E20" s="96">
         <v>30</v>
       </c>
       <c r="F20" s="42"/>
@@ -13357,7 +13388,7 @@
       <c r="D21" s="42">
         <v>27</v>
       </c>
-      <c r="E21" s="94">
+      <c r="E21" s="96">
         <v>21</v>
       </c>
       <c r="F21" s="42"/>
@@ -13380,7 +13411,7 @@
       <c r="D22" s="42">
         <v>33</v>
       </c>
-      <c r="E22" s="94">
+      <c r="E22" s="96">
         <v>39</v>
       </c>
       <c r="F22" s="42"/>
@@ -13403,7 +13434,7 @@
       <c r="D23" s="42">
         <v>31</v>
       </c>
-      <c r="E23" s="95">
+      <c r="E23" s="97">
         <v>26</v>
       </c>
       <c r="F23" s="45"/>
@@ -13426,7 +13457,7 @@
       <c r="D24" s="42">
         <v>31</v>
       </c>
-      <c r="E24" s="94">
+      <c r="E24" s="96">
         <v>32</v>
       </c>
       <c r="F24" s="42"/>
@@ -13449,7 +13480,7 @@
       <c r="D25" s="42">
         <v>44</v>
       </c>
-      <c r="E25" s="94">
+      <c r="E25" s="96">
         <v>45</v>
       </c>
       <c r="F25" s="42"/>
@@ -13472,7 +13503,7 @@
       <c r="D26" s="42">
         <v>35</v>
       </c>
-      <c r="E26" s="94">
+      <c r="E26" s="96">
         <v>45</v>
       </c>
       <c r="F26" s="42"/>
@@ -13495,7 +13526,7 @@
       <c r="D27" s="42">
         <v>23</v>
       </c>
-      <c r="E27" s="94">
+      <c r="E27" s="96">
         <v>12</v>
       </c>
       <c r="F27" s="42"/>
@@ -13518,14 +13549,14 @@
       <c r="D28" s="42">
         <v>35</v>
       </c>
-      <c r="E28" s="94">
-        <v>26</v>
+      <c r="E28" s="96">
+        <v>32</v>
       </c>
       <c r="F28" s="42"/>
       <c r="G28" s="42"/>
       <c r="H28" s="55">
         <f t="shared" si="0"/>
-        <v>6.0666666666666664</v>
+        <v>6.4666666666666659</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1">
@@ -13541,7 +13572,7 @@
       <c r="D29" s="42">
         <v>31</v>
       </c>
-      <c r="E29" s="94">
+      <c r="E29" s="96">
         <v>30</v>
       </c>
       <c r="F29" s="42"/>
@@ -13564,7 +13595,7 @@
       <c r="D30" s="42">
         <v>35</v>
       </c>
-      <c r="E30" s="94">
+      <c r="E30" s="96">
         <v>25</v>
       </c>
       <c r="F30" s="42"/>
@@ -13587,7 +13618,7 @@
       <c r="D31" s="42">
         <v>36</v>
       </c>
-      <c r="E31" s="94">
+      <c r="E31" s="96">
         <v>31</v>
       </c>
       <c r="F31" s="42"/>
@@ -13610,7 +13641,7 @@
       <c r="D32" s="42">
         <v>47</v>
       </c>
-      <c r="E32" s="94">
+      <c r="E32" s="96">
         <v>46</v>
       </c>
       <c r="F32" s="42"/>
@@ -13633,7 +13664,7 @@
       <c r="D33" s="42">
         <v>25</v>
       </c>
-      <c r="E33" s="94">
+      <c r="E33" s="96">
         <v>22</v>
       </c>
       <c r="F33" s="42"/>
@@ -13656,7 +13687,7 @@
       <c r="D34" s="42">
         <v>49</v>
       </c>
-      <c r="E34" s="94">
+      <c r="E34" s="96">
         <v>44</v>
       </c>
       <c r="F34" s="42"/>
@@ -13679,7 +13710,7 @@
       <c r="D35" s="42">
         <v>33</v>
       </c>
-      <c r="E35" s="94">
+      <c r="E35" s="96">
         <v>37</v>
       </c>
       <c r="F35" s="42"/>
@@ -13702,7 +13733,7 @@
       <c r="D36" s="42">
         <v>32</v>
       </c>
-      <c r="E36" s="94">
+      <c r="E36" s="96">
         <v>17</v>
       </c>
       <c r="F36" s="42"/>
@@ -13725,7 +13756,7 @@
       <c r="D37" s="42">
         <v>42</v>
       </c>
-      <c r="E37" s="94">
+      <c r="E37" s="96">
         <v>43</v>
       </c>
       <c r="F37" s="42"/>
@@ -13748,7 +13779,7 @@
       <c r="D38" s="42">
         <v>42</v>
       </c>
-      <c r="E38" s="94">
+      <c r="E38" s="96">
         <v>42</v>
       </c>
       <c r="F38" s="42"/>
@@ -13771,14 +13802,14 @@
       <c r="D39" s="42">
         <v>38</v>
       </c>
-      <c r="E39" s="94">
-        <v>38</v>
+      <c r="E39" s="96">
+        <v>31</v>
       </c>
       <c r="F39" s="42"/>
       <c r="G39" s="42"/>
       <c r="H39" s="55">
         <f t="shared" si="0"/>
-        <v>6.5333333333333332</v>
+        <v>6.0666666666666664</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1">
@@ -13794,14 +13825,14 @@
       <c r="D40" s="42">
         <v>36</v>
       </c>
-      <c r="E40" s="94">
-        <v>31</v>
+      <c r="E40" s="96">
+        <v>38</v>
       </c>
       <c r="F40" s="42"/>
       <c r="G40" s="42"/>
       <c r="H40" s="55">
         <f t="shared" si="0"/>
-        <v>6.8000000000000007</v>
+        <v>7.2666666666666666</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1">
@@ -13817,14 +13848,14 @@
       <c r="D41" s="42">
         <v>34</v>
       </c>
-      <c r="E41" s="94">
-        <v>26</v>
+      <c r="E41" s="96">
+        <v>29</v>
       </c>
       <c r="F41" s="42"/>
       <c r="G41" s="42"/>
       <c r="H41" s="55">
         <f t="shared" si="0"/>
-        <v>5.6666666666666661</v>
+        <v>5.8666666666666671</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1">
@@ -13840,7 +13871,7 @@
       <c r="D42" s="42">
         <v>19</v>
       </c>
-      <c r="E42" s="94">
+      <c r="E42" s="96">
         <v>15</v>
       </c>
       <c r="F42" s="42"/>
@@ -13863,7 +13894,7 @@
       <c r="D43" s="42">
         <v>25</v>
       </c>
-      <c r="E43" s="94">
+      <c r="E43" s="96">
         <v>27</v>
       </c>
       <c r="F43" s="42"/>
@@ -13886,7 +13917,7 @@
       <c r="D44" s="42">
         <v>25</v>
       </c>
-      <c r="E44" s="94">
+      <c r="E44" s="96">
         <v>9</v>
       </c>
       <c r="F44" s="42"/>
@@ -13909,7 +13940,7 @@
       <c r="D45" s="42">
         <v>32</v>
       </c>
-      <c r="E45" s="94">
+      <c r="E45" s="96">
         <v>25</v>
       </c>
       <c r="F45" s="42"/>
@@ -13932,7 +13963,7 @@
       <c r="D46" s="42">
         <v>33</v>
       </c>
-      <c r="E46" s="94">
+      <c r="E46" s="96">
         <v>25</v>
       </c>
       <c r="F46" s="42"/>
@@ -13955,7 +13986,7 @@
       <c r="D47" s="42">
         <v>25</v>
       </c>
-      <c r="E47" s="94">
+      <c r="E47" s="96">
         <v>30</v>
       </c>
       <c r="F47" s="42"/>
@@ -13978,7 +14009,7 @@
       <c r="D48" s="42">
         <v>36</v>
       </c>
-      <c r="E48" s="94">
+      <c r="E48" s="96">
         <v>25</v>
       </c>
       <c r="F48" s="42"/>
@@ -14001,7 +14032,7 @@
       <c r="D49" s="42">
         <v>42</v>
       </c>
-      <c r="E49" s="94">
+      <c r="E49" s="96">
         <v>34</v>
       </c>
       <c r="F49" s="42"/>
@@ -14024,7 +14055,7 @@
       <c r="D50" s="42">
         <v>37</v>
       </c>
-      <c r="E50" s="94">
+      <c r="E50" s="96">
         <v>29</v>
       </c>
       <c r="F50" s="42"/>
@@ -14047,7 +14078,7 @@
       <c r="D51" s="42">
         <v>27</v>
       </c>
-      <c r="E51" s="94">
+      <c r="E51" s="96">
         <v>17</v>
       </c>
       <c r="F51" s="42"/>
@@ -14070,7 +14101,7 @@
       <c r="D52" s="42">
         <v>37</v>
       </c>
-      <c r="E52" s="94">
+      <c r="E52" s="96">
         <v>33</v>
       </c>
       <c r="F52" s="42"/>
@@ -14093,7 +14124,7 @@
       <c r="D53" s="42">
         <v>30</v>
       </c>
-      <c r="E53" s="94">
+      <c r="E53" s="96">
         <v>29</v>
       </c>
       <c r="F53" s="42"/>
@@ -14116,21 +14147,21 @@
       <c r="D54" s="42">
         <v>46</v>
       </c>
-      <c r="E54" s="94">
-        <v>43</v>
+      <c r="E54" s="96">
+        <v>45</v>
       </c>
       <c r="F54" s="42"/>
       <c r="G54" s="42"/>
       <c r="H54" s="55">
         <f t="shared" si="0"/>
-        <v>8.6</v>
+        <v>8.7333333333333325</v>
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="111" t="s">
+      <c r="A55" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="112"/>
+      <c r="B55" s="105"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -14138,17 +14169,17 @@
       <c r="D55" s="42">
         <v>44</v>
       </c>
-      <c r="E55" s="42">
+      <c r="E55" s="96">
         <v>40</v>
       </c>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="109" t="s">
+      <c r="A56" s="101" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="110"/>
+      <c r="B56" s="102"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -14163,10 +14194,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="109" t="s">
+      <c r="A57" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="110"/>
+      <c r="B57" s="102"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -14181,10 +14212,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="109" t="s">
+      <c r="A58" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="110"/>
+      <c r="B58" s="102"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -14200,25 +14231,30 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:E54">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14236,8 +14272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF58"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="AB5" sqref="AB5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -14251,147 +14287,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="112" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="99" t="s">
+      <c r="F1" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="107" t="s">
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="119" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="139" t="s">
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="134" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="140"/>
-      <c r="P1" s="140"/>
-      <c r="Q1" s="140"/>
-      <c r="R1" s="140"/>
-      <c r="S1" s="140"/>
-      <c r="T1" s="140"/>
-      <c r="U1" s="140"/>
-      <c r="V1" s="140"/>
-      <c r="W1" s="140"/>
-      <c r="X1" s="140"/>
-      <c r="Y1" s="140"/>
-      <c r="Z1" s="140"/>
-      <c r="AA1" s="140"/>
-      <c r="AB1" s="140"/>
+      <c r="O1" s="135"/>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="135"/>
+      <c r="R1" s="135"/>
+      <c r="S1" s="135"/>
+      <c r="T1" s="135"/>
+      <c r="U1" s="135"/>
+      <c r="V1" s="135"/>
+      <c r="W1" s="135"/>
+      <c r="X1" s="135"/>
+      <c r="Y1" s="135"/>
+      <c r="Z1" s="135"/>
+      <c r="AA1" s="135"/>
+      <c r="AB1" s="135"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="118"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="111"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="102" t="s">
+      <c r="F2" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="107" t="s">
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="119" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="139" t="s">
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="134" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="140"/>
-      <c r="P2" s="140"/>
-      <c r="Q2" s="140"/>
-      <c r="R2" s="140"/>
-      <c r="S2" s="140"/>
-      <c r="T2" s="140"/>
-      <c r="U2" s="140"/>
-      <c r="V2" s="140"/>
-      <c r="W2" s="140"/>
-      <c r="X2" s="140"/>
-      <c r="Y2" s="140"/>
-      <c r="Z2" s="140"/>
-      <c r="AA2" s="140"/>
-      <c r="AB2" s="140"/>
+      <c r="O2" s="135"/>
+      <c r="P2" s="135"/>
+      <c r="Q2" s="135"/>
+      <c r="R2" s="135"/>
+      <c r="S2" s="135"/>
+      <c r="T2" s="135"/>
+      <c r="U2" s="135"/>
+      <c r="V2" s="135"/>
+      <c r="W2" s="135"/>
+      <c r="X2" s="135"/>
+      <c r="Y2" s="135"/>
+      <c r="Z2" s="135"/>
+      <c r="AA2" s="135"/>
+      <c r="AB2" s="135"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="142" t="s">
+      <c r="A3" s="137" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="143"/>
-      <c r="C3" s="144"/>
+      <c r="B3" s="138"/>
+      <c r="C3" s="139"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="141" t="s">
+      <c r="F3" s="136" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="141"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="150" t="s">
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="145" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="150"/>
-      <c r="L3" s="150"/>
-      <c r="M3" s="150"/>
-      <c r="N3" s="139" t="s">
+      <c r="K3" s="145"/>
+      <c r="L3" s="145"/>
+      <c r="M3" s="145"/>
+      <c r="N3" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="140"/>
-      <c r="P3" s="140"/>
-      <c r="Q3" s="140"/>
-      <c r="R3" s="140"/>
-      <c r="S3" s="140"/>
-      <c r="T3" s="140"/>
-      <c r="U3" s="140"/>
-      <c r="V3" s="140"/>
-      <c r="W3" s="140"/>
-      <c r="X3" s="140"/>
-      <c r="Y3" s="140"/>
-      <c r="Z3" s="140"/>
-      <c r="AA3" s="140"/>
-      <c r="AB3" s="140"/>
+      <c r="O3" s="135"/>
+      <c r="P3" s="135"/>
+      <c r="Q3" s="135"/>
+      <c r="R3" s="135"/>
+      <c r="S3" s="135"/>
+      <c r="T3" s="135"/>
+      <c r="U3" s="135"/>
+      <c r="V3" s="135"/>
+      <c r="W3" s="135"/>
+      <c r="X3" s="135"/>
+      <c r="Y3" s="135"/>
+      <c r="Z3" s="135"/>
+      <c r="AA3" s="135"/>
+      <c r="AB3" s="135"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="145"/>
-      <c r="B4" s="146"/>
-      <c r="C4" s="147"/>
-      <c r="D4" s="148">
+      <c r="A4" s="140"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="143">
         <v>43344</v>
       </c>
-      <c r="E4" s="149"/>
-      <c r="F4" s="149"/>
-      <c r="G4" s="149"/>
-      <c r="H4" s="149"/>
-      <c r="I4" s="149"/>
-      <c r="J4" s="149"/>
-      <c r="K4" s="149"/>
-      <c r="L4" s="149"/>
-      <c r="M4" s="149"/>
+      <c r="E4" s="144"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144"/>
+      <c r="H4" s="144"/>
+      <c r="I4" s="144"/>
+      <c r="J4" s="144"/>
+      <c r="K4" s="144"/>
+      <c r="L4" s="144"/>
+      <c r="M4" s="144"/>
       <c r="N4" s="59"/>
       <c r="O4" s="59"/>
       <c r="P4" s="59"/>
@@ -14404,55 +14440,61 @@
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="113" t="s">
+      <c r="B5" s="106" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="134" t="s">
+      <c r="D5" s="147" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="135"/>
-      <c r="F5" s="135"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="137" t="s">
+      <c r="E5" s="148"/>
+      <c r="F5" s="148"/>
+      <c r="G5" s="149"/>
+      <c r="H5" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="138"/>
-      <c r="J5" s="138"/>
-      <c r="K5" s="138"/>
-      <c r="L5" s="133" t="s">
+      <c r="I5" s="151"/>
+      <c r="J5" s="151"/>
+      <c r="K5" s="151"/>
+      <c r="L5" s="146" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="133"/>
-      <c r="N5" s="137" t="s">
+      <c r="M5" s="146"/>
+      <c r="N5" s="150" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="138"/>
-      <c r="P5" s="138"/>
-      <c r="Q5" s="138"/>
-      <c r="R5" s="133" t="s">
+      <c r="O5" s="151"/>
+      <c r="P5" s="151"/>
+      <c r="Q5" s="151"/>
+      <c r="R5" s="146" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="133"/>
-      <c r="T5" s="119" t="s">
+      <c r="S5" s="146"/>
+      <c r="T5" s="115" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="119"/>
-      <c r="V5" s="119" t="s">
+      <c r="U5" s="115"/>
+      <c r="V5" s="115" t="s">
         <v>117</v>
       </c>
-      <c r="W5" s="119"/>
-      <c r="X5" s="119"/>
-      <c r="Y5" s="119"/>
+      <c r="W5" s="115"/>
+      <c r="X5" s="115"/>
+      <c r="Y5" s="115"/>
+      <c r="Z5" s="115" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA5" s="115"/>
+      <c r="AB5" s="115"/>
+      <c r="AC5" s="115"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="122"/>
-      <c r="B6" s="114"/>
+      <c r="A6" s="127"/>
+      <c r="B6" s="107"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -14522,17 +14564,25 @@
       <c r="Y6" s="93">
         <v>11</v>
       </c>
-      <c r="Z6" s="19"/>
-      <c r="AA6" s="19"/>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="19"/>
+      <c r="Z6" s="19">
+        <v>11</v>
+      </c>
+      <c r="AA6" s="96">
+        <v>11</v>
+      </c>
+      <c r="AB6" s="96">
+        <v>11</v>
+      </c>
+      <c r="AC6" s="96">
+        <v>11</v>
+      </c>
       <c r="AD6" s="19"/>
       <c r="AE6" s="19"/>
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="122"/>
-      <c r="B7" s="114"/>
+      <c r="A7" s="127"/>
+      <c r="B7" s="107"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -14594,25 +14644,33 @@
         <v>1</v>
       </c>
       <c r="W7" s="93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X7" s="93">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y7" s="93">
-        <v>4</v>
-      </c>
-      <c r="Z7" s="19"/>
-      <c r="AA7" s="19"/>
-      <c r="AB7" s="19"/>
-      <c r="AC7" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="Z7" s="19">
+        <v>8</v>
+      </c>
+      <c r="AA7" s="96">
+        <v>8</v>
+      </c>
+      <c r="AB7" s="96">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="96">
+        <v>8</v>
+      </c>
       <c r="AD7" s="19"/>
       <c r="AE7" s="19"/>
       <c r="AF7" s="19"/>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="123"/>
-      <c r="B8" s="115"/>
+      <c r="A8" s="128"/>
+      <c r="B8" s="108"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -14674,18 +14732,26 @@
         <v>5</v>
       </c>
       <c r="W8" s="93">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X8" s="93">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Y8" s="93">
-        <v>5</v>
-      </c>
-      <c r="Z8" s="19"/>
-      <c r="AA8" s="19"/>
-      <c r="AB8" s="19"/>
-      <c r="AC8" s="19"/>
+        <v>8</v>
+      </c>
+      <c r="Z8" s="19">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="96">
+        <v>2</v>
+      </c>
+      <c r="AB8" s="96">
+        <v>3</v>
+      </c>
+      <c r="AC8" s="96">
+        <v>4</v>
+      </c>
       <c r="AD8" s="19"/>
       <c r="AE8" s="19"/>
       <c r="AF8" s="19"/>
@@ -14764,10 +14830,18 @@
       <c r="Y9" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z9" s="19"/>
-      <c r="AA9" s="19"/>
-      <c r="AB9" s="19"/>
-      <c r="AC9" s="19"/>
+      <c r="Z9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC9" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AD9" s="19"/>
       <c r="AE9" s="19"/>
       <c r="AF9" s="19"/>
@@ -14846,10 +14920,18 @@
       <c r="Y10" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z10" s="19"/>
-      <c r="AA10" s="19"/>
-      <c r="AB10" s="19"/>
-      <c r="AC10" s="19"/>
+      <c r="Z10" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA10" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB10" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC10" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD10" s="19"/>
       <c r="AE10" s="19"/>
       <c r="AF10" s="19"/>
@@ -14928,10 +15010,18 @@
       <c r="Y11" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z11" s="19"/>
-      <c r="AA11" s="19"/>
-      <c r="AB11" s="19"/>
-      <c r="AC11" s="19"/>
+      <c r="Z11" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA11" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB11" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC11" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD11" s="19"/>
       <c r="AE11" s="19"/>
       <c r="AF11" s="19"/>
@@ -15010,10 +15100,18 @@
       <c r="Y12" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z12" s="19"/>
-      <c r="AA12" s="19"/>
-      <c r="AB12" s="19"/>
-      <c r="AC12" s="19"/>
+      <c r="Z12" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA12" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB12" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC12" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD12" s="19"/>
       <c r="AE12" s="19"/>
       <c r="AF12" s="19"/>
@@ -15092,10 +15190,18 @@
       <c r="Y13" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z13" s="19"/>
-      <c r="AA13" s="19"/>
-      <c r="AB13" s="19"/>
-      <c r="AC13" s="19"/>
+      <c r="Z13" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA13" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB13" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC13" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD13" s="19"/>
       <c r="AE13" s="19"/>
       <c r="AF13" s="19"/>
@@ -15174,10 +15280,18 @@
       <c r="Y14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="Z14" s="19"/>
-      <c r="AA14" s="19"/>
-      <c r="AB14" s="19"/>
-      <c r="AC14" s="19"/>
+      <c r="Z14" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA14" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB14" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC14" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD14" s="19"/>
       <c r="AE14" s="19"/>
       <c r="AF14" s="19"/>
@@ -15256,10 +15370,18 @@
       <c r="Y15" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z15" s="19"/>
-      <c r="AA15" s="19"/>
-      <c r="AB15" s="19"/>
-      <c r="AC15" s="19"/>
+      <c r="Z15" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA15" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB15" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC15" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD15" s="19"/>
       <c r="AE15" s="19"/>
       <c r="AF15" s="19"/>
@@ -15338,10 +15460,18 @@
       <c r="Y16" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z16" s="19"/>
-      <c r="AA16" s="19"/>
-      <c r="AB16" s="19"/>
-      <c r="AC16" s="19"/>
+      <c r="Z16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC16" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AD16" s="19"/>
       <c r="AE16" s="19"/>
       <c r="AF16" s="19"/>
@@ -15420,10 +15550,18 @@
       <c r="Y17" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z17" s="19"/>
-      <c r="AA17" s="19"/>
-      <c r="AB17" s="19"/>
-      <c r="AC17" s="19"/>
+      <c r="Z17" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA17" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB17" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC17" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD17" s="19"/>
       <c r="AE17" s="19"/>
       <c r="AF17" s="19"/>
@@ -15502,10 +15640,18 @@
       <c r="Y18" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z18" s="19"/>
-      <c r="AA18" s="19"/>
-      <c r="AB18" s="19"/>
-      <c r="AC18" s="19"/>
+      <c r="Z18" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA18" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB18" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC18" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD18" s="19"/>
       <c r="AE18" s="19"/>
       <c r="AF18" s="19"/>
@@ -15584,10 +15730,18 @@
       <c r="Y19" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z19" s="19"/>
-      <c r="AA19" s="19"/>
-      <c r="AB19" s="19"/>
-      <c r="AC19" s="19"/>
+      <c r="Z19" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA19" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB19" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC19" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AD19" s="19"/>
       <c r="AE19" s="19"/>
       <c r="AF19" s="19"/>
@@ -15666,10 +15820,18 @@
       <c r="Y20" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z20" s="19"/>
-      <c r="AA20" s="19"/>
-      <c r="AB20" s="19"/>
-      <c r="AC20" s="19"/>
+      <c r="Z20" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA20" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB20" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC20" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD20" s="19"/>
       <c r="AE20" s="19"/>
       <c r="AF20" s="19"/>
@@ -15748,10 +15910,18 @@
       <c r="Y21" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z21" s="19"/>
-      <c r="AA21" s="19"/>
-      <c r="AB21" s="19"/>
-      <c r="AC21" s="19"/>
+      <c r="Z21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC21" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AD21" s="19"/>
       <c r="AE21" s="19"/>
       <c r="AF21" s="19"/>
@@ -15830,10 +16000,18 @@
       <c r="Y22" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z22" s="19"/>
-      <c r="AA22" s="19"/>
-      <c r="AB22" s="19"/>
-      <c r="AC22" s="19"/>
+      <c r="Z22" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA22" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB22" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC22" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD22" s="19"/>
       <c r="AE22" s="19"/>
       <c r="AF22" s="19"/>
@@ -15912,10 +16090,18 @@
       <c r="Y23" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19"/>
-      <c r="AB23" s="19"/>
-      <c r="AC23" s="19"/>
+      <c r="Z23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC23" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AD23" s="19"/>
       <c r="AE23" s="19"/>
       <c r="AF23" s="19"/>
@@ -15994,10 +16180,18 @@
       <c r="Y24" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z24" s="19"/>
-      <c r="AA24" s="19"/>
-      <c r="AB24" s="19"/>
-      <c r="AC24" s="19"/>
+      <c r="Z24" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA24" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB24" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC24" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD24" s="19"/>
       <c r="AE24" s="19"/>
       <c r="AF24" s="19"/>
@@ -16076,10 +16270,18 @@
       <c r="Y25" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z25" s="19"/>
-      <c r="AA25" s="19"/>
-      <c r="AB25" s="19"/>
-      <c r="AC25" s="19"/>
+      <c r="Z25" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA25" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB25" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC25" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD25" s="19"/>
       <c r="AE25" s="19"/>
       <c r="AF25" s="19"/>
@@ -16158,10 +16360,18 @@
       <c r="Y26" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z26" s="19"/>
-      <c r="AA26" s="19"/>
-      <c r="AB26" s="19"/>
-      <c r="AC26" s="19"/>
+      <c r="Z26" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA26" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB26" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC26" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD26" s="19"/>
       <c r="AE26" s="19"/>
       <c r="AF26" s="19"/>
@@ -16240,10 +16450,18 @@
       <c r="Y27" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z27" s="19"/>
-      <c r="AA27" s="19"/>
-      <c r="AB27" s="19"/>
-      <c r="AC27" s="19"/>
+      <c r="Z27" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA27" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB27" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC27" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AD27" s="19"/>
       <c r="AE27" s="19"/>
       <c r="AF27" s="19"/>
@@ -16322,10 +16540,18 @@
       <c r="Y28" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z28" s="19"/>
-      <c r="AA28" s="19"/>
-      <c r="AB28" s="19"/>
-      <c r="AC28" s="19"/>
+      <c r="Z28" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA28" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB28" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC28" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD28" s="19"/>
       <c r="AE28" s="19"/>
       <c r="AF28" s="19"/>
@@ -16404,10 +16630,18 @@
       <c r="Y29" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z29" s="19"/>
-      <c r="AA29" s="19"/>
-      <c r="AB29" s="19"/>
-      <c r="AC29" s="19"/>
+      <c r="Z29" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA29" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB29" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC29" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD29" s="19"/>
       <c r="AE29" s="19"/>
       <c r="AF29" s="19"/>
@@ -16486,10 +16720,18 @@
       <c r="Y30" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z30" s="19"/>
-      <c r="AA30" s="19"/>
-      <c r="AB30" s="19"/>
-      <c r="AC30" s="19"/>
+      <c r="Z30" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA30" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB30" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC30" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD30" s="19"/>
       <c r="AE30" s="19"/>
       <c r="AF30" s="19"/>
@@ -16568,10 +16810,18 @@
       <c r="Y31" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z31" s="19"/>
-      <c r="AA31" s="19"/>
-      <c r="AB31" s="19"/>
-      <c r="AC31" s="19"/>
+      <c r="Z31" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA31" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB31" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC31" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD31" s="19"/>
       <c r="AE31" s="19"/>
       <c r="AF31" s="19"/>
@@ -16650,10 +16900,18 @@
       <c r="Y32" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z32" s="19"/>
-      <c r="AA32" s="19"/>
-      <c r="AB32" s="19"/>
-      <c r="AC32" s="19"/>
+      <c r="Z32" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA32" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB32" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC32" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD32" s="19"/>
       <c r="AE32" s="19"/>
       <c r="AF32" s="19"/>
@@ -16732,10 +16990,18 @@
       <c r="Y33" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z33" s="19"/>
-      <c r="AA33" s="19"/>
-      <c r="AB33" s="19"/>
-      <c r="AC33" s="19"/>
+      <c r="Z33" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA33" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB33" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC33" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AD33" s="19"/>
       <c r="AE33" s="19"/>
       <c r="AF33" s="19"/>
@@ -16814,10 +17080,18 @@
       <c r="Y34" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z34" s="19"/>
-      <c r="AA34" s="19"/>
-      <c r="AB34" s="19"/>
-      <c r="AC34" s="19"/>
+      <c r="Z34" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA34" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB34" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC34" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD34" s="19"/>
       <c r="AE34" s="19"/>
       <c r="AF34" s="19"/>
@@ -16896,10 +17170,18 @@
       <c r="Y35" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z35" s="19"/>
-      <c r="AA35" s="19"/>
-      <c r="AB35" s="19"/>
-      <c r="AC35" s="19"/>
+      <c r="Z35" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA35" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB35" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC35" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AD35" s="19"/>
       <c r="AE35" s="19"/>
       <c r="AF35" s="19"/>
@@ -16978,10 +17260,18 @@
       <c r="Y36" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z36" s="19"/>
-      <c r="AA36" s="19"/>
-      <c r="AB36" s="19"/>
-      <c r="AC36" s="19"/>
+      <c r="Z36" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA36" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB36" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC36" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD36" s="19"/>
       <c r="AE36" s="19"/>
       <c r="AF36" s="19"/>
@@ -17060,10 +17350,18 @@
       <c r="Y37" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z37" s="19"/>
-      <c r="AA37" s="19"/>
-      <c r="AB37" s="19"/>
-      <c r="AC37" s="19"/>
+      <c r="Z37" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA37" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB37" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC37" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD37" s="19"/>
       <c r="AE37" s="19"/>
       <c r="AF37" s="19"/>
@@ -17142,10 +17440,18 @@
       <c r="Y38" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z38" s="19"/>
-      <c r="AA38" s="19"/>
-      <c r="AB38" s="19"/>
-      <c r="AC38" s="19"/>
+      <c r="Z38" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA38" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB38" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC38" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD38" s="19"/>
       <c r="AE38" s="19"/>
       <c r="AF38" s="19"/>
@@ -17224,10 +17530,18 @@
       <c r="Y39" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z39" s="19"/>
-      <c r="AA39" s="19"/>
-      <c r="AB39" s="19"/>
-      <c r="AC39" s="19"/>
+      <c r="Z39" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA39" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB39" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC39" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD39" s="19"/>
       <c r="AE39" s="19"/>
       <c r="AF39" s="19"/>
@@ -17306,10 +17620,18 @@
       <c r="Y40" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z40" s="19"/>
-      <c r="AA40" s="19"/>
-      <c r="AB40" s="19"/>
-      <c r="AC40" s="19"/>
+      <c r="Z40" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA40" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB40" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC40" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD40" s="19"/>
       <c r="AE40" s="19"/>
       <c r="AF40" s="19"/>
@@ -17388,10 +17710,18 @@
       <c r="Y41" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z41" s="19"/>
-      <c r="AA41" s="19"/>
-      <c r="AB41" s="19"/>
-      <c r="AC41" s="19"/>
+      <c r="Z41" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA41" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB41" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC41" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD41" s="19"/>
       <c r="AE41" s="19"/>
       <c r="AF41" s="19"/>
@@ -17470,10 +17800,18 @@
       <c r="Y42" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z42" s="19"/>
-      <c r="AA42" s="19"/>
-      <c r="AB42" s="19"/>
-      <c r="AC42" s="19"/>
+      <c r="Z42" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA42" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB42" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC42" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD42" s="19"/>
       <c r="AE42" s="19"/>
       <c r="AF42" s="19"/>
@@ -17552,10 +17890,18 @@
       <c r="Y43" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z43" s="19"/>
-      <c r="AA43" s="19"/>
-      <c r="AB43" s="19"/>
-      <c r="AC43" s="19"/>
+      <c r="Z43" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA43" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB43" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC43" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD43" s="19"/>
       <c r="AE43" s="19"/>
       <c r="AF43" s="19"/>
@@ -17634,10 +17980,18 @@
       <c r="Y44" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z44" s="19"/>
-      <c r="AA44" s="19"/>
-      <c r="AB44" s="19"/>
-      <c r="AC44" s="19"/>
+      <c r="Z44" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA44" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB44" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC44" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD44" s="19"/>
       <c r="AE44" s="19"/>
       <c r="AF44" s="19"/>
@@ -17716,10 +18070,18 @@
       <c r="Y45" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z45" s="19"/>
-      <c r="AA45" s="19"/>
-      <c r="AB45" s="19"/>
-      <c r="AC45" s="19"/>
+      <c r="Z45" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA45" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB45" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC45" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD45" s="19"/>
       <c r="AE45" s="19"/>
       <c r="AF45" s="19"/>
@@ -17798,10 +18160,18 @@
       <c r="Y46" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z46" s="19"/>
-      <c r="AA46" s="19"/>
-      <c r="AB46" s="19"/>
-      <c r="AC46" s="19"/>
+      <c r="Z46" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA46" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB46" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC46" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD46" s="19"/>
       <c r="AE46" s="19"/>
       <c r="AF46" s="19"/>
@@ -17880,10 +18250,18 @@
       <c r="Y47" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z47" s="19"/>
-      <c r="AA47" s="19"/>
-      <c r="AB47" s="19"/>
-      <c r="AC47" s="19"/>
+      <c r="Z47" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA47" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB47" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC47" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD47" s="19"/>
       <c r="AE47" s="19"/>
       <c r="AF47" s="19"/>
@@ -17962,10 +18340,18 @@
       <c r="Y48" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z48" s="19"/>
-      <c r="AA48" s="19"/>
-      <c r="AB48" s="19"/>
-      <c r="AC48" s="19"/>
+      <c r="Z48" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA48" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB48" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC48" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD48" s="19"/>
       <c r="AE48" s="19"/>
       <c r="AF48" s="19"/>
@@ -18044,10 +18430,18 @@
       <c r="Y49" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z49" s="19"/>
-      <c r="AA49" s="19"/>
-      <c r="AB49" s="19"/>
-      <c r="AC49" s="19"/>
+      <c r="Z49" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA49" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB49" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC49" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AD49" s="19"/>
       <c r="AE49" s="19"/>
       <c r="AF49" s="19"/>
@@ -18126,10 +18520,18 @@
       <c r="Y50" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z50" s="19"/>
-      <c r="AA50" s="19"/>
-      <c r="AB50" s="19"/>
-      <c r="AC50" s="19"/>
+      <c r="Z50" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA50" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB50" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC50" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD50" s="19"/>
       <c r="AE50" s="19"/>
       <c r="AF50" s="19"/>
@@ -18208,10 +18610,18 @@
       <c r="Y51" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z51" s="19"/>
-      <c r="AA51" s="19"/>
-      <c r="AB51" s="19"/>
-      <c r="AC51" s="19"/>
+      <c r="Z51" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA51" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB51" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC51" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD51" s="19"/>
       <c r="AE51" s="19"/>
       <c r="AF51" s="19"/>
@@ -18290,10 +18700,18 @@
       <c r="Y52" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z52" s="19"/>
-      <c r="AA52" s="19"/>
-      <c r="AB52" s="19"/>
-      <c r="AC52" s="19"/>
+      <c r="Z52" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA52" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB52" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC52" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD52" s="19"/>
       <c r="AE52" s="19"/>
       <c r="AF52" s="19"/>
@@ -18372,10 +18790,18 @@
       <c r="Y53" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z53" s="19"/>
-      <c r="AA53" s="19"/>
-      <c r="AB53" s="19"/>
-      <c r="AC53" s="19"/>
+      <c r="Z53" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA53" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB53" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC53" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD53" s="19"/>
       <c r="AE53" s="19"/>
       <c r="AF53" s="19"/>
@@ -18454,10 +18880,18 @@
       <c r="Y54" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z54" s="19"/>
-      <c r="AA54" s="19"/>
-      <c r="AB54" s="19"/>
-      <c r="AC54" s="19"/>
+      <c r="Z54" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA54" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB54" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC54" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD54" s="19"/>
       <c r="AE54" s="19"/>
       <c r="AF54" s="19"/>
@@ -18536,10 +18970,18 @@
       <c r="Y55" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z55" s="19"/>
-      <c r="AA55" s="19"/>
-      <c r="AB55" s="19"/>
-      <c r="AC55" s="19"/>
+      <c r="Z55" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA55" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB55" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC55" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD55" s="19"/>
       <c r="AE55" s="19"/>
       <c r="AF55" s="19"/>
@@ -18618,19 +19060,27 @@
       <c r="Y56" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="Z56" s="19"/>
-      <c r="AA56" s="19"/>
-      <c r="AB56" s="19"/>
-      <c r="AC56" s="19"/>
+      <c r="Z56" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA56" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB56" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC56" s="96" t="s">
+        <v>54</v>
+      </c>
       <c r="AD56" s="19"/>
       <c r="AE56" s="19"/>
       <c r="AF56" s="19"/>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="111" t="s">
+      <c r="A57" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="112"/>
+      <c r="B57" s="105"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -18722,19 +19172,19 @@
       </c>
       <c r="Z57" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AA57" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AB57" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AC57" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AD57" s="19">
         <f t="shared" si="0"/>
@@ -18750,10 +19200,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="109" t="s">
+      <c r="A58" s="101" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="110"/>
+      <c r="B58" s="102"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -18845,19 +19295,19 @@
       </c>
       <c r="Z58" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AA58" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AB58" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AC58" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AD58" s="24">
         <f t="shared" si="1"/>
@@ -18873,7 +19323,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="N5:Q5"/>
     <mergeCell ref="N1:AB1"/>
     <mergeCell ref="N2:AB2"/>
     <mergeCell ref="N3:AB3"/>
@@ -18887,17 +19349,6 @@
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="N5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18923,28 +19374,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="153" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="154" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="153" t="s">
+      <c r="A3" s="154" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="153"/>
-      <c r="C3" s="153"/>
-      <c r="D3" s="153"/>
+      <c r="B3" s="154"/>
+      <c r="C3" s="154"/>
+      <c r="D3" s="154"/>
     </row>
     <row r="4" spans="1:4" s="84" customFormat="1" ht="28.5">
       <c r="A4" s="82" t="s">
@@ -19675,41 +20126,41 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="151" t="s">
+      <c r="A56" s="152" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="151"/>
-      <c r="C56" s="151"/>
+      <c r="B56" s="152"/>
+      <c r="C56" s="152"/>
       <c r="D56" s="76">
         <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="151" t="s">
+      <c r="A57" s="152" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="151"/>
-      <c r="C57" s="151"/>
+      <c r="B57" s="152"/>
+      <c r="C57" s="152"/>
       <c r="D57" s="77">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="151" t="s">
+      <c r="A58" s="152" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="151"/>
-      <c r="C58" s="151"/>
+      <c r="B58" s="152"/>
+      <c r="C58" s="152"/>
       <c r="D58" s="77">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="151" t="s">
+      <c r="A59" s="152" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="151"/>
-      <c r="C59" s="151"/>
+      <c r="B59" s="152"/>
+      <c r="C59" s="152"/>
       <c r="D59" s="77">
         <v>92</v>
       </c>
@@ -19755,7 +20206,7 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:C55 C8:C23">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Last Update 09-11-2018  7:23:35.05
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Expected Internal Marks" sheetId="6" r:id="rId3"/>
     <sheet name="Lab Attendance" sheetId="4" r:id="rId4"/>
     <sheet name="UT-2-Satement" sheetId="7" r:id="rId5"/>
+    <sheet name="UT-3-Satement" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attendance!$AC$1:$AC$57</definedName>
@@ -920,6 +921,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="AW7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Quick Sort, Tuples</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1203,7 +1228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3833" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4003" uniqueCount="168">
   <si>
     <t>S.NO</t>
   </si>
@@ -1561,6 +1586,153 @@
   <si>
     <t>Lab 6</t>
   </si>
+  <si>
+    <t>Abishraj K</t>
+  </si>
+  <si>
+    <t>Alten C Joseph</t>
+  </si>
+  <si>
+    <t>Anusuya K</t>
+  </si>
+  <si>
+    <t>Aravindraj</t>
+  </si>
+  <si>
+    <t>Balaganapathy V</t>
+  </si>
+  <si>
+    <t>Deepa K</t>
+  </si>
+  <si>
+    <t>Deepak S</t>
+  </si>
+  <si>
+    <t>Dhanush D R</t>
+  </si>
+  <si>
+    <t>Dinesh R</t>
+  </si>
+  <si>
+    <t>Enoch Philip M K</t>
+  </si>
+  <si>
+    <t>Gayathri V</t>
+  </si>
+  <si>
+    <t>Gokul Rajan R</t>
+  </si>
+  <si>
+    <t>Hari Pranav P J</t>
+  </si>
+  <si>
+    <t>Hariharaganesh M</t>
+  </si>
+  <si>
+    <t>Janarthan P</t>
+  </si>
+  <si>
+    <t>Jenah Karthick P</t>
+  </si>
+  <si>
+    <t>Kamatchisundar K</t>
+  </si>
+  <si>
+    <t>Karthikeyan M</t>
+  </si>
+  <si>
+    <t>Kavitha.N</t>
+  </si>
+  <si>
+    <t>Keerthana A</t>
+  </si>
+  <si>
+    <t>Keerthana K</t>
+  </si>
+  <si>
+    <t>Lokesh R Mq</t>
+  </si>
+  <si>
+    <t>Maneesha  S</t>
+  </si>
+  <si>
+    <t>Manoj S</t>
+  </si>
+  <si>
+    <t>Mithun Santhosh Y</t>
+  </si>
+  <si>
+    <t>Nandhini.S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pavithra B </t>
+  </si>
+  <si>
+    <t>Pavithra S</t>
+  </si>
+  <si>
+    <t>Prasanth Kumar P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pravin S </t>
+  </si>
+  <si>
+    <t>Ritesh S</t>
+  </si>
+  <si>
+    <t>Sai Bgm Hemamalini</t>
+  </si>
+  <si>
+    <t>Samuvel S</t>
+  </si>
+  <si>
+    <t>Sanjay J</t>
+  </si>
+  <si>
+    <t>Sathish Kumar P</t>
+  </si>
+  <si>
+    <t>Selvamani P</t>
+  </si>
+  <si>
+    <t>Sri Hari Gupta K</t>
+  </si>
+  <si>
+    <t>Sridhar S R</t>
+  </si>
+  <si>
+    <t>Surya Kumar A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suvetha B </t>
+  </si>
+  <si>
+    <t>Taniya Joseph J</t>
+  </si>
+  <si>
+    <t>Thirumurugan N</t>
+  </si>
+  <si>
+    <t>Tilotham Sd</t>
+  </si>
+  <si>
+    <t>Vijayanand R</t>
+  </si>
+  <si>
+    <t>Vishnupriya K</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Nandhini M</t>
+  </si>
+  <si>
+    <t>Sowmya S</t>
+  </si>
 </sst>
 </file>
 
@@ -1569,7 +1741,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1713,6 +1885,20 @@
       <b/>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="18"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1933,7 +2119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2232,6 +2418,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2241,14 +2463,17 @@
     <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2277,32 +2502,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2316,17 +2529,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2337,11 +2544,23 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2377,24 +2596,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2405,12 +2606,81 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -2775,11 +3045,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BL57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AB5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="AB41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AV7" sqref="AV7"/>
+      <selection pane="bottomRight" activeCell="AW59" sqref="AW59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -2793,29 +3063,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="18.75">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="F1" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="119" t="s">
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -2840,41 +3110,41 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:64" ht="19.5">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="111"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="124"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="103" t="s">
+      <c r="F2" s="108" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="119" t="s">
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="120" t="s">
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="114" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="120"/>
-      <c r="S2" s="120"/>
-      <c r="T2" s="120"/>
-      <c r="U2" s="120"/>
-      <c r="V2" s="120"/>
-      <c r="W2" s="120"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="114"/>
+      <c r="Q2" s="114"/>
+      <c r="R2" s="114"/>
+      <c r="S2" s="114"/>
+      <c r="T2" s="114"/>
+      <c r="U2" s="114"/>
+      <c r="V2" s="114"/>
+      <c r="W2" s="114"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -2887,41 +3157,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:64" ht="18.75">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="113"/>
-      <c r="C3" s="114"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="109"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="103" t="s">
+      <c r="F3" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="119" t="s">
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="119"/>
-      <c r="L3" s="119"/>
-      <c r="M3" s="119"/>
-      <c r="N3" s="120" t="s">
+      <c r="K3" s="113"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="113"/>
+      <c r="N3" s="114" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="120"/>
-      <c r="P3" s="120"/>
-      <c r="Q3" s="120"/>
-      <c r="R3" s="120"/>
-      <c r="S3" s="120"/>
-      <c r="T3" s="120"/>
-      <c r="U3" s="120"/>
-      <c r="V3" s="120"/>
-      <c r="W3" s="120"/>
+      <c r="O3" s="114"/>
+      <c r="P3" s="114"/>
+      <c r="Q3" s="114"/>
+      <c r="R3" s="114"/>
+      <c r="S3" s="114"/>
+      <c r="T3" s="114"/>
+      <c r="U3" s="114"/>
+      <c r="V3" s="114"/>
+      <c r="W3" s="114"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -2934,56 +3204,56 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:64" ht="18.75">
-      <c r="A4" s="112" t="s">
+      <c r="A4" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="113"/>
-      <c r="C4" s="114"/>
-      <c r="D4" s="98">
+      <c r="B4" s="104"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="110">
         <v>43344</v>
       </c>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
-      <c r="N4" s="99"/>
-      <c r="O4" s="99"/>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="99"/>
-      <c r="V4" s="99"/>
-      <c r="W4" s="100"/>
-      <c r="X4" s="98">
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="111"/>
+      <c r="L4" s="111"/>
+      <c r="M4" s="111"/>
+      <c r="N4" s="111"/>
+      <c r="O4" s="111"/>
+      <c r="P4" s="111"/>
+      <c r="Q4" s="111"/>
+      <c r="R4" s="111"/>
+      <c r="S4" s="111"/>
+      <c r="T4" s="111"/>
+      <c r="U4" s="111"/>
+      <c r="V4" s="111"/>
+      <c r="W4" s="112"/>
+      <c r="X4" s="110">
         <v>43374</v>
       </c>
-      <c r="Y4" s="99"/>
-      <c r="Z4" s="99"/>
-      <c r="AA4" s="99"/>
-      <c r="AB4" s="99"/>
-      <c r="AC4" s="99"/>
-      <c r="AD4" s="99"/>
-      <c r="AE4" s="99"/>
-      <c r="AF4" s="99"/>
-      <c r="AG4" s="99"/>
-      <c r="AH4" s="99"/>
-      <c r="AI4" s="99"/>
-      <c r="AJ4" s="99"/>
-      <c r="AK4" s="99"/>
-      <c r="AL4" s="99"/>
-      <c r="AM4" s="99"/>
-      <c r="AN4" s="99"/>
-      <c r="AO4" s="99"/>
-      <c r="AP4" s="99"/>
-      <c r="AQ4" s="99"/>
-      <c r="AR4" s="100"/>
+      <c r="Y4" s="111"/>
+      <c r="Z4" s="111"/>
+      <c r="AA4" s="111"/>
+      <c r="AB4" s="111"/>
+      <c r="AC4" s="111"/>
+      <c r="AD4" s="111"/>
+      <c r="AE4" s="111"/>
+      <c r="AF4" s="111"/>
+      <c r="AG4" s="111"/>
+      <c r="AH4" s="111"/>
+      <c r="AI4" s="111"/>
+      <c r="AJ4" s="111"/>
+      <c r="AK4" s="111"/>
+      <c r="AL4" s="111"/>
+      <c r="AM4" s="111"/>
+      <c r="AN4" s="111"/>
+      <c r="AO4" s="111"/>
+      <c r="AP4" s="111"/>
+      <c r="AQ4" s="111"/>
+      <c r="AR4" s="112"/>
       <c r="AS4" s="61"/>
       <c r="AT4" s="61"/>
       <c r="AU4" s="61"/>
@@ -3006,10 +3276,10 @@
       <c r="BL4" s="61"/>
     </row>
     <row r="5" spans="1:64">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="125" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="119" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -3150,7 +3420,9 @@
       <c r="AV5" s="93">
         <v>11</v>
       </c>
-      <c r="AW5" s="61"/>
+      <c r="AW5" s="98">
+        <v>11</v>
+      </c>
       <c r="AX5" s="61"/>
       <c r="AY5" s="61"/>
       <c r="AZ5" s="61"/>
@@ -3168,8 +3440,8 @@
       <c r="BL5" s="61"/>
     </row>
     <row r="6" spans="1:64">
-      <c r="A6" s="115"/>
-      <c r="B6" s="107"/>
+      <c r="A6" s="125"/>
+      <c r="B6" s="120"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -3308,7 +3580,9 @@
       <c r="AV6" s="93">
         <v>1</v>
       </c>
-      <c r="AW6" s="61"/>
+      <c r="AW6" s="98">
+        <v>8</v>
+      </c>
       <c r="AX6" s="61"/>
       <c r="AY6" s="61"/>
       <c r="AZ6" s="61"/>
@@ -3329,7 +3603,7 @@
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="108"/>
+      <c r="B7" s="121"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -3468,7 +3742,9 @@
       <c r="AV7" s="93">
         <v>4</v>
       </c>
-      <c r="AW7" s="61"/>
+      <c r="AW7" s="98">
+        <v>7</v>
+      </c>
       <c r="AX7" s="61"/>
       <c r="AY7" s="61"/>
       <c r="AZ7" s="61"/>
@@ -3628,7 +3904,9 @@
       <c r="AV8" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW8" s="61"/>
+      <c r="AW8" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AX8" s="61"/>
       <c r="AY8" s="61"/>
       <c r="AZ8" s="61"/>
@@ -3788,7 +4066,9 @@
       <c r="AV9" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW9" s="61"/>
+      <c r="AW9" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX9" s="61"/>
       <c r="AY9" s="61"/>
       <c r="AZ9" s="61"/>
@@ -3948,7 +4228,9 @@
       <c r="AV10" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW10" s="61"/>
+      <c r="AW10" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX10" s="61"/>
       <c r="AY10" s="61"/>
       <c r="AZ10" s="61"/>
@@ -4108,7 +4390,9 @@
       <c r="AV11" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW11" s="61"/>
+      <c r="AW11" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX11" s="61"/>
       <c r="AY11" s="61"/>
       <c r="AZ11" s="61"/>
@@ -4268,7 +4552,9 @@
       <c r="AV12" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW12" s="61"/>
+      <c r="AW12" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX12" s="61"/>
       <c r="AY12" s="61"/>
       <c r="AZ12" s="61"/>
@@ -4428,7 +4714,9 @@
       <c r="AV13" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AW13" s="61"/>
+      <c r="AW13" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX13" s="61"/>
       <c r="AY13" s="61"/>
       <c r="AZ13" s="61"/>
@@ -4588,7 +4876,9 @@
       <c r="AV14" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW14" s="61"/>
+      <c r="AW14" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX14" s="61"/>
       <c r="AY14" s="61"/>
       <c r="AZ14" s="61"/>
@@ -4748,7 +5038,9 @@
       <c r="AV15" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW15" s="61"/>
+      <c r="AW15" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AX15" s="61"/>
       <c r="AY15" s="61"/>
       <c r="AZ15" s="61"/>
@@ -4908,7 +5200,9 @@
       <c r="AV16" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW16" s="61"/>
+      <c r="AW16" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX16" s="61"/>
       <c r="AY16" s="61"/>
       <c r="AZ16" s="61"/>
@@ -5068,7 +5362,9 @@
       <c r="AV17" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW17" s="61"/>
+      <c r="AW17" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX17" s="61"/>
       <c r="AY17" s="61"/>
       <c r="AZ17" s="61"/>
@@ -5228,7 +5524,9 @@
       <c r="AV18" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW18" s="61"/>
+      <c r="AW18" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AX18" s="61"/>
       <c r="AY18" s="61"/>
       <c r="AZ18" s="61"/>
@@ -5388,7 +5686,9 @@
       <c r="AV19" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW19" s="61"/>
+      <c r="AW19" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX19" s="61"/>
       <c r="AY19" s="61"/>
       <c r="AZ19" s="61"/>
@@ -5548,7 +5848,9 @@
       <c r="AV20" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW20" s="61"/>
+      <c r="AW20" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AX20" s="61"/>
       <c r="AY20" s="61"/>
       <c r="AZ20" s="61"/>
@@ -5708,7 +6010,9 @@
       <c r="AV21" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW21" s="61"/>
+      <c r="AW21" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX21" s="61"/>
       <c r="AY21" s="61"/>
       <c r="AZ21" s="61"/>
@@ -5868,7 +6172,9 @@
       <c r="AV22" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW22" s="61"/>
+      <c r="AW22" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AX22" s="61"/>
       <c r="AY22" s="61"/>
       <c r="AZ22" s="61"/>
@@ -6028,7 +6334,9 @@
       <c r="AV23" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW23" s="61"/>
+      <c r="AW23" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX23" s="61"/>
       <c r="AY23" s="61"/>
       <c r="AZ23" s="61"/>
@@ -6188,7 +6496,9 @@
       <c r="AV24" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW24" s="61"/>
+      <c r="AW24" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX24" s="61"/>
       <c r="AY24" s="61"/>
       <c r="AZ24" s="61"/>
@@ -6348,7 +6658,9 @@
       <c r="AV25" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW25" s="61"/>
+      <c r="AW25" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX25" s="61"/>
       <c r="AY25" s="61"/>
       <c r="AZ25" s="61"/>
@@ -6508,7 +6820,9 @@
       <c r="AV26" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW26" s="61"/>
+      <c r="AW26" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AX26" s="61"/>
       <c r="AY26" s="61"/>
       <c r="AZ26" s="61"/>
@@ -6668,7 +6982,9 @@
       <c r="AV27" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW27" s="61"/>
+      <c r="AW27" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX27" s="61"/>
       <c r="AY27" s="61"/>
       <c r="AZ27" s="61"/>
@@ -6828,7 +7144,9 @@
       <c r="AV28" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW28" s="61"/>
+      <c r="AW28" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX28" s="61"/>
       <c r="AY28" s="61"/>
       <c r="AZ28" s="61"/>
@@ -6988,7 +7306,9 @@
       <c r="AV29" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW29" s="61"/>
+      <c r="AW29" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX29" s="61"/>
       <c r="AY29" s="61"/>
       <c r="AZ29" s="61"/>
@@ -7148,7 +7468,9 @@
       <c r="AV30" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW30" s="61"/>
+      <c r="AW30" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX30" s="61"/>
       <c r="AY30" s="61"/>
       <c r="AZ30" s="61"/>
@@ -7308,7 +7630,9 @@
       <c r="AV31" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW31" s="61"/>
+      <c r="AW31" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX31" s="61"/>
       <c r="AY31" s="61"/>
       <c r="AZ31" s="61"/>
@@ -7468,7 +7792,9 @@
       <c r="AV32" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW32" s="61"/>
+      <c r="AW32" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AX32" s="61"/>
       <c r="AY32" s="61"/>
       <c r="AZ32" s="61"/>
@@ -7628,7 +7954,9 @@
       <c r="AV33" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW33" s="61"/>
+      <c r="AW33" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX33" s="61"/>
       <c r="AY33" s="61"/>
       <c r="AZ33" s="61"/>
@@ -7788,7 +8116,9 @@
       <c r="AV34" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW34" s="61"/>
+      <c r="AW34" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AX34" s="61"/>
       <c r="AY34" s="61"/>
       <c r="AZ34" s="61"/>
@@ -7948,7 +8278,9 @@
       <c r="AV35" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW35" s="61"/>
+      <c r="AW35" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX35" s="61"/>
       <c r="AY35" s="61"/>
       <c r="AZ35" s="61"/>
@@ -8108,7 +8440,9 @@
       <c r="AV36" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW36" s="61"/>
+      <c r="AW36" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX36" s="61"/>
       <c r="AY36" s="61"/>
       <c r="AZ36" s="61"/>
@@ -8268,7 +8602,9 @@
       <c r="AV37" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW37" s="61"/>
+      <c r="AW37" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX37" s="61"/>
       <c r="AY37" s="61"/>
       <c r="AZ37" s="61"/>
@@ -8428,7 +8764,9 @@
       <c r="AV38" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW38" s="61"/>
+      <c r="AW38" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX38" s="61"/>
       <c r="AY38" s="61"/>
       <c r="AZ38" s="61"/>
@@ -8588,7 +8926,9 @@
       <c r="AV39" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW39" s="61"/>
+      <c r="AW39" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX39" s="61"/>
       <c r="AY39" s="61"/>
       <c r="AZ39" s="61"/>
@@ -8748,7 +9088,9 @@
       <c r="AV40" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW40" s="61"/>
+      <c r="AW40" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX40" s="61"/>
       <c r="AY40" s="61"/>
       <c r="AZ40" s="61"/>
@@ -8908,7 +9250,9 @@
       <c r="AV41" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW41" s="61"/>
+      <c r="AW41" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX41" s="61"/>
       <c r="AY41" s="61"/>
       <c r="AZ41" s="61"/>
@@ -9068,7 +9412,9 @@
       <c r="AV42" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW42" s="61"/>
+      <c r="AW42" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX42" s="61"/>
       <c r="AY42" s="61"/>
       <c r="AZ42" s="61"/>
@@ -9228,7 +9574,9 @@
       <c r="AV43" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW43" s="61"/>
+      <c r="AW43" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX43" s="61"/>
       <c r="AY43" s="61"/>
       <c r="AZ43" s="61"/>
@@ -9388,7 +9736,9 @@
       <c r="AV44" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW44" s="61"/>
+      <c r="AW44" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX44" s="61"/>
       <c r="AY44" s="61"/>
       <c r="AZ44" s="61"/>
@@ -9548,7 +9898,9 @@
       <c r="AV45" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW45" s="61"/>
+      <c r="AW45" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX45" s="61"/>
       <c r="AY45" s="61"/>
       <c r="AZ45" s="61"/>
@@ -9708,7 +10060,9 @@
       <c r="AV46" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW46" s="61"/>
+      <c r="AW46" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX46" s="61"/>
       <c r="AY46" s="61"/>
       <c r="AZ46" s="61"/>
@@ -9868,7 +10222,9 @@
       <c r="AV47" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW47" s="61"/>
+      <c r="AW47" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX47" s="61"/>
       <c r="AY47" s="61"/>
       <c r="AZ47" s="61"/>
@@ -10028,7 +10384,9 @@
       <c r="AV48" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW48" s="61"/>
+      <c r="AW48" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AX48" s="61"/>
       <c r="AY48" s="61"/>
       <c r="AZ48" s="61"/>
@@ -10188,7 +10546,9 @@
       <c r="AV49" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW49" s="61"/>
+      <c r="AW49" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX49" s="61"/>
       <c r="AY49" s="61"/>
       <c r="AZ49" s="61"/>
@@ -10348,7 +10708,9 @@
       <c r="AV50" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW50" s="61"/>
+      <c r="AW50" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX50" s="61"/>
       <c r="AY50" s="61"/>
       <c r="AZ50" s="61"/>
@@ -10508,7 +10870,9 @@
       <c r="AV51" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW51" s="61"/>
+      <c r="AW51" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX51" s="61"/>
       <c r="AY51" s="61"/>
       <c r="AZ51" s="61"/>
@@ -10668,7 +11032,9 @@
       <c r="AV52" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW52" s="61"/>
+      <c r="AW52" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX52" s="61"/>
       <c r="AY52" s="61"/>
       <c r="AZ52" s="61"/>
@@ -10828,7 +11194,9 @@
       <c r="AV53" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW53" s="61"/>
+      <c r="AW53" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX53" s="61"/>
       <c r="AY53" s="61"/>
       <c r="AZ53" s="61"/>
@@ -10988,7 +11356,9 @@
       <c r="AV54" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW54" s="61"/>
+      <c r="AW54" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX54" s="61"/>
       <c r="AY54" s="61"/>
       <c r="AZ54" s="61"/>
@@ -11148,7 +11518,9 @@
       <c r="AV55" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="AW55" s="61"/>
+      <c r="AW55" s="98" t="s">
+        <v>54</v>
+      </c>
       <c r="AX55" s="61"/>
       <c r="AY55" s="61"/>
       <c r="AZ55" s="61"/>
@@ -11166,10 +11538,10 @@
       <c r="BL55" s="61"/>
     </row>
     <row r="56" spans="1:64">
-      <c r="A56" s="104" t="s">
+      <c r="A56" s="117" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="105"/>
+      <c r="B56" s="118"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -11349,11 +11721,11 @@
       </c>
       <c r="AV56" s="93">
         <f>COUNTIF(AW8:AW55,"A")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AW56" s="61">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AX56" s="61">
         <f t="shared" si="22"/>
@@ -11417,10 +11789,10 @@
       </c>
     </row>
     <row r="57" spans="1:64">
-      <c r="A57" s="101" t="s">
+      <c r="A57" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="102"/>
+      <c r="B57" s="116"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -11600,11 +11972,11 @@
       </c>
       <c r="AV57" s="61">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AW57" s="61">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AX57" s="61">
         <f t="shared" si="23"/>
@@ -11669,6 +12041,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="X4:AR4"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F3:I3"/>
@@ -11679,14 +12059,6 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="X4:AR4"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -11698,8 +12070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F55"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -11714,72 +12086,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="124" t="s">
+      <c r="B1" s="126"/>
+      <c r="C1" s="133" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="124"/>
-      <c r="E1" s="120" t="s">
+      <c r="D1" s="133"/>
+      <c r="E1" s="114" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="131" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="124" t="s">
+      <c r="B2" s="131"/>
+      <c r="C2" s="133" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="124"/>
-      <c r="E2" s="120" t="s">
+      <c r="D2" s="133"/>
+      <c r="E2" s="114" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="132" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="124" t="s">
+      <c r="B3" s="132"/>
+      <c r="C3" s="133" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="124"/>
-      <c r="E3" s="120" t="s">
+      <c r="D3" s="133"/>
+      <c r="E3" s="114" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="126" t="s">
+      <c r="A4" s="127" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="119" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="121" t="s">
+      <c r="C4" s="130" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="121"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="130"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="127"/>
-      <c r="B5" s="107"/>
+      <c r="A5" s="128"/>
+      <c r="B5" s="120"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -11800,8 +12172,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="128"/>
-      <c r="B6" s="108"/>
+      <c r="A6" s="129"/>
+      <c r="B6" s="121"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -12820,10 +13192,10 @@
       <c r="H54" s="42"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="104" t="s">
+      <c r="A55" s="117" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="105"/>
+      <c r="B55" s="118"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -12839,10 +13211,10 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="101" t="s">
+      <c r="A56" s="115" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="102"/>
+      <c r="B56" s="116"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -12858,10 +13230,10 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="101" t="s">
+      <c r="A57" s="115" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="102"/>
+      <c r="B57" s="116"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -12877,10 +13249,10 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="101" t="s">
+      <c r="A58" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="102"/>
+      <c r="B58" s="116"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -12897,13 +13269,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -12913,9 +13278,16 @@
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:H54">
-    <cfRule type="cellIs" dxfId="5" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="17" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12929,7 +13301,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -12946,72 +13318,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="124" t="s">
+      <c r="B1" s="126"/>
+      <c r="C1" s="133" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="124"/>
-      <c r="E1" s="132" t="s">
+      <c r="D1" s="133"/>
+      <c r="E1" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="133"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="135"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="131" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="124" t="s">
+      <c r="B2" s="131"/>
+      <c r="C2" s="133" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="124"/>
-      <c r="E2" s="120" t="s">
+      <c r="D2" s="133"/>
+      <c r="E2" s="114" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="132" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="124" t="s">
+      <c r="B3" s="132"/>
+      <c r="C3" s="133" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="124"/>
-      <c r="E3" s="120" t="s">
+      <c r="D3" s="133"/>
+      <c r="E3" s="114" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="126" t="s">
+      <c r="A4" s="127" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="119" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="129" t="s">
+      <c r="C4" s="136" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="130"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="131"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="137"/>
+      <c r="G4" s="137"/>
+      <c r="H4" s="138"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="127"/>
-      <c r="B5" s="107"/>
+      <c r="A5" s="128"/>
+      <c r="B5" s="120"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -13032,8 +13404,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="128"/>
-      <c r="B6" s="108"/>
+      <c r="A6" s="129"/>
+      <c r="B6" s="121"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -14158,10 +14530,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="104" t="s">
+      <c r="A55" s="117" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="105"/>
+      <c r="B55" s="118"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -14176,10 +14548,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="101" t="s">
+      <c r="A56" s="115" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="102"/>
+      <c r="B56" s="116"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -14194,10 +14566,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="101" t="s">
+      <c r="A57" s="115" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="102"/>
+      <c r="B57" s="116"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -14212,10 +14584,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="101" t="s">
+      <c r="A58" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="102"/>
+      <c r="B58" s="116"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -14231,35 +14603,35 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14272,8 +14644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -14287,147 +14659,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="F1" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="119" t="s">
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="134" t="s">
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="145" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="135"/>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="135"/>
-      <c r="R1" s="135"/>
-      <c r="S1" s="135"/>
-      <c r="T1" s="135"/>
-      <c r="U1" s="135"/>
-      <c r="V1" s="135"/>
-      <c r="W1" s="135"/>
-      <c r="X1" s="135"/>
-      <c r="Y1" s="135"/>
-      <c r="Z1" s="135"/>
-      <c r="AA1" s="135"/>
-      <c r="AB1" s="135"/>
+      <c r="O1" s="146"/>
+      <c r="P1" s="146"/>
+      <c r="Q1" s="146"/>
+      <c r="R1" s="146"/>
+      <c r="S1" s="146"/>
+      <c r="T1" s="146"/>
+      <c r="U1" s="146"/>
+      <c r="V1" s="146"/>
+      <c r="W1" s="146"/>
+      <c r="X1" s="146"/>
+      <c r="Y1" s="146"/>
+      <c r="Z1" s="146"/>
+      <c r="AA1" s="146"/>
+      <c r="AB1" s="146"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="111"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="124"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="103" t="s">
+      <c r="F2" s="108" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="119" t="s">
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="134" t="s">
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="145" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="135"/>
-      <c r="P2" s="135"/>
-      <c r="Q2" s="135"/>
-      <c r="R2" s="135"/>
-      <c r="S2" s="135"/>
-      <c r="T2" s="135"/>
-      <c r="U2" s="135"/>
-      <c r="V2" s="135"/>
-      <c r="W2" s="135"/>
-      <c r="X2" s="135"/>
-      <c r="Y2" s="135"/>
-      <c r="Z2" s="135"/>
-      <c r="AA2" s="135"/>
-      <c r="AB2" s="135"/>
+      <c r="O2" s="146"/>
+      <c r="P2" s="146"/>
+      <c r="Q2" s="146"/>
+      <c r="R2" s="146"/>
+      <c r="S2" s="146"/>
+      <c r="T2" s="146"/>
+      <c r="U2" s="146"/>
+      <c r="V2" s="146"/>
+      <c r="W2" s="146"/>
+      <c r="X2" s="146"/>
+      <c r="Y2" s="146"/>
+      <c r="Z2" s="146"/>
+      <c r="AA2" s="146"/>
+      <c r="AB2" s="146"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="148" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="138"/>
-      <c r="C3" s="139"/>
+      <c r="B3" s="149"/>
+      <c r="C3" s="150"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="136" t="s">
+      <c r="F3" s="147" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="145" t="s">
+      <c r="G3" s="147"/>
+      <c r="H3" s="147"/>
+      <c r="I3" s="147"/>
+      <c r="J3" s="156" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="145"/>
-      <c r="L3" s="145"/>
-      <c r="M3" s="145"/>
-      <c r="N3" s="134" t="s">
+      <c r="K3" s="156"/>
+      <c r="L3" s="156"/>
+      <c r="M3" s="156"/>
+      <c r="N3" s="145" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="135"/>
-      <c r="S3" s="135"/>
-      <c r="T3" s="135"/>
-      <c r="U3" s="135"/>
-      <c r="V3" s="135"/>
-      <c r="W3" s="135"/>
-      <c r="X3" s="135"/>
-      <c r="Y3" s="135"/>
-      <c r="Z3" s="135"/>
-      <c r="AA3" s="135"/>
-      <c r="AB3" s="135"/>
+      <c r="O3" s="146"/>
+      <c r="P3" s="146"/>
+      <c r="Q3" s="146"/>
+      <c r="R3" s="146"/>
+      <c r="S3" s="146"/>
+      <c r="T3" s="146"/>
+      <c r="U3" s="146"/>
+      <c r="V3" s="146"/>
+      <c r="W3" s="146"/>
+      <c r="X3" s="146"/>
+      <c r="Y3" s="146"/>
+      <c r="Z3" s="146"/>
+      <c r="AA3" s="146"/>
+      <c r="AB3" s="146"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="140"/>
-      <c r="B4" s="141"/>
-      <c r="C4" s="142"/>
-      <c r="D4" s="143">
+      <c r="A4" s="151"/>
+      <c r="B4" s="152"/>
+      <c r="C4" s="153"/>
+      <c r="D4" s="154">
         <v>43344</v>
       </c>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="144"/>
-      <c r="I4" s="144"/>
-      <c r="J4" s="144"/>
-      <c r="K4" s="144"/>
-      <c r="L4" s="144"/>
-      <c r="M4" s="144"/>
+      <c r="E4" s="155"/>
+      <c r="F4" s="155"/>
+      <c r="G4" s="155"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
+      <c r="K4" s="155"/>
+      <c r="L4" s="155"/>
+      <c r="M4" s="155"/>
       <c r="N4" s="59"/>
       <c r="O4" s="59"/>
       <c r="P4" s="59"/>
@@ -14440,61 +14812,61 @@
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="119" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="147" t="s">
+      <c r="D5" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="148"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="149"/>
-      <c r="H5" s="150" t="s">
+      <c r="E5" s="141"/>
+      <c r="F5" s="141"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="143" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="151"/>
-      <c r="J5" s="151"/>
-      <c r="K5" s="151"/>
-      <c r="L5" s="146" t="s">
+      <c r="I5" s="144"/>
+      <c r="J5" s="144"/>
+      <c r="K5" s="144"/>
+      <c r="L5" s="139" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="146"/>
-      <c r="N5" s="150" t="s">
+      <c r="M5" s="139"/>
+      <c r="N5" s="143" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="151"/>
-      <c r="P5" s="151"/>
-      <c r="Q5" s="151"/>
-      <c r="R5" s="146" t="s">
+      <c r="O5" s="144"/>
+      <c r="P5" s="144"/>
+      <c r="Q5" s="144"/>
+      <c r="R5" s="139" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="146"/>
-      <c r="T5" s="115" t="s">
+      <c r="S5" s="139"/>
+      <c r="T5" s="125" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="115"/>
-      <c r="V5" s="115" t="s">
+      <c r="U5" s="125"/>
+      <c r="V5" s="125" t="s">
         <v>117</v>
       </c>
-      <c r="W5" s="115"/>
-      <c r="X5" s="115"/>
-      <c r="Y5" s="115"/>
-      <c r="Z5" s="115" t="s">
+      <c r="W5" s="125"/>
+      <c r="X5" s="125"/>
+      <c r="Y5" s="125"/>
+      <c r="Z5" s="125" t="s">
         <v>118</v>
       </c>
-      <c r="AA5" s="115"/>
-      <c r="AB5" s="115"/>
-      <c r="AC5" s="115"/>
+      <c r="AA5" s="125"/>
+      <c r="AB5" s="125"/>
+      <c r="AC5" s="125"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="127"/>
-      <c r="B6" s="107"/>
+      <c r="A6" s="128"/>
+      <c r="B6" s="120"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -14581,8 +14953,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="127"/>
-      <c r="B7" s="107"/>
+      <c r="A7" s="128"/>
+      <c r="B7" s="120"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -14669,8 +15041,8 @@
       <c r="AF7" s="19"/>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="128"/>
-      <c r="B8" s="108"/>
+      <c r="A8" s="129"/>
+      <c r="B8" s="121"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -19077,10 +19449,10 @@
       <c r="AF56" s="19"/>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="104" t="s">
+      <c r="A57" s="117" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="105"/>
+      <c r="B57" s="118"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -19200,10 +19572,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="101" t="s">
+      <c r="A58" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="102"/>
+      <c r="B58" s="116"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -19324,18 +19696,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="N5:Q5"/>
     <mergeCell ref="N1:AB1"/>
     <mergeCell ref="N2:AB2"/>
     <mergeCell ref="N3:AB3"/>
@@ -19349,6 +19709,18 @@
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="N5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -19360,8 +19732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19374,28 +19746,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="158" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="154" t="s">
+      <c r="A2" s="159" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="154"/>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
+      <c r="B2" s="159"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="159" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="154"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
     </row>
     <row r="4" spans="1:4" s="84" customFormat="1" ht="28.5">
       <c r="A4" s="82" t="s">
@@ -20126,41 +20498,41 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="152" t="s">
+      <c r="A56" s="157" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="152"/>
-      <c r="C56" s="152"/>
+      <c r="B56" s="157"/>
+      <c r="C56" s="157"/>
       <c r="D56" s="76">
         <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="152" t="s">
+      <c r="A57" s="157" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="152"/>
-      <c r="C57" s="152"/>
+      <c r="B57" s="157"/>
+      <c r="C57" s="157"/>
       <c r="D57" s="77">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="152" t="s">
+      <c r="A58" s="157" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="152"/>
-      <c r="C58" s="152"/>
+      <c r="B58" s="157"/>
+      <c r="C58" s="157"/>
       <c r="D58" s="77">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="152" t="s">
+      <c r="A59" s="157" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="152"/>
-      <c r="C59" s="152"/>
+      <c r="B59" s="157"/>
+      <c r="C59" s="157"/>
       <c r="D59" s="77">
         <v>92</v>
       </c>
@@ -20213,4 +20585,863 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D63"/>
+  <sheetViews>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="70" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="70" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="70" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="80" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="70"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75">
+      <c r="A1" s="160" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75">
+      <c r="A2" s="161" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="161"/>
+      <c r="C2" s="161"/>
+      <c r="D2" s="161"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="161" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+    </row>
+    <row r="4" spans="1:4" s="84" customFormat="1" ht="31.5">
+      <c r="A4" s="162" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="163" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="164" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="163" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="84" customFormat="1" ht="31.5">
+      <c r="A5" s="162" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="163" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="164" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="163" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="84" customFormat="1" ht="31.5">
+      <c r="A6" s="162" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="163" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="164" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="165">
+        <v>43385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1">
+      <c r="A7" s="99" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="166" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="166" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="167" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A8" s="99">
+        <v>1</v>
+      </c>
+      <c r="B8" s="168" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="98">
+        <v>31</v>
+      </c>
+      <c r="D8" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A9" s="99">
+        <v>2</v>
+      </c>
+      <c r="B9" s="168" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="102">
+        <v>41</v>
+      </c>
+      <c r="D9" s="98" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A10" s="99">
+        <v>3</v>
+      </c>
+      <c r="B10" s="168" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="98">
+        <v>30</v>
+      </c>
+      <c r="D10" s="98" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A11" s="99">
+        <v>4</v>
+      </c>
+      <c r="B11" s="169" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="98">
+        <v>28</v>
+      </c>
+      <c r="D11" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A12" s="99">
+        <v>5</v>
+      </c>
+      <c r="B12" s="168" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="98">
+        <v>35</v>
+      </c>
+      <c r="D12" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A13" s="99">
+        <v>6</v>
+      </c>
+      <c r="B13" s="168" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="98" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A14" s="99">
+        <v>7</v>
+      </c>
+      <c r="B14" s="168" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="98">
+        <v>41</v>
+      </c>
+      <c r="D14" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A15" s="99">
+        <v>8</v>
+      </c>
+      <c r="B15" s="168" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="98">
+        <v>35</v>
+      </c>
+      <c r="D15" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A16" s="99">
+        <v>9</v>
+      </c>
+      <c r="B16" s="168" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="98">
+        <v>22</v>
+      </c>
+      <c r="D16" s="98" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A17" s="99">
+        <v>10</v>
+      </c>
+      <c r="B17" s="168" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="98">
+        <v>27</v>
+      </c>
+      <c r="D17" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A18" s="99">
+        <v>11</v>
+      </c>
+      <c r="B18" s="168" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="98">
+        <v>39</v>
+      </c>
+      <c r="D18" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A19" s="99">
+        <v>12</v>
+      </c>
+      <c r="B19" s="168" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="98">
+        <v>25</v>
+      </c>
+      <c r="D19" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A20" s="99">
+        <v>13</v>
+      </c>
+      <c r="B20" s="168" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="98">
+        <v>29</v>
+      </c>
+      <c r="D20" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A21" s="99">
+        <v>14</v>
+      </c>
+      <c r="B21" s="170" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="98">
+        <v>30</v>
+      </c>
+      <c r="D21" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A22" s="99">
+        <v>15</v>
+      </c>
+      <c r="B22" s="170" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="98">
+        <v>21</v>
+      </c>
+      <c r="D22" s="98" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A23" s="99">
+        <v>16</v>
+      </c>
+      <c r="B23" s="168" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="98">
+        <v>39</v>
+      </c>
+      <c r="D23" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A24" s="99">
+        <v>17</v>
+      </c>
+      <c r="B24" s="168" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="102">
+        <v>26</v>
+      </c>
+      <c r="D24" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A25" s="99">
+        <v>18</v>
+      </c>
+      <c r="B25" s="168" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="98">
+        <v>32</v>
+      </c>
+      <c r="D25" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A26" s="99">
+        <v>19</v>
+      </c>
+      <c r="B26" s="168" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="98">
+        <v>45</v>
+      </c>
+      <c r="D26" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A27" s="99">
+        <v>20</v>
+      </c>
+      <c r="B27" s="168" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="98">
+        <v>45</v>
+      </c>
+      <c r="D27" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A28" s="99">
+        <v>21</v>
+      </c>
+      <c r="B28" s="168" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="98">
+        <v>12</v>
+      </c>
+      <c r="D28" s="98" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A29" s="99">
+        <v>22</v>
+      </c>
+      <c r="B29" s="168" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="98">
+        <v>32</v>
+      </c>
+      <c r="D29" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A30" s="99">
+        <v>23</v>
+      </c>
+      <c r="B30" s="171" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="98">
+        <v>30</v>
+      </c>
+      <c r="D30" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A31" s="99">
+        <v>24</v>
+      </c>
+      <c r="B31" s="172" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="98">
+        <v>25</v>
+      </c>
+      <c r="D31" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A32" s="99">
+        <v>25</v>
+      </c>
+      <c r="B32" s="170" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="98">
+        <v>31</v>
+      </c>
+      <c r="D32" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A33" s="99">
+        <v>26</v>
+      </c>
+      <c r="B33" s="168" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="98">
+        <v>46</v>
+      </c>
+      <c r="D33" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A34" s="99">
+        <v>27</v>
+      </c>
+      <c r="B34" s="172" t="s">
+        <v>166</v>
+      </c>
+      <c r="C34" s="98">
+        <v>22</v>
+      </c>
+      <c r="D34" s="98" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A35" s="99">
+        <v>28</v>
+      </c>
+      <c r="B35" s="168" t="s">
+        <v>144</v>
+      </c>
+      <c r="C35" s="98">
+        <v>44</v>
+      </c>
+      <c r="D35" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A36" s="99">
+        <v>29</v>
+      </c>
+      <c r="B36" s="170" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="98">
+        <v>37</v>
+      </c>
+      <c r="D36" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A37" s="99">
+        <v>30</v>
+      </c>
+      <c r="B37" s="168" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" s="98">
+        <v>17</v>
+      </c>
+      <c r="D37" s="98" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A38" s="99">
+        <v>31</v>
+      </c>
+      <c r="B38" s="170" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="98">
+        <v>43</v>
+      </c>
+      <c r="D38" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A39" s="99">
+        <v>32</v>
+      </c>
+      <c r="B39" s="168" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="98">
+        <v>42</v>
+      </c>
+      <c r="D39" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A40" s="99">
+        <v>33</v>
+      </c>
+      <c r="B40" s="168" t="s">
+        <v>149</v>
+      </c>
+      <c r="C40" s="98">
+        <v>31</v>
+      </c>
+      <c r="D40" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A41" s="99">
+        <v>34</v>
+      </c>
+      <c r="B41" s="168" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="98">
+        <v>38</v>
+      </c>
+      <c r="D41" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A42" s="99">
+        <v>35</v>
+      </c>
+      <c r="B42" s="168" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" s="98">
+        <v>29</v>
+      </c>
+      <c r="D42" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A43" s="99">
+        <v>36</v>
+      </c>
+      <c r="B43" s="168" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" s="98">
+        <v>15</v>
+      </c>
+      <c r="D43" s="98" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A44" s="99">
+        <v>37</v>
+      </c>
+      <c r="B44" s="170" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="98">
+        <v>27</v>
+      </c>
+      <c r="D44" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A45" s="99">
+        <v>38</v>
+      </c>
+      <c r="B45" s="168" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" s="98">
+        <v>9</v>
+      </c>
+      <c r="D45" s="98" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A46" s="99">
+        <v>39</v>
+      </c>
+      <c r="B46" s="172" t="s">
+        <v>167</v>
+      </c>
+      <c r="C46" s="98">
+        <v>25</v>
+      </c>
+      <c r="D46" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A47" s="99">
+        <v>40</v>
+      </c>
+      <c r="B47" s="168" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="98">
+        <v>25</v>
+      </c>
+      <c r="D47" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A48" s="99">
+        <v>41</v>
+      </c>
+      <c r="B48" s="168" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" s="98">
+        <v>30</v>
+      </c>
+      <c r="D48" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A49" s="99">
+        <v>42</v>
+      </c>
+      <c r="B49" s="168" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="98">
+        <v>25</v>
+      </c>
+      <c r="D49" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A50" s="99">
+        <v>43</v>
+      </c>
+      <c r="B50" s="170" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" s="98">
+        <v>34</v>
+      </c>
+      <c r="D50" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A51" s="99">
+        <v>44</v>
+      </c>
+      <c r="B51" s="170" t="s">
+        <v>159</v>
+      </c>
+      <c r="C51" s="98">
+        <v>29</v>
+      </c>
+      <c r="D51" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A52" s="99">
+        <v>45</v>
+      </c>
+      <c r="B52" s="168" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="98">
+        <v>17</v>
+      </c>
+      <c r="D52" s="98" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A53" s="99">
+        <v>46</v>
+      </c>
+      <c r="B53" s="168" t="s">
+        <v>161</v>
+      </c>
+      <c r="C53" s="98">
+        <v>33</v>
+      </c>
+      <c r="D53" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A54" s="99">
+        <v>47</v>
+      </c>
+      <c r="B54" s="168" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" s="98">
+        <v>29</v>
+      </c>
+      <c r="D54" s="98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="84" customFormat="1" ht="15.75">
+      <c r="A55" s="100">
+        <v>48</v>
+      </c>
+      <c r="B55" s="173" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="98">
+        <v>45</v>
+      </c>
+      <c r="D55" s="101" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75">
+      <c r="A56" s="133" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="133"/>
+      <c r="C56" s="133"/>
+      <c r="D56" s="174">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75">
+      <c r="A57" s="133" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="133"/>
+      <c r="C57" s="133"/>
+      <c r="D57" s="175">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75">
+      <c r="A58" s="133" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="133"/>
+      <c r="C58" s="133"/>
+      <c r="D58" s="175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75">
+      <c r="A59" s="133" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" s="133"/>
+      <c r="C59" s="133"/>
+      <c r="D59" s="175">
+        <v>85.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="68"/>
+      <c r="B60" s="68"/>
+      <c r="C60" s="68"/>
+      <c r="D60" s="78"/>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="68"/>
+      <c r="B61" s="68"/>
+      <c r="C61" s="68"/>
+      <c r="D61" s="78"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="74"/>
+      <c r="B62" s="74"/>
+      <c r="C62" s="74"/>
+      <c r="D62" s="78"/>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="69"/>
+      <c r="C63" s="69" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="79" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A58:C58"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C8:C55">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="1.04" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Last Update 10-11-2018  6:02:58.15
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -945,6 +945,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="AX7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dictionaries [Creating, Accessing, Modifying]</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1228,7 +1252,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4003" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4051" uniqueCount="168">
   <si>
     <t>S.NO</t>
   </si>
@@ -2119,7 +2143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2433,6 +2457,59 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2613,74 +2690,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <condense val="0"/>
@@ -3046,10 +3061,10 @@
   <dimension ref="A1:BL57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AB41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="X43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AW59" sqref="AW59"/>
+      <selection pane="bottomRight" activeCell="AX44" sqref="AX44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -3063,29 +3078,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="18.75">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="118" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="105" t="s">
+      <c r="F1" s="120" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="113" t="s">
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="128" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -3110,41 +3125,41 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:64" ht="19.5">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="137" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="124"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="139"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="108" t="s">
+      <c r="F2" s="123" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="113" t="s">
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="128" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="114" t="s">
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="128"/>
+      <c r="N2" s="129" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="114"/>
-      <c r="P2" s="114"/>
-      <c r="Q2" s="114"/>
-      <c r="R2" s="114"/>
-      <c r="S2" s="114"/>
-      <c r="T2" s="114"/>
-      <c r="U2" s="114"/>
-      <c r="V2" s="114"/>
-      <c r="W2" s="114"/>
+      <c r="O2" s="129"/>
+      <c r="P2" s="129"/>
+      <c r="Q2" s="129"/>
+      <c r="R2" s="129"/>
+      <c r="S2" s="129"/>
+      <c r="T2" s="129"/>
+      <c r="U2" s="129"/>
+      <c r="V2" s="129"/>
+      <c r="W2" s="129"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -3157,41 +3172,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:64" ht="18.75">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="104"/>
-      <c r="C3" s="109"/>
+      <c r="B3" s="119"/>
+      <c r="C3" s="124"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="108" t="s">
+      <c r="F3" s="123" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="113" t="s">
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="128" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="113"/>
-      <c r="L3" s="113"/>
-      <c r="M3" s="113"/>
-      <c r="N3" s="114" t="s">
+      <c r="K3" s="128"/>
+      <c r="L3" s="128"/>
+      <c r="M3" s="128"/>
+      <c r="N3" s="129" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="114"/>
-      <c r="P3" s="114"/>
-      <c r="Q3" s="114"/>
-      <c r="R3" s="114"/>
-      <c r="S3" s="114"/>
-      <c r="T3" s="114"/>
-      <c r="U3" s="114"/>
-      <c r="V3" s="114"/>
-      <c r="W3" s="114"/>
+      <c r="O3" s="129"/>
+      <c r="P3" s="129"/>
+      <c r="Q3" s="129"/>
+      <c r="R3" s="129"/>
+      <c r="S3" s="129"/>
+      <c r="T3" s="129"/>
+      <c r="U3" s="129"/>
+      <c r="V3" s="129"/>
+      <c r="W3" s="129"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -3204,56 +3219,56 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:64" ht="18.75">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="110">
+      <c r="B4" s="119"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="125">
         <v>43344</v>
       </c>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="111"/>
-      <c r="M4" s="111"/>
-      <c r="N4" s="111"/>
-      <c r="O4" s="111"/>
-      <c r="P4" s="111"/>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="111"/>
-      <c r="S4" s="111"/>
-      <c r="T4" s="111"/>
-      <c r="U4" s="111"/>
-      <c r="V4" s="111"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="110">
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="126"/>
+      <c r="I4" s="126"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="126"/>
+      <c r="M4" s="126"/>
+      <c r="N4" s="126"/>
+      <c r="O4" s="126"/>
+      <c r="P4" s="126"/>
+      <c r="Q4" s="126"/>
+      <c r="R4" s="126"/>
+      <c r="S4" s="126"/>
+      <c r="T4" s="126"/>
+      <c r="U4" s="126"/>
+      <c r="V4" s="126"/>
+      <c r="W4" s="127"/>
+      <c r="X4" s="125">
         <v>43374</v>
       </c>
-      <c r="Y4" s="111"/>
-      <c r="Z4" s="111"/>
-      <c r="AA4" s="111"/>
-      <c r="AB4" s="111"/>
-      <c r="AC4" s="111"/>
-      <c r="AD4" s="111"/>
-      <c r="AE4" s="111"/>
-      <c r="AF4" s="111"/>
-      <c r="AG4" s="111"/>
-      <c r="AH4" s="111"/>
-      <c r="AI4" s="111"/>
-      <c r="AJ4" s="111"/>
-      <c r="AK4" s="111"/>
-      <c r="AL4" s="111"/>
-      <c r="AM4" s="111"/>
-      <c r="AN4" s="111"/>
-      <c r="AO4" s="111"/>
-      <c r="AP4" s="111"/>
-      <c r="AQ4" s="111"/>
-      <c r="AR4" s="112"/>
+      <c r="Y4" s="126"/>
+      <c r="Z4" s="126"/>
+      <c r="AA4" s="126"/>
+      <c r="AB4" s="126"/>
+      <c r="AC4" s="126"/>
+      <c r="AD4" s="126"/>
+      <c r="AE4" s="126"/>
+      <c r="AF4" s="126"/>
+      <c r="AG4" s="126"/>
+      <c r="AH4" s="126"/>
+      <c r="AI4" s="126"/>
+      <c r="AJ4" s="126"/>
+      <c r="AK4" s="126"/>
+      <c r="AL4" s="126"/>
+      <c r="AM4" s="126"/>
+      <c r="AN4" s="126"/>
+      <c r="AO4" s="126"/>
+      <c r="AP4" s="126"/>
+      <c r="AQ4" s="126"/>
+      <c r="AR4" s="127"/>
       <c r="AS4" s="61"/>
       <c r="AT4" s="61"/>
       <c r="AU4" s="61"/>
@@ -3276,10 +3291,10 @@
       <c r="BL4" s="61"/>
     </row>
     <row r="5" spans="1:64">
-      <c r="A5" s="125" t="s">
+      <c r="A5" s="140" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="119" t="s">
+      <c r="B5" s="134" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -3423,7 +3438,9 @@
       <c r="AW5" s="98">
         <v>11</v>
       </c>
-      <c r="AX5" s="61"/>
+      <c r="AX5" s="61">
+        <v>11</v>
+      </c>
       <c r="AY5" s="61"/>
       <c r="AZ5" s="61"/>
       <c r="BA5" s="61"/>
@@ -3440,8 +3457,8 @@
       <c r="BL5" s="61"/>
     </row>
     <row r="6" spans="1:64">
-      <c r="A6" s="125"/>
-      <c r="B6" s="120"/>
+      <c r="A6" s="140"/>
+      <c r="B6" s="135"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -3583,7 +3600,9 @@
       <c r="AW6" s="98">
         <v>8</v>
       </c>
-      <c r="AX6" s="61"/>
+      <c r="AX6" s="61">
+        <v>9</v>
+      </c>
       <c r="AY6" s="61"/>
       <c r="AZ6" s="61"/>
       <c r="BA6" s="61"/>
@@ -3603,7 +3622,7 @@
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="121"/>
+      <c r="B7" s="136"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -3745,7 +3764,9 @@
       <c r="AW7" s="98">
         <v>7</v>
       </c>
-      <c r="AX7" s="61"/>
+      <c r="AX7" s="61">
+        <v>5</v>
+      </c>
       <c r="AY7" s="61"/>
       <c r="AZ7" s="61"/>
       <c r="BA7" s="61"/>
@@ -3907,7 +3928,9 @@
       <c r="AW8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AX8" s="61"/>
+      <c r="AX8" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AY8" s="61"/>
       <c r="AZ8" s="61"/>
       <c r="BA8" s="61"/>
@@ -4069,7 +4092,9 @@
       <c r="AW9" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX9" s="61"/>
+      <c r="AX9" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY9" s="61"/>
       <c r="AZ9" s="61"/>
       <c r="BA9" s="61"/>
@@ -4231,7 +4256,9 @@
       <c r="AW10" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX10" s="61"/>
+      <c r="AX10" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY10" s="61"/>
       <c r="AZ10" s="61"/>
       <c r="BA10" s="61"/>
@@ -4393,7 +4420,9 @@
       <c r="AW11" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX11" s="61"/>
+      <c r="AX11" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY11" s="61"/>
       <c r="AZ11" s="61"/>
       <c r="BA11" s="61"/>
@@ -4555,7 +4584,9 @@
       <c r="AW12" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX12" s="61"/>
+      <c r="AX12" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY12" s="61"/>
       <c r="AZ12" s="61"/>
       <c r="BA12" s="61"/>
@@ -4717,7 +4748,9 @@
       <c r="AW13" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX13" s="61"/>
+      <c r="AX13" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY13" s="61"/>
       <c r="AZ13" s="61"/>
       <c r="BA13" s="61"/>
@@ -4879,7 +4912,9 @@
       <c r="AW14" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX14" s="61"/>
+      <c r="AX14" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY14" s="61"/>
       <c r="AZ14" s="61"/>
       <c r="BA14" s="61"/>
@@ -5041,7 +5076,9 @@
       <c r="AW15" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AX15" s="61"/>
+      <c r="AX15" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY15" s="61"/>
       <c r="AZ15" s="61"/>
       <c r="BA15" s="61"/>
@@ -5203,7 +5240,9 @@
       <c r="AW16" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX16" s="61"/>
+      <c r="AX16" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY16" s="61"/>
       <c r="AZ16" s="61"/>
       <c r="BA16" s="61"/>
@@ -5365,7 +5404,9 @@
       <c r="AW17" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX17" s="61"/>
+      <c r="AX17" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY17" s="61"/>
       <c r="AZ17" s="61"/>
       <c r="BA17" s="61"/>
@@ -5527,7 +5568,9 @@
       <c r="AW18" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AX18" s="61"/>
+      <c r="AX18" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AY18" s="61"/>
       <c r="AZ18" s="61"/>
       <c r="BA18" s="61"/>
@@ -5689,7 +5732,9 @@
       <c r="AW19" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX19" s="61"/>
+      <c r="AX19" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY19" s="61"/>
       <c r="AZ19" s="61"/>
       <c r="BA19" s="61"/>
@@ -5851,7 +5896,9 @@
       <c r="AW20" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AX20" s="61"/>
+      <c r="AX20" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY20" s="61"/>
       <c r="AZ20" s="61"/>
       <c r="BA20" s="61"/>
@@ -6013,7 +6060,9 @@
       <c r="AW21" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX21" s="61"/>
+      <c r="AX21" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY21" s="61"/>
       <c r="AZ21" s="61"/>
       <c r="BA21" s="61"/>
@@ -6175,7 +6224,9 @@
       <c r="AW22" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AX22" s="61"/>
+      <c r="AX22" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY22" s="61"/>
       <c r="AZ22" s="61"/>
       <c r="BA22" s="61"/>
@@ -6337,7 +6388,9 @@
       <c r="AW23" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX23" s="61"/>
+      <c r="AX23" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY23" s="61"/>
       <c r="AZ23" s="61"/>
       <c r="BA23" s="61"/>
@@ -6499,7 +6552,9 @@
       <c r="AW24" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX24" s="61"/>
+      <c r="AX24" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AY24" s="61"/>
       <c r="AZ24" s="61"/>
       <c r="BA24" s="61"/>
@@ -6661,7 +6716,9 @@
       <c r="AW25" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX25" s="61"/>
+      <c r="AX25" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY25" s="61"/>
       <c r="AZ25" s="61"/>
       <c r="BA25" s="61"/>
@@ -6823,7 +6880,9 @@
       <c r="AW26" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AX26" s="61"/>
+      <c r="AX26" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY26" s="61"/>
       <c r="AZ26" s="61"/>
       <c r="BA26" s="61"/>
@@ -6985,7 +7044,9 @@
       <c r="AW27" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX27" s="61"/>
+      <c r="AX27" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY27" s="61"/>
       <c r="AZ27" s="61"/>
       <c r="BA27" s="61"/>
@@ -7147,7 +7208,9 @@
       <c r="AW28" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX28" s="61"/>
+      <c r="AX28" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY28" s="61"/>
       <c r="AZ28" s="61"/>
       <c r="BA28" s="61"/>
@@ -7309,7 +7372,9 @@
       <c r="AW29" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX29" s="61"/>
+      <c r="AX29" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY29" s="61"/>
       <c r="AZ29" s="61"/>
       <c r="BA29" s="61"/>
@@ -7471,7 +7536,9 @@
       <c r="AW30" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX30" s="61"/>
+      <c r="AX30" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY30" s="61"/>
       <c r="AZ30" s="61"/>
       <c r="BA30" s="61"/>
@@ -7633,7 +7700,9 @@
       <c r="AW31" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX31" s="61"/>
+      <c r="AX31" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY31" s="61"/>
       <c r="AZ31" s="61"/>
       <c r="BA31" s="61"/>
@@ -7795,7 +7864,9 @@
       <c r="AW32" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AX32" s="61"/>
+      <c r="AX32" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY32" s="61"/>
       <c r="AZ32" s="61"/>
       <c r="BA32" s="61"/>
@@ -7957,7 +8028,9 @@
       <c r="AW33" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX33" s="61"/>
+      <c r="AX33" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY33" s="61"/>
       <c r="AZ33" s="61"/>
       <c r="BA33" s="61"/>
@@ -8119,7 +8192,9 @@
       <c r="AW34" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AX34" s="61"/>
+      <c r="AX34" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AY34" s="61"/>
       <c r="AZ34" s="61"/>
       <c r="BA34" s="61"/>
@@ -8281,7 +8356,9 @@
       <c r="AW35" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX35" s="61"/>
+      <c r="AX35" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AY35" s="61"/>
       <c r="AZ35" s="61"/>
       <c r="BA35" s="61"/>
@@ -8443,7 +8520,9 @@
       <c r="AW36" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX36" s="61"/>
+      <c r="AX36" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY36" s="61"/>
       <c r="AZ36" s="61"/>
       <c r="BA36" s="61"/>
@@ -8605,7 +8684,9 @@
       <c r="AW37" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX37" s="61"/>
+      <c r="AX37" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY37" s="61"/>
       <c r="AZ37" s="61"/>
       <c r="BA37" s="61"/>
@@ -8767,7 +8848,9 @@
       <c r="AW38" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX38" s="61"/>
+      <c r="AX38" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY38" s="61"/>
       <c r="AZ38" s="61"/>
       <c r="BA38" s="61"/>
@@ -8929,7 +9012,9 @@
       <c r="AW39" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX39" s="61"/>
+      <c r="AX39" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY39" s="61"/>
       <c r="AZ39" s="61"/>
       <c r="BA39" s="61"/>
@@ -9091,7 +9176,9 @@
       <c r="AW40" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX40" s="61"/>
+      <c r="AX40" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY40" s="61"/>
       <c r="AZ40" s="61"/>
       <c r="BA40" s="61"/>
@@ -9253,7 +9340,9 @@
       <c r="AW41" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX41" s="61"/>
+      <c r="AX41" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY41" s="61"/>
       <c r="AZ41" s="61"/>
       <c r="BA41" s="61"/>
@@ -9415,7 +9504,9 @@
       <c r="AW42" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX42" s="61"/>
+      <c r="AX42" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY42" s="61"/>
       <c r="AZ42" s="61"/>
       <c r="BA42" s="61"/>
@@ -9577,7 +9668,9 @@
       <c r="AW43" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX43" s="61"/>
+      <c r="AX43" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY43" s="61"/>
       <c r="AZ43" s="61"/>
       <c r="BA43" s="61"/>
@@ -9739,7 +9832,9 @@
       <c r="AW44" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX44" s="61"/>
+      <c r="AX44" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY44" s="61"/>
       <c r="AZ44" s="61"/>
       <c r="BA44" s="61"/>
@@ -9901,7 +9996,9 @@
       <c r="AW45" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX45" s="61"/>
+      <c r="AX45" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY45" s="61"/>
       <c r="AZ45" s="61"/>
       <c r="BA45" s="61"/>
@@ -10063,7 +10160,9 @@
       <c r="AW46" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX46" s="61"/>
+      <c r="AX46" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY46" s="61"/>
       <c r="AZ46" s="61"/>
       <c r="BA46" s="61"/>
@@ -10225,7 +10324,9 @@
       <c r="AW47" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX47" s="61"/>
+      <c r="AX47" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY47" s="61"/>
       <c r="AZ47" s="61"/>
       <c r="BA47" s="61"/>
@@ -10387,7 +10488,9 @@
       <c r="AW48" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AX48" s="61"/>
+      <c r="AX48" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY48" s="61"/>
       <c r="AZ48" s="61"/>
       <c r="BA48" s="61"/>
@@ -10549,7 +10652,9 @@
       <c r="AW49" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX49" s="61"/>
+      <c r="AX49" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY49" s="61"/>
       <c r="AZ49" s="61"/>
       <c r="BA49" s="61"/>
@@ -10711,7 +10816,9 @@
       <c r="AW50" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX50" s="61"/>
+      <c r="AX50" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY50" s="61"/>
       <c r="AZ50" s="61"/>
       <c r="BA50" s="61"/>
@@ -10873,7 +10980,9 @@
       <c r="AW51" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX51" s="61"/>
+      <c r="AX51" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY51" s="61"/>
       <c r="AZ51" s="61"/>
       <c r="BA51" s="61"/>
@@ -11035,7 +11144,9 @@
       <c r="AW52" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX52" s="61"/>
+      <c r="AX52" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY52" s="61"/>
       <c r="AZ52" s="61"/>
       <c r="BA52" s="61"/>
@@ -11197,7 +11308,9 @@
       <c r="AW53" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX53" s="61"/>
+      <c r="AX53" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY53" s="61"/>
       <c r="AZ53" s="61"/>
       <c r="BA53" s="61"/>
@@ -11359,7 +11472,9 @@
       <c r="AW54" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX54" s="61"/>
+      <c r="AX54" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY54" s="61"/>
       <c r="AZ54" s="61"/>
       <c r="BA54" s="61"/>
@@ -11521,7 +11636,9 @@
       <c r="AW55" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="AX55" s="61"/>
+      <c r="AX55" s="103" t="s">
+        <v>54</v>
+      </c>
       <c r="AY55" s="61"/>
       <c r="AZ55" s="61"/>
       <c r="BA55" s="61"/>
@@ -11538,10 +11655,10 @@
       <c r="BL55" s="61"/>
     </row>
     <row r="56" spans="1:64">
-      <c r="A56" s="117" t="s">
+      <c r="A56" s="132" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="118"/>
+      <c r="B56" s="133"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -11729,7 +11846,7 @@
       </c>
       <c r="AX56" s="61">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AY56" s="61">
         <f t="shared" si="22"/>
@@ -11789,10 +11906,10 @@
       </c>
     </row>
     <row r="57" spans="1:64">
-      <c r="A57" s="115" t="s">
+      <c r="A57" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="116"/>
+      <c r="B57" s="131"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -11980,7 +12097,7 @@
       </c>
       <c r="AX57" s="61">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AY57" s="61">
         <f t="shared" si="23"/>
@@ -12086,72 +12203,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="141" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="133" t="s">
+      <c r="B1" s="141"/>
+      <c r="C1" s="148" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="133"/>
-      <c r="E1" s="114" t="s">
+      <c r="D1" s="148"/>
+      <c r="E1" s="129" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="146" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="131"/>
-      <c r="C2" s="133" t="s">
+      <c r="B2" s="146"/>
+      <c r="C2" s="148" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="133"/>
-      <c r="E2" s="114" t="s">
+      <c r="D2" s="148"/>
+      <c r="E2" s="129" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="147" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="133" t="s">
+      <c r="B3" s="147"/>
+      <c r="C3" s="148" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="133"/>
-      <c r="E3" s="114" t="s">
+      <c r="D3" s="148"/>
+      <c r="E3" s="129" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="142" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="134" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="130" t="s">
+      <c r="C4" s="145" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="130"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="130"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="145"/>
+      <c r="H4" s="145"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="128"/>
-      <c r="B5" s="120"/>
+      <c r="A5" s="143"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -12172,8 +12289,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="129"/>
-      <c r="B6" s="121"/>
+      <c r="A6" s="144"/>
+      <c r="B6" s="136"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -13192,10 +13309,10 @@
       <c r="H54" s="42"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="117" t="s">
+      <c r="A55" s="132" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="118"/>
+      <c r="B55" s="133"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -13211,10 +13328,10 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="115" t="s">
+      <c r="A56" s="130" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="116"/>
+      <c r="B56" s="131"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -13230,10 +13347,10 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="115" t="s">
+      <c r="A57" s="130" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="116"/>
+      <c r="B57" s="131"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -13249,10 +13366,10 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="115" t="s">
+      <c r="A58" s="130" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="116"/>
+      <c r="B58" s="131"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -13287,7 +13404,7 @@
     <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:H54">
-    <cfRule type="cellIs" dxfId="6" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="17" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13318,72 +13435,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="141" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="133" t="s">
+      <c r="B1" s="141"/>
+      <c r="C1" s="148" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="133"/>
-      <c r="E1" s="134" t="s">
+      <c r="D1" s="148"/>
+      <c r="E1" s="149" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="135"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="150"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="146" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="131"/>
-      <c r="C2" s="133" t="s">
+      <c r="B2" s="146"/>
+      <c r="C2" s="148" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="133"/>
-      <c r="E2" s="114" t="s">
+      <c r="D2" s="148"/>
+      <c r="E2" s="129" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="147" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="133" t="s">
+      <c r="B3" s="147"/>
+      <c r="C3" s="148" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="133"/>
-      <c r="E3" s="114" t="s">
+      <c r="D3" s="148"/>
+      <c r="E3" s="129" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="142" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="134" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="136" t="s">
+      <c r="C4" s="151" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="137"/>
-      <c r="H4" s="138"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="153"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="128"/>
-      <c r="B5" s="120"/>
+      <c r="A5" s="143"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -13404,8 +13521,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="129"/>
-      <c r="B6" s="121"/>
+      <c r="A6" s="144"/>
+      <c r="B6" s="136"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -14530,10 +14647,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="117" t="s">
+      <c r="A55" s="132" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="118"/>
+      <c r="B55" s="133"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -14548,10 +14665,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="115" t="s">
+      <c r="A56" s="130" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="116"/>
+      <c r="B56" s="131"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -14566,10 +14683,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="115" t="s">
+      <c r="A57" s="130" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="116"/>
+      <c r="B57" s="131"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -14584,10 +14701,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="115" t="s">
+      <c r="A58" s="130" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="116"/>
+      <c r="B58" s="131"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -14621,17 +14738,17 @@
     <mergeCell ref="E2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14659,147 +14776,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="118" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="105" t="s">
+      <c r="F1" s="120" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="113" t="s">
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="128" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="145" t="s">
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="160" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="146"/>
-      <c r="P1" s="146"/>
-      <c r="Q1" s="146"/>
-      <c r="R1" s="146"/>
-      <c r="S1" s="146"/>
-      <c r="T1" s="146"/>
-      <c r="U1" s="146"/>
-      <c r="V1" s="146"/>
-      <c r="W1" s="146"/>
-      <c r="X1" s="146"/>
-      <c r="Y1" s="146"/>
-      <c r="Z1" s="146"/>
-      <c r="AA1" s="146"/>
-      <c r="AB1" s="146"/>
+      <c r="O1" s="161"/>
+      <c r="P1" s="161"/>
+      <c r="Q1" s="161"/>
+      <c r="R1" s="161"/>
+      <c r="S1" s="161"/>
+      <c r="T1" s="161"/>
+      <c r="U1" s="161"/>
+      <c r="V1" s="161"/>
+      <c r="W1" s="161"/>
+      <c r="X1" s="161"/>
+      <c r="Y1" s="161"/>
+      <c r="Z1" s="161"/>
+      <c r="AA1" s="161"/>
+      <c r="AB1" s="161"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="137" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="124"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="139"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="108" t="s">
+      <c r="F2" s="123" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="113" t="s">
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="128" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="145" t="s">
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="128"/>
+      <c r="N2" s="160" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="146"/>
-      <c r="P2" s="146"/>
-      <c r="Q2" s="146"/>
-      <c r="R2" s="146"/>
-      <c r="S2" s="146"/>
-      <c r="T2" s="146"/>
-      <c r="U2" s="146"/>
-      <c r="V2" s="146"/>
-      <c r="W2" s="146"/>
-      <c r="X2" s="146"/>
-      <c r="Y2" s="146"/>
-      <c r="Z2" s="146"/>
-      <c r="AA2" s="146"/>
-      <c r="AB2" s="146"/>
+      <c r="O2" s="161"/>
+      <c r="P2" s="161"/>
+      <c r="Q2" s="161"/>
+      <c r="R2" s="161"/>
+      <c r="S2" s="161"/>
+      <c r="T2" s="161"/>
+      <c r="U2" s="161"/>
+      <c r="V2" s="161"/>
+      <c r="W2" s="161"/>
+      <c r="X2" s="161"/>
+      <c r="Y2" s="161"/>
+      <c r="Z2" s="161"/>
+      <c r="AA2" s="161"/>
+      <c r="AB2" s="161"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="163" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="149"/>
-      <c r="C3" s="150"/>
+      <c r="B3" s="164"/>
+      <c r="C3" s="165"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="147" t="s">
+      <c r="F3" s="162" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="147"/>
-      <c r="H3" s="147"/>
-      <c r="I3" s="147"/>
-      <c r="J3" s="156" t="s">
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="171" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="156"/>
-      <c r="L3" s="156"/>
-      <c r="M3" s="156"/>
-      <c r="N3" s="145" t="s">
+      <c r="K3" s="171"/>
+      <c r="L3" s="171"/>
+      <c r="M3" s="171"/>
+      <c r="N3" s="160" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="146"/>
-      <c r="P3" s="146"/>
-      <c r="Q3" s="146"/>
-      <c r="R3" s="146"/>
-      <c r="S3" s="146"/>
-      <c r="T3" s="146"/>
-      <c r="U3" s="146"/>
-      <c r="V3" s="146"/>
-      <c r="W3" s="146"/>
-      <c r="X3" s="146"/>
-      <c r="Y3" s="146"/>
-      <c r="Z3" s="146"/>
-      <c r="AA3" s="146"/>
-      <c r="AB3" s="146"/>
+      <c r="O3" s="161"/>
+      <c r="P3" s="161"/>
+      <c r="Q3" s="161"/>
+      <c r="R3" s="161"/>
+      <c r="S3" s="161"/>
+      <c r="T3" s="161"/>
+      <c r="U3" s="161"/>
+      <c r="V3" s="161"/>
+      <c r="W3" s="161"/>
+      <c r="X3" s="161"/>
+      <c r="Y3" s="161"/>
+      <c r="Z3" s="161"/>
+      <c r="AA3" s="161"/>
+      <c r="AB3" s="161"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="151"/>
-      <c r="B4" s="152"/>
-      <c r="C4" s="153"/>
-      <c r="D4" s="154">
+      <c r="A4" s="166"/>
+      <c r="B4" s="167"/>
+      <c r="C4" s="168"/>
+      <c r="D4" s="169">
         <v>43344</v>
       </c>
-      <c r="E4" s="155"/>
-      <c r="F4" s="155"/>
-      <c r="G4" s="155"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
-      <c r="K4" s="155"/>
-      <c r="L4" s="155"/>
-      <c r="M4" s="155"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
+      <c r="H4" s="170"/>
+      <c r="I4" s="170"/>
+      <c r="J4" s="170"/>
+      <c r="K4" s="170"/>
+      <c r="L4" s="170"/>
+      <c r="M4" s="170"/>
       <c r="N4" s="59"/>
       <c r="O4" s="59"/>
       <c r="P4" s="59"/>
@@ -14812,61 +14929,61 @@
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="127" t="s">
+      <c r="A5" s="142" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="119" t="s">
+      <c r="B5" s="134" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="140" t="s">
+      <c r="D5" s="155" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="141"/>
-      <c r="F5" s="141"/>
-      <c r="G5" s="142"/>
-      <c r="H5" s="143" t="s">
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="157"/>
+      <c r="H5" s="158" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="144"/>
-      <c r="J5" s="144"/>
-      <c r="K5" s="144"/>
-      <c r="L5" s="139" t="s">
+      <c r="I5" s="159"/>
+      <c r="J5" s="159"/>
+      <c r="K5" s="159"/>
+      <c r="L5" s="154" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="139"/>
-      <c r="N5" s="143" t="s">
+      <c r="M5" s="154"/>
+      <c r="N5" s="158" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="144"/>
-      <c r="P5" s="144"/>
-      <c r="Q5" s="144"/>
-      <c r="R5" s="139" t="s">
+      <c r="O5" s="159"/>
+      <c r="P5" s="159"/>
+      <c r="Q5" s="159"/>
+      <c r="R5" s="154" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="139"/>
-      <c r="T5" s="125" t="s">
+      <c r="S5" s="154"/>
+      <c r="T5" s="140" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="125"/>
-      <c r="V5" s="125" t="s">
+      <c r="U5" s="140"/>
+      <c r="V5" s="140" t="s">
         <v>117</v>
       </c>
-      <c r="W5" s="125"/>
-      <c r="X5" s="125"/>
-      <c r="Y5" s="125"/>
-      <c r="Z5" s="125" t="s">
+      <c r="W5" s="140"/>
+      <c r="X5" s="140"/>
+      <c r="Y5" s="140"/>
+      <c r="Z5" s="140" t="s">
         <v>118</v>
       </c>
-      <c r="AA5" s="125"/>
-      <c r="AB5" s="125"/>
-      <c r="AC5" s="125"/>
+      <c r="AA5" s="140"/>
+      <c r="AB5" s="140"/>
+      <c r="AC5" s="140"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="128"/>
-      <c r="B6" s="120"/>
+      <c r="A6" s="143"/>
+      <c r="B6" s="135"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -14953,8 +15070,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="128"/>
-      <c r="B7" s="120"/>
+      <c r="A7" s="143"/>
+      <c r="B7" s="135"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -15041,8 +15158,8 @@
       <c r="AF7" s="19"/>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="129"/>
-      <c r="B8" s="121"/>
+      <c r="A8" s="144"/>
+      <c r="B8" s="136"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -19449,10 +19566,10 @@
       <c r="AF56" s="19"/>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="117" t="s">
+      <c r="A57" s="132" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="118"/>
+      <c r="B57" s="133"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -19572,10 +19689,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="115" t="s">
+      <c r="A58" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="116"/>
+      <c r="B58" s="131"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -19746,28 +19863,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="173" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
+      <c r="B1" s="173"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="174" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="159"/>
-      <c r="C2" s="159"/>
-      <c r="D2" s="159"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="174" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="159"/>
-      <c r="C3" s="159"/>
-      <c r="D3" s="159"/>
+      <c r="B3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
     </row>
     <row r="4" spans="1:4" s="84" customFormat="1" ht="28.5">
       <c r="A4" s="82" t="s">
@@ -20498,41 +20615,41 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="157" t="s">
+      <c r="A56" s="172" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="157"/>
-      <c r="C56" s="157"/>
+      <c r="B56" s="172"/>
+      <c r="C56" s="172"/>
       <c r="D56" s="76">
         <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="157" t="s">
+      <c r="A57" s="172" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="157"/>
-      <c r="C57" s="157"/>
+      <c r="B57" s="172"/>
+      <c r="C57" s="172"/>
       <c r="D57" s="77">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="157" t="s">
+      <c r="A58" s="172" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="157"/>
-      <c r="C58" s="157"/>
+      <c r="B58" s="172"/>
+      <c r="C58" s="172"/>
       <c r="D58" s="77">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="157" t="s">
+      <c r="A59" s="172" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="157"/>
-      <c r="C59" s="157"/>
+      <c r="B59" s="172"/>
+      <c r="C59" s="172"/>
       <c r="D59" s="77">
         <v>92</v>
       </c>
@@ -20578,7 +20695,7 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:C55 C8:C23">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20605,68 +20722,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="175" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="161" t="s">
+      <c r="A2" s="176" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="161"/>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="176" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
     </row>
     <row r="4" spans="1:4" s="84" customFormat="1" ht="31.5">
-      <c r="A4" s="162" t="s">
+      <c r="A4" s="104" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="164" t="s">
+      <c r="C4" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="163" t="s">
+      <c r="D4" s="105" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="84" customFormat="1" ht="31.5">
-      <c r="A5" s="162" t="s">
+      <c r="A5" s="104" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="163" t="s">
+      <c r="B5" s="105" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="164" t="s">
+      <c r="C5" s="106" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="163" t="s">
+      <c r="D5" s="105" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="84" customFormat="1" ht="31.5">
-      <c r="A6" s="162" t="s">
+      <c r="A6" s="104" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="163" t="s">
+      <c r="B6" s="105" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="164" t="s">
+      <c r="C6" s="106" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="165">
+      <c r="D6" s="107">
         <v>43385</v>
       </c>
     </row>
@@ -20674,13 +20791,13 @@
       <c r="A7" s="99" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="166" t="s">
+      <c r="B7" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="166" t="s">
+      <c r="C7" s="108" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="167" t="s">
+      <c r="D7" s="109" t="s">
         <v>106</v>
       </c>
     </row>
@@ -20688,7 +20805,7 @@
       <c r="A8" s="99">
         <v>1</v>
       </c>
-      <c r="B8" s="168" t="s">
+      <c r="B8" s="110" t="s">
         <v>119</v>
       </c>
       <c r="C8" s="98">
@@ -20702,7 +20819,7 @@
       <c r="A9" s="99">
         <v>2</v>
       </c>
-      <c r="B9" s="168" t="s">
+      <c r="B9" s="110" t="s">
         <v>120</v>
       </c>
       <c r="C9" s="102">
@@ -20716,7 +20833,7 @@
       <c r="A10" s="99">
         <v>3</v>
       </c>
-      <c r="B10" s="168" t="s">
+      <c r="B10" s="110" t="s">
         <v>121</v>
       </c>
       <c r="C10" s="98">
@@ -20730,7 +20847,7 @@
       <c r="A11" s="99">
         <v>4</v>
       </c>
-      <c r="B11" s="169" t="s">
+      <c r="B11" s="111" t="s">
         <v>122</v>
       </c>
       <c r="C11" s="98">
@@ -20744,7 +20861,7 @@
       <c r="A12" s="99">
         <v>5</v>
       </c>
-      <c r="B12" s="168" t="s">
+      <c r="B12" s="110" t="s">
         <v>123</v>
       </c>
       <c r="C12" s="98">
@@ -20758,7 +20875,7 @@
       <c r="A13" s="99">
         <v>6</v>
       </c>
-      <c r="B13" s="168" t="s">
+      <c r="B13" s="110" t="s">
         <v>124</v>
       </c>
       <c r="C13" s="45" t="s">
@@ -20772,7 +20889,7 @@
       <c r="A14" s="99">
         <v>7</v>
       </c>
-      <c r="B14" s="168" t="s">
+      <c r="B14" s="110" t="s">
         <v>125</v>
       </c>
       <c r="C14" s="98">
@@ -20786,7 +20903,7 @@
       <c r="A15" s="99">
         <v>8</v>
       </c>
-      <c r="B15" s="168" t="s">
+      <c r="B15" s="110" t="s">
         <v>126</v>
       </c>
       <c r="C15" s="98">
@@ -20800,7 +20917,7 @@
       <c r="A16" s="99">
         <v>9</v>
       </c>
-      <c r="B16" s="168" t="s">
+      <c r="B16" s="110" t="s">
         <v>127</v>
       </c>
       <c r="C16" s="98">
@@ -20814,7 +20931,7 @@
       <c r="A17" s="99">
         <v>10</v>
       </c>
-      <c r="B17" s="168" t="s">
+      <c r="B17" s="110" t="s">
         <v>127</v>
       </c>
       <c r="C17" s="98">
@@ -20828,7 +20945,7 @@
       <c r="A18" s="99">
         <v>11</v>
       </c>
-      <c r="B18" s="168" t="s">
+      <c r="B18" s="110" t="s">
         <v>128</v>
       </c>
       <c r="C18" s="98">
@@ -20842,7 +20959,7 @@
       <c r="A19" s="99">
         <v>12</v>
       </c>
-      <c r="B19" s="168" t="s">
+      <c r="B19" s="110" t="s">
         <v>129</v>
       </c>
       <c r="C19" s="98">
@@ -20856,7 +20973,7 @@
       <c r="A20" s="99">
         <v>13</v>
       </c>
-      <c r="B20" s="168" t="s">
+      <c r="B20" s="110" t="s">
         <v>130</v>
       </c>
       <c r="C20" s="98">
@@ -20870,7 +20987,7 @@
       <c r="A21" s="99">
         <v>14</v>
       </c>
-      <c r="B21" s="170" t="s">
+      <c r="B21" s="112" t="s">
         <v>131</v>
       </c>
       <c r="C21" s="98">
@@ -20884,7 +21001,7 @@
       <c r="A22" s="99">
         <v>15</v>
       </c>
-      <c r="B22" s="170" t="s">
+      <c r="B22" s="112" t="s">
         <v>132</v>
       </c>
       <c r="C22" s="98">
@@ -20898,7 +21015,7 @@
       <c r="A23" s="99">
         <v>16</v>
       </c>
-      <c r="B23" s="168" t="s">
+      <c r="B23" s="110" t="s">
         <v>133</v>
       </c>
       <c r="C23" s="98">
@@ -20912,7 +21029,7 @@
       <c r="A24" s="99">
         <v>17</v>
       </c>
-      <c r="B24" s="168" t="s">
+      <c r="B24" s="110" t="s">
         <v>134</v>
       </c>
       <c r="C24" s="102">
@@ -20926,7 +21043,7 @@
       <c r="A25" s="99">
         <v>18</v>
       </c>
-      <c r="B25" s="168" t="s">
+      <c r="B25" s="110" t="s">
         <v>135</v>
       </c>
       <c r="C25" s="98">
@@ -20940,7 +21057,7 @@
       <c r="A26" s="99">
         <v>19</v>
       </c>
-      <c r="B26" s="168" t="s">
+      <c r="B26" s="110" t="s">
         <v>136</v>
       </c>
       <c r="C26" s="98">
@@ -20954,7 +21071,7 @@
       <c r="A27" s="99">
         <v>20</v>
       </c>
-      <c r="B27" s="168" t="s">
+      <c r="B27" s="110" t="s">
         <v>137</v>
       </c>
       <c r="C27" s="98">
@@ -20968,7 +21085,7 @@
       <c r="A28" s="99">
         <v>21</v>
       </c>
-      <c r="B28" s="168" t="s">
+      <c r="B28" s="110" t="s">
         <v>138</v>
       </c>
       <c r="C28" s="98">
@@ -20982,7 +21099,7 @@
       <c r="A29" s="99">
         <v>22</v>
       </c>
-      <c r="B29" s="168" t="s">
+      <c r="B29" s="110" t="s">
         <v>139</v>
       </c>
       <c r="C29" s="98">
@@ -20996,7 +21113,7 @@
       <c r="A30" s="99">
         <v>23</v>
       </c>
-      <c r="B30" s="171" t="s">
+      <c r="B30" s="113" t="s">
         <v>140</v>
       </c>
       <c r="C30" s="98">
@@ -21010,7 +21127,7 @@
       <c r="A31" s="99">
         <v>24</v>
       </c>
-      <c r="B31" s="172" t="s">
+      <c r="B31" s="114" t="s">
         <v>141</v>
       </c>
       <c r="C31" s="98">
@@ -21024,7 +21141,7 @@
       <c r="A32" s="99">
         <v>25</v>
       </c>
-      <c r="B32" s="170" t="s">
+      <c r="B32" s="112" t="s">
         <v>142</v>
       </c>
       <c r="C32" s="98">
@@ -21038,7 +21155,7 @@
       <c r="A33" s="99">
         <v>26</v>
       </c>
-      <c r="B33" s="168" t="s">
+      <c r="B33" s="110" t="s">
         <v>143</v>
       </c>
       <c r="C33" s="98">
@@ -21052,7 +21169,7 @@
       <c r="A34" s="99">
         <v>27</v>
       </c>
-      <c r="B34" s="172" t="s">
+      <c r="B34" s="114" t="s">
         <v>166</v>
       </c>
       <c r="C34" s="98">
@@ -21066,7 +21183,7 @@
       <c r="A35" s="99">
         <v>28</v>
       </c>
-      <c r="B35" s="168" t="s">
+      <c r="B35" s="110" t="s">
         <v>144</v>
       </c>
       <c r="C35" s="98">
@@ -21080,7 +21197,7 @@
       <c r="A36" s="99">
         <v>29</v>
       </c>
-      <c r="B36" s="170" t="s">
+      <c r="B36" s="112" t="s">
         <v>145</v>
       </c>
       <c r="C36" s="98">
@@ -21094,7 +21211,7 @@
       <c r="A37" s="99">
         <v>30</v>
       </c>
-      <c r="B37" s="168" t="s">
+      <c r="B37" s="110" t="s">
         <v>146</v>
       </c>
       <c r="C37" s="98">
@@ -21108,7 +21225,7 @@
       <c r="A38" s="99">
         <v>31</v>
       </c>
-      <c r="B38" s="170" t="s">
+      <c r="B38" s="112" t="s">
         <v>147</v>
       </c>
       <c r="C38" s="98">
@@ -21122,7 +21239,7 @@
       <c r="A39" s="99">
         <v>32</v>
       </c>
-      <c r="B39" s="168" t="s">
+      <c r="B39" s="110" t="s">
         <v>148</v>
       </c>
       <c r="C39" s="98">
@@ -21136,7 +21253,7 @@
       <c r="A40" s="99">
         <v>33</v>
       </c>
-      <c r="B40" s="168" t="s">
+      <c r="B40" s="110" t="s">
         <v>149</v>
       </c>
       <c r="C40" s="98">
@@ -21150,7 +21267,7 @@
       <c r="A41" s="99">
         <v>34</v>
       </c>
-      <c r="B41" s="168" t="s">
+      <c r="B41" s="110" t="s">
         <v>150</v>
       </c>
       <c r="C41" s="98">
@@ -21164,7 +21281,7 @@
       <c r="A42" s="99">
         <v>35</v>
       </c>
-      <c r="B42" s="168" t="s">
+      <c r="B42" s="110" t="s">
         <v>151</v>
       </c>
       <c r="C42" s="98">
@@ -21178,7 +21295,7 @@
       <c r="A43" s="99">
         <v>36</v>
       </c>
-      <c r="B43" s="168" t="s">
+      <c r="B43" s="110" t="s">
         <v>152</v>
       </c>
       <c r="C43" s="98">
@@ -21192,7 +21309,7 @@
       <c r="A44" s="99">
         <v>37</v>
       </c>
-      <c r="B44" s="170" t="s">
+      <c r="B44" s="112" t="s">
         <v>153</v>
       </c>
       <c r="C44" s="98">
@@ -21206,7 +21323,7 @@
       <c r="A45" s="99">
         <v>38</v>
       </c>
-      <c r="B45" s="168" t="s">
+      <c r="B45" s="110" t="s">
         <v>154</v>
       </c>
       <c r="C45" s="98">
@@ -21220,7 +21337,7 @@
       <c r="A46" s="99">
         <v>39</v>
       </c>
-      <c r="B46" s="172" t="s">
+      <c r="B46" s="114" t="s">
         <v>167</v>
       </c>
       <c r="C46" s="98">
@@ -21234,7 +21351,7 @@
       <c r="A47" s="99">
         <v>40</v>
       </c>
-      <c r="B47" s="168" t="s">
+      <c r="B47" s="110" t="s">
         <v>155</v>
       </c>
       <c r="C47" s="98">
@@ -21248,7 +21365,7 @@
       <c r="A48" s="99">
         <v>41</v>
       </c>
-      <c r="B48" s="168" t="s">
+      <c r="B48" s="110" t="s">
         <v>156</v>
       </c>
       <c r="C48" s="98">
@@ -21262,7 +21379,7 @@
       <c r="A49" s="99">
         <v>42</v>
       </c>
-      <c r="B49" s="168" t="s">
+      <c r="B49" s="110" t="s">
         <v>157</v>
       </c>
       <c r="C49" s="98">
@@ -21276,7 +21393,7 @@
       <c r="A50" s="99">
         <v>43</v>
       </c>
-      <c r="B50" s="170" t="s">
+      <c r="B50" s="112" t="s">
         <v>158</v>
       </c>
       <c r="C50" s="98">
@@ -21290,7 +21407,7 @@
       <c r="A51" s="99">
         <v>44</v>
       </c>
-      <c r="B51" s="170" t="s">
+      <c r="B51" s="112" t="s">
         <v>159</v>
       </c>
       <c r="C51" s="98">
@@ -21304,7 +21421,7 @@
       <c r="A52" s="99">
         <v>45</v>
       </c>
-      <c r="B52" s="168" t="s">
+      <c r="B52" s="110" t="s">
         <v>160</v>
       </c>
       <c r="C52" s="98">
@@ -21318,7 +21435,7 @@
       <c r="A53" s="99">
         <v>46</v>
       </c>
-      <c r="B53" s="168" t="s">
+      <c r="B53" s="110" t="s">
         <v>161</v>
       </c>
       <c r="C53" s="98">
@@ -21332,7 +21449,7 @@
       <c r="A54" s="99">
         <v>47</v>
       </c>
-      <c r="B54" s="168" t="s">
+      <c r="B54" s="110" t="s">
         <v>162</v>
       </c>
       <c r="C54" s="98">
@@ -21346,7 +21463,7 @@
       <c r="A55" s="100">
         <v>48</v>
       </c>
-      <c r="B55" s="173" t="s">
+      <c r="B55" s="115" t="s">
         <v>163</v>
       </c>
       <c r="C55" s="98">
@@ -21357,42 +21474,42 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75">
-      <c r="A56" s="133" t="s">
+      <c r="A56" s="148" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="133"/>
-      <c r="C56" s="133"/>
-      <c r="D56" s="174">
+      <c r="B56" s="148"/>
+      <c r="C56" s="148"/>
+      <c r="D56" s="116">
         <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75">
-      <c r="A57" s="133" t="s">
+      <c r="A57" s="148" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="133"/>
-      <c r="C57" s="133"/>
-      <c r="D57" s="175">
+      <c r="B57" s="148"/>
+      <c r="C57" s="148"/>
+      <c r="D57" s="117">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75">
-      <c r="A58" s="133" t="s">
+      <c r="A58" s="148" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="133"/>
-      <c r="C58" s="133"/>
-      <c r="D58" s="175">
+      <c r="B58" s="148"/>
+      <c r="C58" s="148"/>
+      <c r="D58" s="117">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75">
-      <c r="A59" s="133" t="s">
+      <c r="A59" s="148" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="133"/>
-      <c r="C59" s="133"/>
-      <c r="D59" s="175">
+      <c r="B59" s="148"/>
+      <c r="C59" s="148"/>
+      <c r="D59" s="117">
         <v>85.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Last Update 13-11-2018 14:27:48.06
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -993,6 +993,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="BB7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+File Modes and Operations</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1276,7 +1300,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4195" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4243" uniqueCount="168">
   <si>
     <t>S.NO</t>
   </si>
@@ -2167,7 +2191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2537,6 +2561,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2546,14 +2594,17 @@
     <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2582,32 +2633,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2621,17 +2660,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2642,11 +2675,23 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2680,24 +2725,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3091,7 +3118,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BD2" sqref="BD2"/>
+      <selection pane="bottomRight" activeCell="BF2" sqref="BF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -3105,29 +3132,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="18.75">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="120" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="137" t="s">
+      <c r="F1" s="122" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="140" t="s">
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="130" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="140"/>
-      <c r="L1" s="140"/>
-      <c r="M1" s="140"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -3152,41 +3179,41 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:65" ht="19.5">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="139" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="131"/>
-      <c r="C2" s="132"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="141"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="124" t="s">
+      <c r="F2" s="125" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="140" t="s">
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="140"/>
-      <c r="L2" s="140"/>
-      <c r="M2" s="140"/>
-      <c r="N2" s="141" t="s">
+      <c r="K2" s="130"/>
+      <c r="L2" s="130"/>
+      <c r="M2" s="130"/>
+      <c r="N2" s="131" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="141"/>
-      <c r="P2" s="141"/>
-      <c r="Q2" s="141"/>
-      <c r="R2" s="141"/>
-      <c r="S2" s="141"/>
-      <c r="T2" s="141"/>
-      <c r="U2" s="141"/>
-      <c r="V2" s="141"/>
-      <c r="W2" s="141"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
+      <c r="S2" s="131"/>
+      <c r="T2" s="131"/>
+      <c r="U2" s="131"/>
+      <c r="V2" s="131"/>
+      <c r="W2" s="131"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -3199,41 +3226,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:65" ht="18.75">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="120" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
+      <c r="B3" s="121"/>
+      <c r="C3" s="126"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="124" t="s">
+      <c r="F3" s="125" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="140" t="s">
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="130" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="140"/>
-      <c r="L3" s="140"/>
-      <c r="M3" s="140"/>
-      <c r="N3" s="141" t="s">
+      <c r="K3" s="130"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="130"/>
+      <c r="N3" s="131" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="141"/>
-      <c r="P3" s="141"/>
-      <c r="Q3" s="141"/>
-      <c r="R3" s="141"/>
-      <c r="S3" s="141"/>
-      <c r="T3" s="141"/>
-      <c r="U3" s="141"/>
-      <c r="V3" s="141"/>
-      <c r="W3" s="141"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="131"/>
+      <c r="Q3" s="131"/>
+      <c r="R3" s="131"/>
+      <c r="S3" s="131"/>
+      <c r="T3" s="131"/>
+      <c r="U3" s="131"/>
+      <c r="V3" s="131"/>
+      <c r="W3" s="131"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -3246,57 +3273,57 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:65" ht="18.75">
-      <c r="A4" s="133" t="s">
+      <c r="A4" s="120" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="134"/>
-      <c r="C4" s="135"/>
-      <c r="D4" s="119">
+      <c r="B4" s="121"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="127">
         <v>43344</v>
       </c>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="120"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="120"/>
-      <c r="N4" s="120"/>
-      <c r="O4" s="120"/>
-      <c r="P4" s="120"/>
-      <c r="Q4" s="120"/>
-      <c r="R4" s="120"/>
-      <c r="S4" s="120"/>
-      <c r="T4" s="120"/>
-      <c r="U4" s="120"/>
-      <c r="V4" s="120"/>
-      <c r="W4" s="121"/>
-      <c r="X4" s="119">
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="128"/>
+      <c r="M4" s="128"/>
+      <c r="N4" s="128"/>
+      <c r="O4" s="128"/>
+      <c r="P4" s="128"/>
+      <c r="Q4" s="128"/>
+      <c r="R4" s="128"/>
+      <c r="S4" s="128"/>
+      <c r="T4" s="128"/>
+      <c r="U4" s="128"/>
+      <c r="V4" s="128"/>
+      <c r="W4" s="129"/>
+      <c r="X4" s="127">
         <v>43374</v>
       </c>
-      <c r="Y4" s="120"/>
-      <c r="Z4" s="120"/>
-      <c r="AA4" s="120"/>
-      <c r="AB4" s="120"/>
-      <c r="AC4" s="120"/>
-      <c r="AD4" s="120"/>
-      <c r="AE4" s="120"/>
-      <c r="AF4" s="120"/>
-      <c r="AG4" s="120"/>
-      <c r="AH4" s="120"/>
-      <c r="AI4" s="120"/>
-      <c r="AJ4" s="120"/>
-      <c r="AK4" s="120"/>
-      <c r="AL4" s="120"/>
-      <c r="AM4" s="120"/>
-      <c r="AN4" s="120"/>
-      <c r="AO4" s="120"/>
-      <c r="AP4" s="120"/>
-      <c r="AQ4" s="120"/>
-      <c r="AR4" s="120"/>
-      <c r="AS4" s="121"/>
+      <c r="Y4" s="128"/>
+      <c r="Z4" s="128"/>
+      <c r="AA4" s="128"/>
+      <c r="AB4" s="128"/>
+      <c r="AC4" s="128"/>
+      <c r="AD4" s="128"/>
+      <c r="AE4" s="128"/>
+      <c r="AF4" s="128"/>
+      <c r="AG4" s="128"/>
+      <c r="AH4" s="128"/>
+      <c r="AI4" s="128"/>
+      <c r="AJ4" s="128"/>
+      <c r="AK4" s="128"/>
+      <c r="AL4" s="128"/>
+      <c r="AM4" s="128"/>
+      <c r="AN4" s="128"/>
+      <c r="AO4" s="128"/>
+      <c r="AP4" s="128"/>
+      <c r="AQ4" s="128"/>
+      <c r="AR4" s="128"/>
+      <c r="AS4" s="129"/>
       <c r="AT4" s="60"/>
       <c r="AU4" s="60"/>
       <c r="AV4" s="60"/>
@@ -3319,10 +3346,10 @@
       <c r="BM4" s="60"/>
     </row>
     <row r="5" spans="1:65">
-      <c r="A5" s="136" t="s">
+      <c r="A5" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="127" t="s">
+      <c r="B5" s="136" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -3478,7 +3505,9 @@
       <c r="BA5" s="118">
         <v>11</v>
       </c>
-      <c r="BB5" s="60"/>
+      <c r="BB5" s="60">
+        <v>11</v>
+      </c>
       <c r="BC5" s="60"/>
       <c r="BD5" s="60"/>
       <c r="BE5" s="60"/>
@@ -3492,8 +3521,8 @@
       <c r="BM5" s="60"/>
     </row>
     <row r="6" spans="1:65">
-      <c r="A6" s="136"/>
-      <c r="B6" s="128"/>
+      <c r="A6" s="142"/>
+      <c r="B6" s="137"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -3647,7 +3676,9 @@
       <c r="BA6" s="118">
         <v>10</v>
       </c>
-      <c r="BB6" s="60"/>
+      <c r="BB6" s="60">
+        <v>13</v>
+      </c>
       <c r="BC6" s="60"/>
       <c r="BD6" s="60"/>
       <c r="BE6" s="60"/>
@@ -3664,7 +3695,7 @@
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="129"/>
+      <c r="B7" s="138"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -3818,7 +3849,9 @@
       <c r="BA7" s="118">
         <v>7</v>
       </c>
-      <c r="BB7" s="60"/>
+      <c r="BB7" s="60">
+        <v>5</v>
+      </c>
       <c r="BC7" s="60"/>
       <c r="BD7" s="60"/>
       <c r="BE7" s="60"/>
@@ -3989,7 +4022,9 @@
       <c r="BA8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB8" s="60"/>
+      <c r="BB8" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC8" s="60"/>
       <c r="BD8" s="60"/>
       <c r="BE8" s="60"/>
@@ -4160,7 +4195,9 @@
       <c r="BA9" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB9" s="60"/>
+      <c r="BB9" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC9" s="60"/>
       <c r="BD9" s="60"/>
       <c r="BE9" s="60"/>
@@ -4331,7 +4368,9 @@
       <c r="BA10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB10" s="60"/>
+      <c r="BB10" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC10" s="60"/>
       <c r="BD10" s="60"/>
       <c r="BE10" s="60"/>
@@ -4502,7 +4541,9 @@
       <c r="BA11" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB11" s="60"/>
+      <c r="BB11" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BC11" s="60"/>
       <c r="BD11" s="60"/>
       <c r="BE11" s="60"/>
@@ -4673,7 +4714,9 @@
       <c r="BA12" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB12" s="60"/>
+      <c r="BB12" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC12" s="60"/>
       <c r="BD12" s="60"/>
       <c r="BE12" s="60"/>
@@ -4844,7 +4887,9 @@
       <c r="BA13" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB13" s="60"/>
+      <c r="BB13" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BC13" s="60"/>
       <c r="BD13" s="60"/>
       <c r="BE13" s="60"/>
@@ -5015,7 +5060,9 @@
       <c r="BA14" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB14" s="60"/>
+      <c r="BB14" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC14" s="60"/>
       <c r="BD14" s="60"/>
       <c r="BE14" s="60"/>
@@ -5186,7 +5233,9 @@
       <c r="BA15" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB15" s="60"/>
+      <c r="BB15" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC15" s="60"/>
       <c r="BD15" s="60"/>
       <c r="BE15" s="60"/>
@@ -5357,7 +5406,9 @@
       <c r="BA16" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB16" s="60"/>
+      <c r="BB16" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC16" s="60"/>
       <c r="BD16" s="60"/>
       <c r="BE16" s="60"/>
@@ -5528,7 +5579,9 @@
       <c r="BA17" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB17" s="60"/>
+      <c r="BB17" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC17" s="60"/>
       <c r="BD17" s="60"/>
       <c r="BE17" s="60"/>
@@ -5699,7 +5752,9 @@
       <c r="BA18" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB18" s="60"/>
+      <c r="BB18" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC18" s="60"/>
       <c r="BD18" s="60"/>
       <c r="BE18" s="60"/>
@@ -5870,7 +5925,9 @@
       <c r="BA19" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB19" s="60"/>
+      <c r="BB19" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC19" s="60"/>
       <c r="BD19" s="60"/>
       <c r="BE19" s="60"/>
@@ -6041,7 +6098,9 @@
       <c r="BA20" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB20" s="60"/>
+      <c r="BB20" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC20" s="60"/>
       <c r="BD20" s="60"/>
       <c r="BE20" s="60"/>
@@ -6212,7 +6271,9 @@
       <c r="BA21" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB21" s="60"/>
+      <c r="BB21" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC21" s="60"/>
       <c r="BD21" s="60"/>
       <c r="BE21" s="60"/>
@@ -6383,7 +6444,9 @@
       <c r="BA22" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB22" s="60"/>
+      <c r="BB22" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC22" s="60"/>
       <c r="BD22" s="60"/>
       <c r="BE22" s="60"/>
@@ -6554,7 +6617,9 @@
       <c r="BA23" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB23" s="60"/>
+      <c r="BB23" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC23" s="60"/>
       <c r="BD23" s="60"/>
       <c r="BE23" s="60"/>
@@ -6725,7 +6790,9 @@
       <c r="BA24" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB24" s="60"/>
+      <c r="BB24" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BC24" s="60"/>
       <c r="BD24" s="60"/>
       <c r="BE24" s="60"/>
@@ -6896,7 +6963,9 @@
       <c r="BA25" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB25" s="60"/>
+      <c r="BB25" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC25" s="60"/>
       <c r="BD25" s="60"/>
       <c r="BE25" s="60"/>
@@ -7067,7 +7136,9 @@
       <c r="BA26" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB26" s="60"/>
+      <c r="BB26" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC26" s="60"/>
       <c r="BD26" s="60"/>
       <c r="BE26" s="60"/>
@@ -7238,7 +7309,9 @@
       <c r="BA27" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB27" s="60"/>
+      <c r="BB27" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC27" s="60"/>
       <c r="BD27" s="60"/>
       <c r="BE27" s="60"/>
@@ -7409,7 +7482,9 @@
       <c r="BA28" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB28" s="60"/>
+      <c r="BB28" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC28" s="60"/>
       <c r="BD28" s="60"/>
       <c r="BE28" s="60"/>
@@ -7580,7 +7655,9 @@
       <c r="BA29" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB29" s="60"/>
+      <c r="BB29" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC29" s="60"/>
       <c r="BD29" s="60"/>
       <c r="BE29" s="60"/>
@@ -7751,7 +7828,9 @@
       <c r="BA30" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB30" s="60"/>
+      <c r="BB30" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC30" s="60"/>
       <c r="BD30" s="60"/>
       <c r="BE30" s="60"/>
@@ -7922,7 +8001,9 @@
       <c r="BA31" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB31" s="60"/>
+      <c r="BB31" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC31" s="60"/>
       <c r="BD31" s="60"/>
       <c r="BE31" s="60"/>
@@ -8093,7 +8174,9 @@
       <c r="BA32" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB32" s="60"/>
+      <c r="BB32" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC32" s="60"/>
       <c r="BD32" s="60"/>
       <c r="BE32" s="60"/>
@@ -8264,7 +8347,9 @@
       <c r="BA33" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB33" s="60"/>
+      <c r="BB33" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC33" s="60"/>
       <c r="BD33" s="60"/>
       <c r="BE33" s="60"/>
@@ -8435,7 +8520,9 @@
       <c r="BA34" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB34" s="60"/>
+      <c r="BB34" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC34" s="60"/>
       <c r="BD34" s="60"/>
       <c r="BE34" s="60"/>
@@ -8606,7 +8693,9 @@
       <c r="BA35" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB35" s="60"/>
+      <c r="BB35" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC35" s="60"/>
       <c r="BD35" s="60"/>
       <c r="BE35" s="60"/>
@@ -8777,7 +8866,9 @@
       <c r="BA36" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB36" s="60"/>
+      <c r="BB36" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC36" s="60"/>
       <c r="BD36" s="60"/>
       <c r="BE36" s="60"/>
@@ -8948,7 +9039,9 @@
       <c r="BA37" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB37" s="60"/>
+      <c r="BB37" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC37" s="60"/>
       <c r="BD37" s="60"/>
       <c r="BE37" s="60"/>
@@ -9119,7 +9212,9 @@
       <c r="BA38" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB38" s="60"/>
+      <c r="BB38" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC38" s="60"/>
       <c r="BD38" s="60"/>
       <c r="BE38" s="60"/>
@@ -9290,7 +9385,9 @@
       <c r="BA39" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB39" s="60"/>
+      <c r="BB39" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC39" s="60"/>
       <c r="BD39" s="60"/>
       <c r="BE39" s="60"/>
@@ -9461,7 +9558,9 @@
       <c r="BA40" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB40" s="60"/>
+      <c r="BB40" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BC40" s="60"/>
       <c r="BD40" s="60"/>
       <c r="BE40" s="60"/>
@@ -9632,7 +9731,9 @@
       <c r="BA41" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB41" s="60"/>
+      <c r="BB41" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC41" s="60"/>
       <c r="BD41" s="60"/>
       <c r="BE41" s="60"/>
@@ -9803,7 +9904,9 @@
       <c r="BA42" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB42" s="60"/>
+      <c r="BB42" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC42" s="60"/>
       <c r="BD42" s="60"/>
       <c r="BE42" s="60"/>
@@ -9974,7 +10077,9 @@
       <c r="BA43" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB43" s="60"/>
+      <c r="BB43" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC43" s="60"/>
       <c r="BD43" s="60"/>
       <c r="BE43" s="60"/>
@@ -10145,7 +10250,9 @@
       <c r="BA44" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB44" s="60"/>
+      <c r="BB44" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC44" s="60"/>
       <c r="BD44" s="60"/>
       <c r="BE44" s="60"/>
@@ -10316,7 +10423,9 @@
       <c r="BA45" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB45" s="60"/>
+      <c r="BB45" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC45" s="60"/>
       <c r="BD45" s="60"/>
       <c r="BE45" s="60"/>
@@ -10487,7 +10596,9 @@
       <c r="BA46" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB46" s="60"/>
+      <c r="BB46" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BC46" s="60"/>
       <c r="BD46" s="60"/>
       <c r="BE46" s="60"/>
@@ -10658,7 +10769,9 @@
       <c r="BA47" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB47" s="60"/>
+      <c r="BB47" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC47" s="60"/>
       <c r="BD47" s="60"/>
       <c r="BE47" s="60"/>
@@ -10829,7 +10942,9 @@
       <c r="BA48" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB48" s="60"/>
+      <c r="BB48" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC48" s="60"/>
       <c r="BD48" s="60"/>
       <c r="BE48" s="60"/>
@@ -11000,7 +11115,9 @@
       <c r="BA49" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB49" s="60"/>
+      <c r="BB49" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC49" s="60"/>
       <c r="BD49" s="60"/>
       <c r="BE49" s="60"/>
@@ -11171,7 +11288,9 @@
       <c r="BA50" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB50" s="60"/>
+      <c r="BB50" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BC50" s="60"/>
       <c r="BD50" s="60"/>
       <c r="BE50" s="60"/>
@@ -11342,7 +11461,9 @@
       <c r="BA51" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB51" s="60"/>
+      <c r="BB51" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BC51" s="60"/>
       <c r="BD51" s="60"/>
       <c r="BE51" s="60"/>
@@ -11513,7 +11634,9 @@
       <c r="BA52" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB52" s="60"/>
+      <c r="BB52" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC52" s="60"/>
       <c r="BD52" s="60"/>
       <c r="BE52" s="60"/>
@@ -11684,7 +11807,9 @@
       <c r="BA53" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB53" s="60"/>
+      <c r="BB53" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC53" s="60"/>
       <c r="BD53" s="60"/>
       <c r="BE53" s="60"/>
@@ -11855,7 +11980,9 @@
       <c r="BA54" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="BB54" s="60"/>
+      <c r="BB54" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC54" s="60"/>
       <c r="BD54" s="60"/>
       <c r="BE54" s="60"/>
@@ -12026,7 +12153,9 @@
       <c r="BA55" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BB55" s="60"/>
+      <c r="BB55" s="119" t="s">
+        <v>54</v>
+      </c>
       <c r="BC55" s="60"/>
       <c r="BD55" s="60"/>
       <c r="BE55" s="60"/>
@@ -12040,10 +12169,10 @@
       <c r="BM55" s="60"/>
     </row>
     <row r="56" spans="1:65">
-      <c r="A56" s="125" t="s">
+      <c r="A56" s="134" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="126"/>
+      <c r="B56" s="135"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -12247,7 +12376,7 @@
       </c>
       <c r="BB56" s="60">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BC56" s="60">
         <f t="shared" si="22"/>
@@ -12295,10 +12424,10 @@
       </c>
     </row>
     <row r="57" spans="1:65">
-      <c r="A57" s="122" t="s">
+      <c r="A57" s="132" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="123"/>
+      <c r="B57" s="133"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -12502,7 +12631,7 @@
       </c>
       <c r="BB57" s="60">
         <f t="shared" si="24"/>
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="BC57" s="60">
         <f t="shared" si="24"/>
@@ -12551,6 +12680,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="X4:AS4"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F3:I3"/>
@@ -12561,14 +12698,6 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="X4:AS4"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -12596,72 +12725,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="143" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="145" t="s">
+      <c r="B1" s="143"/>
+      <c r="C1" s="150" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="145"/>
-      <c r="E1" s="141" t="s">
+      <c r="D1" s="150"/>
+      <c r="E1" s="131" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="148" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="145" t="s">
+      <c r="B2" s="148"/>
+      <c r="C2" s="150" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="145"/>
-      <c r="E2" s="141" t="s">
+      <c r="D2" s="150"/>
+      <c r="E2" s="131" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="141"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="144" t="s">
+      <c r="A3" s="149" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="144"/>
-      <c r="C3" s="145" t="s">
+      <c r="B3" s="149"/>
+      <c r="C3" s="150" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="145"/>
-      <c r="E3" s="141" t="s">
+      <c r="D3" s="150"/>
+      <c r="E3" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="141"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="147" t="s">
+      <c r="A4" s="144" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="127" t="s">
+      <c r="B4" s="136" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="142" t="s">
+      <c r="C4" s="147" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="142"/>
-      <c r="E4" s="142"/>
-      <c r="F4" s="142"/>
-      <c r="G4" s="142"/>
-      <c r="H4" s="142"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="147"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="147"/>
+      <c r="H4" s="147"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="148"/>
-      <c r="B5" s="128"/>
+      <c r="A5" s="145"/>
+      <c r="B5" s="137"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -12682,8 +12811,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="149"/>
-      <c r="B6" s="129"/>
+      <c r="A6" s="146"/>
+      <c r="B6" s="138"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -13702,10 +13831,10 @@
       <c r="H54" s="42"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="125" t="s">
+      <c r="A55" s="134" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="126"/>
+      <c r="B55" s="135"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -13721,10 +13850,10 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="122" t="s">
+      <c r="A56" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="123"/>
+      <c r="B56" s="133"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -13740,10 +13869,10 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="122" t="s">
+      <c r="A57" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="123"/>
+      <c r="B57" s="133"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -13759,10 +13888,10 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="122" t="s">
+      <c r="A58" s="132" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="123"/>
+      <c r="B58" s="133"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -13779,13 +13908,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -13795,6 +13917,13 @@
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:H54">
     <cfRule type="cellIs" dxfId="5" priority="17" operator="lessThan">
@@ -13828,72 +13957,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="143" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="145" t="s">
+      <c r="B1" s="143"/>
+      <c r="C1" s="150" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="145"/>
-      <c r="E1" s="153" t="s">
+      <c r="D1" s="150"/>
+      <c r="E1" s="151" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="153"/>
-      <c r="G1" s="153"/>
-      <c r="H1" s="154"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="152"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="148" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="145" t="s">
+      <c r="B2" s="148"/>
+      <c r="C2" s="150" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="145"/>
-      <c r="E2" s="141" t="s">
+      <c r="D2" s="150"/>
+      <c r="E2" s="131" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="141"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="144" t="s">
+      <c r="A3" s="149" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="144"/>
-      <c r="C3" s="145" t="s">
+      <c r="B3" s="149"/>
+      <c r="C3" s="150" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="145"/>
-      <c r="E3" s="141" t="s">
+      <c r="D3" s="150"/>
+      <c r="E3" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="141"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="147" t="s">
+      <c r="A4" s="144" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="127" t="s">
+      <c r="B4" s="136" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="150" t="s">
+      <c r="C4" s="153" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="151"/>
-      <c r="E4" s="151"/>
-      <c r="F4" s="151"/>
-      <c r="G4" s="151"/>
-      <c r="H4" s="152"/>
+      <c r="D4" s="154"/>
+      <c r="E4" s="154"/>
+      <c r="F4" s="154"/>
+      <c r="G4" s="154"/>
+      <c r="H4" s="155"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="148"/>
-      <c r="B5" s="128"/>
+      <c r="A5" s="145"/>
+      <c r="B5" s="137"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -13914,8 +14043,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="149"/>
-      <c r="B6" s="129"/>
+      <c r="A6" s="146"/>
+      <c r="B6" s="138"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -15040,10 +15169,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="125" t="s">
+      <c r="A55" s="134" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="126"/>
+      <c r="B55" s="135"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -15058,10 +15187,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="122" t="s">
+      <c r="A56" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="123"/>
+      <c r="B56" s="133"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -15076,10 +15205,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="122" t="s">
+      <c r="A57" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="123"/>
+      <c r="B57" s="133"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -15094,10 +15223,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="122" t="s">
+      <c r="A58" s="132" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="123"/>
+      <c r="B58" s="133"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -15113,22 +15242,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
@@ -15169,216 +15298,216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="120" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="137" t="s">
+      <c r="F1" s="122" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="140" t="s">
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="130" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="140"/>
-      <c r="L1" s="140"/>
-      <c r="M1" s="140"/>
-      <c r="N1" s="155" t="s">
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="162" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="156"/>
-      <c r="P1" s="156"/>
-      <c r="Q1" s="156"/>
-      <c r="R1" s="156"/>
-      <c r="S1" s="156"/>
-      <c r="T1" s="156"/>
-      <c r="U1" s="156"/>
-      <c r="V1" s="156"/>
-      <c r="W1" s="156"/>
-      <c r="X1" s="156"/>
-      <c r="Y1" s="156"/>
-      <c r="Z1" s="156"/>
-      <c r="AA1" s="156"/>
-      <c r="AB1" s="156"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="163"/>
+      <c r="T1" s="163"/>
+      <c r="U1" s="163"/>
+      <c r="V1" s="163"/>
+      <c r="W1" s="163"/>
+      <c r="X1" s="163"/>
+      <c r="Y1" s="163"/>
+      <c r="Z1" s="163"/>
+      <c r="AA1" s="163"/>
+      <c r="AB1" s="163"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="139" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="131"/>
-      <c r="C2" s="132"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="141"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="124" t="s">
+      <c r="F2" s="125" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="140" t="s">
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="140"/>
-      <c r="L2" s="140"/>
-      <c r="M2" s="140"/>
-      <c r="N2" s="155" t="s">
+      <c r="K2" s="130"/>
+      <c r="L2" s="130"/>
+      <c r="M2" s="130"/>
+      <c r="N2" s="162" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="156"/>
-      <c r="P2" s="156"/>
-      <c r="Q2" s="156"/>
-      <c r="R2" s="156"/>
-      <c r="S2" s="156"/>
-      <c r="T2" s="156"/>
-      <c r="U2" s="156"/>
-      <c r="V2" s="156"/>
-      <c r="W2" s="156"/>
-      <c r="X2" s="156"/>
-      <c r="Y2" s="156"/>
-      <c r="Z2" s="156"/>
-      <c r="AA2" s="156"/>
-      <c r="AB2" s="156"/>
+      <c r="O2" s="163"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
+      <c r="U2" s="163"/>
+      <c r="V2" s="163"/>
+      <c r="W2" s="163"/>
+      <c r="X2" s="163"/>
+      <c r="Y2" s="163"/>
+      <c r="Z2" s="163"/>
+      <c r="AA2" s="163"/>
+      <c r="AB2" s="163"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="158" t="s">
+      <c r="A3" s="165" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="159"/>
-      <c r="C3" s="160"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="167"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="157" t="s">
+      <c r="F3" s="164" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="166" t="s">
+      <c r="G3" s="164"/>
+      <c r="H3" s="164"/>
+      <c r="I3" s="164"/>
+      <c r="J3" s="173" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="166"/>
-      <c r="L3" s="166"/>
-      <c r="M3" s="166"/>
-      <c r="N3" s="155" t="s">
+      <c r="K3" s="173"/>
+      <c r="L3" s="173"/>
+      <c r="M3" s="173"/>
+      <c r="N3" s="162" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="156"/>
-      <c r="P3" s="156"/>
-      <c r="Q3" s="156"/>
-      <c r="R3" s="156"/>
-      <c r="S3" s="156"/>
-      <c r="T3" s="156"/>
-      <c r="U3" s="156"/>
-      <c r="V3" s="156"/>
-      <c r="W3" s="156"/>
-      <c r="X3" s="156"/>
-      <c r="Y3" s="156"/>
-      <c r="Z3" s="156"/>
-      <c r="AA3" s="156"/>
-      <c r="AB3" s="156"/>
+      <c r="O3" s="163"/>
+      <c r="P3" s="163"/>
+      <c r="Q3" s="163"/>
+      <c r="R3" s="163"/>
+      <c r="S3" s="163"/>
+      <c r="T3" s="163"/>
+      <c r="U3" s="163"/>
+      <c r="V3" s="163"/>
+      <c r="W3" s="163"/>
+      <c r="X3" s="163"/>
+      <c r="Y3" s="163"/>
+      <c r="Z3" s="163"/>
+      <c r="AA3" s="163"/>
+      <c r="AB3" s="163"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="161"/>
-      <c r="B4" s="162"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="164">
+      <c r="A4" s="168"/>
+      <c r="B4" s="169"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="171">
         <v>43344</v>
       </c>
-      <c r="E4" s="165"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="165"/>
-      <c r="H4" s="165"/>
-      <c r="I4" s="165"/>
-      <c r="J4" s="165"/>
-      <c r="K4" s="165"/>
-      <c r="L4" s="165"/>
-      <c r="M4" s="165"/>
-      <c r="N4" s="164">
+      <c r="E4" s="172"/>
+      <c r="F4" s="172"/>
+      <c r="G4" s="172"/>
+      <c r="H4" s="172"/>
+      <c r="I4" s="172"/>
+      <c r="J4" s="172"/>
+      <c r="K4" s="172"/>
+      <c r="L4" s="172"/>
+      <c r="M4" s="172"/>
+      <c r="N4" s="171">
         <v>43374</v>
       </c>
-      <c r="O4" s="165"/>
-      <c r="P4" s="165"/>
-      <c r="Q4" s="165"/>
-      <c r="R4" s="165"/>
-      <c r="S4" s="165"/>
-      <c r="T4" s="165"/>
-      <c r="U4" s="165"/>
+      <c r="O4" s="172"/>
+      <c r="P4" s="172"/>
+      <c r="Q4" s="172"/>
+      <c r="R4" s="172"/>
+      <c r="S4" s="172"/>
+      <c r="T4" s="172"/>
+      <c r="U4" s="172"/>
       <c r="V4" s="53"/>
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="147" t="s">
+      <c r="A5" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="127" t="s">
+      <c r="B5" s="136" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="168" t="s">
+      <c r="D5" s="157" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
-      <c r="H5" s="171" t="s">
+      <c r="E5" s="158"/>
+      <c r="F5" s="158"/>
+      <c r="G5" s="159"/>
+      <c r="H5" s="160" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="172"/>
-      <c r="J5" s="172"/>
-      <c r="K5" s="172"/>
-      <c r="L5" s="167" t="s">
+      <c r="I5" s="161"/>
+      <c r="J5" s="161"/>
+      <c r="K5" s="161"/>
+      <c r="L5" s="156" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="167"/>
-      <c r="N5" s="171" t="s">
+      <c r="M5" s="156"/>
+      <c r="N5" s="160" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="172"/>
-      <c r="P5" s="172"/>
-      <c r="Q5" s="172"/>
-      <c r="R5" s="167" t="s">
+      <c r="O5" s="161"/>
+      <c r="P5" s="161"/>
+      <c r="Q5" s="161"/>
+      <c r="R5" s="156" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="167"/>
-      <c r="T5" s="136" t="s">
+      <c r="S5" s="156"/>
+      <c r="T5" s="142" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="136"/>
-      <c r="V5" s="136" t="s">
+      <c r="U5" s="142"/>
+      <c r="V5" s="142" t="s">
         <v>117</v>
       </c>
-      <c r="W5" s="136"/>
-      <c r="X5" s="136"/>
-      <c r="Y5" s="136"/>
-      <c r="Z5" s="136" t="s">
+      <c r="W5" s="142"/>
+      <c r="X5" s="142"/>
+      <c r="Y5" s="142"/>
+      <c r="Z5" s="142" t="s">
         <v>118</v>
       </c>
-      <c r="AA5" s="136"/>
-      <c r="AB5" s="136"/>
-      <c r="AC5" s="136"/>
+      <c r="AA5" s="142"/>
+      <c r="AB5" s="142"/>
+      <c r="AC5" s="142"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="148"/>
-      <c r="B6" s="128"/>
+      <c r="A6" s="145"/>
+      <c r="B6" s="137"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -15465,8 +15594,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="148"/>
-      <c r="B7" s="128"/>
+      <c r="A7" s="145"/>
+      <c r="B7" s="137"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -15553,8 +15682,8 @@
       <c r="AF7" s="19"/>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="149"/>
-      <c r="B8" s="129"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="138"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -19961,10 +20090,10 @@
       <c r="AF56" s="19"/>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="125" t="s">
+      <c r="A57" s="134" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="126"/>
+      <c r="B57" s="135"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -20084,10 +20213,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="122" t="s">
+      <c r="A58" s="132" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="123"/>
+      <c r="B58" s="133"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -20208,18 +20337,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="N5:Q5"/>
     <mergeCell ref="N1:AB1"/>
     <mergeCell ref="N2:AB2"/>
     <mergeCell ref="N3:AB3"/>
@@ -20234,6 +20351,18 @@
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N4:U4"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="N5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -20259,28 +20388,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="175" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="175" t="s">
+      <c r="A2" s="176" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="175" t="s">
+      <c r="A3" s="176" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
     </row>
     <row r="4" spans="1:4" s="83" customFormat="1" ht="28.5">
       <c r="A4" s="81" t="s">
@@ -21011,41 +21140,41 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="173" t="s">
+      <c r="A56" s="174" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="173"/>
-      <c r="C56" s="173"/>
+      <c r="B56" s="174"/>
+      <c r="C56" s="174"/>
       <c r="D56" s="75">
         <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="173" t="s">
+      <c r="A57" s="174" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="173"/>
-      <c r="C57" s="173"/>
+      <c r="B57" s="174"/>
+      <c r="C57" s="174"/>
       <c r="D57" s="76">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="173" t="s">
+      <c r="A58" s="174" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="173"/>
-      <c r="C58" s="173"/>
+      <c r="B58" s="174"/>
+      <c r="C58" s="174"/>
       <c r="D58" s="76">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="173" t="s">
+      <c r="A59" s="174" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="173"/>
-      <c r="C59" s="173"/>
+      <c r="B59" s="174"/>
+      <c r="C59" s="174"/>
       <c r="D59" s="76">
         <v>92</v>
       </c>
@@ -21118,28 +21247,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="177" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="177" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="177"/>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="177" t="s">
+      <c r="A3" s="178" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="177"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
+      <c r="B3" s="178"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="178"/>
     </row>
     <row r="4" spans="1:4" s="83" customFormat="1" ht="31.5">
       <c r="A4" s="103" t="s">
@@ -21870,41 +21999,41 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75">
-      <c r="A56" s="145" t="s">
+      <c r="A56" s="150" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="145"/>
-      <c r="C56" s="145"/>
+      <c r="B56" s="150"/>
+      <c r="C56" s="150"/>
       <c r="D56" s="115">
         <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75">
-      <c r="A57" s="145" t="s">
+      <c r="A57" s="150" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="145"/>
-      <c r="C57" s="145"/>
+      <c r="B57" s="150"/>
+      <c r="C57" s="150"/>
       <c r="D57" s="116">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75">
-      <c r="A58" s="145" t="s">
+      <c r="A58" s="150" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="145"/>
-      <c r="C58" s="145"/>
+      <c r="B58" s="150"/>
+      <c r="C58" s="150"/>
       <c r="D58" s="116">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75">
-      <c r="A59" s="145" t="s">
+      <c r="A59" s="150" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="145"/>
-      <c r="C59" s="145"/>
+      <c r="B59" s="150"/>
+      <c r="C59" s="150"/>
       <c r="D59" s="116">
         <v>85.1</v>
       </c>

</xml_diff>

<commit_message>
Last Update 14-11-2018 15:12:12.35
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -1300,7 +1300,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4243" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4244" uniqueCount="169">
   <si>
     <t>S.NO</t>
   </si>
@@ -1805,6 +1805,9 @@
   <si>
     <t>Sowmya S</t>
   </si>
+  <si>
+    <t>Assignment</t>
+  </si>
 </sst>
 </file>
 
@@ -2191,7 +2194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2564,26 +2567,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2594,17 +2585,14 @@
     <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2633,8 +2621,44 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2648,24 +2672,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2675,23 +2681,11 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2725,6 +2719,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3114,7 +3126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BM57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -3132,29 +3144,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="18.75">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="122" t="s">
+      <c r="F1" s="141" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="130" t="s">
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="143"/>
+      <c r="J1" s="144" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
-      <c r="M1" s="130"/>
+      <c r="K1" s="144"/>
+      <c r="L1" s="144"/>
+      <c r="M1" s="144"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -3179,41 +3191,41 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:65" ht="19.5">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="134" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="140"/>
-      <c r="C2" s="141"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="136"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="125" t="s">
+      <c r="F2" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="130" t="s">
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="144" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="130"/>
-      <c r="L2" s="130"/>
-      <c r="M2" s="130"/>
-      <c r="N2" s="131" t="s">
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="M2" s="144"/>
+      <c r="N2" s="145" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="131"/>
-      <c r="P2" s="131"/>
-      <c r="Q2" s="131"/>
-      <c r="R2" s="131"/>
-      <c r="S2" s="131"/>
-      <c r="T2" s="131"/>
-      <c r="U2" s="131"/>
-      <c r="V2" s="131"/>
-      <c r="W2" s="131"/>
+      <c r="O2" s="145"/>
+      <c r="P2" s="145"/>
+      <c r="Q2" s="145"/>
+      <c r="R2" s="145"/>
+      <c r="S2" s="145"/>
+      <c r="T2" s="145"/>
+      <c r="U2" s="145"/>
+      <c r="V2" s="145"/>
+      <c r="W2" s="145"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -3226,41 +3238,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:65" ht="18.75">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="137" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="121"/>
-      <c r="C3" s="126"/>
+      <c r="B3" s="138"/>
+      <c r="C3" s="139"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="125" t="s">
+      <c r="F3" s="128" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="125"/>
-      <c r="H3" s="125"/>
-      <c r="I3" s="125"/>
-      <c r="J3" s="130" t="s">
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="130"/>
-      <c r="L3" s="130"/>
-      <c r="M3" s="130"/>
-      <c r="N3" s="131" t="s">
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="145" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="131"/>
-      <c r="P3" s="131"/>
-      <c r="Q3" s="131"/>
-      <c r="R3" s="131"/>
-      <c r="S3" s="131"/>
-      <c r="T3" s="131"/>
-      <c r="U3" s="131"/>
-      <c r="V3" s="131"/>
-      <c r="W3" s="131"/>
+      <c r="O3" s="145"/>
+      <c r="P3" s="145"/>
+      <c r="Q3" s="145"/>
+      <c r="R3" s="145"/>
+      <c r="S3" s="145"/>
+      <c r="T3" s="145"/>
+      <c r="U3" s="145"/>
+      <c r="V3" s="145"/>
+      <c r="W3" s="145"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -3273,57 +3285,57 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:65" ht="18.75">
-      <c r="A4" s="120" t="s">
+      <c r="A4" s="137" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="121"/>
-      <c r="C4" s="126"/>
-      <c r="D4" s="127">
+      <c r="B4" s="138"/>
+      <c r="C4" s="139"/>
+      <c r="D4" s="123">
         <v>43344</v>
       </c>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
-      <c r="K4" s="128"/>
-      <c r="L4" s="128"/>
-      <c r="M4" s="128"/>
-      <c r="N4" s="128"/>
-      <c r="O4" s="128"/>
-      <c r="P4" s="128"/>
-      <c r="Q4" s="128"/>
-      <c r="R4" s="128"/>
-      <c r="S4" s="128"/>
-      <c r="T4" s="128"/>
-      <c r="U4" s="128"/>
-      <c r="V4" s="128"/>
-      <c r="W4" s="129"/>
-      <c r="X4" s="127">
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="124"/>
+      <c r="M4" s="124"/>
+      <c r="N4" s="124"/>
+      <c r="O4" s="124"/>
+      <c r="P4" s="124"/>
+      <c r="Q4" s="124"/>
+      <c r="R4" s="124"/>
+      <c r="S4" s="124"/>
+      <c r="T4" s="124"/>
+      <c r="U4" s="124"/>
+      <c r="V4" s="124"/>
+      <c r="W4" s="125"/>
+      <c r="X4" s="123">
         <v>43374</v>
       </c>
-      <c r="Y4" s="128"/>
-      <c r="Z4" s="128"/>
-      <c r="AA4" s="128"/>
-      <c r="AB4" s="128"/>
-      <c r="AC4" s="128"/>
-      <c r="AD4" s="128"/>
-      <c r="AE4" s="128"/>
-      <c r="AF4" s="128"/>
-      <c r="AG4" s="128"/>
-      <c r="AH4" s="128"/>
-      <c r="AI4" s="128"/>
-      <c r="AJ4" s="128"/>
-      <c r="AK4" s="128"/>
-      <c r="AL4" s="128"/>
-      <c r="AM4" s="128"/>
-      <c r="AN4" s="128"/>
-      <c r="AO4" s="128"/>
-      <c r="AP4" s="128"/>
-      <c r="AQ4" s="128"/>
-      <c r="AR4" s="128"/>
-      <c r="AS4" s="129"/>
+      <c r="Y4" s="124"/>
+      <c r="Z4" s="124"/>
+      <c r="AA4" s="124"/>
+      <c r="AB4" s="124"/>
+      <c r="AC4" s="124"/>
+      <c r="AD4" s="124"/>
+      <c r="AE4" s="124"/>
+      <c r="AF4" s="124"/>
+      <c r="AG4" s="124"/>
+      <c r="AH4" s="124"/>
+      <c r="AI4" s="124"/>
+      <c r="AJ4" s="124"/>
+      <c r="AK4" s="124"/>
+      <c r="AL4" s="124"/>
+      <c r="AM4" s="124"/>
+      <c r="AN4" s="124"/>
+      <c r="AO4" s="124"/>
+      <c r="AP4" s="124"/>
+      <c r="AQ4" s="124"/>
+      <c r="AR4" s="124"/>
+      <c r="AS4" s="125"/>
       <c r="AT4" s="60"/>
       <c r="AU4" s="60"/>
       <c r="AV4" s="60"/>
@@ -3346,10 +3358,10 @@
       <c r="BM4" s="60"/>
     </row>
     <row r="5" spans="1:65">
-      <c r="A5" s="142" t="s">
+      <c r="A5" s="140" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="136" t="s">
+      <c r="B5" s="131" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -3521,8 +3533,8 @@
       <c r="BM5" s="60"/>
     </row>
     <row r="6" spans="1:65">
-      <c r="A6" s="142"/>
-      <c r="B6" s="137"/>
+      <c r="A6" s="140"/>
+      <c r="B6" s="132"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -3695,7 +3707,7 @@
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="138"/>
+      <c r="B7" s="133"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -12169,10 +12181,10 @@
       <c r="BM55" s="60"/>
     </row>
     <row r="56" spans="1:65">
-      <c r="A56" s="134" t="s">
+      <c r="A56" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="135"/>
+      <c r="B56" s="130"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -12424,10 +12436,10 @@
       </c>
     </row>
     <row r="57" spans="1:65">
-      <c r="A57" s="132" t="s">
+      <c r="A57" s="126" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="133"/>
+      <c r="B57" s="127"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -12680,14 +12692,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="X4:AS4"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F3:I3"/>
@@ -12698,6 +12702,14 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N2:W2"/>
     <mergeCell ref="N3:W3"/>
+    <mergeCell ref="X4:AS4"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -12707,10 +12719,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -12718,79 +12730,84 @@
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" style="1" customWidth="1"/>
     <col min="3" max="6" width="11.140625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="21" width="9.140625" style="1"/>
-    <col min="22" max="22" width="9.140625" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="12.5703125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="11.140625" style="1" customWidth="1"/>
+    <col min="10" max="22" width="9.140625" style="1"/>
+    <col min="23" max="23" width="9.140625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="143" t="s">
+    <row r="1" spans="1:9" ht="18.75">
+      <c r="A1" s="150" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="150" t="s">
+      <c r="B1" s="150"/>
+      <c r="C1" s="149" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="150"/>
-      <c r="E1" s="131" t="s">
+      <c r="D1" s="149"/>
+      <c r="E1" s="145" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-    </row>
-    <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="148" t="s">
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+    </row>
+    <row r="2" spans="1:9" ht="19.5">
+      <c r="A2" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="150" t="s">
+      <c r="B2" s="147"/>
+      <c r="C2" s="149" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="150"/>
-      <c r="E2" s="131" t="s">
+      <c r="D2" s="149"/>
+      <c r="E2" s="145" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-    </row>
-    <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="149" t="s">
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+    </row>
+    <row r="3" spans="1:9" ht="17.25">
+      <c r="A3" s="148" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="149"/>
-      <c r="C3" s="150" t="s">
+      <c r="B3" s="148"/>
+      <c r="C3" s="149" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="150"/>
-      <c r="E3" s="131" t="s">
+      <c r="D3" s="149"/>
+      <c r="E3" s="145" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131"/>
-      <c r="H3" s="131"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="144" t="s">
+      <c r="F3" s="145"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="145"/>
+      <c r="I3" s="145"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1">
+      <c r="A4" s="151" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="136" t="s">
+      <c r="B4" s="131" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="147" t="s">
+      <c r="C4" s="146" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="147"/>
-      <c r="E4" s="147"/>
-      <c r="F4" s="147"/>
-      <c r="G4" s="147"/>
-      <c r="H4" s="147"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="145"/>
-      <c r="B5" s="137"/>
+      <c r="D4" s="146"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" s="152"/>
+      <c r="B5" s="132"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -12803,16 +12820,19 @@
       <c r="F5" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="121" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="146"/>
-      <c r="B6" s="138"/>
+    <row r="6" spans="1:9" ht="15" customHeight="1">
+      <c r="A6" s="153"/>
+      <c r="B6" s="133"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -12825,14 +12845,17 @@
       <c r="F6" s="43">
         <v>50</v>
       </c>
-      <c r="G6" s="3">
-        <v>50</v>
+      <c r="G6" s="121">
+        <v>20</v>
       </c>
       <c r="H6" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
+      <c r="I6" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -12849,10 +12872,11 @@
       <c r="F7" s="42">
         <v>31</v>
       </c>
-      <c r="G7" s="42"/>
+      <c r="G7" s="120"/>
       <c r="H7" s="42"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
+      <c r="I7" s="42"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -12871,10 +12895,11 @@
       <c r="F8" s="93">
         <v>41</v>
       </c>
-      <c r="G8" s="45"/>
+      <c r="G8" s="122"/>
       <c r="H8" s="45"/>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
+      <c r="I8" s="45"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -12893,10 +12918,11 @@
       <c r="F9" s="42">
         <v>30</v>
       </c>
-      <c r="G9" s="42"/>
+      <c r="G9" s="120"/>
       <c r="H9" s="42"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
+      <c r="I9" s="42"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="3">
         <v>4</v>
       </c>
@@ -12913,10 +12939,13 @@
       <c r="F10" s="42">
         <v>28</v>
       </c>
-      <c r="G10" s="42"/>
+      <c r="G10" s="120">
+        <v>14</v>
+      </c>
       <c r="H10" s="42"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
+      <c r="I10" s="42"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -12933,10 +12962,11 @@
       <c r="F11" s="42">
         <v>35</v>
       </c>
-      <c r="G11" s="42"/>
+      <c r="G11" s="120"/>
       <c r="H11" s="42"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
+      <c r="I11" s="42"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="3">
         <v>6</v>
       </c>
@@ -12955,10 +12985,11 @@
       <c r="F12" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="42"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="42"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1">
+      <c r="I12" s="42"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="3">
         <v>7</v>
       </c>
@@ -12975,10 +13006,11 @@
       <c r="F13" s="42">
         <v>41</v>
       </c>
-      <c r="G13" s="42"/>
+      <c r="G13" s="120"/>
       <c r="H13" s="42"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
+      <c r="I13" s="42"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="3">
         <v>8</v>
       </c>
@@ -12995,10 +13027,11 @@
       <c r="F14" s="42">
         <v>35</v>
       </c>
-      <c r="G14" s="42"/>
+      <c r="G14" s="120"/>
       <c r="H14" s="42"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
+      <c r="I14" s="42"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="3">
         <v>9</v>
       </c>
@@ -13017,10 +13050,13 @@
       <c r="F15" s="42">
         <v>22</v>
       </c>
-      <c r="G15" s="42"/>
+      <c r="G15" s="120">
+        <v>20</v>
+      </c>
       <c r="H15" s="42"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
+      <c r="I15" s="42"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1">
       <c r="A16" s="3">
         <v>10</v>
       </c>
@@ -13037,10 +13073,11 @@
       <c r="F16" s="42">
         <v>27</v>
       </c>
-      <c r="G16" s="42"/>
+      <c r="G16" s="120"/>
       <c r="H16" s="42"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1">
+      <c r="I16" s="42"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1">
       <c r="A17" s="3">
         <v>11</v>
       </c>
@@ -13057,10 +13094,11 @@
       <c r="F17" s="42">
         <v>39</v>
       </c>
-      <c r="G17" s="42"/>
+      <c r="G17" s="120"/>
       <c r="H17" s="42"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1">
+      <c r="I17" s="42"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="3">
         <v>12</v>
       </c>
@@ -13079,10 +13117,11 @@
       <c r="F18" s="42">
         <v>25</v>
       </c>
-      <c r="G18" s="42"/>
+      <c r="G18" s="120"/>
       <c r="H18" s="42"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1">
+      <c r="I18" s="42"/>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="A19" s="3">
         <v>13</v>
       </c>
@@ -13099,10 +13138,11 @@
       <c r="F19" s="42">
         <v>29</v>
       </c>
-      <c r="G19" s="42"/>
+      <c r="G19" s="120"/>
       <c r="H19" s="42"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1">
+      <c r="I19" s="42"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1">
       <c r="A20" s="3">
         <v>14</v>
       </c>
@@ -13119,10 +13159,11 @@
       <c r="F20" s="42">
         <v>30</v>
       </c>
-      <c r="G20" s="42"/>
+      <c r="G20" s="120"/>
       <c r="H20" s="42"/>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1">
+      <c r="I20" s="42"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1">
       <c r="A21" s="3">
         <v>15</v>
       </c>
@@ -13141,10 +13182,13 @@
       <c r="F21" s="42">
         <v>21</v>
       </c>
-      <c r="G21" s="42"/>
+      <c r="G21" s="120">
+        <v>20</v>
+      </c>
       <c r="H21" s="42"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1">
+      <c r="I21" s="42"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1">
       <c r="A22" s="3">
         <v>16</v>
       </c>
@@ -13163,10 +13207,11 @@
       <c r="F22" s="42">
         <v>39</v>
       </c>
-      <c r="G22" s="42"/>
+      <c r="G22" s="120"/>
       <c r="H22" s="42"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1">
+      <c r="I22" s="42"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1">
       <c r="A23" s="3">
         <v>17</v>
       </c>
@@ -13185,10 +13230,11 @@
       <c r="F23" s="93">
         <v>26</v>
       </c>
-      <c r="G23" s="45"/>
+      <c r="G23" s="122"/>
       <c r="H23" s="45"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
+      <c r="I23" s="45"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1">
       <c r="A24" s="3">
         <v>18</v>
       </c>
@@ -13205,10 +13251,11 @@
       <c r="F24" s="42">
         <v>32</v>
       </c>
-      <c r="G24" s="42"/>
+      <c r="G24" s="120"/>
       <c r="H24" s="42"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1">
+      <c r="I24" s="42"/>
+    </row>
+    <row r="25" spans="1:9" ht="15" customHeight="1">
       <c r="A25" s="3">
         <v>19</v>
       </c>
@@ -13225,10 +13272,11 @@
       <c r="F25" s="42">
         <v>45</v>
       </c>
-      <c r="G25" s="42"/>
+      <c r="G25" s="120"/>
       <c r="H25" s="42"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1">
+      <c r="I25" s="42"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" customHeight="1">
       <c r="A26" s="3">
         <v>20</v>
       </c>
@@ -13245,10 +13293,11 @@
       <c r="F26" s="42">
         <v>45</v>
       </c>
-      <c r="G26" s="42"/>
+      <c r="G26" s="120"/>
       <c r="H26" s="42"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1">
+      <c r="I26" s="42"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" customHeight="1">
       <c r="A27" s="3">
         <v>21</v>
       </c>
@@ -13267,10 +13316,11 @@
       <c r="F27" s="42">
         <v>12</v>
       </c>
-      <c r="G27" s="42"/>
+      <c r="G27" s="120"/>
       <c r="H27" s="42"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1">
+      <c r="I27" s="42"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" customHeight="1">
       <c r="A28" s="3">
         <v>22</v>
       </c>
@@ -13287,10 +13337,11 @@
       <c r="F28" s="42">
         <v>32</v>
       </c>
-      <c r="G28" s="42"/>
+      <c r="G28" s="120"/>
       <c r="H28" s="42"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1">
+      <c r="I28" s="42"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" customHeight="1">
       <c r="A29" s="3">
         <v>23</v>
       </c>
@@ -13309,10 +13360,11 @@
       <c r="F29" s="42">
         <v>30</v>
       </c>
-      <c r="G29" s="42"/>
+      <c r="G29" s="120"/>
       <c r="H29" s="42"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1">
+      <c r="I29" s="42"/>
+    </row>
+    <row r="30" spans="1:9" ht="15" customHeight="1">
       <c r="A30" s="3">
         <v>24</v>
       </c>
@@ -13329,10 +13381,11 @@
       <c r="F30" s="42">
         <v>25</v>
       </c>
-      <c r="G30" s="42"/>
+      <c r="G30" s="120"/>
       <c r="H30" s="42"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1">
+      <c r="I30" s="42"/>
+    </row>
+    <row r="31" spans="1:9" ht="15" customHeight="1">
       <c r="A31" s="3">
         <v>25</v>
       </c>
@@ -13351,10 +13404,11 @@
       <c r="F31" s="42">
         <v>31</v>
       </c>
-      <c r="G31" s="42"/>
+      <c r="G31" s="120"/>
       <c r="H31" s="42"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1">
+      <c r="I31" s="42"/>
+    </row>
+    <row r="32" spans="1:9" ht="15" customHeight="1">
       <c r="A32" s="3">
         <v>26</v>
       </c>
@@ -13371,10 +13425,11 @@
       <c r="F32" s="42">
         <v>46</v>
       </c>
-      <c r="G32" s="42"/>
+      <c r="G32" s="120"/>
       <c r="H32" s="42"/>
-    </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1">
+      <c r="I32" s="42"/>
+    </row>
+    <row r="33" spans="1:9" ht="15" customHeight="1">
       <c r="A33" s="3">
         <v>27</v>
       </c>
@@ -13393,10 +13448,11 @@
       <c r="F33" s="42">
         <v>22</v>
       </c>
-      <c r="G33" s="42"/>
+      <c r="G33" s="120"/>
       <c r="H33" s="42"/>
-    </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1">
+      <c r="I33" s="42"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" customHeight="1">
       <c r="A34" s="3">
         <v>28</v>
       </c>
@@ -13413,10 +13469,11 @@
       <c r="F34" s="42">
         <v>44</v>
       </c>
-      <c r="G34" s="42"/>
+      <c r="G34" s="120"/>
       <c r="H34" s="42"/>
-    </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1">
+      <c r="I34" s="42"/>
+    </row>
+    <row r="35" spans="1:9" ht="15" customHeight="1">
       <c r="A35" s="3">
         <v>29</v>
       </c>
@@ -13433,10 +13490,11 @@
       <c r="F35" s="42">
         <v>37</v>
       </c>
-      <c r="G35" s="42"/>
+      <c r="G35" s="120"/>
       <c r="H35" s="42"/>
-    </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1">
+      <c r="I35" s="42"/>
+    </row>
+    <row r="36" spans="1:9" ht="15" customHeight="1">
       <c r="A36" s="3">
         <v>30</v>
       </c>
@@ -13455,10 +13513,11 @@
       <c r="F36" s="42">
         <v>17</v>
       </c>
-      <c r="G36" s="42"/>
+      <c r="G36" s="120"/>
       <c r="H36" s="42"/>
-    </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1">
+      <c r="I36" s="42"/>
+    </row>
+    <row r="37" spans="1:9" ht="15" customHeight="1">
       <c r="A37" s="3">
         <v>31</v>
       </c>
@@ -13475,10 +13534,11 @@
       <c r="F37" s="42">
         <v>43</v>
       </c>
-      <c r="G37" s="42"/>
+      <c r="G37" s="120"/>
       <c r="H37" s="42"/>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1">
+      <c r="I37" s="42"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" customHeight="1">
       <c r="A38" s="3">
         <v>32</v>
       </c>
@@ -13495,10 +13555,11 @@
       <c r="F38" s="42">
         <v>42</v>
       </c>
-      <c r="G38" s="42"/>
+      <c r="G38" s="120"/>
       <c r="H38" s="42"/>
-    </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1">
+      <c r="I38" s="42"/>
+    </row>
+    <row r="39" spans="1:9" ht="15" customHeight="1">
       <c r="A39" s="3">
         <v>33</v>
       </c>
@@ -13517,10 +13578,11 @@
       <c r="F39" s="42">
         <v>31</v>
       </c>
-      <c r="G39" s="42"/>
+      <c r="G39" s="120"/>
       <c r="H39" s="42"/>
-    </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1">
+      <c r="I39" s="42"/>
+    </row>
+    <row r="40" spans="1:9" ht="15" customHeight="1">
       <c r="A40" s="3">
         <v>34</v>
       </c>
@@ -13537,10 +13599,11 @@
       <c r="F40" s="42">
         <v>38</v>
       </c>
-      <c r="G40" s="42"/>
+      <c r="G40" s="120"/>
       <c r="H40" s="42"/>
-    </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1">
+      <c r="I40" s="42"/>
+    </row>
+    <row r="41" spans="1:9" ht="15" customHeight="1">
       <c r="A41" s="3">
         <v>35</v>
       </c>
@@ -13557,10 +13620,11 @@
       <c r="F41" s="42">
         <v>29</v>
       </c>
-      <c r="G41" s="42"/>
+      <c r="G41" s="120"/>
       <c r="H41" s="42"/>
-    </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1">
+      <c r="I41" s="42"/>
+    </row>
+    <row r="42" spans="1:9" ht="15" customHeight="1">
       <c r="A42" s="3">
         <v>36</v>
       </c>
@@ -13579,10 +13643,11 @@
       <c r="F42" s="42">
         <v>15</v>
       </c>
-      <c r="G42" s="42"/>
+      <c r="G42" s="120"/>
       <c r="H42" s="42"/>
-    </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1">
+      <c r="I42" s="42"/>
+    </row>
+    <row r="43" spans="1:9" ht="15" customHeight="1">
       <c r="A43" s="3">
         <v>37</v>
       </c>
@@ -13601,10 +13666,11 @@
       <c r="F43" s="42">
         <v>27</v>
       </c>
-      <c r="G43" s="42"/>
+      <c r="G43" s="120"/>
       <c r="H43" s="42"/>
-    </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1">
+      <c r="I43" s="42"/>
+    </row>
+    <row r="44" spans="1:9" ht="15" customHeight="1">
       <c r="A44" s="3">
         <v>38</v>
       </c>
@@ -13623,10 +13689,13 @@
       <c r="F44" s="42">
         <v>9</v>
       </c>
-      <c r="G44" s="42"/>
+      <c r="G44" s="120">
+        <v>20</v>
+      </c>
       <c r="H44" s="42"/>
-    </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1">
+      <c r="I44" s="42"/>
+    </row>
+    <row r="45" spans="1:9" ht="15" customHeight="1">
       <c r="A45" s="3">
         <v>39</v>
       </c>
@@ -13643,10 +13712,11 @@
       <c r="F45" s="42">
         <v>25</v>
       </c>
-      <c r="G45" s="42"/>
+      <c r="G45" s="120"/>
       <c r="H45" s="42"/>
-    </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1">
+      <c r="I45" s="42"/>
+    </row>
+    <row r="46" spans="1:9" ht="15" customHeight="1">
       <c r="A46" s="3">
         <v>40</v>
       </c>
@@ -13663,10 +13733,13 @@
       <c r="F46" s="42">
         <v>25</v>
       </c>
-      <c r="G46" s="42"/>
+      <c r="G46" s="120">
+        <v>20</v>
+      </c>
       <c r="H46" s="42"/>
-    </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1">
+      <c r="I46" s="42"/>
+    </row>
+    <row r="47" spans="1:9" ht="15" customHeight="1">
       <c r="A47" s="3">
         <v>41</v>
       </c>
@@ -13685,10 +13758,11 @@
       <c r="F47" s="42">
         <v>30</v>
       </c>
-      <c r="G47" s="42"/>
+      <c r="G47" s="120"/>
       <c r="H47" s="42"/>
-    </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1">
+      <c r="I47" s="42"/>
+    </row>
+    <row r="48" spans="1:9" ht="15" customHeight="1">
       <c r="A48" s="3">
         <v>42</v>
       </c>
@@ -13707,10 +13781,11 @@
       <c r="F48" s="42">
         <v>25</v>
       </c>
-      <c r="G48" s="42"/>
+      <c r="G48" s="120"/>
       <c r="H48" s="42"/>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48" s="42"/>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="3">
         <v>43</v>
       </c>
@@ -13727,10 +13802,11 @@
       <c r="F49" s="42">
         <v>34</v>
       </c>
-      <c r="G49" s="42"/>
+      <c r="G49" s="120"/>
       <c r="H49" s="42"/>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49" s="42"/>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="3">
         <v>44</v>
       </c>
@@ -13747,10 +13823,11 @@
       <c r="F50" s="42">
         <v>29</v>
       </c>
-      <c r="G50" s="42"/>
+      <c r="G50" s="120"/>
       <c r="H50" s="42"/>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50" s="42"/>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="3">
         <v>45</v>
       </c>
@@ -13767,10 +13844,11 @@
       <c r="F51" s="42">
         <v>17</v>
       </c>
-      <c r="G51" s="42"/>
+      <c r="G51" s="120"/>
       <c r="H51" s="42"/>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="I51" s="42"/>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="3">
         <v>46</v>
       </c>
@@ -13787,10 +13865,11 @@
       <c r="F52" s="42">
         <v>33</v>
       </c>
-      <c r="G52" s="42"/>
+      <c r="G52" s="120"/>
       <c r="H52" s="42"/>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="I52" s="42"/>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="3">
         <v>47</v>
       </c>
@@ -13807,10 +13886,11 @@
       <c r="F53" s="42">
         <v>29</v>
       </c>
-      <c r="G53" s="42"/>
+      <c r="G53" s="120"/>
       <c r="H53" s="42"/>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="I53" s="42"/>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="3">
         <v>48</v>
       </c>
@@ -13827,14 +13907,15 @@
       <c r="F54" s="42">
         <v>45</v>
       </c>
-      <c r="G54" s="42"/>
+      <c r="G54" s="120"/>
       <c r="H54" s="42"/>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="134" t="s">
+      <c r="I54" s="42"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="129" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="135"/>
+      <c r="B55" s="130"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -13846,14 +13927,15 @@
       <c r="F55" s="42">
         <v>40</v>
       </c>
-      <c r="G55" s="13"/>
+      <c r="G55" s="120"/>
       <c r="H55" s="13"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="132" t="s">
+      <c r="I55" s="13"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="126" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="133"/>
+      <c r="B56" s="127"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -13865,14 +13947,15 @@
       <c r="F56" s="42">
         <v>7</v>
       </c>
-      <c r="G56" s="13"/>
+      <c r="G56" s="120"/>
       <c r="H56" s="13"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="132" t="s">
+      <c r="I56" s="13"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="126" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="133"/>
+      <c r="B57" s="127"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -13884,14 +13967,15 @@
       <c r="F57" s="42">
         <v>1</v>
       </c>
-      <c r="G57" s="13"/>
+      <c r="G57" s="120"/>
       <c r="H57" s="13"/>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="132" t="s">
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="126" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="133"/>
+      <c r="B58" s="127"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -13903,20 +13987,12 @@
       <c r="F58" s="42">
         <v>85.1</v>
       </c>
-      <c r="G58" s="13"/>
+      <c r="G58" s="120"/>
       <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E1:H1"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A55:B55"/>
@@ -13924,9 +14000,18 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:H54">
-    <cfRule type="cellIs" dxfId="5" priority="17" operator="lessThan">
+  <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:I54">
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13957,72 +14042,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="150" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="150" t="s">
+      <c r="B1" s="150"/>
+      <c r="C1" s="149" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="150"/>
-      <c r="E1" s="151" t="s">
+      <c r="D1" s="149"/>
+      <c r="E1" s="157" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="152"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="158"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="150" t="s">
+      <c r="B2" s="147"/>
+      <c r="C2" s="149" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="150"/>
-      <c r="E2" s="131" t="s">
+      <c r="D2" s="149"/>
+      <c r="E2" s="145" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="149" t="s">
+      <c r="A3" s="148" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="149"/>
-      <c r="C3" s="150" t="s">
+      <c r="B3" s="148"/>
+      <c r="C3" s="149" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="150"/>
-      <c r="E3" s="131" t="s">
+      <c r="D3" s="149"/>
+      <c r="E3" s="145" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131"/>
-      <c r="H3" s="131"/>
+      <c r="F3" s="145"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="145"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="144" t="s">
+      <c r="A4" s="151" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="136" t="s">
+      <c r="B4" s="131" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="154" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="154"/>
-      <c r="E4" s="154"/>
-      <c r="F4" s="154"/>
-      <c r="G4" s="154"/>
-      <c r="H4" s="155"/>
+      <c r="D4" s="155"/>
+      <c r="E4" s="155"/>
+      <c r="F4" s="155"/>
+      <c r="G4" s="155"/>
+      <c r="H4" s="156"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="145"/>
-      <c r="B5" s="137"/>
+      <c r="A5" s="152"/>
+      <c r="B5" s="132"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -14043,8 +14128,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="146"/>
-      <c r="B6" s="138"/>
+      <c r="A6" s="153"/>
+      <c r="B6" s="133"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -15169,10 +15254,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="134" t="s">
+      <c r="A55" s="129" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="135"/>
+      <c r="B55" s="130"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -15187,10 +15272,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="132" t="s">
+      <c r="A56" s="126" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="133"/>
+      <c r="B56" s="127"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -15205,10 +15290,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="132" t="s">
+      <c r="A57" s="126" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="133"/>
+      <c r="B57" s="127"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -15223,10 +15308,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="132" t="s">
+      <c r="A58" s="126" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="133"/>
+      <c r="B58" s="127"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -15242,35 +15327,35 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15298,216 +15383,216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="122" t="s">
+      <c r="F1" s="141" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="130" t="s">
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="143"/>
+      <c r="J1" s="144" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
-      <c r="M1" s="130"/>
-      <c r="N1" s="162" t="s">
+      <c r="K1" s="144"/>
+      <c r="L1" s="144"/>
+      <c r="M1" s="144"/>
+      <c r="N1" s="159" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
+      <c r="O1" s="160"/>
+      <c r="P1" s="160"/>
+      <c r="Q1" s="160"/>
+      <c r="R1" s="160"/>
+      <c r="S1" s="160"/>
+      <c r="T1" s="160"/>
+      <c r="U1" s="160"/>
+      <c r="V1" s="160"/>
+      <c r="W1" s="160"/>
+      <c r="X1" s="160"/>
+      <c r="Y1" s="160"/>
+      <c r="Z1" s="160"/>
+      <c r="AA1" s="160"/>
+      <c r="AB1" s="160"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="134" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="140"/>
-      <c r="C2" s="141"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="136"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="125" t="s">
+      <c r="F2" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="130" t="s">
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="144" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="130"/>
-      <c r="L2" s="130"/>
-      <c r="M2" s="130"/>
-      <c r="N2" s="162" t="s">
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="M2" s="144"/>
+      <c r="N2" s="159" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="163"/>
-      <c r="U2" s="163"/>
-      <c r="V2" s="163"/>
-      <c r="W2" s="163"/>
-      <c r="X2" s="163"/>
-      <c r="Y2" s="163"/>
-      <c r="Z2" s="163"/>
-      <c r="AA2" s="163"/>
-      <c r="AB2" s="163"/>
+      <c r="O2" s="160"/>
+      <c r="P2" s="160"/>
+      <c r="Q2" s="160"/>
+      <c r="R2" s="160"/>
+      <c r="S2" s="160"/>
+      <c r="T2" s="160"/>
+      <c r="U2" s="160"/>
+      <c r="V2" s="160"/>
+      <c r="W2" s="160"/>
+      <c r="X2" s="160"/>
+      <c r="Y2" s="160"/>
+      <c r="Z2" s="160"/>
+      <c r="AA2" s="160"/>
+      <c r="AB2" s="160"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="162" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="167"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="164"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="164" t="s">
+      <c r="F3" s="161" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="164"/>
-      <c r="H3" s="164"/>
-      <c r="I3" s="164"/>
-      <c r="J3" s="173" t="s">
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="170" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="173"/>
-      <c r="L3" s="173"/>
-      <c r="M3" s="173"/>
-      <c r="N3" s="162" t="s">
+      <c r="K3" s="170"/>
+      <c r="L3" s="170"/>
+      <c r="M3" s="170"/>
+      <c r="N3" s="159" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="163"/>
-      <c r="P3" s="163"/>
-      <c r="Q3" s="163"/>
-      <c r="R3" s="163"/>
-      <c r="S3" s="163"/>
-      <c r="T3" s="163"/>
-      <c r="U3" s="163"/>
-      <c r="V3" s="163"/>
-      <c r="W3" s="163"/>
-      <c r="X3" s="163"/>
-      <c r="Y3" s="163"/>
-      <c r="Z3" s="163"/>
-      <c r="AA3" s="163"/>
-      <c r="AB3" s="163"/>
+      <c r="O3" s="160"/>
+      <c r="P3" s="160"/>
+      <c r="Q3" s="160"/>
+      <c r="R3" s="160"/>
+      <c r="S3" s="160"/>
+      <c r="T3" s="160"/>
+      <c r="U3" s="160"/>
+      <c r="V3" s="160"/>
+      <c r="W3" s="160"/>
+      <c r="X3" s="160"/>
+      <c r="Y3" s="160"/>
+      <c r="Z3" s="160"/>
+      <c r="AA3" s="160"/>
+      <c r="AB3" s="160"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="168"/>
-      <c r="B4" s="169"/>
-      <c r="C4" s="170"/>
-      <c r="D4" s="171">
+      <c r="A4" s="165"/>
+      <c r="B4" s="166"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="168">
         <v>43344</v>
       </c>
-      <c r="E4" s="172"/>
-      <c r="F4" s="172"/>
-      <c r="G4" s="172"/>
-      <c r="H4" s="172"/>
-      <c r="I4" s="172"/>
-      <c r="J4" s="172"/>
-      <c r="K4" s="172"/>
-      <c r="L4" s="172"/>
-      <c r="M4" s="172"/>
-      <c r="N4" s="171">
+      <c r="E4" s="169"/>
+      <c r="F4" s="169"/>
+      <c r="G4" s="169"/>
+      <c r="H4" s="169"/>
+      <c r="I4" s="169"/>
+      <c r="J4" s="169"/>
+      <c r="K4" s="169"/>
+      <c r="L4" s="169"/>
+      <c r="M4" s="169"/>
+      <c r="N4" s="168">
         <v>43374</v>
       </c>
-      <c r="O4" s="172"/>
-      <c r="P4" s="172"/>
-      <c r="Q4" s="172"/>
-      <c r="R4" s="172"/>
-      <c r="S4" s="172"/>
-      <c r="T4" s="172"/>
-      <c r="U4" s="172"/>
+      <c r="O4" s="169"/>
+      <c r="P4" s="169"/>
+      <c r="Q4" s="169"/>
+      <c r="R4" s="169"/>
+      <c r="S4" s="169"/>
+      <c r="T4" s="169"/>
+      <c r="U4" s="169"/>
       <c r="V4" s="53"/>
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="144" t="s">
+      <c r="A5" s="151" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="136" t="s">
+      <c r="B5" s="131" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="157" t="s">
+      <c r="D5" s="172" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="158"/>
-      <c r="F5" s="158"/>
-      <c r="G5" s="159"/>
-      <c r="H5" s="160" t="s">
+      <c r="E5" s="173"/>
+      <c r="F5" s="173"/>
+      <c r="G5" s="174"/>
+      <c r="H5" s="175" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="161"/>
-      <c r="J5" s="161"/>
-      <c r="K5" s="161"/>
-      <c r="L5" s="156" t="s">
+      <c r="I5" s="176"/>
+      <c r="J5" s="176"/>
+      <c r="K5" s="176"/>
+      <c r="L5" s="171" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="156"/>
-      <c r="N5" s="160" t="s">
+      <c r="M5" s="171"/>
+      <c r="N5" s="175" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="161"/>
-      <c r="P5" s="161"/>
-      <c r="Q5" s="161"/>
-      <c r="R5" s="156" t="s">
+      <c r="O5" s="176"/>
+      <c r="P5" s="176"/>
+      <c r="Q5" s="176"/>
+      <c r="R5" s="171" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="156"/>
-      <c r="T5" s="142" t="s">
+      <c r="S5" s="171"/>
+      <c r="T5" s="140" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="142"/>
-      <c r="V5" s="142" t="s">
+      <c r="U5" s="140"/>
+      <c r="V5" s="140" t="s">
         <v>117</v>
       </c>
-      <c r="W5" s="142"/>
-      <c r="X5" s="142"/>
-      <c r="Y5" s="142"/>
-      <c r="Z5" s="142" t="s">
+      <c r="W5" s="140"/>
+      <c r="X5" s="140"/>
+      <c r="Y5" s="140"/>
+      <c r="Z5" s="140" t="s">
         <v>118</v>
       </c>
-      <c r="AA5" s="142"/>
-      <c r="AB5" s="142"/>
-      <c r="AC5" s="142"/>
+      <c r="AA5" s="140"/>
+      <c r="AB5" s="140"/>
+      <c r="AC5" s="140"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="145"/>
-      <c r="B6" s="137"/>
+      <c r="A6" s="152"/>
+      <c r="B6" s="132"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -15594,8 +15679,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="145"/>
-      <c r="B7" s="137"/>
+      <c r="A7" s="152"/>
+      <c r="B7" s="132"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -15682,8 +15767,8 @@
       <c r="AF7" s="19"/>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="146"/>
-      <c r="B8" s="138"/>
+      <c r="A8" s="153"/>
+      <c r="B8" s="133"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -20090,10 +20175,10 @@
       <c r="AF56" s="19"/>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="134" t="s">
+      <c r="A57" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="135"/>
+      <c r="B57" s="130"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -20213,10 +20298,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="132" t="s">
+      <c r="A58" s="126" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="133"/>
+      <c r="B58" s="127"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -20337,6 +20422,18 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="N5:Q5"/>
     <mergeCell ref="N1:AB1"/>
     <mergeCell ref="N2:AB2"/>
     <mergeCell ref="N3:AB3"/>
@@ -20351,18 +20448,6 @@
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N4:U4"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="N5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -20388,28 +20473,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="178" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="179" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
+      <c r="B2" s="179"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="179" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
     </row>
     <row r="4" spans="1:4" s="83" customFormat="1" ht="28.5">
       <c r="A4" s="81" t="s">
@@ -21140,41 +21225,41 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="174" t="s">
+      <c r="A56" s="177" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="174"/>
-      <c r="C56" s="174"/>
+      <c r="B56" s="177"/>
+      <c r="C56" s="177"/>
       <c r="D56" s="75">
         <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="174" t="s">
+      <c r="A57" s="177" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="174"/>
-      <c r="C57" s="174"/>
+      <c r="B57" s="177"/>
+      <c r="C57" s="177"/>
       <c r="D57" s="76">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="174" t="s">
+      <c r="A58" s="177" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="174"/>
-      <c r="C58" s="174"/>
+      <c r="B58" s="177"/>
+      <c r="C58" s="177"/>
       <c r="D58" s="76">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="174" t="s">
+      <c r="A59" s="177" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="174"/>
-      <c r="C59" s="174"/>
+      <c r="B59" s="177"/>
+      <c r="C59" s="177"/>
       <c r="D59" s="76">
         <v>92</v>
       </c>
@@ -21220,7 +21305,7 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:C55 C8:C23">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21247,28 +21332,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="180" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="178" t="s">
+      <c r="A2" s="181" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="178"/>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
+      <c r="B2" s="181"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="181"/>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="178" t="s">
+      <c r="A3" s="181" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="178"/>
-      <c r="C3" s="178"/>
-      <c r="D3" s="178"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
     </row>
     <row r="4" spans="1:4" s="83" customFormat="1" ht="31.5">
       <c r="A4" s="103" t="s">
@@ -21999,41 +22084,41 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75">
-      <c r="A56" s="150" t="s">
+      <c r="A56" s="149" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="150"/>
-      <c r="C56" s="150"/>
+      <c r="B56" s="149"/>
+      <c r="C56" s="149"/>
       <c r="D56" s="115">
         <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75">
-      <c r="A57" s="150" t="s">
+      <c r="A57" s="149" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="150"/>
-      <c r="C57" s="150"/>
+      <c r="B57" s="149"/>
+      <c r="C57" s="149"/>
       <c r="D57" s="116">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75">
-      <c r="A58" s="150" t="s">
+      <c r="A58" s="149" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="150"/>
-      <c r="C58" s="150"/>
+      <c r="B58" s="149"/>
+      <c r="C58" s="149"/>
       <c r="D58" s="116">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75">
-      <c r="A59" s="150" t="s">
+      <c r="A59" s="149" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="150"/>
-      <c r="C59" s="150"/>
+      <c r="B59" s="149"/>
+      <c r="C59" s="149"/>
       <c r="D59" s="116">
         <v>85.1</v>
       </c>
@@ -22079,7 +22164,7 @@
     <mergeCell ref="A58:C58"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C55">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Last Update 14-11-2018 16:31:42.89
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -2576,6 +2576,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2585,14 +2606,17 @@
     <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2621,32 +2645,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2660,17 +2672,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2681,11 +2687,23 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2719,24 +2737,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3144,29 +3144,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="18.75">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="123" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="141" t="s">
+      <c r="F1" s="125" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="143"/>
-      <c r="J1" s="144" t="s">
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="133" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="144"/>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -3191,11 +3191,11 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:65" ht="19.5">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="142" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="135"/>
-      <c r="C2" s="136"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="144"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
@@ -3208,24 +3208,24 @@
       <c r="G2" s="128"/>
       <c r="H2" s="128"/>
       <c r="I2" s="128"/>
-      <c r="J2" s="144" t="s">
+      <c r="J2" s="133" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="144"/>
-      <c r="L2" s="144"/>
-      <c r="M2" s="144"/>
-      <c r="N2" s="145" t="s">
+      <c r="K2" s="133"/>
+      <c r="L2" s="133"/>
+      <c r="M2" s="133"/>
+      <c r="N2" s="134" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="145"/>
-      <c r="P2" s="145"/>
-      <c r="Q2" s="145"/>
-      <c r="R2" s="145"/>
-      <c r="S2" s="145"/>
-      <c r="T2" s="145"/>
-      <c r="U2" s="145"/>
-      <c r="V2" s="145"/>
-      <c r="W2" s="145"/>
+      <c r="O2" s="134"/>
+      <c r="P2" s="134"/>
+      <c r="Q2" s="134"/>
+      <c r="R2" s="134"/>
+      <c r="S2" s="134"/>
+      <c r="T2" s="134"/>
+      <c r="U2" s="134"/>
+      <c r="V2" s="134"/>
+      <c r="W2" s="134"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -3238,11 +3238,11 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:65" ht="18.75">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="123" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="138"/>
-      <c r="C3" s="139"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="129"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
@@ -3255,24 +3255,24 @@
       <c r="G3" s="128"/>
       <c r="H3" s="128"/>
       <c r="I3" s="128"/>
-      <c r="J3" s="144" t="s">
+      <c r="J3" s="133" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="145" t="s">
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
+      <c r="N3" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="145"/>
-      <c r="P3" s="145"/>
-      <c r="Q3" s="145"/>
-      <c r="R3" s="145"/>
-      <c r="S3" s="145"/>
-      <c r="T3" s="145"/>
-      <c r="U3" s="145"/>
-      <c r="V3" s="145"/>
-      <c r="W3" s="145"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
+      <c r="S3" s="134"/>
+      <c r="T3" s="134"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="134"/>
+      <c r="W3" s="134"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -3285,57 +3285,57 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:65" ht="18.75">
-      <c r="A4" s="137" t="s">
+      <c r="A4" s="123" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="138"/>
-      <c r="C4" s="139"/>
-      <c r="D4" s="123">
+      <c r="B4" s="124"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="130">
         <v>43344</v>
       </c>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="124"/>
-      <c r="M4" s="124"/>
-      <c r="N4" s="124"/>
-      <c r="O4" s="124"/>
-      <c r="P4" s="124"/>
-      <c r="Q4" s="124"/>
-      <c r="R4" s="124"/>
-      <c r="S4" s="124"/>
-      <c r="T4" s="124"/>
-      <c r="U4" s="124"/>
-      <c r="V4" s="124"/>
-      <c r="W4" s="125"/>
-      <c r="X4" s="123">
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="131"/>
+      <c r="L4" s="131"/>
+      <c r="M4" s="131"/>
+      <c r="N4" s="131"/>
+      <c r="O4" s="131"/>
+      <c r="P4" s="131"/>
+      <c r="Q4" s="131"/>
+      <c r="R4" s="131"/>
+      <c r="S4" s="131"/>
+      <c r="T4" s="131"/>
+      <c r="U4" s="131"/>
+      <c r="V4" s="131"/>
+      <c r="W4" s="132"/>
+      <c r="X4" s="130">
         <v>43374</v>
       </c>
-      <c r="Y4" s="124"/>
-      <c r="Z4" s="124"/>
-      <c r="AA4" s="124"/>
-      <c r="AB4" s="124"/>
-      <c r="AC4" s="124"/>
-      <c r="AD4" s="124"/>
-      <c r="AE4" s="124"/>
-      <c r="AF4" s="124"/>
-      <c r="AG4" s="124"/>
-      <c r="AH4" s="124"/>
-      <c r="AI4" s="124"/>
-      <c r="AJ4" s="124"/>
-      <c r="AK4" s="124"/>
-      <c r="AL4" s="124"/>
-      <c r="AM4" s="124"/>
-      <c r="AN4" s="124"/>
-      <c r="AO4" s="124"/>
-      <c r="AP4" s="124"/>
-      <c r="AQ4" s="124"/>
-      <c r="AR4" s="124"/>
-      <c r="AS4" s="125"/>
+      <c r="Y4" s="131"/>
+      <c r="Z4" s="131"/>
+      <c r="AA4" s="131"/>
+      <c r="AB4" s="131"/>
+      <c r="AC4" s="131"/>
+      <c r="AD4" s="131"/>
+      <c r="AE4" s="131"/>
+      <c r="AF4" s="131"/>
+      <c r="AG4" s="131"/>
+      <c r="AH4" s="131"/>
+      <c r="AI4" s="131"/>
+      <c r="AJ4" s="131"/>
+      <c r="AK4" s="131"/>
+      <c r="AL4" s="131"/>
+      <c r="AM4" s="131"/>
+      <c r="AN4" s="131"/>
+      <c r="AO4" s="131"/>
+      <c r="AP4" s="131"/>
+      <c r="AQ4" s="131"/>
+      <c r="AR4" s="131"/>
+      <c r="AS4" s="132"/>
       <c r="AT4" s="60"/>
       <c r="AU4" s="60"/>
       <c r="AV4" s="60"/>
@@ -3358,10 +3358,10 @@
       <c r="BM4" s="60"/>
     </row>
     <row r="5" spans="1:65">
-      <c r="A5" s="140" t="s">
+      <c r="A5" s="145" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="139" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -3533,8 +3533,8 @@
       <c r="BM5" s="60"/>
     </row>
     <row r="6" spans="1:65">
-      <c r="A6" s="140"/>
-      <c r="B6" s="132"/>
+      <c r="A6" s="145"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -3707,7 +3707,7 @@
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="133"/>
+      <c r="B7" s="141"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -12181,10 +12181,10 @@
       <c r="BM55" s="60"/>
     </row>
     <row r="56" spans="1:65">
-      <c r="A56" s="129" t="s">
+      <c r="A56" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="130"/>
+      <c r="B56" s="138"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -12436,10 +12436,10 @@
       </c>
     </row>
     <row r="57" spans="1:65">
-      <c r="A57" s="126" t="s">
+      <c r="A57" s="135" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="127"/>
+      <c r="B57" s="136"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -12692,6 +12692,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="X4:AS4"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F3:I3"/>
@@ -12702,14 +12710,6 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="X4:AS4"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -12721,8 +12721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -12738,76 +12738,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="146" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="149" t="s">
+      <c r="B1" s="146"/>
+      <c r="C1" s="153" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="149"/>
-      <c r="E1" s="145" t="s">
+      <c r="D1" s="153"/>
+      <c r="E1" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
     </row>
     <row r="2" spans="1:9" ht="19.5">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="151" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="149" t="s">
+      <c r="B2" s="151"/>
+      <c r="C2" s="153" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="149"/>
-      <c r="E2" s="145" t="s">
+      <c r="D2" s="153"/>
+      <c r="E2" s="134" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="145"/>
-      <c r="I2" s="145"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
     </row>
     <row r="3" spans="1:9" ht="17.25">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="152" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="148"/>
-      <c r="C3" s="149" t="s">
+      <c r="B3" s="152"/>
+      <c r="C3" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="149"/>
-      <c r="E3" s="145" t="s">
+      <c r="D3" s="153"/>
+      <c r="E3" s="134" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="145"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="151" t="s">
+      <c r="A4" s="147" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="146" t="s">
+      <c r="C4" s="150" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="146"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
+      <c r="D4" s="150"/>
+      <c r="E4" s="150"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="150"/>
+      <c r="H4" s="150"/>
+      <c r="I4" s="150"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="152"/>
-      <c r="B5" s="132"/>
+      <c r="A5" s="148"/>
+      <c r="B5" s="140"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -12831,8 +12831,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="153"/>
-      <c r="B6" s="133"/>
+      <c r="A6" s="149"/>
+      <c r="B6" s="141"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -13620,7 +13620,9 @@
       <c r="F41" s="42">
         <v>29</v>
       </c>
-      <c r="G41" s="120"/>
+      <c r="G41" s="120">
+        <v>18</v>
+      </c>
       <c r="H41" s="42"/>
       <c r="I41" s="42"/>
     </row>
@@ -13912,10 +13914,10 @@
       <c r="I54" s="42"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="129" t="s">
+      <c r="A55" s="137" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="130"/>
+      <c r="B55" s="138"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -13932,10 +13934,10 @@
       <c r="I55" s="13"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="126" t="s">
+      <c r="A56" s="135" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="127"/>
+      <c r="B56" s="136"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -13952,10 +13954,10 @@
       <c r="I56" s="13"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="126" t="s">
+      <c r="A57" s="135" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="127"/>
+      <c r="B57" s="136"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -13972,10 +13974,10 @@
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="126" t="s">
+      <c r="A58" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="127"/>
+      <c r="B58" s="136"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -13993,13 +13995,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -14009,9 +14004,16 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="E1:I1"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:I54">
-    <cfRule type="cellIs" dxfId="0" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="17" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14042,72 +14044,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="146" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="149" t="s">
+      <c r="B1" s="146"/>
+      <c r="C1" s="153" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="149"/>
-      <c r="E1" s="157" t="s">
+      <c r="D1" s="153"/>
+      <c r="E1" s="154" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="158"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="155"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="151" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="149" t="s">
+      <c r="B2" s="151"/>
+      <c r="C2" s="153" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="149"/>
-      <c r="E2" s="145" t="s">
+      <c r="D2" s="153"/>
+      <c r="E2" s="134" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="145"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="152" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="148"/>
-      <c r="C3" s="149" t="s">
+      <c r="B3" s="152"/>
+      <c r="C3" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="149"/>
-      <c r="E3" s="145" t="s">
+      <c r="D3" s="153"/>
+      <c r="E3" s="134" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="145"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="134"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="151" t="s">
+      <c r="A4" s="147" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="154" t="s">
+      <c r="C4" s="156" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="155"/>
-      <c r="E4" s="155"/>
-      <c r="F4" s="155"/>
-      <c r="G4" s="155"/>
-      <c r="H4" s="156"/>
+      <c r="D4" s="157"/>
+      <c r="E4" s="157"/>
+      <c r="F4" s="157"/>
+      <c r="G4" s="157"/>
+      <c r="H4" s="158"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="152"/>
-      <c r="B5" s="132"/>
+      <c r="A5" s="148"/>
+      <c r="B5" s="140"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -14128,8 +14130,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="153"/>
-      <c r="B6" s="133"/>
+      <c r="A6" s="149"/>
+      <c r="B6" s="141"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -15254,10 +15256,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="129" t="s">
+      <c r="A55" s="137" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="130"/>
+      <c r="B55" s="138"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -15272,10 +15274,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="126" t="s">
+      <c r="A56" s="135" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="127"/>
+      <c r="B56" s="136"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -15290,10 +15292,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="126" t="s">
+      <c r="A57" s="135" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="127"/>
+      <c r="B57" s="136"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -15308,10 +15310,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="126" t="s">
+      <c r="A58" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="127"/>
+      <c r="B58" s="136"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -15327,35 +15329,35 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15383,53 +15385,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="123" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="141" t="s">
+      <c r="F1" s="125" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="143"/>
-      <c r="J1" s="144" t="s">
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="133" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="144"/>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
-      <c r="N1" s="159" t="s">
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="165" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="160"/>
-      <c r="P1" s="160"/>
-      <c r="Q1" s="160"/>
-      <c r="R1" s="160"/>
-      <c r="S1" s="160"/>
-      <c r="T1" s="160"/>
-      <c r="U1" s="160"/>
-      <c r="V1" s="160"/>
-      <c r="W1" s="160"/>
-      <c r="X1" s="160"/>
-      <c r="Y1" s="160"/>
-      <c r="Z1" s="160"/>
-      <c r="AA1" s="160"/>
-      <c r="AB1" s="160"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
+      <c r="R1" s="166"/>
+      <c r="S1" s="166"/>
+      <c r="T1" s="166"/>
+      <c r="U1" s="166"/>
+      <c r="V1" s="166"/>
+      <c r="W1" s="166"/>
+      <c r="X1" s="166"/>
+      <c r="Y1" s="166"/>
+      <c r="Z1" s="166"/>
+      <c r="AA1" s="166"/>
+      <c r="AB1" s="166"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="142" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="135"/>
-      <c r="C2" s="136"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="144"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
@@ -15442,157 +15444,157 @@
       <c r="G2" s="128"/>
       <c r="H2" s="128"/>
       <c r="I2" s="128"/>
-      <c r="J2" s="144" t="s">
+      <c r="J2" s="133" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="144"/>
-      <c r="L2" s="144"/>
-      <c r="M2" s="144"/>
-      <c r="N2" s="159" t="s">
+      <c r="K2" s="133"/>
+      <c r="L2" s="133"/>
+      <c r="M2" s="133"/>
+      <c r="N2" s="165" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="160"/>
-      <c r="P2" s="160"/>
-      <c r="Q2" s="160"/>
-      <c r="R2" s="160"/>
-      <c r="S2" s="160"/>
-      <c r="T2" s="160"/>
-      <c r="U2" s="160"/>
-      <c r="V2" s="160"/>
-      <c r="W2" s="160"/>
-      <c r="X2" s="160"/>
-      <c r="Y2" s="160"/>
-      <c r="Z2" s="160"/>
-      <c r="AA2" s="160"/>
-      <c r="AB2" s="160"/>
+      <c r="O2" s="166"/>
+      <c r="P2" s="166"/>
+      <c r="Q2" s="166"/>
+      <c r="R2" s="166"/>
+      <c r="S2" s="166"/>
+      <c r="T2" s="166"/>
+      <c r="U2" s="166"/>
+      <c r="V2" s="166"/>
+      <c r="W2" s="166"/>
+      <c r="X2" s="166"/>
+      <c r="Y2" s="166"/>
+      <c r="Z2" s="166"/>
+      <c r="AA2" s="166"/>
+      <c r="AB2" s="166"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="162" t="s">
+      <c r="A3" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="163"/>
-      <c r="C3" s="164"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="170"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="161" t="s">
+      <c r="F3" s="167" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="170" t="s">
+      <c r="G3" s="167"/>
+      <c r="H3" s="167"/>
+      <c r="I3" s="167"/>
+      <c r="J3" s="176" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="170"/>
-      <c r="L3" s="170"/>
-      <c r="M3" s="170"/>
-      <c r="N3" s="159" t="s">
+      <c r="K3" s="176"/>
+      <c r="L3" s="176"/>
+      <c r="M3" s="176"/>
+      <c r="N3" s="165" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="160"/>
-      <c r="P3" s="160"/>
-      <c r="Q3" s="160"/>
-      <c r="R3" s="160"/>
-      <c r="S3" s="160"/>
-      <c r="T3" s="160"/>
-      <c r="U3" s="160"/>
-      <c r="V3" s="160"/>
-      <c r="W3" s="160"/>
-      <c r="X3" s="160"/>
-      <c r="Y3" s="160"/>
-      <c r="Z3" s="160"/>
-      <c r="AA3" s="160"/>
-      <c r="AB3" s="160"/>
+      <c r="O3" s="166"/>
+      <c r="P3" s="166"/>
+      <c r="Q3" s="166"/>
+      <c r="R3" s="166"/>
+      <c r="S3" s="166"/>
+      <c r="T3" s="166"/>
+      <c r="U3" s="166"/>
+      <c r="V3" s="166"/>
+      <c r="W3" s="166"/>
+      <c r="X3" s="166"/>
+      <c r="Y3" s="166"/>
+      <c r="Z3" s="166"/>
+      <c r="AA3" s="166"/>
+      <c r="AB3" s="166"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="165"/>
-      <c r="B4" s="166"/>
-      <c r="C4" s="167"/>
-      <c r="D4" s="168">
+      <c r="A4" s="171"/>
+      <c r="B4" s="172"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="174">
         <v>43344</v>
       </c>
-      <c r="E4" s="169"/>
-      <c r="F4" s="169"/>
-      <c r="G4" s="169"/>
-      <c r="H4" s="169"/>
-      <c r="I4" s="169"/>
-      <c r="J4" s="169"/>
-      <c r="K4" s="169"/>
-      <c r="L4" s="169"/>
-      <c r="M4" s="169"/>
-      <c r="N4" s="168">
+      <c r="E4" s="175"/>
+      <c r="F4" s="175"/>
+      <c r="G4" s="175"/>
+      <c r="H4" s="175"/>
+      <c r="I4" s="175"/>
+      <c r="J4" s="175"/>
+      <c r="K4" s="175"/>
+      <c r="L4" s="175"/>
+      <c r="M4" s="175"/>
+      <c r="N4" s="174">
         <v>43374</v>
       </c>
-      <c r="O4" s="169"/>
-      <c r="P4" s="169"/>
-      <c r="Q4" s="169"/>
-      <c r="R4" s="169"/>
-      <c r="S4" s="169"/>
-      <c r="T4" s="169"/>
-      <c r="U4" s="169"/>
+      <c r="O4" s="175"/>
+      <c r="P4" s="175"/>
+      <c r="Q4" s="175"/>
+      <c r="R4" s="175"/>
+      <c r="S4" s="175"/>
+      <c r="T4" s="175"/>
+      <c r="U4" s="175"/>
       <c r="V4" s="53"/>
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="151" t="s">
+      <c r="A5" s="147" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="139" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="172" t="s">
+      <c r="D5" s="160" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="173"/>
-      <c r="F5" s="173"/>
-      <c r="G5" s="174"/>
-      <c r="H5" s="175" t="s">
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="162"/>
+      <c r="H5" s="163" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="176"/>
-      <c r="J5" s="176"/>
-      <c r="K5" s="176"/>
-      <c r="L5" s="171" t="s">
+      <c r="I5" s="164"/>
+      <c r="J5" s="164"/>
+      <c r="K5" s="164"/>
+      <c r="L5" s="159" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="171"/>
-      <c r="N5" s="175" t="s">
+      <c r="M5" s="159"/>
+      <c r="N5" s="163" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="176"/>
-      <c r="P5" s="176"/>
-      <c r="Q5" s="176"/>
-      <c r="R5" s="171" t="s">
+      <c r="O5" s="164"/>
+      <c r="P5" s="164"/>
+      <c r="Q5" s="164"/>
+      <c r="R5" s="159" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="171"/>
-      <c r="T5" s="140" t="s">
+      <c r="S5" s="159"/>
+      <c r="T5" s="145" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="140"/>
-      <c r="V5" s="140" t="s">
+      <c r="U5" s="145"/>
+      <c r="V5" s="145" t="s">
         <v>117</v>
       </c>
-      <c r="W5" s="140"/>
-      <c r="X5" s="140"/>
-      <c r="Y5" s="140"/>
-      <c r="Z5" s="140" t="s">
+      <c r="W5" s="145"/>
+      <c r="X5" s="145"/>
+      <c r="Y5" s="145"/>
+      <c r="Z5" s="145" t="s">
         <v>118</v>
       </c>
-      <c r="AA5" s="140"/>
-      <c r="AB5" s="140"/>
-      <c r="AC5" s="140"/>
+      <c r="AA5" s="145"/>
+      <c r="AB5" s="145"/>
+      <c r="AC5" s="145"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="152"/>
-      <c r="B6" s="132"/>
+      <c r="A6" s="148"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -15679,8 +15681,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="152"/>
-      <c r="B7" s="132"/>
+      <c r="A7" s="148"/>
+      <c r="B7" s="140"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -15767,8 +15769,8 @@
       <c r="AF7" s="19"/>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="153"/>
-      <c r="B8" s="133"/>
+      <c r="A8" s="149"/>
+      <c r="B8" s="141"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -20175,10 +20177,10 @@
       <c r="AF56" s="19"/>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="129" t="s">
+      <c r="A57" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="130"/>
+      <c r="B57" s="138"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -20298,10 +20300,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="126" t="s">
+      <c r="A58" s="135" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="127"/>
+      <c r="B58" s="136"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -20422,18 +20424,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="N5:Q5"/>
     <mergeCell ref="N1:AB1"/>
     <mergeCell ref="N2:AB2"/>
     <mergeCell ref="N3:AB3"/>
@@ -20448,6 +20438,18 @@
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N4:U4"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="N5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -21305,7 +21307,7 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:C55 C8:C23">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22084,41 +22086,41 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75">
-      <c r="A56" s="149" t="s">
+      <c r="A56" s="153" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="149"/>
-      <c r="C56" s="149"/>
+      <c r="B56" s="153"/>
+      <c r="C56" s="153"/>
       <c r="D56" s="115">
         <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75">
-      <c r="A57" s="149" t="s">
+      <c r="A57" s="153" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="149"/>
-      <c r="C57" s="149"/>
+      <c r="B57" s="153"/>
+      <c r="C57" s="153"/>
       <c r="D57" s="116">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75">
-      <c r="A58" s="149" t="s">
+      <c r="A58" s="153" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="149"/>
-      <c r="C58" s="149"/>
+      <c r="B58" s="153"/>
+      <c r="C58" s="153"/>
       <c r="D58" s="116">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75">
-      <c r="A59" s="149" t="s">
+      <c r="A59" s="153" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="149"/>
-      <c r="C59" s="149"/>
+      <c r="B59" s="153"/>
+      <c r="C59" s="153"/>
       <c r="D59" s="116">
         <v>85.1</v>
       </c>
@@ -22164,7 +22166,7 @@
     <mergeCell ref="A58:C58"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C55">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Last Update 15-11-2018 15:56:48.19
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -993,6 +993,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="AZ7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Methods in Dictionary</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BA7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+File and I/O</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="BB7" authorId="0">
       <text>
         <r>
@@ -1014,6 +1062,56 @@
           </rPr>
           <t xml:space="preserve">
 File Modes and Operations</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BC7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Command Line Arguments</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BD7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Format Operator
+File Copy
+Shuttle</t>
         </r>
       </text>
     </comment>
@@ -1300,7 +1398,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4244" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4485" uniqueCount="170">
   <si>
     <t>S.NO</t>
   </si>
@@ -1808,6 +1906,9 @@
   <si>
     <t>Assignment</t>
   </si>
+  <si>
+    <t>Lab 7</t>
+  </si>
 </sst>
 </file>
 
@@ -2194,7 +2295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2574,6 +2675,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3126,11 +3233,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BM57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="Z29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BF2" sqref="BF2"/>
+      <selection pane="bottomRight" activeCell="BD46" sqref="BD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -3144,29 +3251,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="18.75">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="125" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="125" t="s">
+      <c r="F1" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="133" t="s">
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="135" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="133"/>
-      <c r="L1" s="133"/>
-      <c r="M1" s="133"/>
+      <c r="K1" s="135"/>
+      <c r="L1" s="135"/>
+      <c r="M1" s="135"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -3191,41 +3298,41 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:65" ht="19.5">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="144" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="144"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="146"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="128" t="s">
+      <c r="F2" s="130" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="133" t="s">
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="135" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="133"/>
-      <c r="L2" s="133"/>
-      <c r="M2" s="133"/>
-      <c r="N2" s="134" t="s">
+      <c r="K2" s="135"/>
+      <c r="L2" s="135"/>
+      <c r="M2" s="135"/>
+      <c r="N2" s="136" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="134"/>
-      <c r="P2" s="134"/>
-      <c r="Q2" s="134"/>
-      <c r="R2" s="134"/>
-      <c r="S2" s="134"/>
-      <c r="T2" s="134"/>
-      <c r="U2" s="134"/>
-      <c r="V2" s="134"/>
-      <c r="W2" s="134"/>
+      <c r="O2" s="136"/>
+      <c r="P2" s="136"/>
+      <c r="Q2" s="136"/>
+      <c r="R2" s="136"/>
+      <c r="S2" s="136"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="136"/>
+      <c r="V2" s="136"/>
+      <c r="W2" s="136"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -3238,41 +3345,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:65" ht="18.75">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="124"/>
-      <c r="C3" s="129"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="131"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="128" t="s">
+      <c r="F3" s="130" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="133" t="s">
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="135" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="133"/>
-      <c r="L3" s="133"/>
-      <c r="M3" s="133"/>
-      <c r="N3" s="134" t="s">
+      <c r="K3" s="135"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="135"/>
+      <c r="N3" s="136" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="134"/>
-      <c r="P3" s="134"/>
-      <c r="Q3" s="134"/>
-      <c r="R3" s="134"/>
-      <c r="S3" s="134"/>
-      <c r="T3" s="134"/>
-      <c r="U3" s="134"/>
-      <c r="V3" s="134"/>
-      <c r="W3" s="134"/>
+      <c r="O3" s="136"/>
+      <c r="P3" s="136"/>
+      <c r="Q3" s="136"/>
+      <c r="R3" s="136"/>
+      <c r="S3" s="136"/>
+      <c r="T3" s="136"/>
+      <c r="U3" s="136"/>
+      <c r="V3" s="136"/>
+      <c r="W3" s="136"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -3285,57 +3392,57 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:65" ht="18.75">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="125" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="124"/>
-      <c r="C4" s="129"/>
-      <c r="D4" s="130">
+      <c r="B4" s="126"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="132">
         <v>43344</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="131"/>
-      <c r="H4" s="131"/>
-      <c r="I4" s="131"/>
-      <c r="J4" s="131"/>
-      <c r="K4" s="131"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="131"/>
-      <c r="N4" s="131"/>
-      <c r="O4" s="131"/>
-      <c r="P4" s="131"/>
-      <c r="Q4" s="131"/>
-      <c r="R4" s="131"/>
-      <c r="S4" s="131"/>
-      <c r="T4" s="131"/>
-      <c r="U4" s="131"/>
-      <c r="V4" s="131"/>
-      <c r="W4" s="132"/>
-      <c r="X4" s="130">
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="133"/>
+      <c r="K4" s="133"/>
+      <c r="L4" s="133"/>
+      <c r="M4" s="133"/>
+      <c r="N4" s="133"/>
+      <c r="O4" s="133"/>
+      <c r="P4" s="133"/>
+      <c r="Q4" s="133"/>
+      <c r="R4" s="133"/>
+      <c r="S4" s="133"/>
+      <c r="T4" s="133"/>
+      <c r="U4" s="133"/>
+      <c r="V4" s="133"/>
+      <c r="W4" s="134"/>
+      <c r="X4" s="132">
         <v>43374</v>
       </c>
-      <c r="Y4" s="131"/>
-      <c r="Z4" s="131"/>
-      <c r="AA4" s="131"/>
-      <c r="AB4" s="131"/>
-      <c r="AC4" s="131"/>
-      <c r="AD4" s="131"/>
-      <c r="AE4" s="131"/>
-      <c r="AF4" s="131"/>
-      <c r="AG4" s="131"/>
-      <c r="AH4" s="131"/>
-      <c r="AI4" s="131"/>
-      <c r="AJ4" s="131"/>
-      <c r="AK4" s="131"/>
-      <c r="AL4" s="131"/>
-      <c r="AM4" s="131"/>
-      <c r="AN4" s="131"/>
-      <c r="AO4" s="131"/>
-      <c r="AP4" s="131"/>
-      <c r="AQ4" s="131"/>
-      <c r="AR4" s="131"/>
-      <c r="AS4" s="132"/>
+      <c r="Y4" s="133"/>
+      <c r="Z4" s="133"/>
+      <c r="AA4" s="133"/>
+      <c r="AB4" s="133"/>
+      <c r="AC4" s="133"/>
+      <c r="AD4" s="133"/>
+      <c r="AE4" s="133"/>
+      <c r="AF4" s="133"/>
+      <c r="AG4" s="133"/>
+      <c r="AH4" s="133"/>
+      <c r="AI4" s="133"/>
+      <c r="AJ4" s="133"/>
+      <c r="AK4" s="133"/>
+      <c r="AL4" s="133"/>
+      <c r="AM4" s="133"/>
+      <c r="AN4" s="133"/>
+      <c r="AO4" s="133"/>
+      <c r="AP4" s="133"/>
+      <c r="AQ4" s="133"/>
+      <c r="AR4" s="133"/>
+      <c r="AS4" s="134"/>
       <c r="AT4" s="60"/>
       <c r="AU4" s="60"/>
       <c r="AV4" s="60"/>
@@ -3358,10 +3465,10 @@
       <c r="BM4" s="60"/>
     </row>
     <row r="5" spans="1:65">
-      <c r="A5" s="145" t="s">
+      <c r="A5" s="147" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="141" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -3520,8 +3627,12 @@
       <c r="BB5" s="60">
         <v>11</v>
       </c>
-      <c r="BC5" s="60"/>
-      <c r="BD5" s="60"/>
+      <c r="BC5" s="60">
+        <v>11</v>
+      </c>
+      <c r="BD5" s="60">
+        <v>11</v>
+      </c>
       <c r="BE5" s="60"/>
       <c r="BF5" s="60"/>
       <c r="BG5" s="60"/>
@@ -3533,8 +3644,8 @@
       <c r="BM5" s="60"/>
     </row>
     <row r="6" spans="1:65">
-      <c r="A6" s="145"/>
-      <c r="B6" s="140"/>
+      <c r="A6" s="147"/>
+      <c r="B6" s="142"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -3691,8 +3802,12 @@
       <c r="BB6" s="60">
         <v>13</v>
       </c>
-      <c r="BC6" s="60"/>
-      <c r="BD6" s="60"/>
+      <c r="BC6" s="60">
+        <v>15</v>
+      </c>
+      <c r="BD6" s="60">
+        <v>15</v>
+      </c>
       <c r="BE6" s="60"/>
       <c r="BF6" s="60"/>
       <c r="BG6" s="60"/>
@@ -3707,7 +3822,7 @@
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="141"/>
+      <c r="B7" s="143"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -3864,8 +3979,12 @@
       <c r="BB7" s="60">
         <v>5</v>
       </c>
-      <c r="BC7" s="60"/>
-      <c r="BD7" s="60"/>
+      <c r="BC7" s="60">
+        <v>4</v>
+      </c>
+      <c r="BD7" s="60">
+        <v>7</v>
+      </c>
       <c r="BE7" s="60"/>
       <c r="BF7" s="60"/>
       <c r="BG7" s="60"/>
@@ -4037,8 +4156,12 @@
       <c r="BB8" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC8" s="60"/>
-      <c r="BD8" s="60"/>
+      <c r="BC8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD8" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BE8" s="60"/>
       <c r="BF8" s="60"/>
       <c r="BG8" s="60"/>
@@ -4210,8 +4333,12 @@
       <c r="BB9" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC9" s="60"/>
-      <c r="BD9" s="60"/>
+      <c r="BC9" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD9" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE9" s="60"/>
       <c r="BF9" s="60"/>
       <c r="BG9" s="60"/>
@@ -4383,8 +4510,12 @@
       <c r="BB10" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC10" s="60"/>
-      <c r="BD10" s="60"/>
+      <c r="BC10" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD10" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE10" s="60"/>
       <c r="BF10" s="60"/>
       <c r="BG10" s="60"/>
@@ -4556,8 +4687,12 @@
       <c r="BB11" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BC11" s="60"/>
-      <c r="BD11" s="60"/>
+      <c r="BC11" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD11" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE11" s="60"/>
       <c r="BF11" s="60"/>
       <c r="BG11" s="60"/>
@@ -4729,8 +4864,12 @@
       <c r="BB12" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC12" s="60"/>
-      <c r="BD12" s="60"/>
+      <c r="BC12" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD12" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE12" s="60"/>
       <c r="BF12" s="60"/>
       <c r="BG12" s="60"/>
@@ -4902,8 +5041,12 @@
       <c r="BB13" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BC13" s="60"/>
-      <c r="BD13" s="60"/>
+      <c r="BC13" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD13" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE13" s="60"/>
       <c r="BF13" s="60"/>
       <c r="BG13" s="60"/>
@@ -5075,8 +5218,12 @@
       <c r="BB14" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC14" s="60"/>
-      <c r="BD14" s="60"/>
+      <c r="BC14" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD14" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE14" s="60"/>
       <c r="BF14" s="60"/>
       <c r="BG14" s="60"/>
@@ -5248,8 +5395,12 @@
       <c r="BB15" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC15" s="60"/>
-      <c r="BD15" s="60"/>
+      <c r="BC15" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD15" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE15" s="60"/>
       <c r="BF15" s="60"/>
       <c r="BG15" s="60"/>
@@ -5421,8 +5572,12 @@
       <c r="BB16" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC16" s="60"/>
-      <c r="BD16" s="60"/>
+      <c r="BC16" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD16" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE16" s="60"/>
       <c r="BF16" s="60"/>
       <c r="BG16" s="60"/>
@@ -5594,8 +5749,12 @@
       <c r="BB17" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC17" s="60"/>
-      <c r="BD17" s="60"/>
+      <c r="BC17" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD17" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BE17" s="60"/>
       <c r="BF17" s="60"/>
       <c r="BG17" s="60"/>
@@ -5767,8 +5926,12 @@
       <c r="BB18" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC18" s="60"/>
-      <c r="BD18" s="60"/>
+      <c r="BC18" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD18" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE18" s="60"/>
       <c r="BF18" s="60"/>
       <c r="BG18" s="60"/>
@@ -5940,8 +6103,12 @@
       <c r="BB19" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC19" s="60"/>
-      <c r="BD19" s="60"/>
+      <c r="BC19" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD19" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE19" s="60"/>
       <c r="BF19" s="60"/>
       <c r="BG19" s="60"/>
@@ -6113,8 +6280,12 @@
       <c r="BB20" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC20" s="60"/>
-      <c r="BD20" s="60"/>
+      <c r="BC20" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD20" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE20" s="60"/>
       <c r="BF20" s="60"/>
       <c r="BG20" s="60"/>
@@ -6286,8 +6457,12 @@
       <c r="BB21" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC21" s="60"/>
-      <c r="BD21" s="60"/>
+      <c r="BC21" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD21" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE21" s="60"/>
       <c r="BF21" s="60"/>
       <c r="BG21" s="60"/>
@@ -6459,8 +6634,12 @@
       <c r="BB22" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC22" s="60"/>
-      <c r="BD22" s="60"/>
+      <c r="BC22" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD22" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE22" s="60"/>
       <c r="BF22" s="60"/>
       <c r="BG22" s="60"/>
@@ -6632,8 +6811,12 @@
       <c r="BB23" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC23" s="60"/>
-      <c r="BD23" s="60"/>
+      <c r="BC23" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD23" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE23" s="60"/>
       <c r="BF23" s="60"/>
       <c r="BG23" s="60"/>
@@ -6805,8 +6988,12 @@
       <c r="BB24" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BC24" s="60"/>
-      <c r="BD24" s="60"/>
+      <c r="BC24" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD24" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BE24" s="60"/>
       <c r="BF24" s="60"/>
       <c r="BG24" s="60"/>
@@ -6978,8 +7165,12 @@
       <c r="BB25" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC25" s="60"/>
-      <c r="BD25" s="60"/>
+      <c r="BC25" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD25" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE25" s="60"/>
       <c r="BF25" s="60"/>
       <c r="BG25" s="60"/>
@@ -7151,8 +7342,12 @@
       <c r="BB26" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC26" s="60"/>
-      <c r="BD26" s="60"/>
+      <c r="BC26" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD26" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BE26" s="60"/>
       <c r="BF26" s="60"/>
       <c r="BG26" s="60"/>
@@ -7324,8 +7519,12 @@
       <c r="BB27" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC27" s="60"/>
-      <c r="BD27" s="60"/>
+      <c r="BC27" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD27" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE27" s="60"/>
       <c r="BF27" s="60"/>
       <c r="BG27" s="60"/>
@@ -7497,8 +7696,12 @@
       <c r="BB28" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC28" s="60"/>
-      <c r="BD28" s="60"/>
+      <c r="BC28" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD28" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE28" s="60"/>
       <c r="BF28" s="60"/>
       <c r="BG28" s="60"/>
@@ -7670,8 +7873,12 @@
       <c r="BB29" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC29" s="60"/>
-      <c r="BD29" s="60"/>
+      <c r="BC29" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD29" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE29" s="60"/>
       <c r="BF29" s="60"/>
       <c r="BG29" s="60"/>
@@ -7843,8 +8050,12 @@
       <c r="BB30" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC30" s="60"/>
-      <c r="BD30" s="60"/>
+      <c r="BC30" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD30" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE30" s="60"/>
       <c r="BF30" s="60"/>
       <c r="BG30" s="60"/>
@@ -8016,8 +8227,12 @@
       <c r="BB31" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC31" s="60"/>
-      <c r="BD31" s="60"/>
+      <c r="BC31" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD31" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE31" s="60"/>
       <c r="BF31" s="60"/>
       <c r="BG31" s="60"/>
@@ -8189,8 +8404,12 @@
       <c r="BB32" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC32" s="60"/>
-      <c r="BD32" s="60"/>
+      <c r="BC32" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD32" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BE32" s="60"/>
       <c r="BF32" s="60"/>
       <c r="BG32" s="60"/>
@@ -8362,8 +8581,12 @@
       <c r="BB33" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC33" s="60"/>
-      <c r="BD33" s="60"/>
+      <c r="BC33" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD33" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE33" s="60"/>
       <c r="BF33" s="60"/>
       <c r="BG33" s="60"/>
@@ -8535,8 +8758,12 @@
       <c r="BB34" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC34" s="60"/>
-      <c r="BD34" s="60"/>
+      <c r="BC34" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD34" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE34" s="60"/>
       <c r="BF34" s="60"/>
       <c r="BG34" s="60"/>
@@ -8708,8 +8935,12 @@
       <c r="BB35" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC35" s="60"/>
-      <c r="BD35" s="60"/>
+      <c r="BC35" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD35" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE35" s="60"/>
       <c r="BF35" s="60"/>
       <c r="BG35" s="60"/>
@@ -8881,8 +9112,12 @@
       <c r="BB36" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC36" s="60"/>
-      <c r="BD36" s="60"/>
+      <c r="BC36" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD36" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE36" s="60"/>
       <c r="BF36" s="60"/>
       <c r="BG36" s="60"/>
@@ -9054,8 +9289,12 @@
       <c r="BB37" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC37" s="60"/>
-      <c r="BD37" s="60"/>
+      <c r="BC37" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD37" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE37" s="60"/>
       <c r="BF37" s="60"/>
       <c r="BG37" s="60"/>
@@ -9227,8 +9466,12 @@
       <c r="BB38" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC38" s="60"/>
-      <c r="BD38" s="60"/>
+      <c r="BC38" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD38" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE38" s="60"/>
       <c r="BF38" s="60"/>
       <c r="BG38" s="60"/>
@@ -9400,8 +9643,12 @@
       <c r="BB39" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC39" s="60"/>
-      <c r="BD39" s="60"/>
+      <c r="BC39" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD39" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE39" s="60"/>
       <c r="BF39" s="60"/>
       <c r="BG39" s="60"/>
@@ -9573,8 +9820,12 @@
       <c r="BB40" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BC40" s="60"/>
-      <c r="BD40" s="60"/>
+      <c r="BC40" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD40" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BE40" s="60"/>
       <c r="BF40" s="60"/>
       <c r="BG40" s="60"/>
@@ -9746,8 +9997,12 @@
       <c r="BB41" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC41" s="60"/>
-      <c r="BD41" s="60"/>
+      <c r="BC41" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD41" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE41" s="60"/>
       <c r="BF41" s="60"/>
       <c r="BG41" s="60"/>
@@ -9919,8 +10174,12 @@
       <c r="BB42" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC42" s="60"/>
-      <c r="BD42" s="60"/>
+      <c r="BC42" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD42" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE42" s="60"/>
       <c r="BF42" s="60"/>
       <c r="BG42" s="60"/>
@@ -10092,8 +10351,12 @@
       <c r="BB43" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC43" s="60"/>
-      <c r="BD43" s="60"/>
+      <c r="BC43" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD43" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE43" s="60"/>
       <c r="BF43" s="60"/>
       <c r="BG43" s="60"/>
@@ -10265,8 +10528,12 @@
       <c r="BB44" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC44" s="60"/>
-      <c r="BD44" s="60"/>
+      <c r="BC44" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD44" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE44" s="60"/>
       <c r="BF44" s="60"/>
       <c r="BG44" s="60"/>
@@ -10438,8 +10705,12 @@
       <c r="BB45" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC45" s="60"/>
-      <c r="BD45" s="60"/>
+      <c r="BC45" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD45" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE45" s="60"/>
       <c r="BF45" s="60"/>
       <c r="BG45" s="60"/>
@@ -10611,8 +10882,12 @@
       <c r="BB46" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BC46" s="60"/>
-      <c r="BD46" s="60"/>
+      <c r="BC46" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD46" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE46" s="60"/>
       <c r="BF46" s="60"/>
       <c r="BG46" s="60"/>
@@ -10784,8 +11059,12 @@
       <c r="BB47" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC47" s="60"/>
-      <c r="BD47" s="60"/>
+      <c r="BC47" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD47" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE47" s="60"/>
       <c r="BF47" s="60"/>
       <c r="BG47" s="60"/>
@@ -10957,8 +11236,12 @@
       <c r="BB48" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC48" s="60"/>
-      <c r="BD48" s="60"/>
+      <c r="BC48" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD48" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE48" s="60"/>
       <c r="BF48" s="60"/>
       <c r="BG48" s="60"/>
@@ -11130,8 +11413,12 @@
       <c r="BB49" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC49" s="60"/>
-      <c r="BD49" s="60"/>
+      <c r="BC49" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD49" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE49" s="60"/>
       <c r="BF49" s="60"/>
       <c r="BG49" s="60"/>
@@ -11303,8 +11590,12 @@
       <c r="BB50" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BC50" s="60"/>
-      <c r="BD50" s="60"/>
+      <c r="BC50" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD50" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE50" s="60"/>
       <c r="BF50" s="60"/>
       <c r="BG50" s="60"/>
@@ -11476,8 +11767,12 @@
       <c r="BB51" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BC51" s="60"/>
-      <c r="BD51" s="60"/>
+      <c r="BC51" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD51" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE51" s="60"/>
       <c r="BF51" s="60"/>
       <c r="BG51" s="60"/>
@@ -11649,8 +11944,12 @@
       <c r="BB52" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC52" s="60"/>
-      <c r="BD52" s="60"/>
+      <c r="BC52" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD52" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE52" s="60"/>
       <c r="BF52" s="60"/>
       <c r="BG52" s="60"/>
@@ -11822,8 +12121,12 @@
       <c r="BB53" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC53" s="60"/>
-      <c r="BD53" s="60"/>
+      <c r="BC53" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD53" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE53" s="60"/>
       <c r="BF53" s="60"/>
       <c r="BG53" s="60"/>
@@ -11995,8 +12298,12 @@
       <c r="BB54" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC54" s="60"/>
-      <c r="BD54" s="60"/>
+      <c r="BC54" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD54" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE54" s="60"/>
       <c r="BF54" s="60"/>
       <c r="BG54" s="60"/>
@@ -12168,8 +12475,12 @@
       <c r="BB55" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="BC55" s="60"/>
-      <c r="BD55" s="60"/>
+      <c r="BC55" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD55" s="124" t="s">
+        <v>54</v>
+      </c>
       <c r="BE55" s="60"/>
       <c r="BF55" s="60"/>
       <c r="BG55" s="60"/>
@@ -12181,10 +12492,10 @@
       <c r="BM55" s="60"/>
     </row>
     <row r="56" spans="1:65">
-      <c r="A56" s="137" t="s">
+      <c r="A56" s="139" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="138"/>
+      <c r="B56" s="140"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -12392,11 +12703,11 @@
       </c>
       <c r="BC56" s="60">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BD56" s="60">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BE56" s="60">
         <f t="shared" si="22"/>
@@ -12436,10 +12747,10 @@
       </c>
     </row>
     <row r="57" spans="1:65">
-      <c r="A57" s="135" t="s">
+      <c r="A57" s="137" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="136"/>
+      <c r="B57" s="138"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -12647,11 +12958,11 @@
       </c>
       <c r="BC57" s="60">
         <f t="shared" si="24"/>
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="BD57" s="60">
         <f t="shared" si="24"/>
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="BE57" s="60">
         <f t="shared" si="24"/>
@@ -12721,7 +13032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
@@ -12738,76 +13049,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="148" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="153" t="s">
+      <c r="B1" s="148"/>
+      <c r="C1" s="155" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="153"/>
-      <c r="E1" s="134" t="s">
+      <c r="D1" s="155"/>
+      <c r="E1" s="136" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
     </row>
     <row r="2" spans="1:9" ht="19.5">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="153" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="153" t="s">
+      <c r="B2" s="153"/>
+      <c r="C2" s="155" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="153"/>
-      <c r="E2" s="134" t="s">
+      <c r="D2" s="155"/>
+      <c r="E2" s="136" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
     </row>
     <row r="3" spans="1:9" ht="17.25">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="154" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="152"/>
-      <c r="C3" s="153" t="s">
+      <c r="B3" s="154"/>
+      <c r="C3" s="155" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="153"/>
-      <c r="E3" s="134" t="s">
+      <c r="D3" s="155"/>
+      <c r="E3" s="136" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="147" t="s">
+      <c r="A4" s="149" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="141" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="150" t="s">
+      <c r="C4" s="152" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="150"/>
-      <c r="E4" s="150"/>
-      <c r="F4" s="150"/>
-      <c r="G4" s="150"/>
-      <c r="H4" s="150"/>
-      <c r="I4" s="150"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="152"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="148"/>
-      <c r="B5" s="140"/>
+      <c r="A5" s="150"/>
+      <c r="B5" s="142"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -12831,8 +13142,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="149"/>
-      <c r="B6" s="141"/>
+      <c r="A6" s="151"/>
+      <c r="B6" s="143"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -13914,10 +14225,10 @@
       <c r="I54" s="42"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="137" t="s">
+      <c r="A55" s="139" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="138"/>
+      <c r="B55" s="140"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -13934,10 +14245,10 @@
       <c r="I55" s="13"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="135" t="s">
+      <c r="A56" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="136"/>
+      <c r="B56" s="138"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -13954,10 +14265,10 @@
       <c r="I56" s="13"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="135" t="s">
+      <c r="A57" s="137" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="136"/>
+      <c r="B57" s="138"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -13974,10 +14285,10 @@
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="135" t="s">
+      <c r="A58" s="137" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="136"/>
+      <c r="B58" s="138"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -14044,72 +14355,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="148" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="153" t="s">
+      <c r="B1" s="148"/>
+      <c r="C1" s="155" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="153"/>
-      <c r="E1" s="154" t="s">
+      <c r="D1" s="155"/>
+      <c r="E1" s="156" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="155"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
+      <c r="H1" s="157"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="153" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="153" t="s">
+      <c r="B2" s="153"/>
+      <c r="C2" s="155" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="153"/>
-      <c r="E2" s="134" t="s">
+      <c r="D2" s="155"/>
+      <c r="E2" s="136" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="154" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="152"/>
-      <c r="C3" s="153" t="s">
+      <c r="B3" s="154"/>
+      <c r="C3" s="155" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="153"/>
-      <c r="E3" s="134" t="s">
+      <c r="D3" s="155"/>
+      <c r="E3" s="136" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="147" t="s">
+      <c r="A4" s="149" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="141" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="156" t="s">
+      <c r="C4" s="158" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="157"/>
-      <c r="E4" s="157"/>
-      <c r="F4" s="157"/>
-      <c r="G4" s="157"/>
-      <c r="H4" s="158"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="159"/>
+      <c r="F4" s="159"/>
+      <c r="G4" s="159"/>
+      <c r="H4" s="160"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="148"/>
-      <c r="B5" s="140"/>
+      <c r="A5" s="150"/>
+      <c r="B5" s="142"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -14130,8 +14441,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="149"/>
-      <c r="B6" s="141"/>
+      <c r="A6" s="151"/>
+      <c r="B6" s="143"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -15256,10 +15567,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="137" t="s">
+      <c r="A55" s="139" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="138"/>
+      <c r="B55" s="140"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -15274,10 +15585,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="135" t="s">
+      <c r="A56" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="136"/>
+      <c r="B56" s="138"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -15292,10 +15603,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="135" t="s">
+      <c r="A57" s="137" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="136"/>
+      <c r="B57" s="138"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -15310,10 +15621,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="135" t="s">
+      <c r="A58" s="137" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="136"/>
+      <c r="B58" s="138"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -15370,8 +15681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF58"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AI3" sqref="AI3"/>
+    <sheetView topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="AI8" sqref="AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -15385,216 +15696,221 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="125" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="125" t="s">
+      <c r="F1" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="133" t="s">
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="135" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="133"/>
-      <c r="L1" s="133"/>
-      <c r="M1" s="133"/>
-      <c r="N1" s="165" t="s">
+      <c r="K1" s="135"/>
+      <c r="L1" s="135"/>
+      <c r="M1" s="135"/>
+      <c r="N1" s="167" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
-      <c r="U1" s="166"/>
-      <c r="V1" s="166"/>
-      <c r="W1" s="166"/>
-      <c r="X1" s="166"/>
-      <c r="Y1" s="166"/>
-      <c r="Z1" s="166"/>
-      <c r="AA1" s="166"/>
-      <c r="AB1" s="166"/>
+      <c r="O1" s="168"/>
+      <c r="P1" s="168"/>
+      <c r="Q1" s="168"/>
+      <c r="R1" s="168"/>
+      <c r="S1" s="168"/>
+      <c r="T1" s="168"/>
+      <c r="U1" s="168"/>
+      <c r="V1" s="168"/>
+      <c r="W1" s="168"/>
+      <c r="X1" s="168"/>
+      <c r="Y1" s="168"/>
+      <c r="Z1" s="168"/>
+      <c r="AA1" s="168"/>
+      <c r="AB1" s="168"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="144" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="144"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="146"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="128" t="s">
+      <c r="F2" s="130" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="133" t="s">
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="135" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="133"/>
-      <c r="L2" s="133"/>
-      <c r="M2" s="133"/>
-      <c r="N2" s="165" t="s">
+      <c r="K2" s="135"/>
+      <c r="L2" s="135"/>
+      <c r="M2" s="135"/>
+      <c r="N2" s="167" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="166"/>
-      <c r="P2" s="166"/>
-      <c r="Q2" s="166"/>
-      <c r="R2" s="166"/>
-      <c r="S2" s="166"/>
-      <c r="T2" s="166"/>
-      <c r="U2" s="166"/>
-      <c r="V2" s="166"/>
-      <c r="W2" s="166"/>
-      <c r="X2" s="166"/>
-      <c r="Y2" s="166"/>
-      <c r="Z2" s="166"/>
-      <c r="AA2" s="166"/>
-      <c r="AB2" s="166"/>
+      <c r="O2" s="168"/>
+      <c r="P2" s="168"/>
+      <c r="Q2" s="168"/>
+      <c r="R2" s="168"/>
+      <c r="S2" s="168"/>
+      <c r="T2" s="168"/>
+      <c r="U2" s="168"/>
+      <c r="V2" s="168"/>
+      <c r="W2" s="168"/>
+      <c r="X2" s="168"/>
+      <c r="Y2" s="168"/>
+      <c r="Z2" s="168"/>
+      <c r="AA2" s="168"/>
+      <c r="AB2" s="168"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="170"/>
+      <c r="B3" s="171"/>
+      <c r="C3" s="172"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="167" t="s">
+      <c r="F3" s="169" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="167"/>
-      <c r="H3" s="167"/>
-      <c r="I3" s="167"/>
-      <c r="J3" s="176" t="s">
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="178" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="176"/>
-      <c r="N3" s="165" t="s">
+      <c r="K3" s="178"/>
+      <c r="L3" s="178"/>
+      <c r="M3" s="178"/>
+      <c r="N3" s="167" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="166"/>
-      <c r="P3" s="166"/>
-      <c r="Q3" s="166"/>
-      <c r="R3" s="166"/>
-      <c r="S3" s="166"/>
-      <c r="T3" s="166"/>
-      <c r="U3" s="166"/>
-      <c r="V3" s="166"/>
-      <c r="W3" s="166"/>
-      <c r="X3" s="166"/>
-      <c r="Y3" s="166"/>
-      <c r="Z3" s="166"/>
-      <c r="AA3" s="166"/>
-      <c r="AB3" s="166"/>
+      <c r="O3" s="168"/>
+      <c r="P3" s="168"/>
+      <c r="Q3" s="168"/>
+      <c r="R3" s="168"/>
+      <c r="S3" s="168"/>
+      <c r="T3" s="168"/>
+      <c r="U3" s="168"/>
+      <c r="V3" s="168"/>
+      <c r="W3" s="168"/>
+      <c r="X3" s="168"/>
+      <c r="Y3" s="168"/>
+      <c r="Z3" s="168"/>
+      <c r="AA3" s="168"/>
+      <c r="AB3" s="168"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="171"/>
-      <c r="B4" s="172"/>
-      <c r="C4" s="173"/>
-      <c r="D4" s="174">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="175"/>
+      <c r="D4" s="176">
         <v>43344</v>
       </c>
-      <c r="E4" s="175"/>
-      <c r="F4" s="175"/>
-      <c r="G4" s="175"/>
-      <c r="H4" s="175"/>
-      <c r="I4" s="175"/>
-      <c r="J4" s="175"/>
-      <c r="K4" s="175"/>
-      <c r="L4" s="175"/>
-      <c r="M4" s="175"/>
-      <c r="N4" s="174">
+      <c r="E4" s="177"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="177"/>
+      <c r="H4" s="177"/>
+      <c r="I4" s="177"/>
+      <c r="J4" s="177"/>
+      <c r="K4" s="177"/>
+      <c r="L4" s="177"/>
+      <c r="M4" s="177"/>
+      <c r="N4" s="176">
         <v>43374</v>
       </c>
-      <c r="O4" s="175"/>
-      <c r="P4" s="175"/>
-      <c r="Q4" s="175"/>
-      <c r="R4" s="175"/>
-      <c r="S4" s="175"/>
-      <c r="T4" s="175"/>
-      <c r="U4" s="175"/>
+      <c r="O4" s="177"/>
+      <c r="P4" s="177"/>
+      <c r="Q4" s="177"/>
+      <c r="R4" s="177"/>
+      <c r="S4" s="177"/>
+      <c r="T4" s="177"/>
+      <c r="U4" s="177"/>
       <c r="V4" s="53"/>
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="147" t="s">
+      <c r="A5" s="149" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="141" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="160" t="s">
+      <c r="D5" s="162" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="161"/>
-      <c r="F5" s="161"/>
-      <c r="G5" s="162"/>
-      <c r="H5" s="163" t="s">
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="164"/>
+      <c r="H5" s="165" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="164"/>
-      <c r="J5" s="164"/>
-      <c r="K5" s="164"/>
-      <c r="L5" s="159" t="s">
+      <c r="I5" s="166"/>
+      <c r="J5" s="166"/>
+      <c r="K5" s="166"/>
+      <c r="L5" s="161" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="159"/>
-      <c r="N5" s="163" t="s">
+      <c r="M5" s="161"/>
+      <c r="N5" s="165" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="164"/>
-      <c r="P5" s="164"/>
-      <c r="Q5" s="164"/>
-      <c r="R5" s="159" t="s">
+      <c r="O5" s="166"/>
+      <c r="P5" s="166"/>
+      <c r="Q5" s="166"/>
+      <c r="R5" s="161" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="159"/>
-      <c r="T5" s="145" t="s">
+      <c r="S5" s="161"/>
+      <c r="T5" s="147" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="145"/>
-      <c r="V5" s="145" t="s">
+      <c r="U5" s="147"/>
+      <c r="V5" s="147" t="s">
         <v>117</v>
       </c>
-      <c r="W5" s="145"/>
-      <c r="X5" s="145"/>
-      <c r="Y5" s="145"/>
-      <c r="Z5" s="145" t="s">
+      <c r="W5" s="147"/>
+      <c r="X5" s="147"/>
+      <c r="Y5" s="147"/>
+      <c r="Z5" s="147" t="s">
         <v>118</v>
       </c>
-      <c r="AA5" s="145"/>
-      <c r="AB5" s="145"/>
-      <c r="AC5" s="145"/>
+      <c r="AA5" s="147"/>
+      <c r="AB5" s="147"/>
+      <c r="AC5" s="147"/>
+      <c r="AD5" s="147" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE5" s="147"/>
+      <c r="AF5" s="147"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="148"/>
-      <c r="B6" s="140"/>
+      <c r="A6" s="150"/>
+      <c r="B6" s="142"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -15676,13 +15992,19 @@
       <c r="AC6" s="95">
         <v>11</v>
       </c>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="19"/>
-      <c r="AF6" s="19"/>
+      <c r="AD6" s="19">
+        <v>11</v>
+      </c>
+      <c r="AE6" s="19">
+        <v>11</v>
+      </c>
+      <c r="AF6" s="19">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="148"/>
-      <c r="B7" s="140"/>
+      <c r="A7" s="150"/>
+      <c r="B7" s="142"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -15764,13 +16086,19 @@
       <c r="AC7" s="95">
         <v>8</v>
       </c>
-      <c r="AD7" s="19"/>
-      <c r="AE7" s="19"/>
-      <c r="AF7" s="19"/>
+      <c r="AD7" s="19">
+        <v>15</v>
+      </c>
+      <c r="AE7" s="19">
+        <v>15</v>
+      </c>
+      <c r="AF7" s="19">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="149"/>
-      <c r="B8" s="141"/>
+      <c r="A8" s="151"/>
+      <c r="B8" s="143"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -15852,9 +16180,15 @@
       <c r="AC8" s="95">
         <v>4</v>
       </c>
-      <c r="AD8" s="19"/>
-      <c r="AE8" s="19"/>
-      <c r="AF8" s="19"/>
+      <c r="AD8" s="19">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="19">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="19">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:32" ht="15" customHeight="1">
       <c r="A9" s="3">
@@ -15942,9 +16276,15 @@
       <c r="AC9" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AD9" s="19"/>
-      <c r="AE9" s="19"/>
-      <c r="AF9" s="19"/>
+      <c r="AD9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF9" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="10" spans="1:32" ht="15" customHeight="1">
       <c r="A10" s="3">
@@ -16032,9 +16372,15 @@
       <c r="AC10" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD10" s="19"/>
-      <c r="AE10" s="19"/>
-      <c r="AF10" s="19"/>
+      <c r="AD10" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE10" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF10" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="11" spans="1:32" ht="15" customHeight="1">
       <c r="A11" s="3">
@@ -16122,9 +16468,15 @@
       <c r="AC11" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD11" s="19"/>
-      <c r="AE11" s="19"/>
-      <c r="AF11" s="19"/>
+      <c r="AD11" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE11" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF11" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="12" spans="1:32" ht="15" customHeight="1">
       <c r="A12" s="3">
@@ -16212,9 +16564,15 @@
       <c r="AC12" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD12" s="19"/>
-      <c r="AE12" s="19"/>
-      <c r="AF12" s="19"/>
+      <c r="AD12" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE12" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF12" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="13" spans="1:32" ht="15" customHeight="1">
       <c r="A13" s="3">
@@ -16302,9 +16660,15 @@
       <c r="AC13" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD13" s="19"/>
-      <c r="AE13" s="19"/>
-      <c r="AF13" s="19"/>
+      <c r="AD13" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE13" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF13" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:32" ht="15" customHeight="1">
       <c r="A14" s="3">
@@ -16392,9 +16756,15 @@
       <c r="AC14" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD14" s="19"/>
-      <c r="AE14" s="19"/>
-      <c r="AF14" s="19"/>
+      <c r="AD14" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE14" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF14" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="15" spans="1:32" ht="15" customHeight="1">
       <c r="A15" s="3">
@@ -16482,9 +16852,15 @@
       <c r="AC15" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD15" s="19"/>
-      <c r="AE15" s="19"/>
-      <c r="AF15" s="19"/>
+      <c r="AD15" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE15" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF15" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="16" spans="1:32" ht="15" customHeight="1">
       <c r="A16" s="3">
@@ -16572,9 +16948,15 @@
       <c r="AC16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AD16" s="19"/>
-      <c r="AE16" s="19"/>
-      <c r="AF16" s="19"/>
+      <c r="AD16" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE16" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF16" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="17" spans="1:32" ht="15" customHeight="1">
       <c r="A17" s="3">
@@ -16662,9 +17044,15 @@
       <c r="AC17" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD17" s="19"/>
-      <c r="AE17" s="19"/>
-      <c r="AF17" s="19"/>
+      <c r="AD17" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE17" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF17" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="18" spans="1:32" ht="15" customHeight="1">
       <c r="A18" s="3">
@@ -16752,9 +17140,15 @@
       <c r="AC18" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD18" s="19"/>
-      <c r="AE18" s="19"/>
-      <c r="AF18" s="19"/>
+      <c r="AD18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF18" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="19" spans="1:32" ht="15" customHeight="1">
       <c r="A19" s="3">
@@ -16842,9 +17236,15 @@
       <c r="AC19" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AD19" s="19"/>
-      <c r="AE19" s="19"/>
-      <c r="AF19" s="19"/>
+      <c r="AD19" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE19" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF19" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="20" spans="1:32" ht="15" customHeight="1">
       <c r="A20" s="3">
@@ -16932,9 +17332,15 @@
       <c r="AC20" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD20" s="19"/>
-      <c r="AE20" s="19"/>
-      <c r="AF20" s="19"/>
+      <c r="AD20" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE20" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF20" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="21" spans="1:32" ht="15" customHeight="1">
       <c r="A21" s="3">
@@ -17022,9 +17428,15 @@
       <c r="AC21" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AD21" s="19"/>
-      <c r="AE21" s="19"/>
-      <c r="AF21" s="19"/>
+      <c r="AD21" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE21" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF21" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="22" spans="1:32" ht="15" customHeight="1">
       <c r="A22" s="3">
@@ -17112,9 +17524,15 @@
       <c r="AC22" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD22" s="19"/>
-      <c r="AE22" s="19"/>
-      <c r="AF22" s="19"/>
+      <c r="AD22" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE22" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF22" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="23" spans="1:32" ht="15" customHeight="1">
       <c r="A23" s="3">
@@ -17202,9 +17620,15 @@
       <c r="AC23" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AD23" s="19"/>
-      <c r="AE23" s="19"/>
-      <c r="AF23" s="19"/>
+      <c r="AD23" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE23" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF23" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="24" spans="1:32" ht="15" customHeight="1">
       <c r="A24" s="3">
@@ -17292,9 +17716,15 @@
       <c r="AC24" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD24" s="19"/>
-      <c r="AE24" s="19"/>
-      <c r="AF24" s="19"/>
+      <c r="AD24" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE24" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF24" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="25" spans="1:32" ht="15" customHeight="1">
       <c r="A25" s="3">
@@ -17382,9 +17812,15 @@
       <c r="AC25" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD25" s="19"/>
-      <c r="AE25" s="19"/>
-      <c r="AF25" s="19"/>
+      <c r="AD25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF25" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="1:32" ht="15" customHeight="1">
       <c r="A26" s="3">
@@ -17472,9 +17908,15 @@
       <c r="AC26" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD26" s="19"/>
-      <c r="AE26" s="19"/>
-      <c r="AF26" s="19"/>
+      <c r="AD26" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE26" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF26" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="27" spans="1:32" ht="15" customHeight="1">
       <c r="A27" s="3">
@@ -17562,9 +18004,15 @@
       <c r="AC27" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AD27" s="19"/>
-      <c r="AE27" s="19"/>
-      <c r="AF27" s="19"/>
+      <c r="AD27" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE27" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF27" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="28" spans="1:32" ht="15" customHeight="1">
       <c r="A28" s="3">
@@ -17652,9 +18100,15 @@
       <c r="AC28" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD28" s="19"/>
-      <c r="AE28" s="19"/>
-      <c r="AF28" s="19"/>
+      <c r="AD28" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE28" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF28" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="29" spans="1:32" ht="15" customHeight="1">
       <c r="A29" s="3">
@@ -17742,9 +18196,15 @@
       <c r="AC29" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD29" s="19"/>
-      <c r="AE29" s="19"/>
-      <c r="AF29" s="19"/>
+      <c r="AD29" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE29" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF29" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="30" spans="1:32" ht="15" customHeight="1">
       <c r="A30" s="3">
@@ -17832,9 +18292,15 @@
       <c r="AC30" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD30" s="19"/>
-      <c r="AE30" s="19"/>
-      <c r="AF30" s="19"/>
+      <c r="AD30" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE30" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF30" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="31" spans="1:32" ht="15" customHeight="1">
       <c r="A31" s="3">
@@ -17922,9 +18388,15 @@
       <c r="AC31" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD31" s="19"/>
-      <c r="AE31" s="19"/>
-      <c r="AF31" s="19"/>
+      <c r="AD31" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE31" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF31" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="32" spans="1:32" ht="15" customHeight="1">
       <c r="A32" s="3">
@@ -18012,9 +18484,15 @@
       <c r="AC32" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD32" s="19"/>
-      <c r="AE32" s="19"/>
-      <c r="AF32" s="19"/>
+      <c r="AD32" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE32" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF32" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="33" spans="1:32" ht="15" customHeight="1">
       <c r="A33" s="3">
@@ -18102,9 +18580,15 @@
       <c r="AC33" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AD33" s="19"/>
-      <c r="AE33" s="19"/>
-      <c r="AF33" s="19"/>
+      <c r="AD33" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE33" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF33" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="34" spans="1:32" ht="15" customHeight="1">
       <c r="A34" s="3">
@@ -18192,9 +18676,15 @@
       <c r="AC34" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD34" s="19"/>
-      <c r="AE34" s="19"/>
-      <c r="AF34" s="19"/>
+      <c r="AD34" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE34" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF34" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="35" spans="1:32" ht="15" customHeight="1">
       <c r="A35" s="3">
@@ -18282,9 +18772,15 @@
       <c r="AC35" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AD35" s="19"/>
-      <c r="AE35" s="19"/>
-      <c r="AF35" s="19"/>
+      <c r="AD35" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE35" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF35" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="1:32" ht="15" customHeight="1">
       <c r="A36" s="3">
@@ -18372,9 +18868,15 @@
       <c r="AC36" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD36" s="19"/>
-      <c r="AE36" s="19"/>
-      <c r="AF36" s="19"/>
+      <c r="AD36" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE36" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF36" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="37" spans="1:32" ht="15" customHeight="1">
       <c r="A37" s="3">
@@ -18462,9 +18964,15 @@
       <c r="AC37" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD37" s="19"/>
-      <c r="AE37" s="19"/>
-      <c r="AF37" s="19"/>
+      <c r="AD37" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE37" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF37" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="38" spans="1:32" ht="15" customHeight="1">
       <c r="A38" s="3">
@@ -18552,9 +19060,15 @@
       <c r="AC38" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD38" s="19"/>
-      <c r="AE38" s="19"/>
-      <c r="AF38" s="19"/>
+      <c r="AD38" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE38" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF38" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="39" spans="1:32" ht="15" customHeight="1">
       <c r="A39" s="3">
@@ -18642,9 +19156,15 @@
       <c r="AC39" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD39" s="19"/>
-      <c r="AE39" s="19"/>
-      <c r="AF39" s="19"/>
+      <c r="AD39" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE39" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF39" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="40" spans="1:32" ht="15" customHeight="1">
       <c r="A40" s="3">
@@ -18732,9 +19252,15 @@
       <c r="AC40" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD40" s="19"/>
-      <c r="AE40" s="19"/>
-      <c r="AF40" s="19"/>
+      <c r="AD40" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE40" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF40" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="41" spans="1:32" ht="15" customHeight="1">
       <c r="A41" s="3">
@@ -18822,9 +19348,15 @@
       <c r="AC41" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD41" s="19"/>
-      <c r="AE41" s="19"/>
-      <c r="AF41" s="19"/>
+      <c r="AD41" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE41" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF41" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="42" spans="1:32" ht="15" customHeight="1">
       <c r="A42" s="3">
@@ -18912,9 +19444,15 @@
       <c r="AC42" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD42" s="19"/>
-      <c r="AE42" s="19"/>
-      <c r="AF42" s="19"/>
+      <c r="AD42" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE42" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF42" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="43" spans="1:32" ht="15" customHeight="1">
       <c r="A43" s="3">
@@ -19002,9 +19540,15 @@
       <c r="AC43" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD43" s="19"/>
-      <c r="AE43" s="19"/>
-      <c r="AF43" s="19"/>
+      <c r="AD43" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE43" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF43" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="44" spans="1:32" ht="15" customHeight="1">
       <c r="A44" s="3">
@@ -19092,9 +19636,15 @@
       <c r="AC44" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD44" s="19"/>
-      <c r="AE44" s="19"/>
-      <c r="AF44" s="19"/>
+      <c r="AD44" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE44" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF44" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="45" spans="1:32" ht="15" customHeight="1">
       <c r="A45" s="3">
@@ -19182,9 +19732,15 @@
       <c r="AC45" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD45" s="19"/>
-      <c r="AE45" s="19"/>
-      <c r="AF45" s="19"/>
+      <c r="AD45" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE45" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF45" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="46" spans="1:32" ht="15" customHeight="1">
       <c r="A46" s="3">
@@ -19272,9 +19828,15 @@
       <c r="AC46" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD46" s="19"/>
-      <c r="AE46" s="19"/>
-      <c r="AF46" s="19"/>
+      <c r="AD46" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE46" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF46" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="47" spans="1:32" ht="15" customHeight="1">
       <c r="A47" s="3">
@@ -19362,9 +19924,15 @@
       <c r="AC47" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD47" s="19"/>
-      <c r="AE47" s="19"/>
-      <c r="AF47" s="19"/>
+      <c r="AD47" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE47" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF47" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="48" spans="1:32" ht="15" customHeight="1">
       <c r="A48" s="3">
@@ -19452,9 +20020,15 @@
       <c r="AC48" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD48" s="19"/>
-      <c r="AE48" s="19"/>
-      <c r="AF48" s="19"/>
+      <c r="AD48" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE48" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF48" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="49" spans="1:32" ht="15" customHeight="1">
       <c r="A49" s="3">
@@ -19542,9 +20116,15 @@
       <c r="AC49" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AD49" s="19"/>
-      <c r="AE49" s="19"/>
-      <c r="AF49" s="19"/>
+      <c r="AD49" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE49" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF49" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="50" spans="1:32" ht="15" customHeight="1">
       <c r="A50" s="3">
@@ -19632,9 +20212,15 @@
       <c r="AC50" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD50" s="19"/>
-      <c r="AE50" s="19"/>
-      <c r="AF50" s="19"/>
+      <c r="AD50" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE50" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF50" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="51" spans="1:32" ht="15" customHeight="1">
       <c r="A51" s="3">
@@ -19722,9 +20308,15 @@
       <c r="AC51" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD51" s="19"/>
-      <c r="AE51" s="19"/>
-      <c r="AF51" s="19"/>
+      <c r="AD51" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE51" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF51" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="52" spans="1:32" ht="15" customHeight="1">
       <c r="A52" s="3">
@@ -19812,9 +20404,15 @@
       <c r="AC52" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD52" s="19"/>
-      <c r="AE52" s="19"/>
-      <c r="AF52" s="19"/>
+      <c r="AD52" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE52" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF52" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="53" spans="1:32" ht="15" customHeight="1">
       <c r="A53" s="3">
@@ -19902,9 +20500,15 @@
       <c r="AC53" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD53" s="19"/>
-      <c r="AE53" s="19"/>
-      <c r="AF53" s="19"/>
+      <c r="AD53" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE53" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF53" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="54" spans="1:32" ht="15" customHeight="1">
       <c r="A54" s="3">
@@ -19992,9 +20596,15 @@
       <c r="AC54" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD54" s="19"/>
-      <c r="AE54" s="19"/>
-      <c r="AF54" s="19"/>
+      <c r="AD54" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE54" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF54" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="55" spans="1:32" ht="15" customHeight="1">
       <c r="A55" s="3">
@@ -20082,9 +20692,15 @@
       <c r="AC55" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD55" s="19"/>
-      <c r="AE55" s="19"/>
-      <c r="AF55" s="19"/>
+      <c r="AD55" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE55" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF55" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="56" spans="1:32" ht="15" customHeight="1">
       <c r="A56" s="3">
@@ -20172,15 +20788,21 @@
       <c r="AC56" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="AD56" s="19"/>
-      <c r="AE56" s="19"/>
-      <c r="AF56" s="19"/>
+      <c r="AD56" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE56" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF56" s="123" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="137" t="s">
+      <c r="A57" s="139" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="138"/>
+      <c r="B57" s="140"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -20288,22 +20910,22 @@
       </c>
       <c r="AD57" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AE57" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AF57" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="135" t="s">
+      <c r="A58" s="137" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="136"/>
+      <c r="B58" s="138"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -20411,19 +21033,19 @@
       </c>
       <c r="AD58" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="AE58" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="AF58" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="27">
     <mergeCell ref="N1:AB1"/>
     <mergeCell ref="N2:AB2"/>
     <mergeCell ref="N3:AB3"/>
@@ -20438,15 +21060,16 @@
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N4:U4"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="B5:B8"/>
+    <mergeCell ref="AD5:AF5"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A57:B57"/>
     <mergeCell ref="T5:U5"/>
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="N5:Q5"/>
@@ -20475,28 +21098,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="180" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="179" t="s">
+      <c r="A2" s="181" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="179"/>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
+      <c r="B2" s="181"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="181"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="179" t="s">
+      <c r="A3" s="181" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="179"/>
-      <c r="C3" s="179"/>
-      <c r="D3" s="179"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
     </row>
     <row r="4" spans="1:4" s="83" customFormat="1" ht="28.5">
       <c r="A4" s="81" t="s">
@@ -21227,41 +21850,41 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="177" t="s">
+      <c r="A56" s="179" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="177"/>
-      <c r="C56" s="177"/>
+      <c r="B56" s="179"/>
+      <c r="C56" s="179"/>
       <c r="D56" s="75">
         <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="177" t="s">
+      <c r="A57" s="179" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="177"/>
-      <c r="C57" s="177"/>
+      <c r="B57" s="179"/>
+      <c r="C57" s="179"/>
       <c r="D57" s="76">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="177" t="s">
+      <c r="A58" s="179" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="177"/>
-      <c r="C58" s="177"/>
+      <c r="B58" s="179"/>
+      <c r="C58" s="179"/>
       <c r="D58" s="76">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="177" t="s">
+      <c r="A59" s="179" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="177"/>
-      <c r="C59" s="177"/>
+      <c r="B59" s="179"/>
+      <c r="C59" s="179"/>
       <c r="D59" s="76">
         <v>92</v>
       </c>
@@ -21334,28 +21957,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="180" t="s">
+      <c r="A1" s="182" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="181" t="s">
+      <c r="A2" s="183" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="181"/>
-      <c r="C2" s="181"/>
-      <c r="D2" s="181"/>
+      <c r="B2" s="183"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="181" t="s">
+      <c r="A3" s="183" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="181"/>
+      <c r="B3" s="183"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="183"/>
     </row>
     <row r="4" spans="1:4" s="83" customFormat="1" ht="31.5">
       <c r="A4" s="103" t="s">
@@ -22086,41 +22709,41 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75">
-      <c r="A56" s="153" t="s">
+      <c r="A56" s="155" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="153"/>
-      <c r="C56" s="153"/>
+      <c r="B56" s="155"/>
+      <c r="C56" s="155"/>
       <c r="D56" s="115">
         <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75">
-      <c r="A57" s="153" t="s">
+      <c r="A57" s="155" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="153"/>
-      <c r="C57" s="153"/>
+      <c r="B57" s="155"/>
+      <c r="C57" s="155"/>
       <c r="D57" s="116">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75">
-      <c r="A58" s="153" t="s">
+      <c r="A58" s="155" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="153"/>
-      <c r="C58" s="153"/>
+      <c r="B58" s="155"/>
+      <c r="C58" s="155"/>
       <c r="D58" s="116">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75">
-      <c r="A59" s="153" t="s">
+      <c r="A59" s="155" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="153"/>
-      <c r="C59" s="153"/>
+      <c r="B59" s="155"/>
+      <c r="C59" s="155"/>
       <c r="D59" s="116">
         <v>85.1</v>
       </c>

</xml_diff>

<commit_message>
Last Update 16-11-2018 13:39:30.79
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -1398,7 +1398,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4485" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4533" uniqueCount="170">
   <si>
     <t>S.NO</t>
   </si>
@@ -2295,7 +2295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2683,26 +2683,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2713,17 +2695,14 @@
     <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2752,8 +2731,44 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2767,24 +2782,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2794,23 +2791,11 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2844,6 +2829,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3234,10 +3237,10 @@
   <dimension ref="A1:BM57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="Z29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="Z37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BD46" sqref="BD46"/>
+      <selection pane="bottomRight" activeCell="BJ40" sqref="BJ40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -3251,29 +3254,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="18.75">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="127" t="s">
+      <c r="F1" s="144" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="135" t="s">
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="147" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="135"/>
-      <c r="L1" s="135"/>
-      <c r="M1" s="135"/>
+      <c r="K1" s="147"/>
+      <c r="L1" s="147"/>
+      <c r="M1" s="147"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -3298,41 +3301,41 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:65" ht="19.5">
-      <c r="A2" s="144" t="s">
+      <c r="A2" s="137" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="145"/>
-      <c r="C2" s="146"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="139"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="130" t="s">
+      <c r="F2" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="135" t="s">
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="135"/>
-      <c r="L2" s="135"/>
-      <c r="M2" s="135"/>
-      <c r="N2" s="136" t="s">
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
+      <c r="M2" s="147"/>
+      <c r="N2" s="148" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="136"/>
-      <c r="P2" s="136"/>
-      <c r="Q2" s="136"/>
-      <c r="R2" s="136"/>
-      <c r="S2" s="136"/>
-      <c r="T2" s="136"/>
-      <c r="U2" s="136"/>
-      <c r="V2" s="136"/>
-      <c r="W2" s="136"/>
+      <c r="O2" s="148"/>
+      <c r="P2" s="148"/>
+      <c r="Q2" s="148"/>
+      <c r="R2" s="148"/>
+      <c r="S2" s="148"/>
+      <c r="T2" s="148"/>
+      <c r="U2" s="148"/>
+      <c r="V2" s="148"/>
+      <c r="W2" s="148"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -3345,41 +3348,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:65" ht="18.75">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="140" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="131"/>
+      <c r="B3" s="141"/>
+      <c r="C3" s="142"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="130" t="s">
+      <c r="F3" s="131" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="135" t="s">
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="147" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="136" t="s">
+      <c r="K3" s="147"/>
+      <c r="L3" s="147"/>
+      <c r="M3" s="147"/>
+      <c r="N3" s="148" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="136"/>
-      <c r="P3" s="136"/>
-      <c r="Q3" s="136"/>
-      <c r="R3" s="136"/>
-      <c r="S3" s="136"/>
-      <c r="T3" s="136"/>
-      <c r="U3" s="136"/>
-      <c r="V3" s="136"/>
-      <c r="W3" s="136"/>
+      <c r="O3" s="148"/>
+      <c r="P3" s="148"/>
+      <c r="Q3" s="148"/>
+      <c r="R3" s="148"/>
+      <c r="S3" s="148"/>
+      <c r="T3" s="148"/>
+      <c r="U3" s="148"/>
+      <c r="V3" s="148"/>
+      <c r="W3" s="148"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -3392,57 +3395,57 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:65" ht="18.75">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="140" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="126"/>
-      <c r="C4" s="131"/>
-      <c r="D4" s="132">
+      <c r="B4" s="141"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="126">
         <v>43344</v>
       </c>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="133"/>
-      <c r="M4" s="133"/>
-      <c r="N4" s="133"/>
-      <c r="O4" s="133"/>
-      <c r="P4" s="133"/>
-      <c r="Q4" s="133"/>
-      <c r="R4" s="133"/>
-      <c r="S4" s="133"/>
-      <c r="T4" s="133"/>
-      <c r="U4" s="133"/>
-      <c r="V4" s="133"/>
-      <c r="W4" s="134"/>
-      <c r="X4" s="132">
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="127"/>
+      <c r="M4" s="127"/>
+      <c r="N4" s="127"/>
+      <c r="O4" s="127"/>
+      <c r="P4" s="127"/>
+      <c r="Q4" s="127"/>
+      <c r="R4" s="127"/>
+      <c r="S4" s="127"/>
+      <c r="T4" s="127"/>
+      <c r="U4" s="127"/>
+      <c r="V4" s="127"/>
+      <c r="W4" s="128"/>
+      <c r="X4" s="126">
         <v>43374</v>
       </c>
-      <c r="Y4" s="133"/>
-      <c r="Z4" s="133"/>
-      <c r="AA4" s="133"/>
-      <c r="AB4" s="133"/>
-      <c r="AC4" s="133"/>
-      <c r="AD4" s="133"/>
-      <c r="AE4" s="133"/>
-      <c r="AF4" s="133"/>
-      <c r="AG4" s="133"/>
-      <c r="AH4" s="133"/>
-      <c r="AI4" s="133"/>
-      <c r="AJ4" s="133"/>
-      <c r="AK4" s="133"/>
-      <c r="AL4" s="133"/>
-      <c r="AM4" s="133"/>
-      <c r="AN4" s="133"/>
-      <c r="AO4" s="133"/>
-      <c r="AP4" s="133"/>
-      <c r="AQ4" s="133"/>
-      <c r="AR4" s="133"/>
-      <c r="AS4" s="134"/>
+      <c r="Y4" s="127"/>
+      <c r="Z4" s="127"/>
+      <c r="AA4" s="127"/>
+      <c r="AB4" s="127"/>
+      <c r="AC4" s="127"/>
+      <c r="AD4" s="127"/>
+      <c r="AE4" s="127"/>
+      <c r="AF4" s="127"/>
+      <c r="AG4" s="127"/>
+      <c r="AH4" s="127"/>
+      <c r="AI4" s="127"/>
+      <c r="AJ4" s="127"/>
+      <c r="AK4" s="127"/>
+      <c r="AL4" s="127"/>
+      <c r="AM4" s="127"/>
+      <c r="AN4" s="127"/>
+      <c r="AO4" s="127"/>
+      <c r="AP4" s="127"/>
+      <c r="AQ4" s="127"/>
+      <c r="AR4" s="127"/>
+      <c r="AS4" s="128"/>
       <c r="AT4" s="60"/>
       <c r="AU4" s="60"/>
       <c r="AV4" s="60"/>
@@ -3465,10 +3468,10 @@
       <c r="BM4" s="60"/>
     </row>
     <row r="5" spans="1:65">
-      <c r="A5" s="147" t="s">
+      <c r="A5" s="143" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="134" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -3633,7 +3636,9 @@
       <c r="BD5" s="60">
         <v>11</v>
       </c>
-      <c r="BE5" s="60"/>
+      <c r="BE5" s="60">
+        <v>11</v>
+      </c>
       <c r="BF5" s="60"/>
       <c r="BG5" s="60"/>
       <c r="BH5" s="60"/>
@@ -3644,8 +3649,8 @@
       <c r="BM5" s="60"/>
     </row>
     <row r="6" spans="1:65">
-      <c r="A6" s="147"/>
-      <c r="B6" s="142"/>
+      <c r="A6" s="143"/>
+      <c r="B6" s="135"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -3808,7 +3813,9 @@
       <c r="BD6" s="60">
         <v>15</v>
       </c>
-      <c r="BE6" s="60"/>
+      <c r="BE6" s="60">
+        <v>16</v>
+      </c>
       <c r="BF6" s="60"/>
       <c r="BG6" s="60"/>
       <c r="BH6" s="60"/>
@@ -3822,7 +3829,7 @@
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="143"/>
+      <c r="B7" s="136"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -3985,7 +3992,9 @@
       <c r="BD7" s="60">
         <v>7</v>
       </c>
-      <c r="BE7" s="60"/>
+      <c r="BE7" s="60">
+        <v>5</v>
+      </c>
       <c r="BF7" s="60"/>
       <c r="BG7" s="60"/>
       <c r="BH7" s="60"/>
@@ -4162,7 +4171,9 @@
       <c r="BD8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BE8" s="60"/>
+      <c r="BE8" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF8" s="60"/>
       <c r="BG8" s="60"/>
       <c r="BH8" s="60"/>
@@ -4339,7 +4350,9 @@
       <c r="BD9" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE9" s="60"/>
+      <c r="BE9" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF9" s="60"/>
       <c r="BG9" s="60"/>
       <c r="BH9" s="60"/>
@@ -4516,7 +4529,9 @@
       <c r="BD10" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE10" s="60"/>
+      <c r="BE10" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF10" s="60"/>
       <c r="BG10" s="60"/>
       <c r="BH10" s="60"/>
@@ -4693,7 +4708,9 @@
       <c r="BD11" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE11" s="60"/>
+      <c r="BE11" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF11" s="60"/>
       <c r="BG11" s="60"/>
       <c r="BH11" s="60"/>
@@ -4870,7 +4887,9 @@
       <c r="BD12" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE12" s="60"/>
+      <c r="BE12" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF12" s="60"/>
       <c r="BG12" s="60"/>
       <c r="BH12" s="60"/>
@@ -5047,7 +5066,9 @@
       <c r="BD13" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE13" s="60"/>
+      <c r="BE13" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF13" s="60"/>
       <c r="BG13" s="60"/>
       <c r="BH13" s="60"/>
@@ -5224,7 +5245,9 @@
       <c r="BD14" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE14" s="60"/>
+      <c r="BE14" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF14" s="60"/>
       <c r="BG14" s="60"/>
       <c r="BH14" s="60"/>
@@ -5401,7 +5424,9 @@
       <c r="BD15" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE15" s="60"/>
+      <c r="BE15" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF15" s="60"/>
       <c r="BG15" s="60"/>
       <c r="BH15" s="60"/>
@@ -5578,7 +5603,9 @@
       <c r="BD16" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE16" s="60"/>
+      <c r="BE16" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF16" s="60"/>
       <c r="BG16" s="60"/>
       <c r="BH16" s="60"/>
@@ -5755,7 +5782,9 @@
       <c r="BD17" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BE17" s="60"/>
+      <c r="BE17" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF17" s="60"/>
       <c r="BG17" s="60"/>
       <c r="BH17" s="60"/>
@@ -5932,7 +5961,9 @@
       <c r="BD18" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE18" s="60"/>
+      <c r="BE18" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF18" s="60"/>
       <c r="BG18" s="60"/>
       <c r="BH18" s="60"/>
@@ -6109,7 +6140,9 @@
       <c r="BD19" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE19" s="60"/>
+      <c r="BE19" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF19" s="60"/>
       <c r="BG19" s="60"/>
       <c r="BH19" s="60"/>
@@ -6286,7 +6319,9 @@
       <c r="BD20" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE20" s="60"/>
+      <c r="BE20" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF20" s="60"/>
       <c r="BG20" s="60"/>
       <c r="BH20" s="60"/>
@@ -6463,7 +6498,9 @@
       <c r="BD21" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE21" s="60"/>
+      <c r="BE21" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF21" s="60"/>
       <c r="BG21" s="60"/>
       <c r="BH21" s="60"/>
@@ -6640,7 +6677,9 @@
       <c r="BD22" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE22" s="60"/>
+      <c r="BE22" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF22" s="60"/>
       <c r="BG22" s="60"/>
       <c r="BH22" s="60"/>
@@ -6817,7 +6856,9 @@
       <c r="BD23" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE23" s="60"/>
+      <c r="BE23" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF23" s="60"/>
       <c r="BG23" s="60"/>
       <c r="BH23" s="60"/>
@@ -6994,7 +7035,9 @@
       <c r="BD24" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BE24" s="60"/>
+      <c r="BE24" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF24" s="60"/>
       <c r="BG24" s="60"/>
       <c r="BH24" s="60"/>
@@ -7171,7 +7214,9 @@
       <c r="BD25" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE25" s="60"/>
+      <c r="BE25" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF25" s="60"/>
       <c r="BG25" s="60"/>
       <c r="BH25" s="60"/>
@@ -7348,7 +7393,9 @@
       <c r="BD26" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BE26" s="60"/>
+      <c r="BE26" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BF26" s="60"/>
       <c r="BG26" s="60"/>
       <c r="BH26" s="60"/>
@@ -7525,7 +7572,9 @@
       <c r="BD27" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE27" s="60"/>
+      <c r="BE27" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF27" s="60"/>
       <c r="BG27" s="60"/>
       <c r="BH27" s="60"/>
@@ -7702,7 +7751,9 @@
       <c r="BD28" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE28" s="60"/>
+      <c r="BE28" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF28" s="60"/>
       <c r="BG28" s="60"/>
       <c r="BH28" s="60"/>
@@ -7879,7 +7930,9 @@
       <c r="BD29" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE29" s="60"/>
+      <c r="BE29" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF29" s="60"/>
       <c r="BG29" s="60"/>
       <c r="BH29" s="60"/>
@@ -8056,7 +8109,9 @@
       <c r="BD30" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE30" s="60"/>
+      <c r="BE30" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF30" s="60"/>
       <c r="BG30" s="60"/>
       <c r="BH30" s="60"/>
@@ -8233,7 +8288,9 @@
       <c r="BD31" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE31" s="60"/>
+      <c r="BE31" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF31" s="60"/>
       <c r="BG31" s="60"/>
       <c r="BH31" s="60"/>
@@ -8410,7 +8467,9 @@
       <c r="BD32" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BE32" s="60"/>
+      <c r="BE32" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF32" s="60"/>
       <c r="BG32" s="60"/>
       <c r="BH32" s="60"/>
@@ -8587,7 +8646,9 @@
       <c r="BD33" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE33" s="60"/>
+      <c r="BE33" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF33" s="60"/>
       <c r="BG33" s="60"/>
       <c r="BH33" s="60"/>
@@ -8764,7 +8825,9 @@
       <c r="BD34" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE34" s="60"/>
+      <c r="BE34" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF34" s="60"/>
       <c r="BG34" s="60"/>
       <c r="BH34" s="60"/>
@@ -8941,7 +9004,9 @@
       <c r="BD35" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE35" s="60"/>
+      <c r="BE35" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF35" s="60"/>
       <c r="BG35" s="60"/>
       <c r="BH35" s="60"/>
@@ -9118,7 +9183,9 @@
       <c r="BD36" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE36" s="60"/>
+      <c r="BE36" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF36" s="60"/>
       <c r="BG36" s="60"/>
       <c r="BH36" s="60"/>
@@ -9295,7 +9362,9 @@
       <c r="BD37" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE37" s="60"/>
+      <c r="BE37" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="BF37" s="60"/>
       <c r="BG37" s="60"/>
       <c r="BH37" s="60"/>
@@ -9472,7 +9541,9 @@
       <c r="BD38" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE38" s="60"/>
+      <c r="BE38" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF38" s="60"/>
       <c r="BG38" s="60"/>
       <c r="BH38" s="60"/>
@@ -9649,7 +9720,9 @@
       <c r="BD39" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE39" s="60"/>
+      <c r="BE39" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF39" s="60"/>
       <c r="BG39" s="60"/>
       <c r="BH39" s="60"/>
@@ -9826,7 +9899,9 @@
       <c r="BD40" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BE40" s="60"/>
+      <c r="BE40" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF40" s="60"/>
       <c r="BG40" s="60"/>
       <c r="BH40" s="60"/>
@@ -10003,7 +10078,9 @@
       <c r="BD41" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE41" s="60"/>
+      <c r="BE41" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF41" s="60"/>
       <c r="BG41" s="60"/>
       <c r="BH41" s="60"/>
@@ -10180,7 +10257,9 @@
       <c r="BD42" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE42" s="60"/>
+      <c r="BE42" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF42" s="60"/>
       <c r="BG42" s="60"/>
       <c r="BH42" s="60"/>
@@ -10357,7 +10436,9 @@
       <c r="BD43" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE43" s="60"/>
+      <c r="BE43" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF43" s="60"/>
       <c r="BG43" s="60"/>
       <c r="BH43" s="60"/>
@@ -10534,7 +10615,9 @@
       <c r="BD44" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE44" s="60"/>
+      <c r="BE44" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF44" s="60"/>
       <c r="BG44" s="60"/>
       <c r="BH44" s="60"/>
@@ -10711,7 +10794,9 @@
       <c r="BD45" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE45" s="60"/>
+      <c r="BE45" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF45" s="60"/>
       <c r="BG45" s="60"/>
       <c r="BH45" s="60"/>
@@ -10888,7 +10973,9 @@
       <c r="BD46" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE46" s="60"/>
+      <c r="BE46" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF46" s="60"/>
       <c r="BG46" s="60"/>
       <c r="BH46" s="60"/>
@@ -11065,7 +11152,9 @@
       <c r="BD47" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE47" s="60"/>
+      <c r="BE47" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF47" s="60"/>
       <c r="BG47" s="60"/>
       <c r="BH47" s="60"/>
@@ -11242,7 +11331,9 @@
       <c r="BD48" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE48" s="60"/>
+      <c r="BE48" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF48" s="60"/>
       <c r="BG48" s="60"/>
       <c r="BH48" s="60"/>
@@ -11419,7 +11510,9 @@
       <c r="BD49" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE49" s="60"/>
+      <c r="BE49" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF49" s="60"/>
       <c r="BG49" s="60"/>
       <c r="BH49" s="60"/>
@@ -11596,7 +11689,9 @@
       <c r="BD50" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE50" s="60"/>
+      <c r="BE50" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF50" s="60"/>
       <c r="BG50" s="60"/>
       <c r="BH50" s="60"/>
@@ -11773,7 +11868,9 @@
       <c r="BD51" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE51" s="60"/>
+      <c r="BE51" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF51" s="60"/>
       <c r="BG51" s="60"/>
       <c r="BH51" s="60"/>
@@ -11950,7 +12047,9 @@
       <c r="BD52" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE52" s="60"/>
+      <c r="BE52" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF52" s="60"/>
       <c r="BG52" s="60"/>
       <c r="BH52" s="60"/>
@@ -12127,7 +12226,9 @@
       <c r="BD53" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE53" s="60"/>
+      <c r="BE53" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF53" s="60"/>
       <c r="BG53" s="60"/>
       <c r="BH53" s="60"/>
@@ -12304,7 +12405,9 @@
       <c r="BD54" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE54" s="60"/>
+      <c r="BE54" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF54" s="60"/>
       <c r="BG54" s="60"/>
       <c r="BH54" s="60"/>
@@ -12481,7 +12584,9 @@
       <c r="BD55" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="BE55" s="60"/>
+      <c r="BE55" s="125" t="s">
+        <v>54</v>
+      </c>
       <c r="BF55" s="60"/>
       <c r="BG55" s="60"/>
       <c r="BH55" s="60"/>
@@ -12492,10 +12597,10 @@
       <c r="BM55" s="60"/>
     </row>
     <row r="56" spans="1:65">
-      <c r="A56" s="139" t="s">
+      <c r="A56" s="132" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="140"/>
+      <c r="B56" s="133"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -12711,7 +12816,7 @@
       </c>
       <c r="BE56" s="60">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BF56" s="60">
         <f t="shared" si="22"/>
@@ -12747,10 +12852,10 @@
       </c>
     </row>
     <row r="57" spans="1:65">
-      <c r="A57" s="137" t="s">
+      <c r="A57" s="129" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="138"/>
+      <c r="B57" s="130"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -12966,7 +13071,7 @@
       </c>
       <c r="BE57" s="60">
         <f t="shared" si="24"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="BF57" s="60">
         <f t="shared" si="24"/>
@@ -13003,14 +13108,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="X4:AS4"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F3:I3"/>
@@ -13021,6 +13118,14 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N2:W2"/>
     <mergeCell ref="N3:W3"/>
+    <mergeCell ref="X4:AS4"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13049,76 +13154,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="155" t="s">
+      <c r="B1" s="153"/>
+      <c r="C1" s="152" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="155"/>
-      <c r="E1" s="136" t="s">
+      <c r="D1" s="152"/>
+      <c r="E1" s="148" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="148"/>
+      <c r="H1" s="148"/>
+      <c r="I1" s="148"/>
     </row>
     <row r="2" spans="1:9" ht="19.5">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="150" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="155" t="s">
+      <c r="B2" s="150"/>
+      <c r="C2" s="152" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="155"/>
-      <c r="E2" s="136" t="s">
+      <c r="D2" s="152"/>
+      <c r="E2" s="148" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
     </row>
     <row r="3" spans="1:9" ht="17.25">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="151" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="154"/>
-      <c r="C3" s="155" t="s">
+      <c r="B3" s="151"/>
+      <c r="C3" s="152" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="155"/>
-      <c r="E3" s="136" t="s">
+      <c r="D3" s="152"/>
+      <c r="E3" s="148" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="136"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
+      <c r="F3" s="148"/>
+      <c r="G3" s="148"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="149" t="s">
+      <c r="A4" s="154" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="134" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="152" t="s">
+      <c r="C4" s="149" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="152"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
+      <c r="D4" s="149"/>
+      <c r="E4" s="149"/>
+      <c r="F4" s="149"/>
+      <c r="G4" s="149"/>
+      <c r="H4" s="149"/>
+      <c r="I4" s="149"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="150"/>
-      <c r="B5" s="142"/>
+      <c r="A5" s="155"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -13142,8 +13247,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="151"/>
-      <c r="B6" s="143"/>
+      <c r="A6" s="156"/>
+      <c r="B6" s="136"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -14225,10 +14330,10 @@
       <c r="I54" s="42"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="139" t="s">
+      <c r="A55" s="132" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="140"/>
+      <c r="B55" s="133"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -14245,10 +14350,10 @@
       <c r="I55" s="13"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="137" t="s">
+      <c r="A56" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="138"/>
+      <c r="B56" s="130"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -14265,10 +14370,10 @@
       <c r="I56" s="13"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="137" t="s">
+      <c r="A57" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="138"/>
+      <c r="B57" s="130"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -14285,10 +14390,10 @@
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="137" t="s">
+      <c r="A58" s="129" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="138"/>
+      <c r="B58" s="130"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -14306,6 +14411,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -14315,13 +14427,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="E1:I1"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:I54">
     <cfRule type="cellIs" dxfId="5" priority="17" operator="lessThan">
@@ -14355,72 +14460,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="155" t="s">
+      <c r="B1" s="153"/>
+      <c r="C1" s="152" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="155"/>
-      <c r="E1" s="156" t="s">
+      <c r="D1" s="152"/>
+      <c r="E1" s="160" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="156"/>
-      <c r="G1" s="156"/>
-      <c r="H1" s="157"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="161"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="150" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="155" t="s">
+      <c r="B2" s="150"/>
+      <c r="C2" s="152" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="155"/>
-      <c r="E2" s="136" t="s">
+      <c r="D2" s="152"/>
+      <c r="E2" s="148" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="151" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="154"/>
-      <c r="C3" s="155" t="s">
+      <c r="B3" s="151"/>
+      <c r="C3" s="152" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="155"/>
-      <c r="E3" s="136" t="s">
+      <c r="D3" s="152"/>
+      <c r="E3" s="148" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="136"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
+      <c r="F3" s="148"/>
+      <c r="G3" s="148"/>
+      <c r="H3" s="148"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="149" t="s">
+      <c r="A4" s="154" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="134" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="158" t="s">
+      <c r="C4" s="157" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="159"/>
-      <c r="E4" s="159"/>
-      <c r="F4" s="159"/>
-      <c r="G4" s="159"/>
-      <c r="H4" s="160"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="159"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="150"/>
-      <c r="B5" s="142"/>
+      <c r="A5" s="155"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -14441,8 +14546,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="151"/>
-      <c r="B6" s="143"/>
+      <c r="A6" s="156"/>
+      <c r="B6" s="136"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -15567,10 +15672,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="139" t="s">
+      <c r="A55" s="132" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="140"/>
+      <c r="B55" s="133"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -15585,10 +15690,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="137" t="s">
+      <c r="A56" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="138"/>
+      <c r="B56" s="130"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -15603,10 +15708,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="137" t="s">
+      <c r="A57" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="138"/>
+      <c r="B57" s="130"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -15621,10 +15726,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="137" t="s">
+      <c r="A58" s="129" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="138"/>
+      <c r="B58" s="130"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -15640,22 +15745,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
@@ -15696,221 +15801,221 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="127" t="s">
+      <c r="F1" s="144" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="135" t="s">
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="147" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="135"/>
-      <c r="L1" s="135"/>
-      <c r="M1" s="135"/>
-      <c r="N1" s="167" t="s">
+      <c r="K1" s="147"/>
+      <c r="L1" s="147"/>
+      <c r="M1" s="147"/>
+      <c r="N1" s="162" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="168"/>
-      <c r="P1" s="168"/>
-      <c r="Q1" s="168"/>
-      <c r="R1" s="168"/>
-      <c r="S1" s="168"/>
-      <c r="T1" s="168"/>
-      <c r="U1" s="168"/>
-      <c r="V1" s="168"/>
-      <c r="W1" s="168"/>
-      <c r="X1" s="168"/>
-      <c r="Y1" s="168"/>
-      <c r="Z1" s="168"/>
-      <c r="AA1" s="168"/>
-      <c r="AB1" s="168"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="163"/>
+      <c r="T1" s="163"/>
+      <c r="U1" s="163"/>
+      <c r="V1" s="163"/>
+      <c r="W1" s="163"/>
+      <c r="X1" s="163"/>
+      <c r="Y1" s="163"/>
+      <c r="Z1" s="163"/>
+      <c r="AA1" s="163"/>
+      <c r="AB1" s="163"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="144" t="s">
+      <c r="A2" s="137" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="145"/>
-      <c r="C2" s="146"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="139"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="130" t="s">
+      <c r="F2" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="135" t="s">
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="135"/>
-      <c r="L2" s="135"/>
-      <c r="M2" s="135"/>
-      <c r="N2" s="167" t="s">
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
+      <c r="M2" s="147"/>
+      <c r="N2" s="162" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="168"/>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="168"/>
-      <c r="R2" s="168"/>
-      <c r="S2" s="168"/>
-      <c r="T2" s="168"/>
-      <c r="U2" s="168"/>
-      <c r="V2" s="168"/>
-      <c r="W2" s="168"/>
-      <c r="X2" s="168"/>
-      <c r="Y2" s="168"/>
-      <c r="Z2" s="168"/>
-      <c r="AA2" s="168"/>
-      <c r="AB2" s="168"/>
+      <c r="O2" s="163"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
+      <c r="U2" s="163"/>
+      <c r="V2" s="163"/>
+      <c r="W2" s="163"/>
+      <c r="X2" s="163"/>
+      <c r="Y2" s="163"/>
+      <c r="Z2" s="163"/>
+      <c r="AA2" s="163"/>
+      <c r="AB2" s="163"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="170" t="s">
+      <c r="A3" s="165" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="171"/>
-      <c r="C3" s="172"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="167"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="169" t="s">
+      <c r="F3" s="164" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="178" t="s">
+      <c r="G3" s="164"/>
+      <c r="H3" s="164"/>
+      <c r="I3" s="164"/>
+      <c r="J3" s="173" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="178"/>
-      <c r="L3" s="178"/>
-      <c r="M3" s="178"/>
-      <c r="N3" s="167" t="s">
+      <c r="K3" s="173"/>
+      <c r="L3" s="173"/>
+      <c r="M3" s="173"/>
+      <c r="N3" s="162" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="168"/>
-      <c r="P3" s="168"/>
-      <c r="Q3" s="168"/>
-      <c r="R3" s="168"/>
-      <c r="S3" s="168"/>
-      <c r="T3" s="168"/>
-      <c r="U3" s="168"/>
-      <c r="V3" s="168"/>
-      <c r="W3" s="168"/>
-      <c r="X3" s="168"/>
-      <c r="Y3" s="168"/>
-      <c r="Z3" s="168"/>
-      <c r="AA3" s="168"/>
-      <c r="AB3" s="168"/>
+      <c r="O3" s="163"/>
+      <c r="P3" s="163"/>
+      <c r="Q3" s="163"/>
+      <c r="R3" s="163"/>
+      <c r="S3" s="163"/>
+      <c r="T3" s="163"/>
+      <c r="U3" s="163"/>
+      <c r="V3" s="163"/>
+      <c r="W3" s="163"/>
+      <c r="X3" s="163"/>
+      <c r="Y3" s="163"/>
+      <c r="Z3" s="163"/>
+      <c r="AA3" s="163"/>
+      <c r="AB3" s="163"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="175"/>
-      <c r="D4" s="176">
+      <c r="A4" s="168"/>
+      <c r="B4" s="169"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="171">
         <v>43344</v>
       </c>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="177"/>
-      <c r="J4" s="177"/>
-      <c r="K4" s="177"/>
-      <c r="L4" s="177"/>
-      <c r="M4" s="177"/>
-      <c r="N4" s="176">
+      <c r="E4" s="172"/>
+      <c r="F4" s="172"/>
+      <c r="G4" s="172"/>
+      <c r="H4" s="172"/>
+      <c r="I4" s="172"/>
+      <c r="J4" s="172"/>
+      <c r="K4" s="172"/>
+      <c r="L4" s="172"/>
+      <c r="M4" s="172"/>
+      <c r="N4" s="171">
         <v>43374</v>
       </c>
-      <c r="O4" s="177"/>
-      <c r="P4" s="177"/>
-      <c r="Q4" s="177"/>
-      <c r="R4" s="177"/>
-      <c r="S4" s="177"/>
-      <c r="T4" s="177"/>
-      <c r="U4" s="177"/>
+      <c r="O4" s="172"/>
+      <c r="P4" s="172"/>
+      <c r="Q4" s="172"/>
+      <c r="R4" s="172"/>
+      <c r="S4" s="172"/>
+      <c r="T4" s="172"/>
+      <c r="U4" s="172"/>
       <c r="V4" s="53"/>
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="149" t="s">
+      <c r="A5" s="154" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="134" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="162" t="s">
+      <c r="D5" s="174" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
-      <c r="H5" s="165" t="s">
+      <c r="E5" s="175"/>
+      <c r="F5" s="175"/>
+      <c r="G5" s="176"/>
+      <c r="H5" s="177" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="166"/>
-      <c r="J5" s="166"/>
-      <c r="K5" s="166"/>
-      <c r="L5" s="161" t="s">
+      <c r="I5" s="178"/>
+      <c r="J5" s="178"/>
+      <c r="K5" s="178"/>
+      <c r="L5" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="161"/>
-      <c r="N5" s="165" t="s">
+      <c r="M5" s="179"/>
+      <c r="N5" s="177" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="166"/>
-      <c r="P5" s="166"/>
-      <c r="Q5" s="166"/>
-      <c r="R5" s="161" t="s">
+      <c r="O5" s="178"/>
+      <c r="P5" s="178"/>
+      <c r="Q5" s="178"/>
+      <c r="R5" s="179" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="161"/>
-      <c r="T5" s="147" t="s">
+      <c r="S5" s="179"/>
+      <c r="T5" s="143" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="147"/>
-      <c r="V5" s="147" t="s">
+      <c r="U5" s="143"/>
+      <c r="V5" s="143" t="s">
         <v>117</v>
       </c>
-      <c r="W5" s="147"/>
-      <c r="X5" s="147"/>
-      <c r="Y5" s="147"/>
-      <c r="Z5" s="147" t="s">
+      <c r="W5" s="143"/>
+      <c r="X5" s="143"/>
+      <c r="Y5" s="143"/>
+      <c r="Z5" s="143" t="s">
         <v>118</v>
       </c>
-      <c r="AA5" s="147"/>
-      <c r="AB5" s="147"/>
-      <c r="AC5" s="147"/>
-      <c r="AD5" s="147" t="s">
+      <c r="AA5" s="143"/>
+      <c r="AB5" s="143"/>
+      <c r="AC5" s="143"/>
+      <c r="AD5" s="143" t="s">
         <v>169</v>
       </c>
-      <c r="AE5" s="147"/>
-      <c r="AF5" s="147"/>
+      <c r="AE5" s="143"/>
+      <c r="AF5" s="143"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="150"/>
-      <c r="B6" s="142"/>
+      <c r="A6" s="155"/>
+      <c r="B6" s="135"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -16003,8 +16108,8 @@
       </c>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="150"/>
-      <c r="B7" s="142"/>
+      <c r="A7" s="155"/>
+      <c r="B7" s="135"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -16097,8 +16202,8 @@
       </c>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="151"/>
-      <c r="B8" s="143"/>
+      <c r="A8" s="156"/>
+      <c r="B8" s="136"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -20799,10 +20904,10 @@
       </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="139" t="s">
+      <c r="A57" s="132" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="140"/>
+      <c r="B57" s="133"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -20922,10 +21027,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="137" t="s">
+      <c r="A58" s="129" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="138"/>
+      <c r="B58" s="130"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -21046,6 +21151,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="AD5:AF5"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
     <mergeCell ref="N1:AB1"/>
     <mergeCell ref="N2:AB2"/>
     <mergeCell ref="N3:AB3"/>
@@ -21060,19 +21178,6 @@
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N4:U4"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="AD5:AF5"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="N5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -21098,28 +21203,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="180" t="s">
+      <c r="A1" s="181" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="181" t="s">
+      <c r="A2" s="182" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="181"/>
-      <c r="C2" s="181"/>
-      <c r="D2" s="181"/>
+      <c r="B2" s="182"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="181" t="s">
+      <c r="A3" s="182" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="181"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
     </row>
     <row r="4" spans="1:4" s="83" customFormat="1" ht="28.5">
       <c r="A4" s="81" t="s">
@@ -21850,41 +21955,41 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="179" t="s">
+      <c r="A56" s="180" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="179"/>
-      <c r="C56" s="179"/>
+      <c r="B56" s="180"/>
+      <c r="C56" s="180"/>
       <c r="D56" s="75">
         <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="179" t="s">
+      <c r="A57" s="180" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="179"/>
-      <c r="C57" s="179"/>
+      <c r="B57" s="180"/>
+      <c r="C57" s="180"/>
       <c r="D57" s="76">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="179" t="s">
+      <c r="A58" s="180" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="179"/>
-      <c r="C58" s="179"/>
+      <c r="B58" s="180"/>
+      <c r="C58" s="180"/>
       <c r="D58" s="76">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="179" t="s">
+      <c r="A59" s="180" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="179"/>
-      <c r="C59" s="179"/>
+      <c r="B59" s="180"/>
+      <c r="C59" s="180"/>
       <c r="D59" s="76">
         <v>92</v>
       </c>
@@ -21957,28 +22062,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="183" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
+      <c r="B1" s="183"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="183"/>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="184" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
+      <c r="B2" s="184"/>
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="183" t="s">
+      <c r="A3" s="184" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="183"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="183"/>
+      <c r="B3" s="184"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="184"/>
     </row>
     <row r="4" spans="1:4" s="83" customFormat="1" ht="31.5">
       <c r="A4" s="103" t="s">
@@ -22709,41 +22814,41 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75">
-      <c r="A56" s="155" t="s">
+      <c r="A56" s="152" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="155"/>
-      <c r="C56" s="155"/>
+      <c r="B56" s="152"/>
+      <c r="C56" s="152"/>
       <c r="D56" s="115">
         <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75">
-      <c r="A57" s="155" t="s">
+      <c r="A57" s="152" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="155"/>
-      <c r="C57" s="155"/>
+      <c r="B57" s="152"/>
+      <c r="C57" s="152"/>
       <c r="D57" s="116">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75">
-      <c r="A58" s="155" t="s">
+      <c r="A58" s="152" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="155"/>
-      <c r="C58" s="155"/>
+      <c r="B58" s="152"/>
+      <c r="C58" s="152"/>
       <c r="D58" s="116">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75">
-      <c r="A59" s="155" t="s">
+      <c r="A59" s="152" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="155"/>
-      <c r="C59" s="155"/>
+      <c r="B59" s="152"/>
+      <c r="C59" s="152"/>
       <c r="D59" s="116">
         <v>85.1</v>
       </c>

</xml_diff>

<commit_message>
Last Update 27-11-2018 12:10:06.01
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -2736,27 +2736,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2766,17 +2758,14 @@
     <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2805,8 +2794,44 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2820,24 +2845,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2847,23 +2854,11 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2899,6 +2894,24 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2916,19 +2929,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3299,7 +3299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BM57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="AC5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -3317,29 +3317,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="18.75">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="145" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="129" t="s">
+      <c r="F1" s="149" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="137" t="s">
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
+      <c r="I1" s="151"/>
+      <c r="J1" s="152" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="137"/>
-      <c r="L1" s="137"/>
-      <c r="M1" s="137"/>
+      <c r="K1" s="152"/>
+      <c r="L1" s="152"/>
+      <c r="M1" s="152"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -3364,41 +3364,41 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:65" ht="19.5">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="142" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="148"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="144"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="132" t="s">
+      <c r="F2" s="136" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="137" t="s">
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="152" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="137"/>
-      <c r="L2" s="137"/>
-      <c r="M2" s="137"/>
-      <c r="N2" s="138" t="s">
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="153" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="138"/>
-      <c r="P2" s="138"/>
-      <c r="Q2" s="138"/>
-      <c r="R2" s="138"/>
-      <c r="S2" s="138"/>
-      <c r="T2" s="138"/>
-      <c r="U2" s="138"/>
-      <c r="V2" s="138"/>
-      <c r="W2" s="138"/>
+      <c r="O2" s="153"/>
+      <c r="P2" s="153"/>
+      <c r="Q2" s="153"/>
+      <c r="R2" s="153"/>
+      <c r="S2" s="153"/>
+      <c r="T2" s="153"/>
+      <c r="U2" s="153"/>
+      <c r="V2" s="153"/>
+      <c r="W2" s="153"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -3411,41 +3411,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:65" ht="18.75">
-      <c r="A3" s="127" t="s">
+      <c r="A3" s="145" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="128"/>
-      <c r="C3" s="133"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="147"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="132" t="s">
+      <c r="F3" s="136" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="137" t="s">
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="152" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="137"/>
-      <c r="L3" s="137"/>
-      <c r="M3" s="137"/>
-      <c r="N3" s="138" t="s">
+      <c r="K3" s="152"/>
+      <c r="L3" s="152"/>
+      <c r="M3" s="152"/>
+      <c r="N3" s="153" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="138"/>
-      <c r="P3" s="138"/>
-      <c r="Q3" s="138"/>
-      <c r="R3" s="138"/>
-      <c r="S3" s="138"/>
-      <c r="T3" s="138"/>
-      <c r="U3" s="138"/>
-      <c r="V3" s="138"/>
-      <c r="W3" s="138"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
+      <c r="Q3" s="153"/>
+      <c r="R3" s="153"/>
+      <c r="S3" s="153"/>
+      <c r="T3" s="153"/>
+      <c r="U3" s="153"/>
+      <c r="V3" s="153"/>
+      <c r="W3" s="153"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -3458,57 +3458,57 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:65" ht="18.75">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="145" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="128"/>
-      <c r="C4" s="133"/>
-      <c r="D4" s="134">
+      <c r="B4" s="146"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="131">
         <v>43344</v>
       </c>
-      <c r="E4" s="135"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="135"/>
-      <c r="H4" s="135"/>
-      <c r="I4" s="135"/>
-      <c r="J4" s="135"/>
-      <c r="K4" s="135"/>
-      <c r="L4" s="135"/>
-      <c r="M4" s="135"/>
-      <c r="N4" s="135"/>
-      <c r="O4" s="135"/>
-      <c r="P4" s="135"/>
-      <c r="Q4" s="135"/>
-      <c r="R4" s="135"/>
-      <c r="S4" s="135"/>
-      <c r="T4" s="135"/>
-      <c r="U4" s="135"/>
-      <c r="V4" s="135"/>
-      <c r="W4" s="136"/>
-      <c r="X4" s="134">
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
+      <c r="H4" s="132"/>
+      <c r="I4" s="132"/>
+      <c r="J4" s="132"/>
+      <c r="K4" s="132"/>
+      <c r="L4" s="132"/>
+      <c r="M4" s="132"/>
+      <c r="N4" s="132"/>
+      <c r="O4" s="132"/>
+      <c r="P4" s="132"/>
+      <c r="Q4" s="132"/>
+      <c r="R4" s="132"/>
+      <c r="S4" s="132"/>
+      <c r="T4" s="132"/>
+      <c r="U4" s="132"/>
+      <c r="V4" s="132"/>
+      <c r="W4" s="133"/>
+      <c r="X4" s="131">
         <v>43374</v>
       </c>
-      <c r="Y4" s="135"/>
-      <c r="Z4" s="135"/>
-      <c r="AA4" s="135"/>
-      <c r="AB4" s="135"/>
-      <c r="AC4" s="135"/>
-      <c r="AD4" s="135"/>
-      <c r="AE4" s="135"/>
-      <c r="AF4" s="135"/>
-      <c r="AG4" s="135"/>
-      <c r="AH4" s="135"/>
-      <c r="AI4" s="135"/>
-      <c r="AJ4" s="135"/>
-      <c r="AK4" s="135"/>
-      <c r="AL4" s="135"/>
-      <c r="AM4" s="135"/>
-      <c r="AN4" s="135"/>
-      <c r="AO4" s="135"/>
-      <c r="AP4" s="135"/>
-      <c r="AQ4" s="135"/>
-      <c r="AR4" s="135"/>
-      <c r="AS4" s="136"/>
+      <c r="Y4" s="132"/>
+      <c r="Z4" s="132"/>
+      <c r="AA4" s="132"/>
+      <c r="AB4" s="132"/>
+      <c r="AC4" s="132"/>
+      <c r="AD4" s="132"/>
+      <c r="AE4" s="132"/>
+      <c r="AF4" s="132"/>
+      <c r="AG4" s="132"/>
+      <c r="AH4" s="132"/>
+      <c r="AI4" s="132"/>
+      <c r="AJ4" s="132"/>
+      <c r="AK4" s="132"/>
+      <c r="AL4" s="132"/>
+      <c r="AM4" s="132"/>
+      <c r="AN4" s="132"/>
+      <c r="AO4" s="132"/>
+      <c r="AP4" s="132"/>
+      <c r="AQ4" s="132"/>
+      <c r="AR4" s="132"/>
+      <c r="AS4" s="133"/>
       <c r="AT4" s="59"/>
       <c r="AU4" s="59"/>
       <c r="AV4" s="59"/>
@@ -3531,10 +3531,10 @@
       <c r="BM4" s="59"/>
     </row>
     <row r="5" spans="1:65">
-      <c r="A5" s="149" t="s">
+      <c r="A5" s="148" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="139" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -3718,8 +3718,8 @@
       <c r="BM5" s="59"/>
     </row>
     <row r="6" spans="1:65">
-      <c r="A6" s="149"/>
-      <c r="B6" s="144"/>
+      <c r="A6" s="148"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -3904,7 +3904,7 @@
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="145"/>
+      <c r="B7" s="141"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -4089,7 +4089,7 @@
       <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="186" t="s">
+      <c r="B8" s="127" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="5"/>
@@ -4274,7 +4274,7 @@
       <c r="A9" s="3">
         <v>2</v>
       </c>
-      <c r="B9" s="187" t="s">
+      <c r="B9" s="128" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="4"/>
@@ -4459,7 +4459,7 @@
       <c r="A10" s="3">
         <v>3</v>
       </c>
-      <c r="B10" s="187" t="s">
+      <c r="B10" s="128" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="4"/>
@@ -4644,7 +4644,7 @@
       <c r="A11" s="3">
         <v>4</v>
       </c>
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="127" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="5"/>
@@ -4829,7 +4829,7 @@
       <c r="A12" s="3">
         <v>5</v>
       </c>
-      <c r="B12" s="187" t="s">
+      <c r="B12" s="128" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="4"/>
@@ -5014,7 +5014,7 @@
       <c r="A13" s="3">
         <v>6</v>
       </c>
-      <c r="B13" s="187" t="s">
+      <c r="B13" s="128" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="4"/>
@@ -5199,7 +5199,7 @@
       <c r="A14" s="3">
         <v>7</v>
       </c>
-      <c r="B14" s="187" t="s">
+      <c r="B14" s="128" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="4"/>
@@ -5384,7 +5384,7 @@
       <c r="A15" s="3">
         <v>8</v>
       </c>
-      <c r="B15" s="187" t="s">
+      <c r="B15" s="128" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="4"/>
@@ -5569,7 +5569,7 @@
       <c r="A16" s="3">
         <v>9</v>
       </c>
-      <c r="B16" s="187" t="s">
+      <c r="B16" s="128" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="4"/>
@@ -5754,7 +5754,7 @@
       <c r="A17" s="3">
         <v>10</v>
       </c>
-      <c r="B17" s="187" t="s">
+      <c r="B17" s="128" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="4"/>
@@ -5939,7 +5939,7 @@
       <c r="A18" s="3">
         <v>11</v>
       </c>
-      <c r="B18" s="187" t="s">
+      <c r="B18" s="128" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="4"/>
@@ -6124,7 +6124,7 @@
       <c r="A19" s="3">
         <v>12</v>
       </c>
-      <c r="B19" s="187" t="s">
+      <c r="B19" s="128" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="4"/>
@@ -6309,7 +6309,7 @@
       <c r="A20" s="3">
         <v>13</v>
       </c>
-      <c r="B20" s="187" t="s">
+      <c r="B20" s="128" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="4"/>
@@ -6494,7 +6494,7 @@
       <c r="A21" s="3">
         <v>14</v>
       </c>
-      <c r="B21" s="188" t="s">
+      <c r="B21" s="129" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="6"/>
@@ -6679,7 +6679,7 @@
       <c r="A22" s="3">
         <v>15</v>
       </c>
-      <c r="B22" s="189" t="s">
+      <c r="B22" s="130" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="13"/>
@@ -6864,7 +6864,7 @@
       <c r="A23" s="3">
         <v>16</v>
       </c>
-      <c r="B23" s="187" t="s">
+      <c r="B23" s="128" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="4"/>
@@ -7049,7 +7049,7 @@
       <c r="A24" s="3">
         <v>17</v>
       </c>
-      <c r="B24" s="187" t="s">
+      <c r="B24" s="128" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="4"/>
@@ -12966,10 +12966,10 @@
       <c r="BM55" s="59"/>
     </row>
     <row r="56" spans="1:65">
-      <c r="A56" s="141" t="s">
+      <c r="A56" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="142"/>
+      <c r="B56" s="138"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f t="shared" ref="D56:Q56" si="0">COUNTIF(D8:D55,"A")</f>
@@ -13221,10 +13221,10 @@
       </c>
     </row>
     <row r="57" spans="1:65">
-      <c r="A57" s="139" t="s">
+      <c r="A57" s="134" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="140"/>
+      <c r="B57" s="135"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -13477,14 +13477,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="X4:AS4"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F3:I3"/>
@@ -13495,6 +13487,14 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N2:W2"/>
     <mergeCell ref="N3:W3"/>
+    <mergeCell ref="X4:AS4"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13523,21 +13523,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="158" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="150"/>
+      <c r="B1" s="158"/>
       <c r="C1" s="157" t="s">
         <v>75</v>
       </c>
       <c r="D1" s="157"/>
-      <c r="E1" s="138" t="s">
+      <c r="E1" s="153" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
     </row>
     <row r="2" spans="1:9" ht="19.5">
       <c r="A2" s="155" t="s">
@@ -13548,13 +13548,13 @@
         <v>76</v>
       </c>
       <c r="D2" s="157"/>
-      <c r="E2" s="138" t="s">
+      <c r="E2" s="153" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
     </row>
     <row r="3" spans="1:9" ht="17.25">
       <c r="A3" s="156" t="s">
@@ -13565,19 +13565,19 @@
         <v>77</v>
       </c>
       <c r="D3" s="157"/>
-      <c r="E3" s="138" t="s">
+      <c r="E3" s="153" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="138"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="151" t="s">
+      <c r="A4" s="159" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="139" t="s">
         <v>84</v>
       </c>
       <c r="C4" s="154" t="s">
@@ -13591,8 +13591,8 @@
       <c r="I4" s="154"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="152"/>
-      <c r="B5" s="144"/>
+      <c r="A5" s="160"/>
+      <c r="B5" s="140"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -13616,8 +13616,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="153"/>
-      <c r="B6" s="145"/>
+      <c r="A6" s="161"/>
+      <c r="B6" s="141"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -14699,10 +14699,10 @@
       <c r="I54" s="42"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="141" t="s">
+      <c r="A55" s="137" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="142"/>
+      <c r="B55" s="138"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -14719,10 +14719,10 @@
       <c r="I55" s="13"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="139" t="s">
+      <c r="A56" s="134" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="140"/>
+      <c r="B56" s="135"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -14739,10 +14739,10 @@
       <c r="I56" s="13"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="139" t="s">
+      <c r="A57" s="134" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="140"/>
+      <c r="B57" s="135"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -14759,10 +14759,10 @@
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="139" t="s">
+      <c r="A58" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="140"/>
+      <c r="B58" s="135"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -14780,6 +14780,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -14789,13 +14796,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="E1:I1"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:I54">
     <cfRule type="cellIs" dxfId="5" priority="17" operator="lessThan">
@@ -14829,20 +14829,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="158" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="150"/>
+      <c r="B1" s="158"/>
       <c r="C1" s="157" t="s">
         <v>75</v>
       </c>
       <c r="D1" s="157"/>
-      <c r="E1" s="158" t="s">
+      <c r="E1" s="165" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="159"/>
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="166"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
       <c r="A2" s="155" t="s">
@@ -14853,12 +14853,12 @@
         <v>76</v>
       </c>
       <c r="D2" s="157"/>
-      <c r="E2" s="138" t="s">
+      <c r="E2" s="153" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
       <c r="A3" s="156" t="s">
@@ -14869,32 +14869,32 @@
         <v>77</v>
       </c>
       <c r="D3" s="157"/>
-      <c r="E3" s="138" t="s">
+      <c r="E3" s="153" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="151" t="s">
+      <c r="A4" s="159" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="160" t="s">
+      <c r="C4" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
-      <c r="H4" s="162"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="164"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="152"/>
-      <c r="B5" s="144"/>
+      <c r="A5" s="160"/>
+      <c r="B5" s="140"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -14915,8 +14915,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="153"/>
-      <c r="B6" s="145"/>
+      <c r="A6" s="161"/>
+      <c r="B6" s="141"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -16041,10 +16041,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="141" t="s">
+      <c r="A55" s="137" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="142"/>
+      <c r="B55" s="138"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -16059,10 +16059,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="139" t="s">
+      <c r="A56" s="134" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="140"/>
+      <c r="B56" s="135"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -16077,10 +16077,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="139" t="s">
+      <c r="A57" s="134" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="140"/>
+      <c r="B57" s="135"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -16095,10 +16095,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="139" t="s">
+      <c r="A58" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="140"/>
+      <c r="B58" s="135"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -16114,22 +16114,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
@@ -16155,8 +16155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF58"/>
   <sheetViews>
-    <sheetView topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="AI8" sqref="AI8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -16170,221 +16170,221 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="145" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="129" t="s">
+      <c r="F1" s="149" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="137" t="s">
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
+      <c r="I1" s="151"/>
+      <c r="J1" s="152" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="137"/>
-      <c r="L1" s="137"/>
-      <c r="M1" s="137"/>
-      <c r="N1" s="169" t="s">
+      <c r="K1" s="152"/>
+      <c r="L1" s="152"/>
+      <c r="M1" s="152"/>
+      <c r="N1" s="167" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="170"/>
-      <c r="P1" s="170"/>
-      <c r="Q1" s="170"/>
-      <c r="R1" s="170"/>
-      <c r="S1" s="170"/>
-      <c r="T1" s="170"/>
-      <c r="U1" s="170"/>
-      <c r="V1" s="170"/>
-      <c r="W1" s="170"/>
-      <c r="X1" s="170"/>
-      <c r="Y1" s="170"/>
-      <c r="Z1" s="170"/>
-      <c r="AA1" s="170"/>
-      <c r="AB1" s="170"/>
+      <c r="O1" s="168"/>
+      <c r="P1" s="168"/>
+      <c r="Q1" s="168"/>
+      <c r="R1" s="168"/>
+      <c r="S1" s="168"/>
+      <c r="T1" s="168"/>
+      <c r="U1" s="168"/>
+      <c r="V1" s="168"/>
+      <c r="W1" s="168"/>
+      <c r="X1" s="168"/>
+      <c r="Y1" s="168"/>
+      <c r="Z1" s="168"/>
+      <c r="AA1" s="168"/>
+      <c r="AB1" s="168"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="142" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="148"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="144"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="132" t="s">
+      <c r="F2" s="136" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="137" t="s">
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="152" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="137"/>
-      <c r="L2" s="137"/>
-      <c r="M2" s="137"/>
-      <c r="N2" s="169" t="s">
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="167" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="170"/>
-      <c r="P2" s="170"/>
-      <c r="Q2" s="170"/>
-      <c r="R2" s="170"/>
-      <c r="S2" s="170"/>
-      <c r="T2" s="170"/>
-      <c r="U2" s="170"/>
-      <c r="V2" s="170"/>
-      <c r="W2" s="170"/>
-      <c r="X2" s="170"/>
-      <c r="Y2" s="170"/>
-      <c r="Z2" s="170"/>
-      <c r="AA2" s="170"/>
-      <c r="AB2" s="170"/>
+      <c r="O2" s="168"/>
+      <c r="P2" s="168"/>
+      <c r="Q2" s="168"/>
+      <c r="R2" s="168"/>
+      <c r="S2" s="168"/>
+      <c r="T2" s="168"/>
+      <c r="U2" s="168"/>
+      <c r="V2" s="168"/>
+      <c r="W2" s="168"/>
+      <c r="X2" s="168"/>
+      <c r="Y2" s="168"/>
+      <c r="Z2" s="168"/>
+      <c r="AA2" s="168"/>
+      <c r="AB2" s="168"/>
     </row>
     <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="172" t="s">
+      <c r="A3" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="173"/>
-      <c r="C3" s="174"/>
+      <c r="B3" s="171"/>
+      <c r="C3" s="172"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="171" t="s">
+      <c r="F3" s="169" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="171"/>
-      <c r="H3" s="171"/>
-      <c r="I3" s="171"/>
-      <c r="J3" s="180" t="s">
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="178" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="180"/>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="169" t="s">
+      <c r="K3" s="178"/>
+      <c r="L3" s="178"/>
+      <c r="M3" s="178"/>
+      <c r="N3" s="167" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="170"/>
-      <c r="P3" s="170"/>
-      <c r="Q3" s="170"/>
-      <c r="R3" s="170"/>
-      <c r="S3" s="170"/>
-      <c r="T3" s="170"/>
-      <c r="U3" s="170"/>
-      <c r="V3" s="170"/>
-      <c r="W3" s="170"/>
-      <c r="X3" s="170"/>
-      <c r="Y3" s="170"/>
-      <c r="Z3" s="170"/>
-      <c r="AA3" s="170"/>
-      <c r="AB3" s="170"/>
+      <c r="O3" s="168"/>
+      <c r="P3" s="168"/>
+      <c r="Q3" s="168"/>
+      <c r="R3" s="168"/>
+      <c r="S3" s="168"/>
+      <c r="T3" s="168"/>
+      <c r="U3" s="168"/>
+      <c r="V3" s="168"/>
+      <c r="W3" s="168"/>
+      <c r="X3" s="168"/>
+      <c r="Y3" s="168"/>
+      <c r="Z3" s="168"/>
+      <c r="AA3" s="168"/>
+      <c r="AB3" s="168"/>
     </row>
     <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="175"/>
-      <c r="B4" s="176"/>
-      <c r="C4" s="177"/>
-      <c r="D4" s="178">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="175"/>
+      <c r="D4" s="176">
         <v>43344</v>
       </c>
-      <c r="E4" s="179"/>
-      <c r="F4" s="179"/>
-      <c r="G4" s="179"/>
-      <c r="H4" s="179"/>
-      <c r="I4" s="179"/>
-      <c r="J4" s="179"/>
-      <c r="K4" s="179"/>
-      <c r="L4" s="179"/>
-      <c r="M4" s="179"/>
-      <c r="N4" s="178">
+      <c r="E4" s="177"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="177"/>
+      <c r="H4" s="177"/>
+      <c r="I4" s="177"/>
+      <c r="J4" s="177"/>
+      <c r="K4" s="177"/>
+      <c r="L4" s="177"/>
+      <c r="M4" s="177"/>
+      <c r="N4" s="176">
         <v>43374</v>
       </c>
-      <c r="O4" s="179"/>
-      <c r="P4" s="179"/>
-      <c r="Q4" s="179"/>
-      <c r="R4" s="179"/>
-      <c r="S4" s="179"/>
-      <c r="T4" s="179"/>
-      <c r="U4" s="179"/>
+      <c r="O4" s="177"/>
+      <c r="P4" s="177"/>
+      <c r="Q4" s="177"/>
+      <c r="R4" s="177"/>
+      <c r="S4" s="177"/>
+      <c r="T4" s="177"/>
+      <c r="U4" s="177"/>
       <c r="V4" s="53"/>
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="151" t="s">
+      <c r="A5" s="159" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="139" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="166" t="s">
+      <c r="D5" s="179" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="167"/>
-      <c r="F5" s="167"/>
-      <c r="G5" s="168"/>
-      <c r="H5" s="164" t="s">
+      <c r="E5" s="180"/>
+      <c r="F5" s="180"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="182" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="165"/>
-      <c r="J5" s="165"/>
-      <c r="K5" s="165"/>
-      <c r="L5" s="163" t="s">
+      <c r="I5" s="183"/>
+      <c r="J5" s="183"/>
+      <c r="K5" s="183"/>
+      <c r="L5" s="184" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="163"/>
-      <c r="N5" s="164" t="s">
+      <c r="M5" s="184"/>
+      <c r="N5" s="182" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="165"/>
-      <c r="P5" s="165"/>
-      <c r="Q5" s="165"/>
-      <c r="R5" s="163" t="s">
+      <c r="O5" s="183"/>
+      <c r="P5" s="183"/>
+      <c r="Q5" s="183"/>
+      <c r="R5" s="184" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="163"/>
-      <c r="T5" s="149" t="s">
+      <c r="S5" s="184"/>
+      <c r="T5" s="148" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="149"/>
-      <c r="V5" s="149" t="s">
+      <c r="U5" s="148"/>
+      <c r="V5" s="148" t="s">
         <v>117</v>
       </c>
-      <c r="W5" s="149"/>
-      <c r="X5" s="149"/>
-      <c r="Y5" s="149"/>
-      <c r="Z5" s="149" t="s">
+      <c r="W5" s="148"/>
+      <c r="X5" s="148"/>
+      <c r="Y5" s="148"/>
+      <c r="Z5" s="148" t="s">
         <v>118</v>
       </c>
-      <c r="AA5" s="149"/>
-      <c r="AB5" s="149"/>
-      <c r="AC5" s="149"/>
-      <c r="AD5" s="149" t="s">
+      <c r="AA5" s="148"/>
+      <c r="AB5" s="148"/>
+      <c r="AC5" s="148"/>
+      <c r="AD5" s="148" t="s">
         <v>169</v>
       </c>
-      <c r="AE5" s="149"/>
-      <c r="AF5" s="149"/>
+      <c r="AE5" s="148"/>
+      <c r="AF5" s="148"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="152"/>
-      <c r="B6" s="144"/>
+      <c r="A6" s="160"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -16477,8 +16477,8 @@
       </c>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="152"/>
-      <c r="B7" s="144"/>
+      <c r="A7" s="160"/>
+      <c r="B7" s="140"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -16571,8 +16571,8 @@
       </c>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="153"/>
-      <c r="B8" s="145"/>
+      <c r="A8" s="161"/>
+      <c r="B8" s="141"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -21273,10 +21273,10 @@
       </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="141" t="s">
+      <c r="A57" s="137" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="142"/>
+      <c r="B57" s="138"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -21396,10 +21396,10 @@
       </c>
     </row>
     <row r="58" spans="1:32">
-      <c r="A58" s="139" t="s">
+      <c r="A58" s="134" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="140"/>
+      <c r="B58" s="135"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -21520,6 +21520,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="AD5:AF5"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
     <mergeCell ref="N1:AB1"/>
     <mergeCell ref="N2:AB2"/>
     <mergeCell ref="N3:AB3"/>
@@ -21534,19 +21547,6 @@
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N4:U4"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="AD5:AF5"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="N5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -21572,28 +21572,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="186" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="187" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="183" t="s">
+      <c r="A3" s="187" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="183"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="183"/>
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
     </row>
     <row r="4" spans="1:4" s="82" customFormat="1" ht="28.5">
       <c r="A4" s="80" t="s">
@@ -22324,41 +22324,41 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="181" t="s">
+      <c r="A56" s="185" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="181"/>
-      <c r="C56" s="181"/>
+      <c r="B56" s="185"/>
+      <c r="C56" s="185"/>
       <c r="D56" s="74">
         <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="181" t="s">
+      <c r="A57" s="185" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="181"/>
-      <c r="C57" s="181"/>
+      <c r="B57" s="185"/>
+      <c r="C57" s="185"/>
       <c r="D57" s="75">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="181" t="s">
+      <c r="A58" s="185" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="181"/>
-      <c r="C58" s="181"/>
+      <c r="B58" s="185"/>
+      <c r="C58" s="185"/>
       <c r="D58" s="75">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="181" t="s">
+      <c r="A59" s="185" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="181"/>
-      <c r="C59" s="181"/>
+      <c r="B59" s="185"/>
+      <c r="C59" s="185"/>
       <c r="D59" s="75">
         <v>92</v>
       </c>
@@ -22431,28 +22431,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="184" t="s">
+      <c r="A1" s="188" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="185" t="s">
+      <c r="A2" s="189" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="185"/>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
+      <c r="B2" s="189"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="185" t="s">
+      <c r="A3" s="189" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="185"/>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
+      <c r="B3" s="189"/>
+      <c r="C3" s="189"/>
+      <c r="D3" s="189"/>
     </row>
     <row r="4" spans="1:4" s="82" customFormat="1" ht="31.5">
       <c r="A4" s="102" t="s">

</xml_diff>

<commit_message>
Last Update 29-11-2018 11:13:38.86
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Lab Attendance" sheetId="4" r:id="rId4"/>
     <sheet name="UT-2-Satement" sheetId="7" r:id="rId5"/>
     <sheet name="UT-3-Satement" sheetId="8" r:id="rId6"/>
+    <sheet name="Record Submission Status" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attendance!$AZ$1:$AZ$57</definedName>
@@ -1446,7 +1447,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4677" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4985" uniqueCount="182">
   <si>
     <t>S.NO</t>
   </si>
@@ -1957,6 +1958,42 @@
   <si>
     <t>Lab 7</t>
   </si>
+  <si>
+    <t>Lab 8</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Not Completed</t>
+  </si>
+  <si>
+    <t>Not Submitted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Record Status - Batch 1</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Back to Back Writing</t>
+  </si>
+  <si>
+    <t>Flowchart</t>
+  </si>
+  <si>
+    <t>Handwriting Mismatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lokesh R </t>
+  </si>
+  <si>
+    <t>Output written in leftside</t>
+  </si>
+  <si>
+    <t>Result page missing</t>
+  </si>
 </sst>
 </file>
 
@@ -2343,7 +2380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2749,6 +2786,42 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="17" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2758,14 +2831,17 @@
     <xf numFmtId="17" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2794,32 +2870,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2833,17 +2897,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2854,11 +2912,23 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2894,24 +2964,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2934,7 +2986,535 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="80">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -3317,29 +3897,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="18.75">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="136" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="149" t="s">
+      <c r="F1" s="138" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="150"/>
-      <c r="H1" s="150"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="152" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="146" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="152"/>
-      <c r="L1" s="152"/>
-      <c r="M1" s="152"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -3364,41 +3944,41 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:65" ht="19.5">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="155" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="144"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="157"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="136" t="s">
+      <c r="F2" s="141" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="152" t="s">
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="146" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="152"/>
-      <c r="L2" s="152"/>
-      <c r="M2" s="152"/>
-      <c r="N2" s="153" t="s">
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="147" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="153"/>
-      <c r="P2" s="153"/>
-      <c r="Q2" s="153"/>
-      <c r="R2" s="153"/>
-      <c r="S2" s="153"/>
-      <c r="T2" s="153"/>
-      <c r="U2" s="153"/>
-      <c r="V2" s="153"/>
-      <c r="W2" s="153"/>
+      <c r="O2" s="147"/>
+      <c r="P2" s="147"/>
+      <c r="Q2" s="147"/>
+      <c r="R2" s="147"/>
+      <c r="S2" s="147"/>
+      <c r="T2" s="147"/>
+      <c r="U2" s="147"/>
+      <c r="V2" s="147"/>
+      <c r="W2" s="147"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -3411,41 +3991,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:65" ht="18.75">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="146"/>
-      <c r="C3" s="147"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="142"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="136" t="s">
+      <c r="F3" s="141" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="152" t="s">
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="146" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="152"/>
-      <c r="L3" s="152"/>
-      <c r="M3" s="152"/>
-      <c r="N3" s="153" t="s">
+      <c r="K3" s="146"/>
+      <c r="L3" s="146"/>
+      <c r="M3" s="146"/>
+      <c r="N3" s="147" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="153"/>
-      <c r="P3" s="153"/>
-      <c r="Q3" s="153"/>
-      <c r="R3" s="153"/>
-      <c r="S3" s="153"/>
-      <c r="T3" s="153"/>
-      <c r="U3" s="153"/>
-      <c r="V3" s="153"/>
-      <c r="W3" s="153"/>
+      <c r="O3" s="147"/>
+      <c r="P3" s="147"/>
+      <c r="Q3" s="147"/>
+      <c r="R3" s="147"/>
+      <c r="S3" s="147"/>
+      <c r="T3" s="147"/>
+      <c r="U3" s="147"/>
+      <c r="V3" s="147"/>
+      <c r="W3" s="147"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -3458,57 +4038,57 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:65" ht="18.75">
-      <c r="A4" s="145" t="s">
+      <c r="A4" s="136" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="146"/>
-      <c r="C4" s="147"/>
-      <c r="D4" s="131">
+      <c r="B4" s="137"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="143">
         <v>43344</v>
       </c>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="132"/>
-      <c r="K4" s="132"/>
-      <c r="L4" s="132"/>
-      <c r="M4" s="132"/>
-      <c r="N4" s="132"/>
-      <c r="O4" s="132"/>
-      <c r="P4" s="132"/>
-      <c r="Q4" s="132"/>
-      <c r="R4" s="132"/>
-      <c r="S4" s="132"/>
-      <c r="T4" s="132"/>
-      <c r="U4" s="132"/>
-      <c r="V4" s="132"/>
-      <c r="W4" s="133"/>
-      <c r="X4" s="131">
+      <c r="E4" s="144"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144"/>
+      <c r="H4" s="144"/>
+      <c r="I4" s="144"/>
+      <c r="J4" s="144"/>
+      <c r="K4" s="144"/>
+      <c r="L4" s="144"/>
+      <c r="M4" s="144"/>
+      <c r="N4" s="144"/>
+      <c r="O4" s="144"/>
+      <c r="P4" s="144"/>
+      <c r="Q4" s="144"/>
+      <c r="R4" s="144"/>
+      <c r="S4" s="144"/>
+      <c r="T4" s="144"/>
+      <c r="U4" s="144"/>
+      <c r="V4" s="144"/>
+      <c r="W4" s="145"/>
+      <c r="X4" s="143">
         <v>43374</v>
       </c>
-      <c r="Y4" s="132"/>
-      <c r="Z4" s="132"/>
-      <c r="AA4" s="132"/>
-      <c r="AB4" s="132"/>
-      <c r="AC4" s="132"/>
-      <c r="AD4" s="132"/>
-      <c r="AE4" s="132"/>
-      <c r="AF4" s="132"/>
-      <c r="AG4" s="132"/>
-      <c r="AH4" s="132"/>
-      <c r="AI4" s="132"/>
-      <c r="AJ4" s="132"/>
-      <c r="AK4" s="132"/>
-      <c r="AL4" s="132"/>
-      <c r="AM4" s="132"/>
-      <c r="AN4" s="132"/>
-      <c r="AO4" s="132"/>
-      <c r="AP4" s="132"/>
-      <c r="AQ4" s="132"/>
-      <c r="AR4" s="132"/>
-      <c r="AS4" s="133"/>
+      <c r="Y4" s="144"/>
+      <c r="Z4" s="144"/>
+      <c r="AA4" s="144"/>
+      <c r="AB4" s="144"/>
+      <c r="AC4" s="144"/>
+      <c r="AD4" s="144"/>
+      <c r="AE4" s="144"/>
+      <c r="AF4" s="144"/>
+      <c r="AG4" s="144"/>
+      <c r="AH4" s="144"/>
+      <c r="AI4" s="144"/>
+      <c r="AJ4" s="144"/>
+      <c r="AK4" s="144"/>
+      <c r="AL4" s="144"/>
+      <c r="AM4" s="144"/>
+      <c r="AN4" s="144"/>
+      <c r="AO4" s="144"/>
+      <c r="AP4" s="144"/>
+      <c r="AQ4" s="144"/>
+      <c r="AR4" s="144"/>
+      <c r="AS4" s="145"/>
       <c r="AT4" s="59"/>
       <c r="AU4" s="59"/>
       <c r="AV4" s="59"/>
@@ -3531,10 +4111,10 @@
       <c r="BM4" s="59"/>
     </row>
     <row r="5" spans="1:65">
-      <c r="A5" s="148" t="s">
+      <c r="A5" s="158" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="152" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -3718,8 +4298,8 @@
       <c r="BM5" s="59"/>
     </row>
     <row r="6" spans="1:65">
-      <c r="A6" s="148"/>
-      <c r="B6" s="140"/>
+      <c r="A6" s="158"/>
+      <c r="B6" s="153"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -3904,7 +4484,7 @@
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="141"/>
+      <c r="B7" s="154"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -12966,10 +13546,10 @@
       <c r="BM55" s="59"/>
     </row>
     <row r="56" spans="1:65">
-      <c r="A56" s="137" t="s">
+      <c r="A56" s="150" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="138"/>
+      <c r="B56" s="151"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f t="shared" ref="D56:Q56" si="0">COUNTIF(D8:D55,"A")</f>
@@ -13221,10 +13801,10 @@
       </c>
     </row>
     <row r="57" spans="1:65">
-      <c r="A57" s="134" t="s">
+      <c r="A57" s="148" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="135"/>
+      <c r="B57" s="149"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -13477,6 +14057,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="X4:AS4"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F3:I3"/>
@@ -13487,14 +14075,6 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="X4:AS4"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13506,8 +14086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -13523,76 +14103,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="157" t="s">
+      <c r="B1" s="159"/>
+      <c r="C1" s="166" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="157"/>
-      <c r="E1" s="153" t="s">
+      <c r="D1" s="166"/>
+      <c r="E1" s="147" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="153"/>
-      <c r="G1" s="153"/>
-      <c r="H1" s="153"/>
-      <c r="I1" s="153"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
     </row>
     <row r="2" spans="1:9" ht="19.5">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="164" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="157" t="s">
+      <c r="B2" s="164"/>
+      <c r="C2" s="166" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="157"/>
-      <c r="E2" s="153" t="s">
+      <c r="D2" s="166"/>
+      <c r="E2" s="147" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147"/>
+      <c r="I2" s="147"/>
     </row>
     <row r="3" spans="1:9" ht="17.25">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="165" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="156"/>
-      <c r="C3" s="157" t="s">
+      <c r="B3" s="165"/>
+      <c r="C3" s="166" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="157"/>
-      <c r="E3" s="153" t="s">
+      <c r="D3" s="166"/>
+      <c r="E3" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="147"/>
+      <c r="I3" s="147"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="159" t="s">
+      <c r="A4" s="160" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="152" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="154" t="s">
+      <c r="C4" s="163" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="154"/>
-      <c r="E4" s="154"/>
-      <c r="F4" s="154"/>
-      <c r="G4" s="154"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="154"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="163"/>
+      <c r="I4" s="163"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="160"/>
-      <c r="B5" s="140"/>
+      <c r="A5" s="161"/>
+      <c r="B5" s="153"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -13616,8 +14196,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="161"/>
-      <c r="B6" s="141"/>
+      <c r="A6" s="162"/>
+      <c r="B6" s="154"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -13658,7 +14238,9 @@
         <v>31</v>
       </c>
       <c r="G7" s="119"/>
-      <c r="H7" s="42"/>
+      <c r="H7" s="42">
+        <v>35</v>
+      </c>
       <c r="I7" s="42"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1">
@@ -13681,7 +14263,9 @@
         <v>41</v>
       </c>
       <c r="G8" s="121"/>
-      <c r="H8" s="45"/>
+      <c r="H8" s="45">
+        <v>21</v>
+      </c>
       <c r="I8" s="45"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1">
@@ -13704,7 +14288,9 @@
         <v>30</v>
       </c>
       <c r="G9" s="119"/>
-      <c r="H9" s="42"/>
+      <c r="H9" s="42">
+        <v>29</v>
+      </c>
       <c r="I9" s="42"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1">
@@ -13727,7 +14313,9 @@
       <c r="G10" s="119">
         <v>14</v>
       </c>
-      <c r="H10" s="42"/>
+      <c r="H10" s="42">
+        <v>22</v>
+      </c>
       <c r="I10" s="42"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1">
@@ -13748,7 +14336,9 @@
         <v>35</v>
       </c>
       <c r="G11" s="119"/>
-      <c r="H11" s="42"/>
+      <c r="H11" s="42">
+        <v>36</v>
+      </c>
       <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1">
@@ -13771,7 +14361,9 @@
         <v>63</v>
       </c>
       <c r="G12" s="45"/>
-      <c r="H12" s="42"/>
+      <c r="H12" s="42">
+        <v>12</v>
+      </c>
       <c r="I12" s="42"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
@@ -13792,7 +14384,9 @@
         <v>41</v>
       </c>
       <c r="G13" s="119"/>
-      <c r="H13" s="42"/>
+      <c r="H13" s="42">
+        <v>40</v>
+      </c>
       <c r="I13" s="42"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
@@ -13813,7 +14407,9 @@
         <v>35</v>
       </c>
       <c r="G14" s="119"/>
-      <c r="H14" s="42"/>
+      <c r="H14" s="42">
+        <v>36</v>
+      </c>
       <c r="I14" s="42"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1">
@@ -13838,7 +14434,9 @@
       <c r="G15" s="119">
         <v>20</v>
       </c>
-      <c r="H15" s="42"/>
+      <c r="H15" s="42">
+        <v>22</v>
+      </c>
       <c r="I15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1">
@@ -13859,7 +14457,9 @@
         <v>27</v>
       </c>
       <c r="G16" s="119"/>
-      <c r="H16" s="42"/>
+      <c r="H16" s="42">
+        <v>23</v>
+      </c>
       <c r="I16" s="42"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1">
@@ -13880,7 +14480,9 @@
         <v>39</v>
       </c>
       <c r="G17" s="119"/>
-      <c r="H17" s="42"/>
+      <c r="H17" s="42">
+        <v>33</v>
+      </c>
       <c r="I17" s="42"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1">
@@ -13903,7 +14505,9 @@
         <v>25</v>
       </c>
       <c r="G18" s="119"/>
-      <c r="H18" s="42"/>
+      <c r="H18" s="42">
+        <v>26</v>
+      </c>
       <c r="I18" s="42"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1">
@@ -13924,7 +14528,9 @@
         <v>29</v>
       </c>
       <c r="G19" s="119"/>
-      <c r="H19" s="42"/>
+      <c r="H19" s="42">
+        <v>29</v>
+      </c>
       <c r="I19" s="42"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1">
@@ -13945,7 +14551,9 @@
         <v>30</v>
       </c>
       <c r="G20" s="119"/>
-      <c r="H20" s="42"/>
+      <c r="H20" s="42">
+        <v>8</v>
+      </c>
       <c r="I20" s="42"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1">
@@ -13970,7 +14578,9 @@
       <c r="G21" s="119">
         <v>20</v>
       </c>
-      <c r="H21" s="42"/>
+      <c r="H21" s="45" t="s">
+        <v>63</v>
+      </c>
       <c r="I21" s="42"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1">
@@ -13993,7 +14603,9 @@
         <v>39</v>
       </c>
       <c r="G22" s="119"/>
-      <c r="H22" s="42"/>
+      <c r="H22" s="42">
+        <v>13</v>
+      </c>
       <c r="I22" s="42"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1">
@@ -14016,7 +14628,9 @@
         <v>26</v>
       </c>
       <c r="G23" s="121"/>
-      <c r="H23" s="45"/>
+      <c r="H23" s="131">
+        <v>28</v>
+      </c>
       <c r="I23" s="45"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1">
@@ -14037,7 +14651,9 @@
         <v>32</v>
       </c>
       <c r="G24" s="119"/>
-      <c r="H24" s="42"/>
+      <c r="H24" s="42">
+        <v>25</v>
+      </c>
       <c r="I24" s="42"/>
     </row>
     <row r="25" spans="1:9" ht="15" customHeight="1">
@@ -14058,7 +14674,9 @@
         <v>45</v>
       </c>
       <c r="G25" s="119"/>
-      <c r="H25" s="42"/>
+      <c r="H25" s="42">
+        <v>31</v>
+      </c>
       <c r="I25" s="42"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1">
@@ -14079,7 +14697,9 @@
         <v>45</v>
       </c>
       <c r="G26" s="119"/>
-      <c r="H26" s="42"/>
+      <c r="H26" s="42">
+        <v>42</v>
+      </c>
       <c r="I26" s="42"/>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1">
@@ -14102,7 +14722,9 @@
         <v>12</v>
       </c>
       <c r="G27" s="119"/>
-      <c r="H27" s="42"/>
+      <c r="H27" s="42">
+        <v>25</v>
+      </c>
       <c r="I27" s="42"/>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1">
@@ -14123,7 +14745,9 @@
         <v>32</v>
       </c>
       <c r="G28" s="119"/>
-      <c r="H28" s="42"/>
+      <c r="H28" s="42">
+        <v>31</v>
+      </c>
       <c r="I28" s="42"/>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1">
@@ -14146,7 +14770,9 @@
         <v>30</v>
       </c>
       <c r="G29" s="119"/>
-      <c r="H29" s="42"/>
+      <c r="H29" s="42">
+        <v>26</v>
+      </c>
       <c r="I29" s="42"/>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1">
@@ -14167,7 +14793,9 @@
         <v>25</v>
       </c>
       <c r="G30" s="119"/>
-      <c r="H30" s="42"/>
+      <c r="H30" s="42">
+        <v>13</v>
+      </c>
       <c r="I30" s="42"/>
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1">
@@ -14190,7 +14818,9 @@
         <v>31</v>
       </c>
       <c r="G31" s="119"/>
-      <c r="H31" s="42"/>
+      <c r="H31" s="42">
+        <v>12</v>
+      </c>
       <c r="I31" s="42"/>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1">
@@ -14211,7 +14841,9 @@
         <v>46</v>
       </c>
       <c r="G32" s="119"/>
-      <c r="H32" s="42"/>
+      <c r="H32" s="42">
+        <v>46</v>
+      </c>
       <c r="I32" s="42"/>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1">
@@ -14234,7 +14866,9 @@
         <v>22</v>
       </c>
       <c r="G33" s="119"/>
-      <c r="H33" s="42"/>
+      <c r="H33" s="45" t="s">
+        <v>63</v>
+      </c>
       <c r="I33" s="42"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1">
@@ -14255,7 +14889,9 @@
         <v>44</v>
       </c>
       <c r="G34" s="119"/>
-      <c r="H34" s="42"/>
+      <c r="H34" s="42">
+        <v>49</v>
+      </c>
       <c r="I34" s="42"/>
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1">
@@ -14276,7 +14912,9 @@
         <v>37</v>
       </c>
       <c r="G35" s="119"/>
-      <c r="H35" s="42"/>
+      <c r="H35" s="42">
+        <v>39</v>
+      </c>
       <c r="I35" s="42"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1">
@@ -14299,7 +14937,9 @@
         <v>17</v>
       </c>
       <c r="G36" s="119"/>
-      <c r="H36" s="42"/>
+      <c r="H36" s="42">
+        <v>13</v>
+      </c>
       <c r="I36" s="42"/>
     </row>
     <row r="37" spans="1:9" ht="15" customHeight="1">
@@ -14320,7 +14960,9 @@
         <v>43</v>
       </c>
       <c r="G37" s="119"/>
-      <c r="H37" s="42"/>
+      <c r="H37" s="42">
+        <v>47</v>
+      </c>
       <c r="I37" s="42"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1">
@@ -14341,7 +14983,9 @@
         <v>42</v>
       </c>
       <c r="G38" s="119"/>
-      <c r="H38" s="42"/>
+      <c r="H38" s="42">
+        <v>39</v>
+      </c>
       <c r="I38" s="42"/>
     </row>
     <row r="39" spans="1:9" ht="15" customHeight="1">
@@ -14364,7 +15008,9 @@
         <v>31</v>
       </c>
       <c r="G39" s="119"/>
-      <c r="H39" s="42"/>
+      <c r="H39" s="42">
+        <v>33</v>
+      </c>
       <c r="I39" s="42"/>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1">
@@ -14385,7 +15031,9 @@
         <v>38</v>
       </c>
       <c r="G40" s="119"/>
-      <c r="H40" s="42"/>
+      <c r="H40" s="42">
+        <v>35</v>
+      </c>
       <c r="I40" s="42"/>
     </row>
     <row r="41" spans="1:9" ht="15" customHeight="1">
@@ -14408,7 +15056,9 @@
       <c r="G41" s="119">
         <v>18</v>
       </c>
-      <c r="H41" s="42"/>
+      <c r="H41" s="42">
+        <v>34</v>
+      </c>
       <c r="I41" s="42"/>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1">
@@ -14431,7 +15081,9 @@
         <v>15</v>
       </c>
       <c r="G42" s="119"/>
-      <c r="H42" s="42"/>
+      <c r="H42" s="42">
+        <v>25</v>
+      </c>
       <c r="I42" s="42"/>
     </row>
     <row r="43" spans="1:9" ht="15" customHeight="1">
@@ -14454,7 +15106,9 @@
         <v>27</v>
       </c>
       <c r="G43" s="119"/>
-      <c r="H43" s="42"/>
+      <c r="H43" s="45" t="s">
+        <v>63</v>
+      </c>
       <c r="I43" s="42"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1">
@@ -14479,7 +15133,9 @@
       <c r="G44" s="119">
         <v>20</v>
       </c>
-      <c r="H44" s="42"/>
+      <c r="H44" s="42">
+        <v>21</v>
+      </c>
       <c r="I44" s="42"/>
     </row>
     <row r="45" spans="1:9" ht="15" customHeight="1">
@@ -14500,7 +15156,9 @@
         <v>25</v>
       </c>
       <c r="G45" s="119"/>
-      <c r="H45" s="42"/>
+      <c r="H45" s="42">
+        <v>27</v>
+      </c>
       <c r="I45" s="42"/>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1">
@@ -14523,7 +15181,9 @@
       <c r="G46" s="119">
         <v>20</v>
       </c>
-      <c r="H46" s="42"/>
+      <c r="H46" s="42">
+        <v>32</v>
+      </c>
       <c r="I46" s="42"/>
     </row>
     <row r="47" spans="1:9" ht="15" customHeight="1">
@@ -14546,7 +15206,9 @@
         <v>30</v>
       </c>
       <c r="G47" s="119"/>
-      <c r="H47" s="42"/>
+      <c r="H47" s="45" t="s">
+        <v>63</v>
+      </c>
       <c r="I47" s="42"/>
     </row>
     <row r="48" spans="1:9" ht="15" customHeight="1">
@@ -14569,7 +15231,9 @@
         <v>25</v>
       </c>
       <c r="G48" s="119"/>
-      <c r="H48" s="42"/>
+      <c r="H48" s="42">
+        <v>36</v>
+      </c>
       <c r="I48" s="42"/>
     </row>
     <row r="49" spans="1:9">
@@ -14590,7 +15254,9 @@
         <v>34</v>
       </c>
       <c r="G49" s="119"/>
-      <c r="H49" s="42"/>
+      <c r="H49" s="42">
+        <v>44</v>
+      </c>
       <c r="I49" s="42"/>
     </row>
     <row r="50" spans="1:9">
@@ -14611,7 +15277,9 @@
         <v>29</v>
       </c>
       <c r="G50" s="119"/>
-      <c r="H50" s="42"/>
+      <c r="H50" s="42">
+        <v>40</v>
+      </c>
       <c r="I50" s="42"/>
     </row>
     <row r="51" spans="1:9">
@@ -14632,7 +15300,9 @@
         <v>17</v>
       </c>
       <c r="G51" s="119"/>
-      <c r="H51" s="42"/>
+      <c r="H51" s="42">
+        <v>19</v>
+      </c>
       <c r="I51" s="42"/>
     </row>
     <row r="52" spans="1:9">
@@ -14653,7 +15323,9 @@
         <v>33</v>
       </c>
       <c r="G52" s="119"/>
-      <c r="H52" s="42"/>
+      <c r="H52" s="42">
+        <v>36</v>
+      </c>
       <c r="I52" s="42"/>
     </row>
     <row r="53" spans="1:9">
@@ -14674,7 +15346,9 @@
         <v>29</v>
       </c>
       <c r="G53" s="119"/>
-      <c r="H53" s="42"/>
+      <c r="H53" s="42">
+        <v>33</v>
+      </c>
       <c r="I53" s="42"/>
     </row>
     <row r="54" spans="1:9">
@@ -14695,14 +15369,16 @@
         <v>45</v>
       </c>
       <c r="G54" s="119"/>
-      <c r="H54" s="42"/>
+      <c r="H54" s="42">
+        <v>49</v>
+      </c>
       <c r="I54" s="42"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="137" t="s">
+      <c r="A55" s="150" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="138"/>
+      <c r="B55" s="151"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -14719,10 +15395,10 @@
       <c r="I55" s="13"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="134" t="s">
+      <c r="A56" s="148" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="135"/>
+      <c r="B56" s="149"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -14739,10 +15415,10 @@
       <c r="I56" s="13"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="134" t="s">
+      <c r="A57" s="148" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="135"/>
+      <c r="B57" s="149"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -14759,10 +15435,10 @@
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="134" t="s">
+      <c r="A58" s="148" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="135"/>
+      <c r="B58" s="149"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -14780,13 +15456,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -14796,9 +15465,16 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="E1:I1"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:I54">
-    <cfRule type="cellIs" dxfId="5" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="17" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14811,7 +15487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -14829,72 +15505,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="157" t="s">
+      <c r="B1" s="159"/>
+      <c r="C1" s="166" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="157"/>
-      <c r="E1" s="165" t="s">
+      <c r="D1" s="166"/>
+      <c r="E1" s="167" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="166"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="168"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="164" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="157" t="s">
+      <c r="B2" s="164"/>
+      <c r="C2" s="166" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="157"/>
-      <c r="E2" s="153" t="s">
+      <c r="D2" s="166"/>
+      <c r="E2" s="147" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="165" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="156"/>
-      <c r="C3" s="157" t="s">
+      <c r="B3" s="165"/>
+      <c r="C3" s="166" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="157"/>
-      <c r="E3" s="153" t="s">
+      <c r="D3" s="166"/>
+      <c r="E3" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="147"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="159" t="s">
+      <c r="A4" s="160" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="152" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="162" t="s">
+      <c r="C4" s="169" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="164"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
+      <c r="H4" s="171"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="160"/>
-      <c r="B5" s="140"/>
+      <c r="A5" s="161"/>
+      <c r="B5" s="153"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -14915,8 +15591,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="161"/>
-      <c r="B6" s="141"/>
+      <c r="A6" s="162"/>
+      <c r="B6" s="154"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -16041,10 +16717,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="137" t="s">
+      <c r="A55" s="150" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="138"/>
+      <c r="B55" s="151"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -16059,10 +16735,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="134" t="s">
+      <c r="A56" s="148" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="135"/>
+      <c r="B56" s="149"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -16077,10 +16753,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="134" t="s">
+      <c r="A57" s="148" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="135"/>
+      <c r="B57" s="149"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -16095,10 +16771,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="134" t="s">
+      <c r="A58" s="148" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="135"/>
+      <c r="B58" s="149"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -16114,35 +16790,35 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="3" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="77" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16153,10 +16829,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF58"/>
+  <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AI6" sqref="AI6"/>
+    <sheetView topLeftCell="B52" workbookViewId="0">
+      <selection activeCell="AK57" sqref="AK57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -16164,227 +16840,233 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
-    <col min="4" max="32" width="4.140625" style="2" customWidth="1"/>
-    <col min="33" max="33" width="4.85546875" style="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="35" width="4.140625" style="2" customWidth="1"/>
+    <col min="36" max="36" width="4.85546875" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="145" t="s">
+    <row r="1" spans="1:36" ht="18.75">
+      <c r="A1" s="136" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="149" t="s">
+      <c r="F1" s="138" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="150"/>
-      <c r="H1" s="150"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="152" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="146" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="152"/>
-      <c r="L1" s="152"/>
-      <c r="M1" s="152"/>
-      <c r="N1" s="167" t="s">
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="178" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="168"/>
-      <c r="P1" s="168"/>
-      <c r="Q1" s="168"/>
-      <c r="R1" s="168"/>
-      <c r="S1" s="168"/>
-      <c r="T1" s="168"/>
-      <c r="U1" s="168"/>
-      <c r="V1" s="168"/>
-      <c r="W1" s="168"/>
-      <c r="X1" s="168"/>
-      <c r="Y1" s="168"/>
-      <c r="Z1" s="168"/>
-      <c r="AA1" s="168"/>
-      <c r="AB1" s="168"/>
-    </row>
-    <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="142" t="s">
+      <c r="O1" s="179"/>
+      <c r="P1" s="179"/>
+      <c r="Q1" s="179"/>
+      <c r="R1" s="179"/>
+      <c r="S1" s="179"/>
+      <c r="T1" s="179"/>
+      <c r="U1" s="179"/>
+      <c r="V1" s="179"/>
+      <c r="W1" s="179"/>
+      <c r="X1" s="179"/>
+      <c r="Y1" s="179"/>
+      <c r="Z1" s="179"/>
+      <c r="AA1" s="179"/>
+      <c r="AB1" s="179"/>
+    </row>
+    <row r="2" spans="1:36" ht="19.5">
+      <c r="A2" s="155" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="144"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="157"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="136" t="s">
+      <c r="F2" s="141" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="152" t="s">
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="146" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="152"/>
-      <c r="L2" s="152"/>
-      <c r="M2" s="152"/>
-      <c r="N2" s="167" t="s">
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="178" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="168"/>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="168"/>
-      <c r="R2" s="168"/>
-      <c r="S2" s="168"/>
-      <c r="T2" s="168"/>
-      <c r="U2" s="168"/>
-      <c r="V2" s="168"/>
-      <c r="W2" s="168"/>
-      <c r="X2" s="168"/>
-      <c r="Y2" s="168"/>
-      <c r="Z2" s="168"/>
-      <c r="AA2" s="168"/>
-      <c r="AB2" s="168"/>
-    </row>
-    <row r="3" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A3" s="170" t="s">
+      <c r="O2" s="179"/>
+      <c r="P2" s="179"/>
+      <c r="Q2" s="179"/>
+      <c r="R2" s="179"/>
+      <c r="S2" s="179"/>
+      <c r="T2" s="179"/>
+      <c r="U2" s="179"/>
+      <c r="V2" s="179"/>
+      <c r="W2" s="179"/>
+      <c r="X2" s="179"/>
+      <c r="Y2" s="179"/>
+      <c r="Z2" s="179"/>
+      <c r="AA2" s="179"/>
+      <c r="AB2" s="179"/>
+    </row>
+    <row r="3" spans="1:36" ht="18.75" customHeight="1">
+      <c r="A3" s="181" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="171"/>
-      <c r="C3" s="172"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="183"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="169" t="s">
+      <c r="F3" s="180" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="178" t="s">
+      <c r="G3" s="180"/>
+      <c r="H3" s="180"/>
+      <c r="I3" s="180"/>
+      <c r="J3" s="189" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="178"/>
-      <c r="L3" s="178"/>
-      <c r="M3" s="178"/>
-      <c r="N3" s="167" t="s">
+      <c r="K3" s="189"/>
+      <c r="L3" s="189"/>
+      <c r="M3" s="189"/>
+      <c r="N3" s="178" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="168"/>
-      <c r="P3" s="168"/>
-      <c r="Q3" s="168"/>
-      <c r="R3" s="168"/>
-      <c r="S3" s="168"/>
-      <c r="T3" s="168"/>
-      <c r="U3" s="168"/>
-      <c r="V3" s="168"/>
-      <c r="W3" s="168"/>
-      <c r="X3" s="168"/>
-      <c r="Y3" s="168"/>
-      <c r="Z3" s="168"/>
-      <c r="AA3" s="168"/>
-      <c r="AB3" s="168"/>
-    </row>
-    <row r="4" spans="1:32" ht="18.75" customHeight="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="175"/>
-      <c r="D4" s="176">
+      <c r="O3" s="179"/>
+      <c r="P3" s="179"/>
+      <c r="Q3" s="179"/>
+      <c r="R3" s="179"/>
+      <c r="S3" s="179"/>
+      <c r="T3" s="179"/>
+      <c r="U3" s="179"/>
+      <c r="V3" s="179"/>
+      <c r="W3" s="179"/>
+      <c r="X3" s="179"/>
+      <c r="Y3" s="179"/>
+      <c r="Z3" s="179"/>
+      <c r="AA3" s="179"/>
+      <c r="AB3" s="179"/>
+    </row>
+    <row r="4" spans="1:36" ht="18.75" customHeight="1">
+      <c r="A4" s="184"/>
+      <c r="B4" s="185"/>
+      <c r="C4" s="186"/>
+      <c r="D4" s="187">
         <v>43344</v>
       </c>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="177"/>
-      <c r="J4" s="177"/>
-      <c r="K4" s="177"/>
-      <c r="L4" s="177"/>
-      <c r="M4" s="177"/>
-      <c r="N4" s="176">
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="188"/>
+      <c r="J4" s="188"/>
+      <c r="K4" s="188"/>
+      <c r="L4" s="188"/>
+      <c r="M4" s="188"/>
+      <c r="N4" s="187">
         <v>43374</v>
       </c>
-      <c r="O4" s="177"/>
-      <c r="P4" s="177"/>
-      <c r="Q4" s="177"/>
-      <c r="R4" s="177"/>
-      <c r="S4" s="177"/>
-      <c r="T4" s="177"/>
-      <c r="U4" s="177"/>
+      <c r="O4" s="188"/>
+      <c r="P4" s="188"/>
+      <c r="Q4" s="188"/>
+      <c r="R4" s="188"/>
+      <c r="S4" s="188"/>
+      <c r="T4" s="188"/>
+      <c r="U4" s="188"/>
       <c r="V4" s="53"/>
       <c r="W4" s="53"/>
     </row>
-    <row r="5" spans="1:32">
-      <c r="A5" s="159" t="s">
+    <row r="5" spans="1:36">
+      <c r="A5" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="152" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="179" t="s">
+      <c r="D5" s="175" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="180"/>
-      <c r="F5" s="180"/>
-      <c r="G5" s="181"/>
-      <c r="H5" s="182" t="s">
+      <c r="E5" s="176"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="173" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="183"/>
-      <c r="J5" s="183"/>
-      <c r="K5" s="183"/>
-      <c r="L5" s="184" t="s">
+      <c r="I5" s="174"/>
+      <c r="J5" s="174"/>
+      <c r="K5" s="174"/>
+      <c r="L5" s="172" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="184"/>
-      <c r="N5" s="182" t="s">
+      <c r="M5" s="172"/>
+      <c r="N5" s="173" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="183"/>
-      <c r="P5" s="183"/>
-      <c r="Q5" s="183"/>
-      <c r="R5" s="184" t="s">
+      <c r="O5" s="174"/>
+      <c r="P5" s="174"/>
+      <c r="Q5" s="174"/>
+      <c r="R5" s="172" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="184"/>
-      <c r="T5" s="148" t="s">
+      <c r="S5" s="172"/>
+      <c r="T5" s="158" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="148" t="s">
+      <c r="U5" s="158"/>
+      <c r="V5" s="158" t="s">
         <v>117</v>
       </c>
-      <c r="W5" s="148"/>
-      <c r="X5" s="148"/>
-      <c r="Y5" s="148"/>
-      <c r="Z5" s="148" t="s">
+      <c r="W5" s="158"/>
+      <c r="X5" s="158"/>
+      <c r="Y5" s="158"/>
+      <c r="Z5" s="158" t="s">
         <v>118</v>
       </c>
-      <c r="AA5" s="148"/>
-      <c r="AB5" s="148"/>
-      <c r="AC5" s="148"/>
-      <c r="AD5" s="148" t="s">
+      <c r="AA5" s="158"/>
+      <c r="AB5" s="158"/>
+      <c r="AC5" s="158"/>
+      <c r="AD5" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="AE5" s="148"/>
-      <c r="AF5" s="148"/>
-    </row>
-    <row r="6" spans="1:32">
-      <c r="A6" s="160"/>
-      <c r="B6" s="140"/>
+      <c r="AE5" s="158"/>
+      <c r="AF5" s="158"/>
+      <c r="AG5" s="158" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH5" s="158"/>
+      <c r="AI5" s="158"/>
+      <c r="AJ5" s="158"/>
+    </row>
+    <row r="6" spans="1:36">
+      <c r="A6" s="161"/>
+      <c r="B6" s="153"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -16475,10 +17157,22 @@
       <c r="AF6" s="19">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:32">
-      <c r="A7" s="160"/>
-      <c r="B7" s="140"/>
+      <c r="AG6" s="131">
+        <v>11</v>
+      </c>
+      <c r="AH6" s="131">
+        <v>11</v>
+      </c>
+      <c r="AI6" s="131">
+        <v>11</v>
+      </c>
+      <c r="AJ6" s="131">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36">
+      <c r="A7" s="161"/>
+      <c r="B7" s="153"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -16569,10 +17263,22 @@
       <c r="AF7" s="19">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="161"/>
-      <c r="B8" s="141"/>
+      <c r="AG7" s="131">
+        <v>27</v>
+      </c>
+      <c r="AH7" s="131">
+        <v>27</v>
+      </c>
+      <c r="AI7" s="131">
+        <v>27</v>
+      </c>
+      <c r="AJ7" s="131">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" ht="15" customHeight="1">
+      <c r="A8" s="162"/>
+      <c r="B8" s="154"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -16663,8 +17369,20 @@
       <c r="AF8" s="19">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:32" ht="15" customHeight="1">
+      <c r="AG8" s="131">
+        <v>5</v>
+      </c>
+      <c r="AH8" s="131">
+        <v>5</v>
+      </c>
+      <c r="AI8" s="131">
+        <v>5</v>
+      </c>
+      <c r="AJ8" s="131">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" ht="15" customHeight="1">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -16759,8 +17477,20 @@
       <c r="AF9" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:32" ht="15" customHeight="1">
+      <c r="AG9" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH9" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI9" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ9" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" ht="15" customHeight="1">
       <c r="A10" s="3">
         <v>2</v>
       </c>
@@ -16855,8 +17585,20 @@
       <c r="AF10" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:32" ht="15" customHeight="1">
+      <c r="AG10" s="132" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH10" s="132" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI10" s="132" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ10" s="132" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" ht="15" customHeight="1">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -16951,8 +17693,20 @@
       <c r="AF11" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:32" ht="15" customHeight="1">
+      <c r="AG11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ11" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" ht="15" customHeight="1">
       <c r="A12" s="3">
         <v>4</v>
       </c>
@@ -17047,8 +17801,20 @@
       <c r="AF12" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:32" ht="15" customHeight="1">
+      <c r="AG12" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH12" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI12" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ12" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" ht="15" customHeight="1">
       <c r="A13" s="3">
         <v>5</v>
       </c>
@@ -17143,8 +17909,20 @@
       <c r="AF13" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:32" ht="15" customHeight="1">
+      <c r="AG13" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH13" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI13" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ13" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" ht="15" customHeight="1">
       <c r="A14" s="3">
         <v>6</v>
       </c>
@@ -17239,8 +18017,20 @@
       <c r="AF14" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:32" ht="15" customHeight="1">
+      <c r="AG14" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH14" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI14" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ14" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" ht="15" customHeight="1">
       <c r="A15" s="3">
         <v>7</v>
       </c>
@@ -17335,8 +18125,20 @@
       <c r="AF15" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:32" ht="15" customHeight="1">
+      <c r="AG15" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH15" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI15" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ15" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" ht="15" customHeight="1">
       <c r="A16" s="3">
         <v>8</v>
       </c>
@@ -17431,8 +18233,20 @@
       <c r="AF16" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" ht="15" customHeight="1">
+      <c r="AG16" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH16" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI16" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ16" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" ht="15" customHeight="1">
       <c r="A17" s="3">
         <v>9</v>
       </c>
@@ -17527,8 +18341,20 @@
       <c r="AF17" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:32" ht="15" customHeight="1">
+      <c r="AG17" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH17" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI17" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ17" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" ht="15" customHeight="1">
       <c r="A18" s="3">
         <v>10</v>
       </c>
@@ -17623,8 +18449,20 @@
       <c r="AF18" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="19" spans="1:32" ht="15" customHeight="1">
+      <c r="AG18" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH18" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI18" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ18" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" ht="15" customHeight="1">
       <c r="A19" s="3">
         <v>11</v>
       </c>
@@ -17719,8 +18557,20 @@
       <c r="AF19" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" ht="15" customHeight="1">
+      <c r="AG19" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH19" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI19" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ19" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" ht="15" customHeight="1">
       <c r="A20" s="3">
         <v>12</v>
       </c>
@@ -17815,8 +18665,20 @@
       <c r="AF20" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:32" ht="15" customHeight="1">
+      <c r="AG20" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH20" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI20" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ20" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" ht="15" customHeight="1">
       <c r="A21" s="3">
         <v>13</v>
       </c>
@@ -17911,8 +18773,20 @@
       <c r="AF21" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="1:32" ht="15" customHeight="1">
+      <c r="AG21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ21" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" ht="15" customHeight="1">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -18007,8 +18881,20 @@
       <c r="AF22" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:32" ht="15" customHeight="1">
+      <c r="AG22" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH22" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI22" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ22" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" ht="15" customHeight="1">
       <c r="A23" s="3">
         <v>15</v>
       </c>
@@ -18103,8 +18989,20 @@
       <c r="AF23" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="1:32" ht="15" customHeight="1">
+      <c r="AG23" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH23" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI23" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ23" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" ht="15" customHeight="1">
       <c r="A24" s="3">
         <v>16</v>
       </c>
@@ -18199,8 +19097,20 @@
       <c r="AF24" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="25" spans="1:32" ht="15" customHeight="1">
+      <c r="AG24" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH24" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI24" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ24" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" ht="15" customHeight="1">
       <c r="A25" s="3">
         <v>17</v>
       </c>
@@ -18295,8 +19205,20 @@
       <c r="AF25" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:32" ht="15" customHeight="1">
+      <c r="AG25" s="132" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH25" s="132" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI25" s="132" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ25" s="132" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" ht="15" customHeight="1">
       <c r="A26" s="3">
         <v>18</v>
       </c>
@@ -18391,8 +19313,20 @@
       <c r="AF26" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:32" ht="15" customHeight="1">
+      <c r="AG26" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH26" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI26" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ26" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" ht="15" customHeight="1">
       <c r="A27" s="3">
         <v>19</v>
       </c>
@@ -18487,8 +19421,20 @@
       <c r="AF27" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:32" ht="15" customHeight="1">
+      <c r="AG27" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH27" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI27" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ27" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" ht="15" customHeight="1">
       <c r="A28" s="3">
         <v>20</v>
       </c>
@@ -18583,8 +19529,20 @@
       <c r="AF28" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:32" ht="15" customHeight="1">
+      <c r="AG28" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH28" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI28" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ28" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" ht="15" customHeight="1">
       <c r="A29" s="3">
         <v>21</v>
       </c>
@@ -18679,8 +19637,20 @@
       <c r="AF29" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="1:32" ht="15" customHeight="1">
+      <c r="AG29" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH29" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI29" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ29" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" ht="15" customHeight="1">
       <c r="A30" s="3">
         <v>22</v>
       </c>
@@ -18775,8 +19745,20 @@
       <c r="AF30" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:32" ht="15" customHeight="1">
+      <c r="AG30" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH30" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI30" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ30" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" ht="15" customHeight="1">
       <c r="A31" s="3">
         <v>23</v>
       </c>
@@ -18871,8 +19853,20 @@
       <c r="AF31" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="32" spans="1:32" ht="15" customHeight="1">
+      <c r="AG31" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH31" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI31" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ31" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" ht="15" customHeight="1">
       <c r="A32" s="3">
         <v>24</v>
       </c>
@@ -18967,8 +19961,20 @@
       <c r="AF32" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" spans="1:32" ht="15" customHeight="1">
+      <c r="AG32" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH32" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI32" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ32" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" ht="15" customHeight="1">
       <c r="A33" s="3">
         <v>25</v>
       </c>
@@ -19063,8 +20069,20 @@
       <c r="AF33" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:32" ht="15" customHeight="1">
+      <c r="AG33" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH33" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI33" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ33" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" ht="15" customHeight="1">
       <c r="A34" s="3">
         <v>26</v>
       </c>
@@ -19159,8 +20177,20 @@
       <c r="AF34" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="35" spans="1:32" ht="15" customHeight="1">
+      <c r="AG34" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH34" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI34" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ34" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" ht="15" customHeight="1">
       <c r="A35" s="3">
         <v>27</v>
       </c>
@@ -19255,8 +20285,20 @@
       <c r="AF35" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:32" ht="15" customHeight="1">
+      <c r="AG35" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH35" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI35" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ35" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" ht="15" customHeight="1">
       <c r="A36" s="3">
         <v>28</v>
       </c>
@@ -19351,8 +20393,20 @@
       <c r="AF36" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="37" spans="1:32" ht="15" customHeight="1">
+      <c r="AG36" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH36" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI36" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ36" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" ht="15" customHeight="1">
       <c r="A37" s="3">
         <v>29</v>
       </c>
@@ -19447,8 +20501,20 @@
       <c r="AF37" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="38" spans="1:32" ht="15" customHeight="1">
+      <c r="AG37" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH37" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI37" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ37" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" ht="15" customHeight="1">
       <c r="A38" s="3">
         <v>30</v>
       </c>
@@ -19543,8 +20609,20 @@
       <c r="AF38" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="39" spans="1:32" ht="15" customHeight="1">
+      <c r="AG38" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH38" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI38" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ38" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" ht="15" customHeight="1">
       <c r="A39" s="3">
         <v>31</v>
       </c>
@@ -19639,8 +20717,20 @@
       <c r="AF39" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="40" spans="1:32" ht="15" customHeight="1">
+      <c r="AG39" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH39" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI39" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ39" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" ht="15" customHeight="1">
       <c r="A40" s="3">
         <v>32</v>
       </c>
@@ -19735,8 +20825,20 @@
       <c r="AF40" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="41" spans="1:32" ht="15" customHeight="1">
+      <c r="AG40" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH40" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI40" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ40" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" ht="15" customHeight="1">
       <c r="A41" s="3">
         <v>33</v>
       </c>
@@ -19831,8 +20933,20 @@
       <c r="AF41" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="42" spans="1:32" ht="15" customHeight="1">
+      <c r="AG41" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH41" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI41" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ41" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36" ht="15" customHeight="1">
       <c r="A42" s="3">
         <v>34</v>
       </c>
@@ -19927,8 +21041,20 @@
       <c r="AF42" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="43" spans="1:32" ht="15" customHeight="1">
+      <c r="AG42" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH42" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI42" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ42" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36" ht="15" customHeight="1">
       <c r="A43" s="3">
         <v>35</v>
       </c>
@@ -20023,8 +21149,20 @@
       <c r="AF43" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="44" spans="1:32" ht="15" customHeight="1">
+      <c r="AG43" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH43" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI43" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ43" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:36" ht="15" customHeight="1">
       <c r="A44" s="3">
         <v>36</v>
       </c>
@@ -20119,8 +21257,20 @@
       <c r="AF44" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="45" spans="1:32" ht="15" customHeight="1">
+      <c r="AG44" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH44" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI44" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ44" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:36" ht="15" customHeight="1">
       <c r="A45" s="3">
         <v>37</v>
       </c>
@@ -20215,8 +21365,20 @@
       <c r="AF45" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:32" ht="15" customHeight="1">
+      <c r="AG45" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH45" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI45" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ45" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:36" ht="15" customHeight="1">
       <c r="A46" s="3">
         <v>38</v>
       </c>
@@ -20311,8 +21473,20 @@
       <c r="AF46" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="47" spans="1:32" ht="15" customHeight="1">
+      <c r="AG46" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH46" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI46" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ46" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36" ht="15" customHeight="1">
       <c r="A47" s="3">
         <v>39</v>
       </c>
@@ -20407,8 +21581,20 @@
       <c r="AF47" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:32" ht="15" customHeight="1">
+      <c r="AG47" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH47" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI47" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ47" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:36" ht="15" customHeight="1">
       <c r="A48" s="3">
         <v>40</v>
       </c>
@@ -20503,8 +21689,20 @@
       <c r="AF48" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="49" spans="1:32" ht="15" customHeight="1">
+      <c r="AG48" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH48" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI48" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ48" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:36" ht="15" customHeight="1">
       <c r="A49" s="3">
         <v>41</v>
       </c>
@@ -20599,8 +21797,20 @@
       <c r="AF49" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="50" spans="1:32" ht="15" customHeight="1">
+      <c r="AG49" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH49" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI49" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ49" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:36" ht="15" customHeight="1">
       <c r="A50" s="3">
         <v>42</v>
       </c>
@@ -20695,8 +21905,20 @@
       <c r="AF50" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="51" spans="1:32" ht="15" customHeight="1">
+      <c r="AG50" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH50" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI50" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ50" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:36" ht="15" customHeight="1">
       <c r="A51" s="3">
         <v>43</v>
       </c>
@@ -20791,8 +22013,20 @@
       <c r="AF51" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="52" spans="1:32" ht="15" customHeight="1">
+      <c r="AG51" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH51" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI51" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ51" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:36" ht="15" customHeight="1">
       <c r="A52" s="3">
         <v>44</v>
       </c>
@@ -20887,8 +22121,20 @@
       <c r="AF52" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="53" spans="1:32" ht="15" customHeight="1">
+      <c r="AG52" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH52" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI52" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ52" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" ht="15" customHeight="1">
       <c r="A53" s="3">
         <v>45</v>
       </c>
@@ -20983,8 +22229,20 @@
       <c r="AF53" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="54" spans="1:32" ht="15" customHeight="1">
+      <c r="AG53" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH53" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI53" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ53" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" ht="15" customHeight="1">
       <c r="A54" s="3">
         <v>46</v>
       </c>
@@ -21079,8 +22337,20 @@
       <c r="AF54" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:32" ht="15" customHeight="1">
+      <c r="AG54" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH54" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI54" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ54" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" ht="15" customHeight="1">
       <c r="A55" s="3">
         <v>47</v>
       </c>
@@ -21175,8 +22445,20 @@
       <c r="AF55" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:32" ht="15" customHeight="1">
+      <c r="AG55" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH55" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI55" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ55" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:36" ht="15" customHeight="1">
       <c r="A56" s="3">
         <v>48</v>
       </c>
@@ -21271,19 +22553,31 @@
       <c r="AF56" s="122" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:32">
-      <c r="A57" s="137" t="s">
+      <c r="AG56" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH56" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI56" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ56" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:36">
+      <c r="A57" s="150" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="138"/>
+      <c r="B57" s="151"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
         <v>2</v>
       </c>
       <c r="E57" s="19">
-        <f t="shared" ref="E57:AF57" si="0">COUNTIF(E9:E56,"A")</f>
+        <f t="shared" ref="E57:AJ57" si="0">COUNTIF(E9:E56,"A")</f>
         <v>2</v>
       </c>
       <c r="F57" s="19">
@@ -21394,19 +22688,35 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:32">
-      <c r="A58" s="134" t="s">
+      <c r="AG57" s="132">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AH57" s="132">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AI57" s="132">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AJ57" s="131">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:36">
+      <c r="A58" s="148" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="135"/>
+      <c r="B58" s="149"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
         <v>46</v>
       </c>
       <c r="E58" s="24">
-        <f t="shared" ref="E58:AF58" si="1">(48-E57)</f>
+        <f t="shared" ref="E58:AJ58" si="1">(48-E57)</f>
         <v>46</v>
       </c>
       <c r="F58" s="24">
@@ -21517,22 +22827,26 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
+      <c r="AG58" s="132">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="AH58" s="132">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="AI58" s="132">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="AJ58" s="131">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="AD5:AF5"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
+  <mergeCells count="28">
+    <mergeCell ref="AG5:AJ5"/>
     <mergeCell ref="N1:AB1"/>
     <mergeCell ref="N2:AB2"/>
     <mergeCell ref="N3:AB3"/>
@@ -21547,6 +22861,19 @@
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N4:U4"/>
+    <mergeCell ref="AD5:AF5"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="N5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -21572,28 +22899,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="191" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="187" t="s">
+      <c r="A2" s="192" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="187"/>
-      <c r="C2" s="187"/>
-      <c r="D2" s="187"/>
+      <c r="B2" s="192"/>
+      <c r="C2" s="192"/>
+      <c r="D2" s="192"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="187" t="s">
+      <c r="A3" s="192" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="187"/>
-      <c r="C3" s="187"/>
-      <c r="D3" s="187"/>
+      <c r="B3" s="192"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
     </row>
     <row r="4" spans="1:4" s="82" customFormat="1" ht="28.5">
       <c r="A4" s="80" t="s">
@@ -22324,41 +23651,41 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="185" t="s">
+      <c r="A56" s="190" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="185"/>
-      <c r="C56" s="185"/>
+      <c r="B56" s="190"/>
+      <c r="C56" s="190"/>
       <c r="D56" s="74">
         <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="185" t="s">
+      <c r="A57" s="190" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="185"/>
-      <c r="C57" s="185"/>
+      <c r="B57" s="190"/>
+      <c r="C57" s="190"/>
       <c r="D57" s="75">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="185" t="s">
+      <c r="A58" s="190" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="185"/>
-      <c r="C58" s="185"/>
+      <c r="B58" s="190"/>
+      <c r="C58" s="190"/>
       <c r="D58" s="75">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="185" t="s">
+      <c r="A59" s="190" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="185"/>
-      <c r="C59" s="185"/>
+      <c r="B59" s="190"/>
+      <c r="C59" s="190"/>
       <c r="D59" s="75">
         <v>92</v>
       </c>
@@ -22404,7 +23731,7 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:C55 C8:C23">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="75" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22431,28 +23758,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="193" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
+      <c r="B1" s="193"/>
+      <c r="C1" s="193"/>
+      <c r="D1" s="193"/>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="189" t="s">
+      <c r="A2" s="194" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="189"/>
-      <c r="C2" s="189"/>
-      <c r="D2" s="189"/>
+      <c r="B2" s="194"/>
+      <c r="C2" s="194"/>
+      <c r="D2" s="194"/>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="194" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="189"/>
-      <c r="C3" s="189"/>
-      <c r="D3" s="189"/>
+      <c r="B3" s="194"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
     </row>
     <row r="4" spans="1:4" s="82" customFormat="1" ht="31.5">
       <c r="A4" s="102" t="s">
@@ -23183,41 +24510,41 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75">
-      <c r="A56" s="157" t="s">
+      <c r="A56" s="166" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="157"/>
-      <c r="C56" s="157"/>
+      <c r="B56" s="166"/>
+      <c r="C56" s="166"/>
       <c r="D56" s="114">
         <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75">
-      <c r="A57" s="157" t="s">
+      <c r="A57" s="166" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="157"/>
-      <c r="C57" s="157"/>
+      <c r="B57" s="166"/>
+      <c r="C57" s="166"/>
       <c r="D57" s="115">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75">
-      <c r="A58" s="157" t="s">
+      <c r="A58" s="166" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="157"/>
-      <c r="C58" s="157"/>
+      <c r="B58" s="166"/>
+      <c r="C58" s="166"/>
       <c r="D58" s="115">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75">
-      <c r="A59" s="157" t="s">
+      <c r="A59" s="166" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="157"/>
-      <c r="C59" s="157"/>
+      <c r="B59" s="166"/>
+      <c r="C59" s="166"/>
       <c r="D59" s="115">
         <v>85.1</v>
       </c>
@@ -23263,11 +24590,680 @@
     <mergeCell ref="A58:C58"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C55">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="1.04" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="68" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="68" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="68" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="78" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="68"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75">
+      <c r="A1" s="193" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="193"/>
+      <c r="C1" s="193"/>
+      <c r="D1" s="193"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75">
+      <c r="A2" s="194" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="194"/>
+      <c r="C2" s="194"/>
+      <c r="D2" s="194"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="194" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="194"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1">
+      <c r="A4" s="134" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="106" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="106" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="107" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A5" s="134">
+        <v>1</v>
+      </c>
+      <c r="B5" s="108" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" s="133"/>
+    </row>
+    <row r="6" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A6" s="134">
+        <v>2</v>
+      </c>
+      <c r="B6" s="108" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="133"/>
+    </row>
+    <row r="7" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A7" s="134">
+        <v>3</v>
+      </c>
+      <c r="B7" s="108" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="133"/>
+    </row>
+    <row r="8" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A8" s="134">
+        <v>4</v>
+      </c>
+      <c r="B8" s="109" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D8" s="133"/>
+    </row>
+    <row r="9" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A9" s="134">
+        <v>5</v>
+      </c>
+      <c r="B9" s="108" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" s="133"/>
+    </row>
+    <row r="10" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A10" s="134">
+        <v>6</v>
+      </c>
+      <c r="B10" s="108" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="133"/>
+    </row>
+    <row r="11" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A11" s="134">
+        <v>7</v>
+      </c>
+      <c r="B11" s="108" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="133"/>
+    </row>
+    <row r="12" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A12" s="134">
+        <v>8</v>
+      </c>
+      <c r="B12" s="108" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" s="133"/>
+    </row>
+    <row r="13" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A13" s="134">
+        <v>9</v>
+      </c>
+      <c r="B13" s="108" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" s="133"/>
+    </row>
+    <row r="14" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A14" s="134">
+        <v>10</v>
+      </c>
+      <c r="B14" s="108" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" s="133"/>
+    </row>
+    <row r="15" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A15" s="134">
+        <v>11</v>
+      </c>
+      <c r="B15" s="108" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="133"/>
+    </row>
+    <row r="16" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A16" s="134">
+        <v>12</v>
+      </c>
+      <c r="B16" s="108" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="133"/>
+    </row>
+    <row r="17" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A17" s="134">
+        <v>13</v>
+      </c>
+      <c r="B17" s="108" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="133"/>
+    </row>
+    <row r="18" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A18" s="134">
+        <v>14</v>
+      </c>
+      <c r="B18" s="110" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="133"/>
+    </row>
+    <row r="19" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A19" s="134">
+        <v>15</v>
+      </c>
+      <c r="B19" s="110" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" s="133"/>
+    </row>
+    <row r="20" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A20" s="134">
+        <v>16</v>
+      </c>
+      <c r="B20" s="108" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D20" s="133"/>
+    </row>
+    <row r="21" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A21" s="134">
+        <v>17</v>
+      </c>
+      <c r="B21" s="108" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D21" s="133"/>
+    </row>
+    <row r="22" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A22" s="134">
+        <v>18</v>
+      </c>
+      <c r="B22" s="108" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22" s="133"/>
+    </row>
+    <row r="23" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A23" s="134">
+        <v>19</v>
+      </c>
+      <c r="B23" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D23" s="133"/>
+    </row>
+    <row r="24" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A24" s="134">
+        <v>20</v>
+      </c>
+      <c r="B24" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" s="133"/>
+    </row>
+    <row r="25" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A25" s="134">
+        <v>21</v>
+      </c>
+      <c r="B25" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D25" s="133"/>
+    </row>
+    <row r="26" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A26" s="134">
+        <v>22</v>
+      </c>
+      <c r="B26" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" s="133"/>
+    </row>
+    <row r="27" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A27" s="134">
+        <v>23</v>
+      </c>
+      <c r="B27" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="C27" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D27" s="133"/>
+    </row>
+    <row r="28" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A28" s="134">
+        <v>24</v>
+      </c>
+      <c r="B28" s="112" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D28" s="133"/>
+    </row>
+    <row r="29" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A29" s="134">
+        <v>25</v>
+      </c>
+      <c r="B29" s="110" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" s="133"/>
+    </row>
+    <row r="30" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A30" s="134">
+        <v>26</v>
+      </c>
+      <c r="B30" s="108" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D30" s="133"/>
+    </row>
+    <row r="31" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A31" s="134">
+        <v>27</v>
+      </c>
+      <c r="B31" s="112" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" s="133"/>
+    </row>
+    <row r="32" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A32" s="134">
+        <v>28</v>
+      </c>
+      <c r="B32" s="108" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D32" s="133"/>
+    </row>
+    <row r="33" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A33" s="134">
+        <v>29</v>
+      </c>
+      <c r="B33" s="110" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" s="133" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A34" s="134">
+        <v>30</v>
+      </c>
+      <c r="B34" s="108" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" s="133" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A35" s="134">
+        <v>31</v>
+      </c>
+      <c r="B35" s="110" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" s="133" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A36" s="134">
+        <v>32</v>
+      </c>
+      <c r="B36" s="108" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D36" s="133"/>
+    </row>
+    <row r="37" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A37" s="134">
+        <v>33</v>
+      </c>
+      <c r="B37" s="108" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D37" s="133" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A38" s="134">
+        <v>34</v>
+      </c>
+      <c r="B38" s="108" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" s="133"/>
+    </row>
+    <row r="39" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A39" s="134">
+        <v>35</v>
+      </c>
+      <c r="B39" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D39" s="133" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A40" s="134">
+        <v>36</v>
+      </c>
+      <c r="B40" s="108" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D40" s="133" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A41" s="134">
+        <v>37</v>
+      </c>
+      <c r="B41" s="110" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" s="133"/>
+    </row>
+    <row r="42" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A42" s="134">
+        <v>38</v>
+      </c>
+      <c r="B42" s="108" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" s="133"/>
+    </row>
+    <row r="43" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A43" s="134">
+        <v>39</v>
+      </c>
+      <c r="B43" s="112" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D43" s="133" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A44" s="134">
+        <v>40</v>
+      </c>
+      <c r="B44" s="108" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" s="133"/>
+    </row>
+    <row r="45" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A45" s="134">
+        <v>41</v>
+      </c>
+      <c r="B45" s="108" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D45" s="133"/>
+    </row>
+    <row r="46" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A46" s="134">
+        <v>42</v>
+      </c>
+      <c r="B46" s="108" t="s">
+        <v>157</v>
+      </c>
+      <c r="C46" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46" s="133"/>
+    </row>
+    <row r="47" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A47" s="134">
+        <v>43</v>
+      </c>
+      <c r="B47" s="110" t="s">
+        <v>158</v>
+      </c>
+      <c r="C47" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D47" s="133"/>
+    </row>
+    <row r="48" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A48" s="134">
+        <v>44</v>
+      </c>
+      <c r="B48" s="110" t="s">
+        <v>159</v>
+      </c>
+      <c r="C48" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D48" s="133" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A49" s="134">
+        <v>45</v>
+      </c>
+      <c r="B49" s="108" t="s">
+        <v>160</v>
+      </c>
+      <c r="C49" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D49" s="133"/>
+    </row>
+    <row r="50" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A50" s="134">
+        <v>46</v>
+      </c>
+      <c r="B50" s="108" t="s">
+        <v>161</v>
+      </c>
+      <c r="C50" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="133"/>
+    </row>
+    <row r="51" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A51" s="134">
+        <v>47</v>
+      </c>
+      <c r="B51" s="108" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D51" s="133"/>
+    </row>
+    <row r="52" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A52" s="134">
+        <v>48</v>
+      </c>
+      <c r="B52" s="108" t="s">
+        <v>163</v>
+      </c>
+      <c r="C52" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D52" s="133"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5:C52">
+    <cfRule type="cellIs" dxfId="65" priority="3" operator="equal">
+      <formula>"Not Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="2" operator="equal">
+      <formula>"Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
+      <formula>"Not Submitted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="1.04" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Last Update 01-12-2018 11:18:15.11
</commit_message>
<xml_diff>
--- a/Acadamic Log Book PSPP-18_19.xlsx
+++ b/Acadamic Log Book PSPP-18_19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,8 @@
     <sheet name="Lab Attendance" sheetId="4" r:id="rId4"/>
     <sheet name="UT-2-Satement" sheetId="7" r:id="rId5"/>
     <sheet name="UT-3-Satement" sheetId="8" r:id="rId6"/>
-    <sheet name="Record Submission Status" sheetId="9" r:id="rId7"/>
+    <sheet name="UT-4-Satement" sheetId="10" r:id="rId7"/>
+    <sheet name="Record Submission Status" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attendance!$AZ$1:$AZ$57</definedName>
@@ -1447,7 +1448,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4985" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5159" uniqueCount="184">
   <si>
     <t>S.NO</t>
   </si>
@@ -1962,9 +1963,6 @@
     <t>Lab 8</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Not Completed</t>
   </si>
   <si>
@@ -1994,13 +1992,23 @@
   <si>
     <t>Result page missing</t>
   </si>
+  <si>
+    <t>Status 1</t>
+  </si>
+  <si>
+    <t>Status 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Statement of Marks - Unit Test-IV-NOV-2018</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -2380,7 +2388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2801,6 +2809,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2981,464 +3001,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="12">
     <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3459,59 +3063,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3897,29 +3449,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="18.75">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="138" t="s">
+      <c r="F1" s="142" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="146" t="s">
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="144"/>
+      <c r="J1" s="150" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
+      <c r="K1" s="150"/>
+      <c r="L1" s="150"/>
+      <c r="M1" s="150"/>
       <c r="N1" s="9" t="s">
         <v>78</v>
       </c>
@@ -3944,41 +3496,41 @@
       <c r="AG1" s="50"/>
     </row>
     <row r="2" spans="1:65" ht="19.5">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="159" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="157"/>
+      <c r="B2" s="160"/>
+      <c r="C2" s="161"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="141" t="s">
+      <c r="F2" s="145" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
-      <c r="J2" s="146" t="s">
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="150" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="146"/>
-      <c r="L2" s="146"/>
-      <c r="M2" s="146"/>
-      <c r="N2" s="147" t="s">
+      <c r="K2" s="150"/>
+      <c r="L2" s="150"/>
+      <c r="M2" s="150"/>
+      <c r="N2" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="147"/>
-      <c r="P2" s="147"/>
-      <c r="Q2" s="147"/>
-      <c r="R2" s="147"/>
-      <c r="S2" s="147"/>
-      <c r="T2" s="147"/>
-      <c r="U2" s="147"/>
-      <c r="V2" s="147"/>
-      <c r="W2" s="147"/>
+      <c r="O2" s="151"/>
+      <c r="P2" s="151"/>
+      <c r="Q2" s="151"/>
+      <c r="R2" s="151"/>
+      <c r="S2" s="151"/>
+      <c r="T2" s="151"/>
+      <c r="U2" s="151"/>
+      <c r="V2" s="151"/>
+      <c r="W2" s="151"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
       <c r="Z2" s="50"/>
@@ -3991,41 +3543,41 @@
       <c r="AG2" s="50"/>
     </row>
     <row r="3" spans="1:65" ht="18.75">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="140" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="137"/>
-      <c r="C3" s="142"/>
+      <c r="B3" s="141"/>
+      <c r="C3" s="146"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="141" t="s">
+      <c r="F3" s="145" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="141"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="146" t="s">
+      <c r="G3" s="145"/>
+      <c r="H3" s="145"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="150" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="146"/>
-      <c r="L3" s="146"/>
-      <c r="M3" s="146"/>
-      <c r="N3" s="147" t="s">
+      <c r="K3" s="150"/>
+      <c r="L3" s="150"/>
+      <c r="M3" s="150"/>
+      <c r="N3" s="151" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="147"/>
-      <c r="P3" s="147"/>
-      <c r="Q3" s="147"/>
-      <c r="R3" s="147"/>
-      <c r="S3" s="147"/>
-      <c r="T3" s="147"/>
-      <c r="U3" s="147"/>
-      <c r="V3" s="147"/>
-      <c r="W3" s="147"/>
+      <c r="O3" s="151"/>
+      <c r="P3" s="151"/>
+      <c r="Q3" s="151"/>
+      <c r="R3" s="151"/>
+      <c r="S3" s="151"/>
+      <c r="T3" s="151"/>
+      <c r="U3" s="151"/>
+      <c r="V3" s="151"/>
+      <c r="W3" s="151"/>
       <c r="X3" s="51"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
@@ -4038,57 +3590,57 @@
       <c r="AG3" s="51"/>
     </row>
     <row r="4" spans="1:65" ht="18.75">
-      <c r="A4" s="136" t="s">
+      <c r="A4" s="140" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="137"/>
-      <c r="C4" s="142"/>
-      <c r="D4" s="143">
+      <c r="B4" s="141"/>
+      <c r="C4" s="146"/>
+      <c r="D4" s="147">
         <v>43344</v>
       </c>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="144"/>
-      <c r="I4" s="144"/>
-      <c r="J4" s="144"/>
-      <c r="K4" s="144"/>
-      <c r="L4" s="144"/>
-      <c r="M4" s="144"/>
-      <c r="N4" s="144"/>
-      <c r="O4" s="144"/>
-      <c r="P4" s="144"/>
-      <c r="Q4" s="144"/>
-      <c r="R4" s="144"/>
-      <c r="S4" s="144"/>
-      <c r="T4" s="144"/>
-      <c r="U4" s="144"/>
-      <c r="V4" s="144"/>
-      <c r="W4" s="145"/>
-      <c r="X4" s="143">
+      <c r="E4" s="148"/>
+      <c r="F4" s="148"/>
+      <c r="G4" s="148"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="148"/>
+      <c r="M4" s="148"/>
+      <c r="N4" s="148"/>
+      <c r="O4" s="148"/>
+      <c r="P4" s="148"/>
+      <c r="Q4" s="148"/>
+      <c r="R4" s="148"/>
+      <c r="S4" s="148"/>
+      <c r="T4" s="148"/>
+      <c r="U4" s="148"/>
+      <c r="V4" s="148"/>
+      <c r="W4" s="149"/>
+      <c r="X4" s="147">
         <v>43374</v>
       </c>
-      <c r="Y4" s="144"/>
-      <c r="Z4" s="144"/>
-      <c r="AA4" s="144"/>
-      <c r="AB4" s="144"/>
-      <c r="AC4" s="144"/>
-      <c r="AD4" s="144"/>
-      <c r="AE4" s="144"/>
-      <c r="AF4" s="144"/>
-      <c r="AG4" s="144"/>
-      <c r="AH4" s="144"/>
-      <c r="AI4" s="144"/>
-      <c r="AJ4" s="144"/>
-      <c r="AK4" s="144"/>
-      <c r="AL4" s="144"/>
-      <c r="AM4" s="144"/>
-      <c r="AN4" s="144"/>
-      <c r="AO4" s="144"/>
-      <c r="AP4" s="144"/>
-      <c r="AQ4" s="144"/>
-      <c r="AR4" s="144"/>
-      <c r="AS4" s="145"/>
+      <c r="Y4" s="148"/>
+      <c r="Z4" s="148"/>
+      <c r="AA4" s="148"/>
+      <c r="AB4" s="148"/>
+      <c r="AC4" s="148"/>
+      <c r="AD4" s="148"/>
+      <c r="AE4" s="148"/>
+      <c r="AF4" s="148"/>
+      <c r="AG4" s="148"/>
+      <c r="AH4" s="148"/>
+      <c r="AI4" s="148"/>
+      <c r="AJ4" s="148"/>
+      <c r="AK4" s="148"/>
+      <c r="AL4" s="148"/>
+      <c r="AM4" s="148"/>
+      <c r="AN4" s="148"/>
+      <c r="AO4" s="148"/>
+      <c r="AP4" s="148"/>
+      <c r="AQ4" s="148"/>
+      <c r="AR4" s="148"/>
+      <c r="AS4" s="149"/>
       <c r="AT4" s="59"/>
       <c r="AU4" s="59"/>
       <c r="AV4" s="59"/>
@@ -4111,10 +3663,10 @@
       <c r="BM4" s="59"/>
     </row>
     <row r="5" spans="1:65">
-      <c r="A5" s="158" t="s">
+      <c r="A5" s="162" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="152" t="s">
+      <c r="B5" s="156" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -4298,8 +3850,8 @@
       <c r="BM5" s="59"/>
     </row>
     <row r="6" spans="1:65">
-      <c r="A6" s="158"/>
-      <c r="B6" s="153"/>
+      <c r="A6" s="162"/>
+      <c r="B6" s="157"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -4484,7 +4036,7 @@
       <c r="A7" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="154"/>
+      <c r="B7" s="158"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -13546,10 +13098,10 @@
       <c r="BM55" s="59"/>
     </row>
     <row r="56" spans="1:65">
-      <c r="A56" s="150" t="s">
+      <c r="A56" s="154" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="151"/>
+      <c r="B56" s="155"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f t="shared" ref="D56:Q56" si="0">COUNTIF(D8:D55,"A")</f>
@@ -13801,10 +13353,10 @@
       </c>
     </row>
     <row r="57" spans="1:65">
-      <c r="A57" s="148" t="s">
+      <c r="A57" s="152" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="149"/>
+      <c r="B57" s="153"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -14086,8 +13638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -14103,76 +13655,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="163" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="166" t="s">
+      <c r="B1" s="163"/>
+      <c r="C1" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="166"/>
-      <c r="E1" s="147" t="s">
+      <c r="D1" s="170"/>
+      <c r="E1" s="151" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="147"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="151"/>
     </row>
     <row r="2" spans="1:9" ht="19.5">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="164"/>
-      <c r="C2" s="166" t="s">
+      <c r="B2" s="168"/>
+      <c r="C2" s="170" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="166"/>
-      <c r="E2" s="147" t="s">
+      <c r="D2" s="170"/>
+      <c r="E2" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
+      <c r="I2" s="151"/>
     </row>
     <row r="3" spans="1:9" ht="17.25">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="169" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="165"/>
-      <c r="C3" s="166" t="s">
+      <c r="B3" s="169"/>
+      <c r="C3" s="170" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="166"/>
-      <c r="E3" s="147" t="s">
+      <c r="D3" s="170"/>
+      <c r="E3" s="151" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="147"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="147"/>
-      <c r="I3" s="147"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="164" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="152" t="s">
+      <c r="B4" s="156" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="163" t="s">
+      <c r="C4" s="167" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163"/>
-      <c r="I4" s="163"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
+      <c r="H4" s="167"/>
+      <c r="I4" s="167"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="161"/>
-      <c r="B5" s="153"/>
+      <c r="A5" s="165"/>
+      <c r="B5" s="157"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -14196,8 +13748,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="162"/>
-      <c r="B6" s="154"/>
+      <c r="A6" s="166"/>
+      <c r="B6" s="158"/>
       <c r="C6" s="43">
         <v>50</v>
       </c>
@@ -15375,10 +14927,10 @@
       <c r="I54" s="42"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="150" t="s">
+      <c r="A55" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="151"/>
+      <c r="B55" s="155"/>
       <c r="C55" s="31">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -15395,10 +14947,10 @@
       <c r="I55" s="13"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="148" t="s">
+      <c r="A56" s="152" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="149"/>
+      <c r="B56" s="153"/>
       <c r="C56" s="31">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -15415,10 +14967,10 @@
       <c r="I56" s="13"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="148" t="s">
+      <c r="A57" s="152" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="149"/>
+      <c r="B57" s="153"/>
       <c r="C57" s="31">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -15435,10 +14987,10 @@
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="148" t="s">
+      <c r="A58" s="152" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="149"/>
+      <c r="B58" s="153"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
@@ -15474,7 +15026,7 @@
     <mergeCell ref="B4:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:D54 E12 E33 E39 E47 E43:E44 E36 E31 E21:E22 E8:E9 F7:I54">
-    <cfRule type="cellIs" dxfId="79" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15505,72 +15057,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="163" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="166" t="s">
+      <c r="B1" s="163"/>
+      <c r="C1" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="166"/>
-      <c r="E1" s="167" t="s">
+      <c r="D1" s="170"/>
+      <c r="E1" s="171" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="168"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="172"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="164"/>
-      <c r="C2" s="166" t="s">
+      <c r="B2" s="168"/>
+      <c r="C2" s="170" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="166"/>
-      <c r="E2" s="147" t="s">
+      <c r="D2" s="170"/>
+      <c r="E2" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="169" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="165"/>
-      <c r="C3" s="166" t="s">
+      <c r="B3" s="169"/>
+      <c r="C3" s="170" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="166"/>
-      <c r="E3" s="147" t="s">
+      <c r="D3" s="170"/>
+      <c r="E3" s="151" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="147"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="147"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="164" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="152" t="s">
+      <c r="B4" s="156" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="169" t="s">
+      <c r="C4" s="173" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
-      <c r="H4" s="171"/>
+      <c r="D4" s="174"/>
+      <c r="E4" s="174"/>
+      <c r="F4" s="174"/>
+      <c r="G4" s="174"/>
+      <c r="H4" s="175"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="161"/>
-      <c r="B5" s="153"/>
+      <c r="A5" s="165"/>
+      <c r="B5" s="157"/>
       <c r="C5" s="43" t="s">
         <v>62</v>
       </c>
@@ -15591,8 +15143,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="162"/>
-      <c r="B6" s="154"/>
+      <c r="A6" s="166"/>
+      <c r="B6" s="158"/>
       <c r="C6" s="32">
         <v>50</v>
       </c>
@@ -16717,10 +16269,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="150" t="s">
+      <c r="A55" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="151"/>
+      <c r="B55" s="155"/>
       <c r="C55" s="42">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -16735,10 +16287,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="148" t="s">
+      <c r="A56" s="152" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="149"/>
+      <c r="B56" s="153"/>
       <c r="C56" s="42">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -16753,10 +16305,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="148" t="s">
+      <c r="A57" s="152" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="149"/>
+      <c r="B57" s="153"/>
       <c r="C57" s="42">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -16771,10 +16323,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="148" t="s">
+      <c r="A58" s="152" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="149"/>
+      <c r="B58" s="153"/>
       <c r="C58" s="33">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -16808,17 +16360,17 @@
     <mergeCell ref="E2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
-    <cfRule type="cellIs" dxfId="78" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="77" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="76" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16831,8 +16383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView topLeftCell="B52" workbookViewId="0">
-      <selection activeCell="AK57" sqref="AK57"/>
+    <sheetView topLeftCell="B61" workbookViewId="0">
+      <selection activeCell="AK5" sqref="AK5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -16846,227 +16398,227 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="18.75">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
       <c r="D1" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="138" t="s">
+      <c r="F1" s="142" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="146" t="s">
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="144"/>
+      <c r="J1" s="150" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="178" t="s">
+      <c r="K1" s="150"/>
+      <c r="L1" s="150"/>
+      <c r="M1" s="150"/>
+      <c r="N1" s="182" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="179"/>
-      <c r="P1" s="179"/>
-      <c r="Q1" s="179"/>
-      <c r="R1" s="179"/>
-      <c r="S1" s="179"/>
-      <c r="T1" s="179"/>
-      <c r="U1" s="179"/>
-      <c r="V1" s="179"/>
-      <c r="W1" s="179"/>
-      <c r="X1" s="179"/>
-      <c r="Y1" s="179"/>
-      <c r="Z1" s="179"/>
-      <c r="AA1" s="179"/>
-      <c r="AB1" s="179"/>
+      <c r="O1" s="183"/>
+      <c r="P1" s="183"/>
+      <c r="Q1" s="183"/>
+      <c r="R1" s="183"/>
+      <c r="S1" s="183"/>
+      <c r="T1" s="183"/>
+      <c r="U1" s="183"/>
+      <c r="V1" s="183"/>
+      <c r="W1" s="183"/>
+      <c r="X1" s="183"/>
+      <c r="Y1" s="183"/>
+      <c r="Z1" s="183"/>
+      <c r="AA1" s="183"/>
+      <c r="AB1" s="183"/>
     </row>
     <row r="2" spans="1:36" ht="19.5">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="159" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="157"/>
+      <c r="B2" s="160"/>
+      <c r="C2" s="161"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="141" t="s">
+      <c r="F2" s="145" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
-      <c r="J2" s="146" t="s">
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="150" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="146"/>
-      <c r="L2" s="146"/>
-      <c r="M2" s="146"/>
-      <c r="N2" s="178" t="s">
+      <c r="K2" s="150"/>
+      <c r="L2" s="150"/>
+      <c r="M2" s="150"/>
+      <c r="N2" s="182" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="179"/>
-      <c r="P2" s="179"/>
-      <c r="Q2" s="179"/>
-      <c r="R2" s="179"/>
-      <c r="S2" s="179"/>
-      <c r="T2" s="179"/>
-      <c r="U2" s="179"/>
-      <c r="V2" s="179"/>
-      <c r="W2" s="179"/>
-      <c r="X2" s="179"/>
-      <c r="Y2" s="179"/>
-      <c r="Z2" s="179"/>
-      <c r="AA2" s="179"/>
-      <c r="AB2" s="179"/>
+      <c r="O2" s="183"/>
+      <c r="P2" s="183"/>
+      <c r="Q2" s="183"/>
+      <c r="R2" s="183"/>
+      <c r="S2" s="183"/>
+      <c r="T2" s="183"/>
+      <c r="U2" s="183"/>
+      <c r="V2" s="183"/>
+      <c r="W2" s="183"/>
+      <c r="X2" s="183"/>
+      <c r="Y2" s="183"/>
+      <c r="Z2" s="183"/>
+      <c r="AA2" s="183"/>
+      <c r="AB2" s="183"/>
     </row>
     <row r="3" spans="1:36" ht="18.75" customHeight="1">
-      <c r="A3" s="181" t="s">
+      <c r="A3" s="185" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="182"/>
-      <c r="C3" s="183"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="187"/>
       <c r="D3" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="180" t="s">
+      <c r="F3" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="180"/>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="189" t="s">
+      <c r="G3" s="184"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="193" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="189"/>
-      <c r="L3" s="189"/>
-      <c r="M3" s="189"/>
-      <c r="N3" s="178" t="s">
+      <c r="K3" s="193"/>
+      <c r="L3" s="193"/>
+      <c r="M3" s="193"/>
+      <c r="N3" s="182" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="179"/>
-      <c r="P3" s="179"/>
-      <c r="Q3" s="179"/>
-      <c r="R3" s="179"/>
-      <c r="S3" s="179"/>
-      <c r="T3" s="179"/>
-      <c r="U3" s="179"/>
-      <c r="V3" s="179"/>
-      <c r="W3" s="179"/>
-      <c r="X3" s="179"/>
-      <c r="Y3" s="179"/>
-      <c r="Z3" s="179"/>
-      <c r="AA3" s="179"/>
-      <c r="AB3" s="179"/>
+      <c r="O3" s="183"/>
+      <c r="P3" s="183"/>
+      <c r="Q3" s="183"/>
+      <c r="R3" s="183"/>
+      <c r="S3" s="183"/>
+      <c r="T3" s="183"/>
+      <c r="U3" s="183"/>
+      <c r="V3" s="183"/>
+      <c r="W3" s="183"/>
+      <c r="X3" s="183"/>
+      <c r="Y3" s="183"/>
+      <c r="Z3" s="183"/>
+      <c r="AA3" s="183"/>
+      <c r="AB3" s="183"/>
     </row>
     <row r="4" spans="1:36" ht="18.75" customHeight="1">
-      <c r="A4" s="184"/>
-      <c r="B4" s="185"/>
-      <c r="C4" s="186"/>
-      <c r="D4" s="187">
+      <c r="A4" s="188"/>
+      <c r="B4" s="189"/>
+      <c r="C4" s="190"/>
+      <c r="D4" s="191">
         <v>43344</v>
       </c>
-      <c r="E4" s="188"/>
-      <c r="F4" s="188"/>
-      <c r="G4" s="188"/>
-      <c r="H4" s="188"/>
-      <c r="I4" s="188"/>
-      <c r="J4" s="188"/>
-      <c r="K4" s="188"/>
-      <c r="L4" s="188"/>
-      <c r="M4" s="188"/>
-      <c r="N4" s="187">
+      <c r="E4" s="192"/>
+      <c r="F4" s="192"/>
+      <c r="G4" s="192"/>
+      <c r="H4" s="192"/>
+      <c r="I4" s="192"/>
+      <c r="J4" s="192"/>
+      <c r="K4" s="192"/>
+      <c r="L4" s="192"/>
+      <c r="M4" s="192"/>
+      <c r="N4" s="191">
         <v>43374</v>
       </c>
-      <c r="O4" s="188"/>
-      <c r="P4" s="188"/>
-      <c r="Q4" s="188"/>
-      <c r="R4" s="188"/>
-      <c r="S4" s="188"/>
-      <c r="T4" s="188"/>
-      <c r="U4" s="188"/>
+      <c r="O4" s="192"/>
+      <c r="P4" s="192"/>
+      <c r="Q4" s="192"/>
+      <c r="R4" s="192"/>
+      <c r="S4" s="192"/>
+      <c r="T4" s="192"/>
+      <c r="U4" s="192"/>
       <c r="V4" s="53"/>
       <c r="W4" s="53"/>
     </row>
     <row r="5" spans="1:36">
-      <c r="A5" s="160" t="s">
+      <c r="A5" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="152" t="s">
+      <c r="B5" s="156" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="175" t="s">
+      <c r="D5" s="179" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="176"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="177"/>
-      <c r="H5" s="173" t="s">
+      <c r="E5" s="180"/>
+      <c r="F5" s="180"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="177" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="174"/>
-      <c r="J5" s="174"/>
-      <c r="K5" s="174"/>
-      <c r="L5" s="172" t="s">
+      <c r="I5" s="178"/>
+      <c r="J5" s="178"/>
+      <c r="K5" s="178"/>
+      <c r="L5" s="176" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="172"/>
-      <c r="N5" s="173" t="s">
+      <c r="M5" s="176"/>
+      <c r="N5" s="177" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="174"/>
-      <c r="P5" s="174"/>
-      <c r="Q5" s="174"/>
-      <c r="R5" s="172" t="s">
+      <c r="O5" s="178"/>
+      <c r="P5" s="178"/>
+      <c r="Q5" s="178"/>
+      <c r="R5" s="176" t="s">
         <v>71</v>
       </c>
-      <c r="S5" s="172"/>
-      <c r="T5" s="158" t="s">
+      <c r="S5" s="176"/>
+      <c r="T5" s="162" t="s">
         <v>95</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="158" t="s">
+      <c r="U5" s="162"/>
+      <c r="V5" s="162" t="s">
         <v>117</v>
       </c>
-      <c r="W5" s="158"/>
-      <c r="X5" s="158"/>
-      <c r="Y5" s="158"/>
-      <c r="Z5" s="158" t="s">
+      <c r="W5" s="162"/>
+      <c r="X5" s="162"/>
+      <c r="Y5" s="162"/>
+      <c r="Z5" s="162" t="s">
         <v>118</v>
       </c>
-      <c r="AA5" s="158"/>
-      <c r="AB5" s="158"/>
-      <c r="AC5" s="158"/>
-      <c r="AD5" s="158" t="s">
+      <c r="AA5" s="162"/>
+      <c r="AB5" s="162"/>
+      <c r="AC5" s="162"/>
+      <c r="AD5" s="162" t="s">
         <v>169</v>
       </c>
-      <c r="AE5" s="158"/>
-      <c r="AF5" s="158"/>
-      <c r="AG5" s="158" t="s">
+      <c r="AE5" s="162"/>
+      <c r="AF5" s="162"/>
+      <c r="AG5" s="162" t="s">
         <v>170</v>
       </c>
-      <c r="AH5" s="158"/>
-      <c r="AI5" s="158"/>
-      <c r="AJ5" s="158"/>
+      <c r="AH5" s="162"/>
+      <c r="AI5" s="162"/>
+      <c r="AJ5" s="162"/>
     </row>
     <row r="6" spans="1:36">
-      <c r="A6" s="161"/>
-      <c r="B6" s="153"/>
+      <c r="A6" s="165"/>
+      <c r="B6" s="157"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -17171,8 +16723,8 @@
       </c>
     </row>
     <row r="7" spans="1:36">
-      <c r="A7" s="161"/>
-      <c r="B7" s="153"/>
+      <c r="A7" s="165"/>
+      <c r="B7" s="157"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -17277,8 +16829,8 @@
       </c>
     </row>
     <row r="8" spans="1:36" ht="15" customHeight="1">
-      <c r="A8" s="162"/>
-      <c r="B8" s="154"/>
+      <c r="A8" s="166"/>
+      <c r="B8" s="158"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -22567,10 +22119,10 @@
       </c>
     </row>
     <row r="57" spans="1:36">
-      <c r="A57" s="150" t="s">
+      <c r="A57" s="154" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="151"/>
+      <c r="B57" s="155"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -22706,10 +22258,10 @@
       </c>
     </row>
     <row r="58" spans="1:36">
-      <c r="A58" s="148" t="s">
+      <c r="A58" s="152" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="149"/>
+      <c r="B58" s="153"/>
       <c r="C58" s="13"/>
       <c r="D58" s="19">
         <f>(48-D57)</f>
@@ -22899,28 +22451,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="191" t="s">
+      <c r="A1" s="195" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="192" t="s">
+      <c r="A2" s="196" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="192"/>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
+      <c r="B2" s="196"/>
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="196" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="192"/>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
+      <c r="B3" s="196"/>
+      <c r="C3" s="196"/>
+      <c r="D3" s="196"/>
     </row>
     <row r="4" spans="1:4" s="82" customFormat="1" ht="28.5">
       <c r="A4" s="80" t="s">
@@ -23651,41 +23203,41 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="190" t="s">
+      <c r="A56" s="194" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="190"/>
-      <c r="C56" s="190"/>
+      <c r="B56" s="194"/>
+      <c r="C56" s="194"/>
       <c r="D56" s="74">
         <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="190" t="s">
+      <c r="A57" s="194" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="190"/>
-      <c r="C57" s="190"/>
+      <c r="B57" s="194"/>
+      <c r="C57" s="194"/>
       <c r="D57" s="75">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="190" t="s">
+      <c r="A58" s="194" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="190"/>
-      <c r="C58" s="190"/>
+      <c r="B58" s="194"/>
+      <c r="C58" s="194"/>
       <c r="D58" s="75">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="190" t="s">
+      <c r="A59" s="194" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="190"/>
-      <c r="C59" s="190"/>
+      <c r="B59" s="194"/>
+      <c r="C59" s="194"/>
       <c r="D59" s="75">
         <v>92</v>
       </c>
@@ -23731,7 +23283,7 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:C55 C8:C23">
-    <cfRule type="cellIs" dxfId="75" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23758,28 +23310,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="197" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="198" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="194"/>
-      <c r="C2" s="194"/>
-      <c r="D2" s="194"/>
+      <c r="B2" s="198"/>
+      <c r="C2" s="198"/>
+      <c r="D2" s="198"/>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="198" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="194"/>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
+      <c r="B3" s="198"/>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
     </row>
     <row r="4" spans="1:4" s="82" customFormat="1" ht="31.5">
       <c r="A4" s="102" t="s">
@@ -24510,41 +24062,41 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75">
-      <c r="A56" s="166" t="s">
+      <c r="A56" s="170" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="166"/>
-      <c r="C56" s="166"/>
+      <c r="B56" s="170"/>
+      <c r="C56" s="170"/>
       <c r="D56" s="114">
         <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75">
-      <c r="A57" s="166" t="s">
+      <c r="A57" s="170" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="166"/>
-      <c r="C57" s="166"/>
+      <c r="B57" s="170"/>
+      <c r="C57" s="170"/>
       <c r="D57" s="115">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75">
-      <c r="A58" s="166" t="s">
+      <c r="A58" s="170" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="166"/>
-      <c r="C58" s="166"/>
+      <c r="B58" s="170"/>
+      <c r="C58" s="170"/>
       <c r="D58" s="115">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75">
-      <c r="A59" s="166" t="s">
+      <c r="A59" s="170" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="166"/>
-      <c r="C59" s="166"/>
+      <c r="B59" s="170"/>
+      <c r="C59" s="170"/>
       <c r="D59" s="115">
         <v>85.1</v>
       </c>
@@ -24590,7 +24142,7 @@
     <mergeCell ref="A58:C58"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C55">
-    <cfRule type="cellIs" dxfId="74" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24601,666 +24153,1681 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D52"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="68" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" style="68" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="68" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="68" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" style="78" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="68"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="197" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="198" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="194"/>
-      <c r="C2" s="194"/>
-      <c r="D2" s="194"/>
+      <c r="B2" s="198"/>
+      <c r="C2" s="198"/>
+      <c r="D2" s="198"/>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="194" t="s">
-        <v>174</v>
-      </c>
-      <c r="B3" s="194"/>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1">
-      <c r="A4" s="134" t="s">
+      <c r="A3" s="198" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="198"/>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+    </row>
+    <row r="4" spans="1:4" s="82" customFormat="1" ht="31.5">
+      <c r="A4" s="102" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="103" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="104" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="103" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="82" customFormat="1" ht="31.5">
+      <c r="A5" s="102" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="103" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="104" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="103" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="82" customFormat="1" ht="31.5">
+      <c r="A6" s="102" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="103" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="104" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="105">
+        <v>43385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1">
+      <c r="A7" s="138" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="106" t="s">
+      <c r="B7" s="106" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="106" t="s">
-        <v>171</v>
-      </c>
-      <c r="D4" s="107" t="s">
+      <c r="C7" s="106" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="107" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A5" s="134">
+    <row r="8" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A8" s="138">
         <v>1</v>
       </c>
-      <c r="B5" s="108" t="s">
+      <c r="B8" s="108" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D5" s="133"/>
-    </row>
-    <row r="6" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A6" s="134">
+      <c r="C8" s="137">
+        <v>35</v>
+      </c>
+      <c r="D8" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A9" s="138">
         <v>2</v>
       </c>
-      <c r="B6" s="108" t="s">
+      <c r="B9" s="108" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D6" s="133"/>
-    </row>
-    <row r="7" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A7" s="134">
+      <c r="C9" s="45">
+        <v>21</v>
+      </c>
+      <c r="D9" s="137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A10" s="138">
         <v>3</v>
       </c>
-      <c r="B7" s="108" t="s">
+      <c r="B10" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="C7" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D7" s="133"/>
-    </row>
-    <row r="8" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A8" s="134">
+      <c r="C10" s="137">
+        <v>29</v>
+      </c>
+      <c r="D10" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A11" s="138">
         <v>4</v>
       </c>
-      <c r="B8" s="109" t="s">
+      <c r="B11" s="109" t="s">
         <v>122</v>
       </c>
-      <c r="C8" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D8" s="133"/>
-    </row>
-    <row r="9" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A9" s="134">
+      <c r="C11" s="137">
+        <v>22</v>
+      </c>
+      <c r="D11" s="137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A12" s="138">
         <v>5</v>
       </c>
-      <c r="B9" s="108" t="s">
+      <c r="B12" s="108" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D9" s="133"/>
-    </row>
-    <row r="10" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A10" s="134">
+      <c r="C12" s="137">
+        <v>36</v>
+      </c>
+      <c r="D12" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A13" s="138">
         <v>6</v>
       </c>
-      <c r="B10" s="108" t="s">
+      <c r="B13" s="108" t="s">
         <v>124</v>
       </c>
-      <c r="C10" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D10" s="133"/>
-    </row>
-    <row r="11" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A11" s="134">
+      <c r="C13" s="137">
+        <v>12</v>
+      </c>
+      <c r="D13" s="137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A14" s="138">
         <v>7</v>
       </c>
-      <c r="B11" s="108" t="s">
+      <c r="B14" s="108" t="s">
         <v>125</v>
       </c>
-      <c r="C11" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D11" s="133"/>
-    </row>
-    <row r="12" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A12" s="134">
+      <c r="C14" s="137">
+        <v>40</v>
+      </c>
+      <c r="D14" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A15" s="138">
         <v>8</v>
       </c>
-      <c r="B12" s="108" t="s">
+      <c r="B15" s="108" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D12" s="133"/>
-    </row>
-    <row r="13" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A13" s="134">
+      <c r="C15" s="137">
+        <v>36</v>
+      </c>
+      <c r="D15" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A16" s="138">
         <v>9</v>
       </c>
-      <c r="B13" s="108" t="s">
+      <c r="B16" s="108" t="s">
         <v>127</v>
       </c>
-      <c r="C13" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D13" s="133"/>
-    </row>
-    <row r="14" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A14" s="134">
+      <c r="C16" s="137">
+        <v>22</v>
+      </c>
+      <c r="D16" s="137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A17" s="138">
         <v>10</v>
       </c>
-      <c r="B14" s="108" t="s">
+      <c r="B17" s="108" t="s">
         <v>127</v>
       </c>
-      <c r="C14" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D14" s="133"/>
-    </row>
-    <row r="15" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A15" s="134">
+      <c r="C17" s="137">
+        <v>23</v>
+      </c>
+      <c r="D17" s="137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A18" s="138">
         <v>11</v>
       </c>
-      <c r="B15" s="108" t="s">
+      <c r="B18" s="108" t="s">
         <v>128</v>
       </c>
-      <c r="C15" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D15" s="133"/>
-    </row>
-    <row r="16" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A16" s="134">
+      <c r="C18" s="137">
+        <v>33</v>
+      </c>
+      <c r="D18" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A19" s="138">
         <v>12</v>
       </c>
-      <c r="B16" s="108" t="s">
+      <c r="B19" s="108" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="D16" s="133"/>
-    </row>
-    <row r="17" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A17" s="134">
+      <c r="C19" s="137">
+        <v>26</v>
+      </c>
+      <c r="D19" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A20" s="138">
         <v>13</v>
       </c>
-      <c r="B17" s="108" t="s">
+      <c r="B20" s="108" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D17" s="133"/>
-    </row>
-    <row r="18" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A18" s="134">
+      <c r="C20" s="137">
+        <v>29</v>
+      </c>
+      <c r="D20" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A21" s="138">
         <v>14</v>
       </c>
-      <c r="B18" s="110" t="s">
+      <c r="B21" s="110" t="s">
         <v>131</v>
       </c>
-      <c r="C18" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D18" s="133"/>
-    </row>
-    <row r="19" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A19" s="134">
+      <c r="C21" s="137">
+        <v>8</v>
+      </c>
+      <c r="D21" s="137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A22" s="138">
         <v>15</v>
       </c>
-      <c r="B19" s="110" t="s">
+      <c r="B22" s="110" t="s">
         <v>132</v>
       </c>
-      <c r="C19" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D19" s="133"/>
-    </row>
-    <row r="20" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A20" s="134">
+      <c r="C22" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="137" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A23" s="138">
         <v>16</v>
       </c>
-      <c r="B20" s="108" t="s">
+      <c r="B23" s="108" t="s">
         <v>133</v>
       </c>
-      <c r="C20" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D20" s="133"/>
-    </row>
-    <row r="21" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A21" s="134">
+      <c r="C23" s="137">
+        <v>13</v>
+      </c>
+      <c r="D23" s="137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A24" s="138">
         <v>17</v>
       </c>
-      <c r="B21" s="108" t="s">
+      <c r="B24" s="108" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D21" s="133"/>
-    </row>
-    <row r="22" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A22" s="134">
+      <c r="C24" s="137">
+        <v>28</v>
+      </c>
+      <c r="D24" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A25" s="138">
         <v>18</v>
       </c>
-      <c r="B22" s="108" t="s">
+      <c r="B25" s="108" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D22" s="133"/>
-    </row>
-    <row r="23" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A23" s="134">
+      <c r="C25" s="137">
+        <v>25</v>
+      </c>
+      <c r="D25" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A26" s="138">
         <v>19</v>
       </c>
-      <c r="B23" s="108" t="s">
+      <c r="B26" s="108" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="D23" s="133"/>
-    </row>
-    <row r="24" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A24" s="134">
+      <c r="C26" s="137">
+        <v>31</v>
+      </c>
+      <c r="D26" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A27" s="138">
         <v>20</v>
       </c>
-      <c r="B24" s="108" t="s">
+      <c r="B27" s="108" t="s">
         <v>137</v>
       </c>
-      <c r="C24" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="D24" s="133"/>
-    </row>
-    <row r="25" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A25" s="134">
+      <c r="C27" s="137">
+        <v>42</v>
+      </c>
+      <c r="D27" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A28" s="138">
         <v>21</v>
       </c>
-      <c r="B25" s="108" t="s">
+      <c r="B28" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="D25" s="133"/>
-    </row>
-    <row r="26" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A26" s="134">
+      <c r="C28" s="137">
+        <v>25</v>
+      </c>
+      <c r="D28" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A29" s="138">
         <v>22</v>
       </c>
-      <c r="B26" s="108" t="s">
+      <c r="B29" s="108" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="D26" s="133"/>
-    </row>
-    <row r="27" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A27" s="134">
+      <c r="C29" s="137">
+        <v>31</v>
+      </c>
+      <c r="D29" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A30" s="138">
         <v>23</v>
       </c>
-      <c r="B27" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="C27" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="D27" s="133"/>
-    </row>
-    <row r="28" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A28" s="134">
+      <c r="B30" s="111" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="137">
+        <v>26</v>
+      </c>
+      <c r="D30" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A31" s="138">
         <v>24</v>
       </c>
-      <c r="B28" s="112" t="s">
+      <c r="B31" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D28" s="133"/>
-    </row>
-    <row r="29" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A29" s="134">
+      <c r="C31" s="137">
+        <v>13</v>
+      </c>
+      <c r="D31" s="137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A32" s="138">
         <v>25</v>
       </c>
-      <c r="B29" s="110" t="s">
+      <c r="B32" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D29" s="133"/>
-    </row>
-    <row r="30" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A30" s="134">
+      <c r="C32" s="137">
+        <v>12</v>
+      </c>
+      <c r="D32" s="137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A33" s="138">
         <v>26</v>
       </c>
-      <c r="B30" s="108" t="s">
+      <c r="B33" s="108" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="D30" s="133"/>
-    </row>
-    <row r="31" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A31" s="134">
+      <c r="C33" s="137">
+        <v>46</v>
+      </c>
+      <c r="D33" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A34" s="138">
         <v>27</v>
       </c>
-      <c r="B31" s="112" t="s">
+      <c r="B34" s="112" t="s">
         <v>166</v>
       </c>
-      <c r="C31" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D31" s="133"/>
-    </row>
-    <row r="32" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A32" s="134">
+      <c r="C34" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="137" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A35" s="138">
         <v>28</v>
       </c>
-      <c r="B32" s="108" t="s">
+      <c r="B35" s="108" t="s">
         <v>144</v>
       </c>
-      <c r="C32" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="D32" s="133"/>
-    </row>
-    <row r="33" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A33" s="134">
+      <c r="C35" s="137">
+        <v>49</v>
+      </c>
+      <c r="D35" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A36" s="138">
         <v>29</v>
       </c>
-      <c r="B33" s="110" t="s">
+      <c r="B36" s="110" t="s">
         <v>145</v>
       </c>
-      <c r="C33" s="135" t="s">
-        <v>172</v>
-      </c>
-      <c r="D33" s="133" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A34" s="134">
+      <c r="C36" s="137">
+        <v>39</v>
+      </c>
+      <c r="D36" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A37" s="138">
         <v>30</v>
       </c>
-      <c r="B34" s="108" t="s">
+      <c r="B37" s="108" t="s">
         <v>146</v>
       </c>
-      <c r="C34" s="135" t="s">
-        <v>172</v>
-      </c>
-      <c r="D34" s="133" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A35" s="134">
+      <c r="C37" s="137">
+        <v>13</v>
+      </c>
+      <c r="D37" s="137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A38" s="138">
         <v>31</v>
       </c>
-      <c r="B35" s="110" t="s">
+      <c r="B38" s="110" t="s">
         <v>147</v>
       </c>
-      <c r="C35" s="135" t="s">
-        <v>172</v>
-      </c>
-      <c r="D35" s="133" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A36" s="134">
+      <c r="C38" s="137">
+        <v>47</v>
+      </c>
+      <c r="D38" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A39" s="138">
         <v>32</v>
       </c>
-      <c r="B36" s="108" t="s">
+      <c r="B39" s="108" t="s">
         <v>148</v>
       </c>
-      <c r="C36" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="D36" s="133"/>
-    </row>
-    <row r="37" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A37" s="134">
+      <c r="C39" s="137">
+        <v>39</v>
+      </c>
+      <c r="D39" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A40" s="138">
         <v>33</v>
       </c>
-      <c r="B37" s="108" t="s">
+      <c r="B40" s="108" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="135" t="s">
-        <v>172</v>
-      </c>
-      <c r="D37" s="133" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A38" s="134">
+      <c r="C40" s="137">
+        <v>33</v>
+      </c>
+      <c r="D40" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A41" s="138">
         <v>34</v>
       </c>
-      <c r="B38" s="108" t="s">
+      <c r="B41" s="108" t="s">
         <v>150</v>
       </c>
-      <c r="C38" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D38" s="133"/>
-    </row>
-    <row r="39" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A39" s="134">
+      <c r="C41" s="137">
         <v>35</v>
       </c>
-      <c r="B39" s="108" t="s">
+      <c r="D41" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A42" s="138">
+        <v>35</v>
+      </c>
+      <c r="B42" s="108" t="s">
         <v>151</v>
       </c>
-      <c r="C39" s="135" t="s">
-        <v>172</v>
-      </c>
-      <c r="D39" s="133" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A40" s="134">
+      <c r="C42" s="137">
+        <v>34</v>
+      </c>
+      <c r="D42" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A43" s="138">
         <v>36</v>
       </c>
-      <c r="B40" s="108" t="s">
+      <c r="B43" s="108" t="s">
         <v>152</v>
       </c>
-      <c r="C40" s="135" t="s">
-        <v>172</v>
-      </c>
-      <c r="D40" s="133" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A41" s="134">
+      <c r="C43" s="137">
+        <v>25</v>
+      </c>
+      <c r="D43" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A44" s="138">
         <v>37</v>
       </c>
-      <c r="B41" s="110" t="s">
+      <c r="B44" s="110" t="s">
         <v>153</v>
       </c>
-      <c r="C41" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D41" s="133"/>
-    </row>
-    <row r="42" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A42" s="134">
+      <c r="C44" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="137" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A45" s="138">
         <v>38</v>
       </c>
-      <c r="B42" s="108" t="s">
+      <c r="B45" s="108" t="s">
         <v>154</v>
       </c>
-      <c r="C42" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D42" s="133"/>
-    </row>
-    <row r="43" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A43" s="134">
+      <c r="C45" s="137">
+        <v>21</v>
+      </c>
+      <c r="D45" s="137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A46" s="138">
         <v>39</v>
       </c>
-      <c r="B43" s="112" t="s">
+      <c r="B46" s="112" t="s">
         <v>167</v>
       </c>
-      <c r="C43" s="135" t="s">
-        <v>172</v>
-      </c>
-      <c r="D43" s="133" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A44" s="134">
+      <c r="C46" s="137">
+        <v>27</v>
+      </c>
+      <c r="D46" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A47" s="138">
         <v>40</v>
       </c>
-      <c r="B44" s="108" t="s">
+      <c r="B47" s="108" t="s">
         <v>155</v>
       </c>
-      <c r="C44" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D44" s="133"/>
-    </row>
-    <row r="45" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A45" s="134">
+      <c r="C47" s="137">
+        <v>32</v>
+      </c>
+      <c r="D47" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A48" s="138">
         <v>41</v>
       </c>
-      <c r="B45" s="108" t="s">
+      <c r="B48" s="108" t="s">
         <v>156</v>
       </c>
-      <c r="C45" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D45" s="133"/>
-    </row>
-    <row r="46" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A46" s="134">
+      <c r="C48" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="137" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A49" s="138">
         <v>42</v>
       </c>
-      <c r="B46" s="108" t="s">
+      <c r="B49" s="108" t="s">
         <v>157</v>
       </c>
-      <c r="C46" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D46" s="133"/>
-    </row>
-    <row r="47" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A47" s="134">
+      <c r="C49" s="137">
+        <v>36</v>
+      </c>
+      <c r="D49" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A50" s="138">
         <v>43</v>
       </c>
-      <c r="B47" s="110" t="s">
+      <c r="B50" s="110" t="s">
         <v>158</v>
       </c>
-      <c r="C47" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D47" s="133"/>
-    </row>
-    <row r="48" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A48" s="134">
+      <c r="C50" s="137">
         <v>44</v>
       </c>
-      <c r="B48" s="110" t="s">
+      <c r="D50" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A51" s="138">
+        <v>44</v>
+      </c>
+      <c r="B51" s="110" t="s">
         <v>159</v>
       </c>
-      <c r="C48" s="135" t="s">
-        <v>172</v>
-      </c>
-      <c r="D48" s="133" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A49" s="134">
+      <c r="C51" s="137">
+        <v>40</v>
+      </c>
+      <c r="D51" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A52" s="138">
         <v>45</v>
       </c>
-      <c r="B49" s="108" t="s">
+      <c r="B52" s="108" t="s">
         <v>160</v>
       </c>
-      <c r="C49" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="D49" s="133"/>
-    </row>
-    <row r="50" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A50" s="134">
+      <c r="C52" s="137">
+        <v>19</v>
+      </c>
+      <c r="D52" s="137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A53" s="138">
         <v>46</v>
       </c>
-      <c r="B50" s="108" t="s">
+      <c r="B53" s="108" t="s">
         <v>161</v>
       </c>
-      <c r="C50" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D50" s="133"/>
-    </row>
-    <row r="51" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A51" s="134">
+      <c r="C53" s="137">
+        <v>36</v>
+      </c>
+      <c r="D53" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A54" s="138">
         <v>47</v>
       </c>
-      <c r="B51" s="108" t="s">
+      <c r="B54" s="108" t="s">
         <v>162</v>
       </c>
-      <c r="C51" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="D51" s="133"/>
-    </row>
-    <row r="52" spans="1:4" s="82" customFormat="1" ht="15.75">
-      <c r="A52" s="134">
+      <c r="C54" s="137">
+        <v>33</v>
+      </c>
+      <c r="D54" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="82" customFormat="1" ht="15.75">
+      <c r="A55" s="139">
         <v>48</v>
       </c>
-      <c r="B52" s="108" t="s">
+      <c r="B55" s="113" t="s">
         <v>163</v>
       </c>
-      <c r="C52" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="D52" s="133"/>
+      <c r="C55" s="137">
+        <v>49</v>
+      </c>
+      <c r="D55" s="137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75">
+      <c r="A56" s="170" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="170"/>
+      <c r="C56" s="170"/>
+      <c r="D56" s="114">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75">
+      <c r="A57" s="170" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="170"/>
+      <c r="C57" s="170"/>
+      <c r="D57" s="115">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75">
+      <c r="A58" s="170" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="170"/>
+      <c r="C58" s="170"/>
+      <c r="D58" s="115">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75">
+      <c r="A59" s="170" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" s="170"/>
+      <c r="C59" s="170"/>
+      <c r="D59" s="199">
+        <f>(D56/48)*100</f>
+        <v>66.666666666666657</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="66"/>
+      <c r="B60" s="66"/>
+      <c r="C60" s="66"/>
+      <c r="D60" s="76"/>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="66"/>
+      <c r="B61" s="66"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="76"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="72"/>
+      <c r="B62" s="72"/>
+      <c r="C62" s="72"/>
+      <c r="D62" s="76"/>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="67"/>
+      <c r="C63" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="77" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="A59:C59"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A58:C58"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:C52">
-    <cfRule type="cellIs" dxfId="65" priority="3" operator="equal">
-      <formula>"Not Completed"</formula>
+  <conditionalFormatting sqref="C8:C55">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="2" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:C55">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="1.04" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="68" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="68" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="68" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="78" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="68"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75">
+      <c r="A1" s="197" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
+      <c r="A2" s="198" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="198"/>
+      <c r="C2" s="198"/>
+      <c r="D2" s="198"/>
+      <c r="E2" s="198"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75">
+      <c r="A3" s="198" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="198"/>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="198"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="134" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="106" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="106" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="106" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="107" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A5" s="134">
+        <v>1</v>
+      </c>
+      <c r="B5" s="108" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" s="133"/>
+    </row>
+    <row r="6" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A6" s="134">
+        <v>2</v>
+      </c>
+      <c r="B6" s="108" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="133"/>
+    </row>
+    <row r="7" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A7" s="134">
+        <v>3</v>
+      </c>
+      <c r="B7" s="108" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="133"/>
+    </row>
+    <row r="8" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A8" s="134">
+        <v>4</v>
+      </c>
+      <c r="B8" s="109" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E8" s="133"/>
+    </row>
+    <row r="9" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A9" s="134">
+        <v>5</v>
+      </c>
+      <c r="B9" s="108" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" s="133"/>
+    </row>
+    <row r="10" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A10" s="134">
+        <v>6</v>
+      </c>
+      <c r="B10" s="108" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="133"/>
+    </row>
+    <row r="11" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A11" s="134">
+        <v>7</v>
+      </c>
+      <c r="B11" s="108" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" s="133"/>
+    </row>
+    <row r="12" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A12" s="134">
+        <v>8</v>
+      </c>
+      <c r="B12" s="108" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="133"/>
+    </row>
+    <row r="13" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A13" s="134">
+        <v>9</v>
+      </c>
+      <c r="B13" s="108" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" s="133"/>
+    </row>
+    <row r="14" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A14" s="134">
+        <v>10</v>
+      </c>
+      <c r="B14" s="108" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="133"/>
+    </row>
+    <row r="15" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A15" s="134">
+        <v>11</v>
+      </c>
+      <c r="B15" s="108" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" s="133"/>
+    </row>
+    <row r="16" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A16" s="134">
+        <v>12</v>
+      </c>
+      <c r="B16" s="108" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E16" s="133"/>
+    </row>
+    <row r="17" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A17" s="134">
+        <v>13</v>
+      </c>
+      <c r="B17" s="108" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E17" s="133"/>
+    </row>
+    <row r="18" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A18" s="134">
+        <v>14</v>
+      </c>
+      <c r="B18" s="110" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="133"/>
+    </row>
+    <row r="19" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A19" s="134">
+        <v>15</v>
+      </c>
+      <c r="B19" s="110" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="133"/>
+    </row>
+    <row r="20" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A20" s="134">
+        <v>16</v>
+      </c>
+      <c r="B20" s="108" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D20" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E20" s="133"/>
+    </row>
+    <row r="21" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A21" s="134">
+        <v>17</v>
+      </c>
+      <c r="B21" s="108" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E21" s="133"/>
+    </row>
+    <row r="22" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A22" s="134">
+        <v>18</v>
+      </c>
+      <c r="B22" s="108" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E22" s="133"/>
+    </row>
+    <row r="23" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A23" s="134">
+        <v>19</v>
+      </c>
+      <c r="B23" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E23" s="133"/>
+    </row>
+    <row r="24" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A24" s="134">
+        <v>20</v>
+      </c>
+      <c r="B24" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" s="136" t="s">
+        <v>174</v>
+      </c>
+      <c r="E24" s="133"/>
+    </row>
+    <row r="25" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A25" s="134">
+        <v>21</v>
+      </c>
+      <c r="B25" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E25" s="133"/>
+    </row>
+    <row r="26" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A26" s="134">
+        <v>22</v>
+      </c>
+      <c r="B26" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="D26" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E26" s="133"/>
+    </row>
+    <row r="27" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A27" s="134">
+        <v>23</v>
+      </c>
+      <c r="B27" s="111" t="s">
+        <v>178</v>
+      </c>
+      <c r="C27" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="D27" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E27" s="133"/>
+    </row>
+    <row r="28" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A28" s="134">
+        <v>24</v>
+      </c>
+      <c r="B28" s="112" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E28" s="133"/>
+    </row>
+    <row r="29" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A29" s="134">
+        <v>25</v>
+      </c>
+      <c r="B29" s="110" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E29" s="133"/>
+    </row>
+    <row r="30" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A30" s="134">
+        <v>26</v>
+      </c>
+      <c r="B30" s="108" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" s="136" t="s">
+        <v>174</v>
+      </c>
+      <c r="E30" s="133"/>
+    </row>
+    <row r="31" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A31" s="134">
+        <v>27</v>
+      </c>
+      <c r="B31" s="112" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E31" s="133"/>
+    </row>
+    <row r="32" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A32" s="134">
+        <v>28</v>
+      </c>
+      <c r="B32" s="108" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" s="136" t="s">
+        <v>174</v>
+      </c>
+      <c r="E32" s="133"/>
+    </row>
+    <row r="33" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A33" s="134">
+        <v>29</v>
+      </c>
+      <c r="B33" s="110" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="135" t="s">
+        <v>171</v>
+      </c>
+      <c r="D33" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E33" s="133" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A34" s="134">
+        <v>30</v>
+      </c>
+      <c r="B34" s="108" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="135" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E34" s="133" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A35" s="134">
+        <v>31</v>
+      </c>
+      <c r="B35" s="110" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="135" t="s">
+        <v>171</v>
+      </c>
+      <c r="D35" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E35" s="133" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A36" s="134">
+        <v>32</v>
+      </c>
+      <c r="B36" s="108" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="D36" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E36" s="133"/>
+    </row>
+    <row r="37" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A37" s="134">
+        <v>33</v>
+      </c>
+      <c r="B37" s="108" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" s="135" t="s">
+        <v>171</v>
+      </c>
+      <c r="D37" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" s="133" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A38" s="134">
+        <v>34</v>
+      </c>
+      <c r="B38" s="108" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D38" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E38" s="133"/>
+    </row>
+    <row r="39" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A39" s="134">
+        <v>35</v>
+      </c>
+      <c r="B39" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="135" t="s">
+        <v>171</v>
+      </c>
+      <c r="D39" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E39" s="133" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A40" s="134">
+        <v>36</v>
+      </c>
+      <c r="B40" s="108" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" s="135" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="133" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A41" s="134">
+        <v>37</v>
+      </c>
+      <c r="B41" s="110" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D41" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E41" s="133"/>
+    </row>
+    <row r="42" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A42" s="134">
+        <v>38</v>
+      </c>
+      <c r="B42" s="108" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D42" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E42" s="133"/>
+    </row>
+    <row r="43" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A43" s="134">
+        <v>39</v>
+      </c>
+      <c r="B43" s="112" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="135" t="s">
+        <v>171</v>
+      </c>
+      <c r="D43" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E43" s="133" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A44" s="134">
+        <v>40</v>
+      </c>
+      <c r="B44" s="108" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E44" s="133"/>
+    </row>
+    <row r="45" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A45" s="134">
+        <v>41</v>
+      </c>
+      <c r="B45" s="108" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D45" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E45" s="133"/>
+    </row>
+    <row r="46" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A46" s="134">
+        <v>42</v>
+      </c>
+      <c r="B46" s="108" t="s">
+        <v>157</v>
+      </c>
+      <c r="C46" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D46" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E46" s="133"/>
+    </row>
+    <row r="47" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A47" s="134">
+        <v>43</v>
+      </c>
+      <c r="B47" s="110" t="s">
+        <v>158</v>
+      </c>
+      <c r="C47" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D47" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E47" s="133"/>
+    </row>
+    <row r="48" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A48" s="134">
+        <v>44</v>
+      </c>
+      <c r="B48" s="110" t="s">
+        <v>159</v>
+      </c>
+      <c r="C48" s="135" t="s">
+        <v>171</v>
+      </c>
+      <c r="D48" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E48" s="133" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A49" s="134">
+        <v>45</v>
+      </c>
+      <c r="B49" s="108" t="s">
+        <v>160</v>
+      </c>
+      <c r="C49" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E49" s="133"/>
+    </row>
+    <row r="50" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A50" s="134">
+        <v>46</v>
+      </c>
+      <c r="B50" s="108" t="s">
+        <v>161</v>
+      </c>
+      <c r="C50" s="135" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E50" s="133"/>
+    </row>
+    <row r="51" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A51" s="134">
+        <v>47</v>
+      </c>
+      <c r="B51" s="108" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="D51" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E51" s="133"/>
+    </row>
+    <row r="52" spans="1:5" s="82" customFormat="1" ht="15.75">
+      <c r="A52" s="134">
+        <v>48</v>
+      </c>
+      <c r="B52" s="108" t="s">
+        <v>163</v>
+      </c>
+      <c r="C52" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="D52" s="136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="133"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5:D52">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"Not Submitted"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
-      <formula>"Not Submitted"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Not Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="1.04" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>